<commit_message>
Bien avancé dans le TreeView.
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA3ADEC-1C3F-4737-8179-6AA34E897140}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D426E95-9E1B-4CA1-857B-AD12987933E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="98">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -25579,8 +25579,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="AO22" sqref="AO22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="AU38" sqref="AU38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25588,7 +25588,7 @@
     <col min="1" max="1" width="5" style="3" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="7" width="2.85546875" customWidth="1"/>
     <col min="8" max="8" width="2.28515625" customWidth="1"/>
@@ -29951,6 +29951,9 @@
       <c r="AD23" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AE23" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="AI23" s="71" t="s">
         <v>28</v>
       </c>
@@ -30276,7 +30279,7 @@
       <c r="Q25" s="5"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="20"/>
-      <c r="AE25" s="3" t="s">
+      <c r="AF25" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AJ25" s="71" t="s">
@@ -30603,6 +30606,9 @@
       <c r="Q27" s="5"/>
       <c r="Z27" s="18"/>
       <c r="AA27" s="20"/>
+      <c r="AG27" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="AK27" s="71" t="s">
         <v>28</v>
       </c>
@@ -31604,7 +31610,12 @@
       <c r="Q33" s="5"/>
       <c r="Z33" s="18"/>
       <c r="AA33" s="20"/>
-      <c r="AJ33" s="18"/>
+      <c r="AI33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ33" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="AK33" s="20"/>
       <c r="AU33" s="20"/>
       <c r="AV33" s="71" t="s">
@@ -32268,6 +32279,9 @@
       <c r="Q37" s="5"/>
       <c r="Z37" s="18"/>
       <c r="AA37" s="20"/>
+      <c r="AH37" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="AJ37" s="18"/>
       <c r="AK37" s="20"/>
       <c r="AT37" s="18"/>

</xml_diff>

<commit_message>
Gestion de plusieurs adresses ip sur le pc du professeur.
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D426E95-9E1B-4CA1-857B-AD12987933E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7443D554-B7DB-421F-8B6C-44C1CC9BD90C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,9 +184,6 @@
     <t>Informations supplémentaires avec les miniatures</t>
   </si>
   <si>
-    <t>Zoom dans le Treeview</t>
-  </si>
-  <si>
     <t>Affichage ou non des branches du Treeview</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>[L3] Historique</t>
+  </si>
+  <si>
+    <t>Zoom dans les captures d'écrans</t>
   </si>
 </sst>
 </file>
@@ -916,43 +916,70 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -961,10 +988,7 @@
     <xf numFmtId="14" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -973,41 +997,8 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,53 +1021,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -25579,8 +25579,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="AU38" sqref="AU38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25626,11 +25626,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="Q3" s="109">
+      <c r="Q3" s="106">
         <f>MAX(K13:K163)</f>
         <v>64</v>
       </c>
-      <c r="R3" s="110"/>
+      <c r="R3" s="107"/>
       <c r="S3" s="28" t="s">
         <v>23</v>
       </c>
@@ -25655,11 +25655,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="Q4" s="111">
+      <c r="Q4" s="108">
         <f>MAX(L13:L163)-L12</f>
         <v>13</v>
       </c>
-      <c r="R4" s="112"/>
+      <c r="R4" s="109"/>
       <c r="S4" s="29" t="s">
         <v>24</v>
       </c>
@@ -25676,31 +25676,31 @@
       <c r="AD4" s="26"/>
       <c r="AE4" s="27"/>
       <c r="AI4" s="66"/>
-      <c r="AJ4" s="115" t="s">
+      <c r="AJ4" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="AK4" s="115"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="115"/>
-      <c r="AN4" s="115"/>
-      <c r="AO4" s="115"/>
-      <c r="AP4" s="115"/>
-      <c r="AQ4" s="115"/>
-      <c r="AR4" s="115"/>
+      <c r="AK4" s="112"/>
+      <c r="AL4" s="112"/>
+      <c r="AM4" s="112"/>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="115" t="s">
+      <c r="AU4" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="AV4" s="115"/>
-      <c r="AW4" s="115"/>
-      <c r="AX4" s="115"/>
-      <c r="AY4" s="115"/>
-      <c r="AZ4" s="115"/>
-      <c r="BA4" s="115"/>
-      <c r="BB4" s="115"/>
-      <c r="BC4" s="115"/>
-      <c r="BD4" s="115"/>
-      <c r="BE4" s="115"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112"/>
+      <c r="AZ4" s="112"/>
+      <c r="BA4" s="112"/>
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="112"/>
       <c r="BG4" s="8"/>
       <c r="BH4" s="3" t="s">
         <v>2</v>
@@ -25712,11 +25712,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="Q5" s="113">
+      <c r="Q5" s="110">
         <f>MAX(M13:M163)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="114"/>
+      <c r="R5" s="111"/>
       <c r="S5" s="30" t="s">
         <v>25</v>
       </c>
@@ -25733,31 +25733,31 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="12"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="115" t="s">
+      <c r="AJ5" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="115"/>
-      <c r="AM5" s="115"/>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
+      <c r="AK5" s="112"/>
+      <c r="AL5" s="112"/>
+      <c r="AM5" s="112"/>
+      <c r="AN5" s="112"/>
+      <c r="AO5" s="112"/>
+      <c r="AP5" s="112"/>
+      <c r="AQ5" s="112"/>
+      <c r="AR5" s="112"/>
       <c r="AT5" s="65"/>
-      <c r="AU5" s="115" t="s">
+      <c r="AU5" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="115"/>
-      <c r="BA5" s="115"/>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
+      <c r="AV5" s="112"/>
+      <c r="AW5" s="112"/>
+      <c r="AX5" s="112"/>
+      <c r="AY5" s="112"/>
+      <c r="AZ5" s="112"/>
+      <c r="BA5" s="112"/>
+      <c r="BB5" s="112"/>
+      <c r="BC5" s="112"/>
+      <c r="BD5" s="112"/>
+      <c r="BE5" s="112"/>
     </row>
     <row r="6" spans="1:226" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -25768,889 +25768,889 @@
     </row>
     <row r="7" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B7" s="69"/>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="105" t="s">
+      <c r="H7" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="105"/>
-      <c r="J7" s="102" t="s">
+      <c r="I7" s="89"/>
+      <c r="J7" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="129" t="s">
+      <c r="K7" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="124" t="s">
+      <c r="M7" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="124" t="s">
+      <c r="N7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="124" t="s">
+      <c r="O7" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="121" t="s">
+      <c r="P7" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="120">
+      <c r="Q7" s="92">
         <v>1</v>
       </c>
-      <c r="R7" s="88"/>
-      <c r="S7" s="88"/>
-      <c r="T7" s="88"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="88"/>
-      <c r="W7" s="88"/>
-      <c r="X7" s="88"/>
-      <c r="Y7" s="88"/>
-      <c r="Z7" s="98"/>
-      <c r="AA7" s="87">
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="93"/>
+      <c r="V7" s="93"/>
+      <c r="W7" s="93"/>
+      <c r="X7" s="93"/>
+      <c r="Y7" s="93"/>
+      <c r="Z7" s="94"/>
+      <c r="AA7" s="105">
         <v>2</v>
       </c>
-      <c r="AB7" s="88"/>
-      <c r="AC7" s="88"/>
-      <c r="AD7" s="88"/>
-      <c r="AE7" s="88"/>
-      <c r="AF7" s="88"/>
-      <c r="AG7" s="88"/>
-      <c r="AH7" s="88"/>
-      <c r="AI7" s="88"/>
-      <c r="AJ7" s="98"/>
-      <c r="AK7" s="87">
+      <c r="AB7" s="93"/>
+      <c r="AC7" s="93"/>
+      <c r="AD7" s="93"/>
+      <c r="AE7" s="93"/>
+      <c r="AF7" s="93"/>
+      <c r="AG7" s="93"/>
+      <c r="AH7" s="93"/>
+      <c r="AI7" s="93"/>
+      <c r="AJ7" s="94"/>
+      <c r="AK7" s="105">
         <v>3</v>
       </c>
-      <c r="AL7" s="88"/>
-      <c r="AM7" s="88"/>
-      <c r="AN7" s="88"/>
-      <c r="AO7" s="88"/>
-      <c r="AP7" s="88"/>
-      <c r="AQ7" s="88"/>
-      <c r="AR7" s="88"/>
-      <c r="AS7" s="88"/>
-      <c r="AT7" s="98"/>
-      <c r="AU7" s="87">
+      <c r="AL7" s="93"/>
+      <c r="AM7" s="93"/>
+      <c r="AN7" s="93"/>
+      <c r="AO7" s="93"/>
+      <c r="AP7" s="93"/>
+      <c r="AQ7" s="93"/>
+      <c r="AR7" s="93"/>
+      <c r="AS7" s="93"/>
+      <c r="AT7" s="94"/>
+      <c r="AU7" s="105">
         <v>4</v>
       </c>
-      <c r="AV7" s="88"/>
-      <c r="AW7" s="88"/>
-      <c r="AX7" s="88"/>
-      <c r="AY7" s="88"/>
-      <c r="AZ7" s="88"/>
-      <c r="BA7" s="88"/>
-      <c r="BB7" s="88"/>
-      <c r="BC7" s="88"/>
-      <c r="BD7" s="98"/>
-      <c r="BE7" s="87">
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="93"/>
+      <c r="AX7" s="93"/>
+      <c r="AY7" s="93"/>
+      <c r="AZ7" s="93"/>
+      <c r="BA7" s="93"/>
+      <c r="BB7" s="93"/>
+      <c r="BC7" s="93"/>
+      <c r="BD7" s="94"/>
+      <c r="BE7" s="105">
         <v>5</v>
       </c>
-      <c r="BF7" s="88"/>
-      <c r="BG7" s="88"/>
-      <c r="BH7" s="88"/>
-      <c r="BI7" s="88"/>
-      <c r="BJ7" s="88"/>
-      <c r="BK7" s="88"/>
-      <c r="BL7" s="88"/>
-      <c r="BM7" s="88"/>
-      <c r="BN7" s="98"/>
-      <c r="BO7" s="87">
+      <c r="BF7" s="93"/>
+      <c r="BG7" s="93"/>
+      <c r="BH7" s="93"/>
+      <c r="BI7" s="93"/>
+      <c r="BJ7" s="93"/>
+      <c r="BK7" s="93"/>
+      <c r="BL7" s="93"/>
+      <c r="BM7" s="93"/>
+      <c r="BN7" s="94"/>
+      <c r="BO7" s="105">
         <v>6</v>
       </c>
-      <c r="BP7" s="88"/>
-      <c r="BQ7" s="88"/>
-      <c r="BR7" s="88"/>
-      <c r="BS7" s="88"/>
-      <c r="BT7" s="88"/>
-      <c r="BU7" s="88"/>
-      <c r="BV7" s="88"/>
-      <c r="BW7" s="88"/>
-      <c r="BX7" s="98"/>
-      <c r="BY7" s="87">
+      <c r="BP7" s="93"/>
+      <c r="BQ7" s="93"/>
+      <c r="BR7" s="93"/>
+      <c r="BS7" s="93"/>
+      <c r="BT7" s="93"/>
+      <c r="BU7" s="93"/>
+      <c r="BV7" s="93"/>
+      <c r="BW7" s="93"/>
+      <c r="BX7" s="94"/>
+      <c r="BY7" s="105">
         <v>7</v>
       </c>
-      <c r="BZ7" s="88"/>
-      <c r="CA7" s="88"/>
-      <c r="CB7" s="88"/>
-      <c r="CC7" s="88"/>
-      <c r="CD7" s="88"/>
-      <c r="CE7" s="88"/>
-      <c r="CF7" s="88"/>
-      <c r="CG7" s="88"/>
-      <c r="CH7" s="98"/>
-      <c r="CI7" s="87">
+      <c r="BZ7" s="93"/>
+      <c r="CA7" s="93"/>
+      <c r="CB7" s="93"/>
+      <c r="CC7" s="93"/>
+      <c r="CD7" s="93"/>
+      <c r="CE7" s="93"/>
+      <c r="CF7" s="93"/>
+      <c r="CG7" s="93"/>
+      <c r="CH7" s="94"/>
+      <c r="CI7" s="105">
         <v>8</v>
       </c>
-      <c r="CJ7" s="88"/>
-      <c r="CK7" s="88"/>
-      <c r="CL7" s="88"/>
-      <c r="CM7" s="88"/>
-      <c r="CN7" s="88"/>
-      <c r="CO7" s="88"/>
-      <c r="CP7" s="88"/>
-      <c r="CQ7" s="88"/>
-      <c r="CR7" s="98"/>
-      <c r="CS7" s="87">
+      <c r="CJ7" s="93"/>
+      <c r="CK7" s="93"/>
+      <c r="CL7" s="93"/>
+      <c r="CM7" s="93"/>
+      <c r="CN7" s="93"/>
+      <c r="CO7" s="93"/>
+      <c r="CP7" s="93"/>
+      <c r="CQ7" s="93"/>
+      <c r="CR7" s="94"/>
+      <c r="CS7" s="105">
         <v>9</v>
       </c>
-      <c r="CT7" s="88"/>
-      <c r="CU7" s="88"/>
-      <c r="CV7" s="88"/>
-      <c r="CW7" s="88"/>
-      <c r="CX7" s="88"/>
-      <c r="CY7" s="88"/>
-      <c r="CZ7" s="88"/>
-      <c r="DA7" s="88"/>
-      <c r="DB7" s="88"/>
-      <c r="DC7" s="87">
+      <c r="CT7" s="93"/>
+      <c r="CU7" s="93"/>
+      <c r="CV7" s="93"/>
+      <c r="CW7" s="93"/>
+      <c r="CX7" s="93"/>
+      <c r="CY7" s="93"/>
+      <c r="CZ7" s="93"/>
+      <c r="DA7" s="93"/>
+      <c r="DB7" s="93"/>
+      <c r="DC7" s="105">
         <v>10</v>
       </c>
-      <c r="DD7" s="88"/>
-      <c r="DE7" s="88"/>
-      <c r="DF7" s="88"/>
-      <c r="DG7" s="88"/>
-      <c r="DH7" s="88"/>
-      <c r="DI7" s="88"/>
-      <c r="DJ7" s="88"/>
-      <c r="DK7" s="88"/>
-      <c r="DL7" s="98"/>
-      <c r="DM7" s="87">
+      <c r="DD7" s="93"/>
+      <c r="DE7" s="93"/>
+      <c r="DF7" s="93"/>
+      <c r="DG7" s="93"/>
+      <c r="DH7" s="93"/>
+      <c r="DI7" s="93"/>
+      <c r="DJ7" s="93"/>
+      <c r="DK7" s="93"/>
+      <c r="DL7" s="94"/>
+      <c r="DM7" s="105">
         <v>11</v>
       </c>
-      <c r="DN7" s="88"/>
-      <c r="DO7" s="88"/>
-      <c r="DP7" s="88"/>
-      <c r="DQ7" s="88"/>
-      <c r="DR7" s="88"/>
-      <c r="DS7" s="88"/>
-      <c r="DT7" s="88"/>
-      <c r="DU7" s="88"/>
-      <c r="DV7" s="98"/>
-      <c r="DW7" s="87">
+      <c r="DN7" s="93"/>
+      <c r="DO7" s="93"/>
+      <c r="DP7" s="93"/>
+      <c r="DQ7" s="93"/>
+      <c r="DR7" s="93"/>
+      <c r="DS7" s="93"/>
+      <c r="DT7" s="93"/>
+      <c r="DU7" s="93"/>
+      <c r="DV7" s="94"/>
+      <c r="DW7" s="105">
         <v>12</v>
       </c>
-      <c r="DX7" s="88"/>
-      <c r="DY7" s="88"/>
-      <c r="DZ7" s="88"/>
-      <c r="EA7" s="88"/>
-      <c r="EB7" s="88"/>
-      <c r="EC7" s="88"/>
-      <c r="ED7" s="88"/>
-      <c r="EE7" s="88"/>
-      <c r="EF7" s="98"/>
-      <c r="EG7" s="87">
+      <c r="DX7" s="93"/>
+      <c r="DY7" s="93"/>
+      <c r="DZ7" s="93"/>
+      <c r="EA7" s="93"/>
+      <c r="EB7" s="93"/>
+      <c r="EC7" s="93"/>
+      <c r="ED7" s="93"/>
+      <c r="EE7" s="93"/>
+      <c r="EF7" s="94"/>
+      <c r="EG7" s="105">
         <v>13</v>
       </c>
-      <c r="EH7" s="88"/>
-      <c r="EI7" s="88"/>
-      <c r="EJ7" s="88"/>
-      <c r="EK7" s="88"/>
-      <c r="EL7" s="88"/>
-      <c r="EM7" s="88"/>
-      <c r="EN7" s="88"/>
-      <c r="EO7" s="88"/>
-      <c r="EP7" s="89"/>
-      <c r="EQ7" s="88">
+      <c r="EH7" s="93"/>
+      <c r="EI7" s="93"/>
+      <c r="EJ7" s="93"/>
+      <c r="EK7" s="93"/>
+      <c r="EL7" s="93"/>
+      <c r="EM7" s="93"/>
+      <c r="EN7" s="93"/>
+      <c r="EO7" s="93"/>
+      <c r="EP7" s="123"/>
+      <c r="EQ7" s="93">
         <v>14</v>
       </c>
-      <c r="ER7" s="88"/>
-      <c r="ES7" s="88"/>
-      <c r="ET7" s="88"/>
-      <c r="EU7" s="88"/>
-      <c r="EV7" s="88"/>
-      <c r="EW7" s="88"/>
-      <c r="EX7" s="88"/>
-      <c r="EY7" s="88"/>
-      <c r="EZ7" s="98"/>
-      <c r="FA7" s="87">
+      <c r="ER7" s="93"/>
+      <c r="ES7" s="93"/>
+      <c r="ET7" s="93"/>
+      <c r="EU7" s="93"/>
+      <c r="EV7" s="93"/>
+      <c r="EW7" s="93"/>
+      <c r="EX7" s="93"/>
+      <c r="EY7" s="93"/>
+      <c r="EZ7" s="94"/>
+      <c r="FA7" s="105">
         <v>15</v>
       </c>
-      <c r="FB7" s="88"/>
-      <c r="FC7" s="88"/>
-      <c r="FD7" s="88"/>
-      <c r="FE7" s="88"/>
-      <c r="FF7" s="88"/>
-      <c r="FG7" s="88"/>
-      <c r="FH7" s="88"/>
-      <c r="FI7" s="88"/>
-      <c r="FJ7" s="98"/>
-      <c r="FK7" s="87">
+      <c r="FB7" s="93"/>
+      <c r="FC7" s="93"/>
+      <c r="FD7" s="93"/>
+      <c r="FE7" s="93"/>
+      <c r="FF7" s="93"/>
+      <c r="FG7" s="93"/>
+      <c r="FH7" s="93"/>
+      <c r="FI7" s="93"/>
+      <c r="FJ7" s="94"/>
+      <c r="FK7" s="105">
         <v>16</v>
       </c>
-      <c r="FL7" s="88"/>
-      <c r="FM7" s="88"/>
-      <c r="FN7" s="88"/>
-      <c r="FO7" s="88"/>
-      <c r="FP7" s="88"/>
-      <c r="FQ7" s="88"/>
-      <c r="FR7" s="88"/>
-      <c r="FS7" s="88"/>
-      <c r="FT7" s="98"/>
-      <c r="FU7" s="87">
+      <c r="FL7" s="93"/>
+      <c r="FM7" s="93"/>
+      <c r="FN7" s="93"/>
+      <c r="FO7" s="93"/>
+      <c r="FP7" s="93"/>
+      <c r="FQ7" s="93"/>
+      <c r="FR7" s="93"/>
+      <c r="FS7" s="93"/>
+      <c r="FT7" s="94"/>
+      <c r="FU7" s="105">
         <v>17</v>
       </c>
-      <c r="FV7" s="88"/>
-      <c r="FW7" s="88"/>
-      <c r="FX7" s="88"/>
-      <c r="FY7" s="88"/>
-      <c r="FZ7" s="88"/>
-      <c r="GA7" s="88"/>
-      <c r="GB7" s="88"/>
-      <c r="GC7" s="88"/>
-      <c r="GD7" s="98"/>
-      <c r="GE7" s="87">
+      <c r="FV7" s="93"/>
+      <c r="FW7" s="93"/>
+      <c r="FX7" s="93"/>
+      <c r="FY7" s="93"/>
+      <c r="FZ7" s="93"/>
+      <c r="GA7" s="93"/>
+      <c r="GB7" s="93"/>
+      <c r="GC7" s="93"/>
+      <c r="GD7" s="94"/>
+      <c r="GE7" s="105">
         <v>18</v>
       </c>
-      <c r="GF7" s="88"/>
-      <c r="GG7" s="88"/>
-      <c r="GH7" s="88"/>
-      <c r="GI7" s="88"/>
-      <c r="GJ7" s="88"/>
-      <c r="GK7" s="88"/>
-      <c r="GL7" s="88"/>
-      <c r="GM7" s="88"/>
-      <c r="GN7" s="98"/>
-      <c r="GO7" s="87">
+      <c r="GF7" s="93"/>
+      <c r="GG7" s="93"/>
+      <c r="GH7" s="93"/>
+      <c r="GI7" s="93"/>
+      <c r="GJ7" s="93"/>
+      <c r="GK7" s="93"/>
+      <c r="GL7" s="93"/>
+      <c r="GM7" s="93"/>
+      <c r="GN7" s="94"/>
+      <c r="GO7" s="105">
         <v>19</v>
       </c>
-      <c r="GP7" s="88"/>
-      <c r="GQ7" s="88"/>
-      <c r="GR7" s="88"/>
-      <c r="GS7" s="88"/>
-      <c r="GT7" s="88"/>
-      <c r="GU7" s="88"/>
-      <c r="GV7" s="88"/>
-      <c r="GW7" s="88"/>
-      <c r="GX7" s="98"/>
-      <c r="GY7" s="87">
+      <c r="GP7" s="93"/>
+      <c r="GQ7" s="93"/>
+      <c r="GR7" s="93"/>
+      <c r="GS7" s="93"/>
+      <c r="GT7" s="93"/>
+      <c r="GU7" s="93"/>
+      <c r="GV7" s="93"/>
+      <c r="GW7" s="93"/>
+      <c r="GX7" s="94"/>
+      <c r="GY7" s="105">
         <v>20</v>
       </c>
-      <c r="GZ7" s="88"/>
-      <c r="HA7" s="88"/>
-      <c r="HB7" s="88"/>
-      <c r="HC7" s="88"/>
-      <c r="HD7" s="88"/>
-      <c r="HE7" s="88"/>
-      <c r="HF7" s="88"/>
-      <c r="HG7" s="88"/>
-      <c r="HH7" s="98"/>
-      <c r="HI7" s="87">
+      <c r="GZ7" s="93"/>
+      <c r="HA7" s="93"/>
+      <c r="HB7" s="93"/>
+      <c r="HC7" s="93"/>
+      <c r="HD7" s="93"/>
+      <c r="HE7" s="93"/>
+      <c r="HF7" s="93"/>
+      <c r="HG7" s="93"/>
+      <c r="HH7" s="94"/>
+      <c r="HI7" s="105">
         <v>21</v>
       </c>
-      <c r="HJ7" s="88"/>
-      <c r="HK7" s="88"/>
-      <c r="HL7" s="88"/>
-      <c r="HM7" s="88"/>
-      <c r="HN7" s="88"/>
-      <c r="HO7" s="88"/>
-      <c r="HP7" s="88"/>
-      <c r="HQ7" s="88"/>
-      <c r="HR7" s="89"/>
+      <c r="HJ7" s="93"/>
+      <c r="HK7" s="93"/>
+      <c r="HL7" s="93"/>
+      <c r="HM7" s="93"/>
+      <c r="HN7" s="93"/>
+      <c r="HO7" s="93"/>
+      <c r="HP7" s="93"/>
+      <c r="HQ7" s="93"/>
+      <c r="HR7" s="123"/>
     </row>
     <row r="8" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="130"/>
-      <c r="L8" s="125"/>
-      <c r="M8" s="125"/>
-      <c r="N8" s="125"/>
-      <c r="O8" s="125"/>
-      <c r="P8" s="122"/>
-      <c r="Q8" s="127">
+      <c r="D8" s="121"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="117"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="99">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],Q7),"")</f>
         <v>45041</v>
       </c>
-      <c r="R8" s="91"/>
-      <c r="S8" s="91"/>
-      <c r="T8" s="91"/>
-      <c r="U8" s="91"/>
-      <c r="V8" s="91"/>
-      <c r="W8" s="91"/>
-      <c r="X8" s="91"/>
-      <c r="Y8" s="91"/>
-      <c r="Z8" s="92"/>
-      <c r="AA8" s="90">
+      <c r="R8" s="100"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="100"/>
+      <c r="V8" s="100"/>
+      <c r="W8" s="100"/>
+      <c r="X8" s="100"/>
+      <c r="Y8" s="100"/>
+      <c r="Z8" s="101"/>
+      <c r="AA8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AA7),"")</f>
         <v>45042</v>
       </c>
-      <c r="AB8" s="91"/>
-      <c r="AC8" s="91"/>
-      <c r="AD8" s="91"/>
-      <c r="AE8" s="91"/>
-      <c r="AF8" s="91"/>
-      <c r="AG8" s="91"/>
-      <c r="AH8" s="91"/>
-      <c r="AI8" s="91"/>
-      <c r="AJ8" s="92"/>
-      <c r="AK8" s="90">
+      <c r="AB8" s="100"/>
+      <c r="AC8" s="100"/>
+      <c r="AD8" s="100"/>
+      <c r="AE8" s="100"/>
+      <c r="AF8" s="100"/>
+      <c r="AG8" s="100"/>
+      <c r="AH8" s="100"/>
+      <c r="AI8" s="100"/>
+      <c r="AJ8" s="101"/>
+      <c r="AK8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AK7),"")</f>
         <v>45043</v>
       </c>
-      <c r="AL8" s="91"/>
-      <c r="AM8" s="91"/>
-      <c r="AN8" s="91"/>
-      <c r="AO8" s="91"/>
-      <c r="AP8" s="91"/>
-      <c r="AQ8" s="91"/>
-      <c r="AR8" s="91"/>
-      <c r="AS8" s="91"/>
-      <c r="AT8" s="92"/>
-      <c r="AU8" s="90">
+      <c r="AL8" s="100"/>
+      <c r="AM8" s="100"/>
+      <c r="AN8" s="100"/>
+      <c r="AO8" s="100"/>
+      <c r="AP8" s="100"/>
+      <c r="AQ8" s="100"/>
+      <c r="AR8" s="100"/>
+      <c r="AS8" s="100"/>
+      <c r="AT8" s="101"/>
+      <c r="AU8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AU7),"")</f>
         <v>45049</v>
       </c>
-      <c r="AV8" s="91"/>
-      <c r="AW8" s="91"/>
-      <c r="AX8" s="91"/>
-      <c r="AY8" s="91"/>
-      <c r="AZ8" s="91"/>
-      <c r="BA8" s="91"/>
-      <c r="BB8" s="91"/>
-      <c r="BC8" s="91"/>
-      <c r="BD8" s="92"/>
-      <c r="BE8" s="90">
+      <c r="AV8" s="100"/>
+      <c r="AW8" s="100"/>
+      <c r="AX8" s="100"/>
+      <c r="AY8" s="100"/>
+      <c r="AZ8" s="100"/>
+      <c r="BA8" s="100"/>
+      <c r="BB8" s="100"/>
+      <c r="BC8" s="100"/>
+      <c r="BD8" s="101"/>
+      <c r="BE8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BE7),"")</f>
         <v>45050</v>
       </c>
-      <c r="BF8" s="91"/>
-      <c r="BG8" s="91"/>
-      <c r="BH8" s="91"/>
-      <c r="BI8" s="91"/>
-      <c r="BJ8" s="91"/>
-      <c r="BK8" s="91"/>
-      <c r="BL8" s="91"/>
-      <c r="BM8" s="91"/>
-      <c r="BN8" s="92"/>
-      <c r="BO8" s="90">
+      <c r="BF8" s="100"/>
+      <c r="BG8" s="100"/>
+      <c r="BH8" s="100"/>
+      <c r="BI8" s="100"/>
+      <c r="BJ8" s="100"/>
+      <c r="BK8" s="100"/>
+      <c r="BL8" s="100"/>
+      <c r="BM8" s="100"/>
+      <c r="BN8" s="101"/>
+      <c r="BO8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BO7),"")</f>
         <v>45055</v>
       </c>
-      <c r="BP8" s="91"/>
-      <c r="BQ8" s="91"/>
-      <c r="BR8" s="91"/>
-      <c r="BS8" s="91"/>
-      <c r="BT8" s="91"/>
-      <c r="BU8" s="91"/>
-      <c r="BV8" s="91"/>
-      <c r="BW8" s="91"/>
-      <c r="BX8" s="92"/>
-      <c r="BY8" s="90">
+      <c r="BP8" s="100"/>
+      <c r="BQ8" s="100"/>
+      <c r="BR8" s="100"/>
+      <c r="BS8" s="100"/>
+      <c r="BT8" s="100"/>
+      <c r="BU8" s="100"/>
+      <c r="BV8" s="100"/>
+      <c r="BW8" s="100"/>
+      <c r="BX8" s="101"/>
+      <c r="BY8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BY7),"")</f>
         <v>45056</v>
       </c>
-      <c r="BZ8" s="91"/>
-      <c r="CA8" s="91"/>
-      <c r="CB8" s="91"/>
-      <c r="CC8" s="91"/>
-      <c r="CD8" s="91"/>
-      <c r="CE8" s="91"/>
-      <c r="CF8" s="91"/>
-      <c r="CG8" s="91"/>
-      <c r="CH8" s="92"/>
-      <c r="CI8" s="90">
+      <c r="BZ8" s="100"/>
+      <c r="CA8" s="100"/>
+      <c r="CB8" s="100"/>
+      <c r="CC8" s="100"/>
+      <c r="CD8" s="100"/>
+      <c r="CE8" s="100"/>
+      <c r="CF8" s="100"/>
+      <c r="CG8" s="100"/>
+      <c r="CH8" s="101"/>
+      <c r="CI8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CI7),"")</f>
         <v>45057</v>
       </c>
-      <c r="CJ8" s="91"/>
-      <c r="CK8" s="91"/>
-      <c r="CL8" s="91"/>
-      <c r="CM8" s="91"/>
-      <c r="CN8" s="91"/>
-      <c r="CO8" s="91"/>
-      <c r="CP8" s="91"/>
-      <c r="CQ8" s="91"/>
-      <c r="CR8" s="92"/>
-      <c r="CS8" s="90">
+      <c r="CJ8" s="100"/>
+      <c r="CK8" s="100"/>
+      <c r="CL8" s="100"/>
+      <c r="CM8" s="100"/>
+      <c r="CN8" s="100"/>
+      <c r="CO8" s="100"/>
+      <c r="CP8" s="100"/>
+      <c r="CQ8" s="100"/>
+      <c r="CR8" s="101"/>
+      <c r="CS8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CS7),"")</f>
         <v>45062</v>
       </c>
-      <c r="CT8" s="91"/>
-      <c r="CU8" s="91"/>
-      <c r="CV8" s="91"/>
-      <c r="CW8" s="91"/>
-      <c r="CX8" s="91"/>
-      <c r="CY8" s="91"/>
-      <c r="CZ8" s="91"/>
-      <c r="DA8" s="91"/>
-      <c r="DB8" s="91"/>
-      <c r="DC8" s="90">
+      <c r="CT8" s="100"/>
+      <c r="CU8" s="100"/>
+      <c r="CV8" s="100"/>
+      <c r="CW8" s="100"/>
+      <c r="CX8" s="100"/>
+      <c r="CY8" s="100"/>
+      <c r="CZ8" s="100"/>
+      <c r="DA8" s="100"/>
+      <c r="DB8" s="100"/>
+      <c r="DC8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DC7),"")</f>
         <v>45063</v>
       </c>
-      <c r="DD8" s="91"/>
-      <c r="DE8" s="91"/>
-      <c r="DF8" s="91"/>
-      <c r="DG8" s="91"/>
-      <c r="DH8" s="91"/>
-      <c r="DI8" s="91"/>
-      <c r="DJ8" s="91"/>
-      <c r="DK8" s="91"/>
-      <c r="DL8" s="92"/>
-      <c r="DM8" s="90">
+      <c r="DD8" s="100"/>
+      <c r="DE8" s="100"/>
+      <c r="DF8" s="100"/>
+      <c r="DG8" s="100"/>
+      <c r="DH8" s="100"/>
+      <c r="DI8" s="100"/>
+      <c r="DJ8" s="100"/>
+      <c r="DK8" s="100"/>
+      <c r="DL8" s="101"/>
+      <c r="DM8" s="114">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DM7),"")</f>
         <v>45064</v>
       </c>
-      <c r="DN8" s="91"/>
-      <c r="DO8" s="91"/>
-      <c r="DP8" s="91"/>
-      <c r="DQ8" s="91"/>
-      <c r="DR8" s="91"/>
-      <c r="DS8" s="91"/>
-      <c r="DT8" s="91"/>
-      <c r="DU8" s="91"/>
-      <c r="DV8" s="92"/>
-      <c r="DW8" s="90" t="str">
+      <c r="DN8" s="100"/>
+      <c r="DO8" s="100"/>
+      <c r="DP8" s="100"/>
+      <c r="DQ8" s="100"/>
+      <c r="DR8" s="100"/>
+      <c r="DS8" s="100"/>
+      <c r="DT8" s="100"/>
+      <c r="DU8" s="100"/>
+      <c r="DV8" s="101"/>
+      <c r="DW8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DW7),"")</f>
         <v/>
       </c>
-      <c r="DX8" s="91"/>
-      <c r="DY8" s="91"/>
-      <c r="DZ8" s="91"/>
-      <c r="EA8" s="91"/>
-      <c r="EB8" s="91"/>
-      <c r="EC8" s="91"/>
-      <c r="ED8" s="91"/>
-      <c r="EE8" s="91"/>
-      <c r="EF8" s="92"/>
-      <c r="EG8" s="90" t="str">
+      <c r="DX8" s="100"/>
+      <c r="DY8" s="100"/>
+      <c r="DZ8" s="100"/>
+      <c r="EA8" s="100"/>
+      <c r="EB8" s="100"/>
+      <c r="EC8" s="100"/>
+      <c r="ED8" s="100"/>
+      <c r="EE8" s="100"/>
+      <c r="EF8" s="101"/>
+      <c r="EG8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EG7),"")</f>
         <v/>
       </c>
-      <c r="EH8" s="91"/>
-      <c r="EI8" s="91"/>
-      <c r="EJ8" s="91"/>
-      <c r="EK8" s="91"/>
-      <c r="EL8" s="91"/>
-      <c r="EM8" s="91"/>
-      <c r="EN8" s="91"/>
-      <c r="EO8" s="91"/>
-      <c r="EP8" s="93"/>
-      <c r="EQ8" s="91" t="str">
+      <c r="EH8" s="100"/>
+      <c r="EI8" s="100"/>
+      <c r="EJ8" s="100"/>
+      <c r="EK8" s="100"/>
+      <c r="EL8" s="100"/>
+      <c r="EM8" s="100"/>
+      <c r="EN8" s="100"/>
+      <c r="EO8" s="100"/>
+      <c r="EP8" s="115"/>
+      <c r="EQ8" s="100" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EQ7),"")</f>
         <v/>
       </c>
-      <c r="ER8" s="91"/>
-      <c r="ES8" s="91"/>
-      <c r="ET8" s="91"/>
-      <c r="EU8" s="91"/>
-      <c r="EV8" s="91"/>
-      <c r="EW8" s="91"/>
-      <c r="EX8" s="91"/>
-      <c r="EY8" s="91"/>
-      <c r="EZ8" s="92"/>
-      <c r="FA8" s="90" t="str">
+      <c r="ER8" s="100"/>
+      <c r="ES8" s="100"/>
+      <c r="ET8" s="100"/>
+      <c r="EU8" s="100"/>
+      <c r="EV8" s="100"/>
+      <c r="EW8" s="100"/>
+      <c r="EX8" s="100"/>
+      <c r="EY8" s="100"/>
+      <c r="EZ8" s="101"/>
+      <c r="FA8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FA7),"")</f>
         <v/>
       </c>
-      <c r="FB8" s="91"/>
-      <c r="FC8" s="91"/>
-      <c r="FD8" s="91"/>
-      <c r="FE8" s="91"/>
-      <c r="FF8" s="91"/>
-      <c r="FG8" s="91"/>
-      <c r="FH8" s="91"/>
-      <c r="FI8" s="91"/>
-      <c r="FJ8" s="92"/>
-      <c r="FK8" s="90" t="str">
+      <c r="FB8" s="100"/>
+      <c r="FC8" s="100"/>
+      <c r="FD8" s="100"/>
+      <c r="FE8" s="100"/>
+      <c r="FF8" s="100"/>
+      <c r="FG8" s="100"/>
+      <c r="FH8" s="100"/>
+      <c r="FI8" s="100"/>
+      <c r="FJ8" s="101"/>
+      <c r="FK8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FK7),"")</f>
         <v/>
       </c>
-      <c r="FL8" s="91"/>
-      <c r="FM8" s="91"/>
-      <c r="FN8" s="91"/>
-      <c r="FO8" s="91"/>
-      <c r="FP8" s="91"/>
-      <c r="FQ8" s="91"/>
-      <c r="FR8" s="91"/>
-      <c r="FS8" s="91"/>
-      <c r="FT8" s="92"/>
-      <c r="FU8" s="90" t="str">
+      <c r="FL8" s="100"/>
+      <c r="FM8" s="100"/>
+      <c r="FN8" s="100"/>
+      <c r="FO8" s="100"/>
+      <c r="FP8" s="100"/>
+      <c r="FQ8" s="100"/>
+      <c r="FR8" s="100"/>
+      <c r="FS8" s="100"/>
+      <c r="FT8" s="101"/>
+      <c r="FU8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FU7),"")</f>
         <v/>
       </c>
-      <c r="FV8" s="91"/>
-      <c r="FW8" s="91"/>
-      <c r="FX8" s="91"/>
-      <c r="FY8" s="91"/>
-      <c r="FZ8" s="91"/>
-      <c r="GA8" s="91"/>
-      <c r="GB8" s="91"/>
-      <c r="GC8" s="91"/>
-      <c r="GD8" s="92"/>
-      <c r="GE8" s="90" t="str">
+      <c r="FV8" s="100"/>
+      <c r="FW8" s="100"/>
+      <c r="FX8" s="100"/>
+      <c r="FY8" s="100"/>
+      <c r="FZ8" s="100"/>
+      <c r="GA8" s="100"/>
+      <c r="GB8" s="100"/>
+      <c r="GC8" s="100"/>
+      <c r="GD8" s="101"/>
+      <c r="GE8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GE7),"")</f>
         <v/>
       </c>
-      <c r="GF8" s="91"/>
-      <c r="GG8" s="91"/>
-      <c r="GH8" s="91"/>
-      <c r="GI8" s="91"/>
-      <c r="GJ8" s="91"/>
-      <c r="GK8" s="91"/>
-      <c r="GL8" s="91"/>
-      <c r="GM8" s="91"/>
-      <c r="GN8" s="92"/>
-      <c r="GO8" s="90" t="str">
+      <c r="GF8" s="100"/>
+      <c r="GG8" s="100"/>
+      <c r="GH8" s="100"/>
+      <c r="GI8" s="100"/>
+      <c r="GJ8" s="100"/>
+      <c r="GK8" s="100"/>
+      <c r="GL8" s="100"/>
+      <c r="GM8" s="100"/>
+      <c r="GN8" s="101"/>
+      <c r="GO8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GO7),"")</f>
         <v/>
       </c>
-      <c r="GP8" s="91"/>
-      <c r="GQ8" s="91"/>
-      <c r="GR8" s="91"/>
-      <c r="GS8" s="91"/>
-      <c r="GT8" s="91"/>
-      <c r="GU8" s="91"/>
-      <c r="GV8" s="91"/>
-      <c r="GW8" s="91"/>
-      <c r="GX8" s="92"/>
-      <c r="GY8" s="90" t="str">
+      <c r="GP8" s="100"/>
+      <c r="GQ8" s="100"/>
+      <c r="GR8" s="100"/>
+      <c r="GS8" s="100"/>
+      <c r="GT8" s="100"/>
+      <c r="GU8" s="100"/>
+      <c r="GV8" s="100"/>
+      <c r="GW8" s="100"/>
+      <c r="GX8" s="101"/>
+      <c r="GY8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GY7),"")</f>
         <v/>
       </c>
-      <c r="GZ8" s="91"/>
-      <c r="HA8" s="91"/>
-      <c r="HB8" s="91"/>
-      <c r="HC8" s="91"/>
-      <c r="HD8" s="91"/>
-      <c r="HE8" s="91"/>
-      <c r="HF8" s="91"/>
-      <c r="HG8" s="91"/>
-      <c r="HH8" s="92"/>
-      <c r="HI8" s="90" t="str">
+      <c r="GZ8" s="100"/>
+      <c r="HA8" s="100"/>
+      <c r="HB8" s="100"/>
+      <c r="HC8" s="100"/>
+      <c r="HD8" s="100"/>
+      <c r="HE8" s="100"/>
+      <c r="HF8" s="100"/>
+      <c r="HG8" s="100"/>
+      <c r="HH8" s="101"/>
+      <c r="HI8" s="114" t="str">
         <f ca="1">IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],HI7),"")</f>
         <v/>
       </c>
-      <c r="HJ8" s="91"/>
-      <c r="HK8" s="91"/>
-      <c r="HL8" s="91"/>
-      <c r="HM8" s="91"/>
-      <c r="HN8" s="91"/>
-      <c r="HO8" s="91"/>
-      <c r="HP8" s="91"/>
-      <c r="HQ8" s="91"/>
-      <c r="HR8" s="93"/>
+      <c r="HJ8" s="100"/>
+      <c r="HK8" s="100"/>
+      <c r="HL8" s="100"/>
+      <c r="HM8" s="100"/>
+      <c r="HN8" s="100"/>
+      <c r="HO8" s="100"/>
+      <c r="HP8" s="100"/>
+      <c r="HQ8" s="100"/>
+      <c r="HR8" s="115"/>
     </row>
     <row r="9" spans="1:226" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="125"/>
-      <c r="M9" s="125"/>
-      <c r="N9" s="125"/>
-      <c r="O9" s="125"/>
-      <c r="P9" s="122"/>
-      <c r="Q9" s="128">
+      <c r="D9" s="121"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="117"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="102">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(Q8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="R9" s="95"/>
-      <c r="S9" s="95"/>
-      <c r="T9" s="95"/>
-      <c r="U9" s="95"/>
-      <c r="V9" s="95"/>
-      <c r="W9" s="95"/>
-      <c r="X9" s="95"/>
-      <c r="Y9" s="95"/>
-      <c r="Z9" s="96"/>
-      <c r="AA9" s="94" t="str">
+      <c r="R9" s="103"/>
+      <c r="S9" s="103"/>
+      <c r="T9" s="103"/>
+      <c r="U9" s="103"/>
+      <c r="V9" s="103"/>
+      <c r="W9" s="103"/>
+      <c r="X9" s="103"/>
+      <c r="Y9" s="103"/>
+      <c r="Z9" s="104"/>
+      <c r="AA9" s="113" t="str">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L1] Connexion</v>
       </c>
-      <c r="AB9" s="95"/>
-      <c r="AC9" s="95"/>
-      <c r="AD9" s="95"/>
-      <c r="AE9" s="95"/>
-      <c r="AF9" s="95"/>
-      <c r="AG9" s="95"/>
-      <c r="AH9" s="95"/>
-      <c r="AI9" s="95"/>
-      <c r="AJ9" s="96"/>
-      <c r="AK9" s="94">
+      <c r="AB9" s="103"/>
+      <c r="AC9" s="103"/>
+      <c r="AD9" s="103"/>
+      <c r="AE9" s="103"/>
+      <c r="AF9" s="103"/>
+      <c r="AG9" s="103"/>
+      <c r="AH9" s="103"/>
+      <c r="AI9" s="103"/>
+      <c r="AJ9" s="104"/>
+      <c r="AK9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="95"/>
-      <c r="AM9" s="95"/>
-      <c r="AN9" s="95"/>
-      <c r="AO9" s="95"/>
-      <c r="AP9" s="95"/>
-      <c r="AQ9" s="95"/>
-      <c r="AR9" s="95"/>
-      <c r="AS9" s="95"/>
-      <c r="AT9" s="96"/>
-      <c r="AU9" s="94" t="str">
+      <c r="AL9" s="103"/>
+      <c r="AM9" s="103"/>
+      <c r="AN9" s="103"/>
+      <c r="AO9" s="103"/>
+      <c r="AP9" s="103"/>
+      <c r="AQ9" s="103"/>
+      <c r="AR9" s="103"/>
+      <c r="AS9" s="103"/>
+      <c r="AT9" s="104"/>
+      <c r="AU9" s="113" t="str">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L2] Affichage Professeur</v>
       </c>
-      <c r="AV9" s="95"/>
-      <c r="AW9" s="95"/>
-      <c r="AX9" s="95"/>
-      <c r="AY9" s="95"/>
-      <c r="AZ9" s="95"/>
-      <c r="BA9" s="95"/>
-      <c r="BB9" s="95"/>
-      <c r="BC9" s="95"/>
-      <c r="BD9" s="96"/>
-      <c r="BE9" s="94">
+      <c r="AV9" s="103"/>
+      <c r="AW9" s="103"/>
+      <c r="AX9" s="103"/>
+      <c r="AY9" s="103"/>
+      <c r="AZ9" s="103"/>
+      <c r="BA9" s="103"/>
+      <c r="BB9" s="103"/>
+      <c r="BC9" s="103"/>
+      <c r="BD9" s="104"/>
+      <c r="BE9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BF9" s="95"/>
-      <c r="BG9" s="95"/>
-      <c r="BH9" s="95"/>
-      <c r="BI9" s="95"/>
-      <c r="BJ9" s="95"/>
-      <c r="BK9" s="95"/>
-      <c r="BL9" s="95"/>
-      <c r="BM9" s="95"/>
-      <c r="BN9" s="96"/>
-      <c r="BO9" s="94" t="str">
+      <c r="BF9" s="103"/>
+      <c r="BG9" s="103"/>
+      <c r="BH9" s="103"/>
+      <c r="BI9" s="103"/>
+      <c r="BJ9" s="103"/>
+      <c r="BK9" s="103"/>
+      <c r="BL9" s="103"/>
+      <c r="BM9" s="103"/>
+      <c r="BN9" s="104"/>
+      <c r="BO9" s="113" t="str">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L3] Historique</v>
       </c>
-      <c r="BP9" s="95"/>
-      <c r="BQ9" s="95"/>
-      <c r="BR9" s="95"/>
-      <c r="BS9" s="95"/>
-      <c r="BT9" s="95"/>
-      <c r="BU9" s="95"/>
-      <c r="BV9" s="95"/>
-      <c r="BW9" s="95"/>
-      <c r="BX9" s="96"/>
-      <c r="BY9" s="94">
+      <c r="BP9" s="103"/>
+      <c r="BQ9" s="103"/>
+      <c r="BR9" s="103"/>
+      <c r="BS9" s="103"/>
+      <c r="BT9" s="103"/>
+      <c r="BU9" s="103"/>
+      <c r="BV9" s="103"/>
+      <c r="BW9" s="103"/>
+      <c r="BX9" s="104"/>
+      <c r="BY9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BZ9" s="95"/>
-      <c r="CA9" s="95"/>
-      <c r="CB9" s="95"/>
-      <c r="CC9" s="95"/>
-      <c r="CD9" s="95"/>
-      <c r="CE9" s="95"/>
-      <c r="CF9" s="95"/>
-      <c r="CG9" s="95"/>
-      <c r="CH9" s="96"/>
-      <c r="CI9" s="94" t="str">
+      <c r="BZ9" s="103"/>
+      <c r="CA9" s="103"/>
+      <c r="CB9" s="103"/>
+      <c r="CC9" s="103"/>
+      <c r="CD9" s="103"/>
+      <c r="CE9" s="103"/>
+      <c r="CF9" s="103"/>
+      <c r="CG9" s="103"/>
+      <c r="CH9" s="104"/>
+      <c r="CI9" s="113" t="str">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L4] Filtrage</v>
       </c>
-      <c r="CJ9" s="95"/>
-      <c r="CK9" s="95"/>
-      <c r="CL9" s="95"/>
-      <c r="CM9" s="95"/>
-      <c r="CN9" s="95"/>
-      <c r="CO9" s="95"/>
-      <c r="CP9" s="95"/>
-      <c r="CQ9" s="95"/>
-      <c r="CR9" s="96"/>
-      <c r="CS9" s="94" t="str">
+      <c r="CJ9" s="103"/>
+      <c r="CK9" s="103"/>
+      <c r="CL9" s="103"/>
+      <c r="CM9" s="103"/>
+      <c r="CN9" s="103"/>
+      <c r="CO9" s="103"/>
+      <c r="CP9" s="103"/>
+      <c r="CQ9" s="103"/>
+      <c r="CR9" s="104"/>
+      <c r="CS9" s="113" t="str">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CS8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L5] Streaming multicast</v>
       </c>
-      <c r="CT9" s="95"/>
-      <c r="CU9" s="95"/>
-      <c r="CV9" s="95"/>
-      <c r="CW9" s="95"/>
-      <c r="CX9" s="95"/>
-      <c r="CY9" s="95"/>
-      <c r="CZ9" s="95"/>
-      <c r="DA9" s="95"/>
-      <c r="DB9" s="95"/>
-      <c r="DC9" s="94">
+      <c r="CT9" s="103"/>
+      <c r="CU9" s="103"/>
+      <c r="CV9" s="103"/>
+      <c r="CW9" s="103"/>
+      <c r="CX9" s="103"/>
+      <c r="CY9" s="103"/>
+      <c r="CZ9" s="103"/>
+      <c r="DA9" s="103"/>
+      <c r="DB9" s="103"/>
+      <c r="DC9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DC8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DD9" s="95"/>
-      <c r="DE9" s="95"/>
-      <c r="DF9" s="95"/>
-      <c r="DG9" s="95"/>
-      <c r="DH9" s="95"/>
-      <c r="DI9" s="95"/>
-      <c r="DJ9" s="95"/>
-      <c r="DK9" s="95"/>
-      <c r="DL9" s="96"/>
-      <c r="DM9" s="94" t="str">
+      <c r="DD9" s="103"/>
+      <c r="DE9" s="103"/>
+      <c r="DF9" s="103"/>
+      <c r="DG9" s="103"/>
+      <c r="DH9" s="103"/>
+      <c r="DI9" s="103"/>
+      <c r="DJ9" s="103"/>
+      <c r="DK9" s="103"/>
+      <c r="DL9" s="104"/>
+      <c r="DM9" s="113" t="str">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DM8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L6] Contrôle à distance</v>
       </c>
-      <c r="DN9" s="95"/>
-      <c r="DO9" s="95"/>
-      <c r="DP9" s="95"/>
-      <c r="DQ9" s="95"/>
-      <c r="DR9" s="95"/>
-      <c r="DS9" s="95"/>
-      <c r="DT9" s="95"/>
-      <c r="DU9" s="95"/>
-      <c r="DV9" s="96"/>
-      <c r="DW9" s="94">
+      <c r="DN9" s="103"/>
+      <c r="DO9" s="103"/>
+      <c r="DP9" s="103"/>
+      <c r="DQ9" s="103"/>
+      <c r="DR9" s="103"/>
+      <c r="DS9" s="103"/>
+      <c r="DT9" s="103"/>
+      <c r="DU9" s="103"/>
+      <c r="DV9" s="104"/>
+      <c r="DW9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DW8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DX9" s="95"/>
-      <c r="DY9" s="95"/>
-      <c r="DZ9" s="95"/>
-      <c r="EA9" s="95"/>
-      <c r="EB9" s="95"/>
-      <c r="EC9" s="95"/>
-      <c r="ED9" s="95"/>
-      <c r="EE9" s="95"/>
-      <c r="EF9" s="96"/>
-      <c r="EG9" s="94">
+      <c r="DX9" s="103"/>
+      <c r="DY9" s="103"/>
+      <c r="DZ9" s="103"/>
+      <c r="EA9" s="103"/>
+      <c r="EB9" s="103"/>
+      <c r="EC9" s="103"/>
+      <c r="ED9" s="103"/>
+      <c r="EE9" s="103"/>
+      <c r="EF9" s="104"/>
+      <c r="EG9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EG8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="EH9" s="95"/>
-      <c r="EI9" s="95"/>
-      <c r="EJ9" s="95"/>
-      <c r="EK9" s="95"/>
-      <c r="EL9" s="95"/>
-      <c r="EM9" s="95"/>
-      <c r="EN9" s="95"/>
-      <c r="EO9" s="95"/>
-      <c r="EP9" s="97"/>
-      <c r="EQ9" s="95">
+      <c r="EH9" s="103"/>
+      <c r="EI9" s="103"/>
+      <c r="EJ9" s="103"/>
+      <c r="EK9" s="103"/>
+      <c r="EL9" s="103"/>
+      <c r="EM9" s="103"/>
+      <c r="EN9" s="103"/>
+      <c r="EO9" s="103"/>
+      <c r="EP9" s="119"/>
+      <c r="EQ9" s="103">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EQ8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="ER9" s="95"/>
-      <c r="ES9" s="95"/>
-      <c r="ET9" s="95"/>
-      <c r="EU9" s="95"/>
-      <c r="EV9" s="95"/>
-      <c r="EW9" s="95"/>
-      <c r="EX9" s="95"/>
-      <c r="EY9" s="95"/>
-      <c r="EZ9" s="96"/>
-      <c r="FA9" s="94">
+      <c r="ER9" s="103"/>
+      <c r="ES9" s="103"/>
+      <c r="ET9" s="103"/>
+      <c r="EU9" s="103"/>
+      <c r="EV9" s="103"/>
+      <c r="EW9" s="103"/>
+      <c r="EX9" s="103"/>
+      <c r="EY9" s="103"/>
+      <c r="EZ9" s="104"/>
+      <c r="FA9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FB9" s="95"/>
-      <c r="FC9" s="95"/>
-      <c r="FD9" s="95"/>
-      <c r="FE9" s="95"/>
-      <c r="FF9" s="95"/>
-      <c r="FG9" s="95"/>
-      <c r="FH9" s="95"/>
-      <c r="FI9" s="95"/>
-      <c r="FJ9" s="96"/>
-      <c r="FK9" s="94">
+      <c r="FB9" s="103"/>
+      <c r="FC9" s="103"/>
+      <c r="FD9" s="103"/>
+      <c r="FE9" s="103"/>
+      <c r="FF9" s="103"/>
+      <c r="FG9" s="103"/>
+      <c r="FH9" s="103"/>
+      <c r="FI9" s="103"/>
+      <c r="FJ9" s="104"/>
+      <c r="FK9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FL9" s="95"/>
-      <c r="FM9" s="95"/>
-      <c r="FN9" s="95"/>
-      <c r="FO9" s="95"/>
-      <c r="FP9" s="95"/>
-      <c r="FQ9" s="95"/>
-      <c r="FR9" s="95"/>
-      <c r="FS9" s="95"/>
-      <c r="FT9" s="96"/>
-      <c r="FU9" s="94">
+      <c r="FL9" s="103"/>
+      <c r="FM9" s="103"/>
+      <c r="FN9" s="103"/>
+      <c r="FO9" s="103"/>
+      <c r="FP9" s="103"/>
+      <c r="FQ9" s="103"/>
+      <c r="FR9" s="103"/>
+      <c r="FS9" s="103"/>
+      <c r="FT9" s="104"/>
+      <c r="FU9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FV9" s="95"/>
-      <c r="FW9" s="95"/>
-      <c r="FX9" s="95"/>
-      <c r="FY9" s="95"/>
-      <c r="FZ9" s="95"/>
-      <c r="GA9" s="95"/>
-      <c r="GB9" s="95"/>
-      <c r="GC9" s="95"/>
-      <c r="GD9" s="96"/>
-      <c r="GE9" s="94">
+      <c r="FV9" s="103"/>
+      <c r="FW9" s="103"/>
+      <c r="FX9" s="103"/>
+      <c r="FY9" s="103"/>
+      <c r="FZ9" s="103"/>
+      <c r="GA9" s="103"/>
+      <c r="GB9" s="103"/>
+      <c r="GC9" s="103"/>
+      <c r="GD9" s="104"/>
+      <c r="GE9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GF9" s="95"/>
-      <c r="GG9" s="95"/>
-      <c r="GH9" s="95"/>
-      <c r="GI9" s="95"/>
-      <c r="GJ9" s="95"/>
-      <c r="GK9" s="95"/>
-      <c r="GL9" s="95"/>
-      <c r="GM9" s="95"/>
-      <c r="GN9" s="96"/>
-      <c r="GO9" s="94">
+      <c r="GF9" s="103"/>
+      <c r="GG9" s="103"/>
+      <c r="GH9" s="103"/>
+      <c r="GI9" s="103"/>
+      <c r="GJ9" s="103"/>
+      <c r="GK9" s="103"/>
+      <c r="GL9" s="103"/>
+      <c r="GM9" s="103"/>
+      <c r="GN9" s="104"/>
+      <c r="GO9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GP9" s="95"/>
-      <c r="GQ9" s="95"/>
-      <c r="GR9" s="95"/>
-      <c r="GS9" s="95"/>
-      <c r="GT9" s="95"/>
-      <c r="GU9" s="95"/>
-      <c r="GV9" s="95"/>
-      <c r="GW9" s="95"/>
-      <c r="GX9" s="96"/>
-      <c r="GY9" s="94">
+      <c r="GP9" s="103"/>
+      <c r="GQ9" s="103"/>
+      <c r="GR9" s="103"/>
+      <c r="GS9" s="103"/>
+      <c r="GT9" s="103"/>
+      <c r="GU9" s="103"/>
+      <c r="GV9" s="103"/>
+      <c r="GW9" s="103"/>
+      <c r="GX9" s="104"/>
+      <c r="GY9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GZ9" s="95"/>
-      <c r="HA9" s="95"/>
-      <c r="HB9" s="95"/>
-      <c r="HC9" s="95"/>
-      <c r="HD9" s="95"/>
-      <c r="HE9" s="95"/>
-      <c r="HF9" s="95"/>
-      <c r="HG9" s="95"/>
-      <c r="HH9" s="96"/>
-      <c r="HI9" s="94">
+      <c r="GZ9" s="103"/>
+      <c r="HA9" s="103"/>
+      <c r="HB9" s="103"/>
+      <c r="HC9" s="103"/>
+      <c r="HD9" s="103"/>
+      <c r="HE9" s="103"/>
+      <c r="HF9" s="103"/>
+      <c r="HG9" s="103"/>
+      <c r="HH9" s="104"/>
+      <c r="HI9" s="113">
         <f ca="1">INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(HI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="HJ9" s="95"/>
-      <c r="HK9" s="95"/>
-      <c r="HL9" s="95"/>
-      <c r="HM9" s="95"/>
-      <c r="HN9" s="95"/>
-      <c r="HO9" s="95"/>
-      <c r="HP9" s="95"/>
-      <c r="HQ9" s="95"/>
-      <c r="HR9" s="97"/>
+      <c r="HJ9" s="103"/>
+      <c r="HK9" s="103"/>
+      <c r="HL9" s="103"/>
+      <c r="HM9" s="103"/>
+      <c r="HN9" s="103"/>
+      <c r="HO9" s="103"/>
+      <c r="HP9" s="103"/>
+      <c r="HQ9" s="103"/>
+      <c r="HR9" s="119"/>
     </row>
     <row r="10" spans="1:226" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="130"/>
-      <c r="L10" s="125"/>
-      <c r="M10" s="125"/>
-      <c r="N10" s="125"/>
-      <c r="O10" s="125"/>
-      <c r="P10" s="122"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="117"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="96"/>
       <c r="Q10" s="5"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="20"/>
@@ -26696,19 +26696,19 @@
       <c r="A11" s="68"/>
       <c r="B11" s="5"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="126"/>
-      <c r="M11" s="126"/>
-      <c r="N11" s="126"/>
-      <c r="O11" s="126"/>
-      <c r="P11" s="123"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="97"/>
       <c r="Q11" s="51">
         <v>0</v>
       </c>
@@ -28132,7 +28132,7 @@
         <v>0</v>
       </c>
       <c r="HA12" s="33">
-        <f t="shared" ref="HA12:JL12" si="3">IF(COUNTIF(HA13:HA163,"r")&gt;0,COUNTIF(HA13:HA163,"r")-1,0)</f>
+        <f t="shared" ref="HA12:HR12" si="3">IF(COUNTIF(HA13:HA163,"r")&gt;0,COUNTIF(HA13:HA163,"r")-1,0)</f>
         <v>0</v>
       </c>
       <c r="HB12" s="33">
@@ -28205,15 +28205,15 @@
       </c>
     </row>
     <row r="13" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="108" t="s">
+      <c r="D13" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="80"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82" t="str">
+      <c r="E13" s="98"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="116" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
       </c>
@@ -28319,11 +28319,11 @@
       <c r="HR13" s="4"/>
     </row>
     <row r="14" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="78"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="80"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="82"/>
+      <c r="B14" s="131"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="98"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="116"/>
       <c r="I14" s="45" t="s">
         <v>1</v>
       </c>
@@ -28575,20 +28575,20 @@
       <c r="HR14" s="31"/>
     </row>
     <row r="15" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="108" t="s">
+      <c r="D15" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="80">
+      <c r="F15" s="98">
         <v>1</v>
       </c>
-      <c r="G15" s="81"/>
-      <c r="H15" s="82" t="str">
+      <c r="G15" s="84"/>
+      <c r="H15" s="116" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
       </c>
@@ -28659,12 +28659,12 @@
       <c r="HR15" s="4"/>
     </row>
     <row r="16" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="78"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="82"/>
+      <c r="B16" s="131"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="116"/>
       <c r="I16" s="45" t="s">
         <v>1</v>
       </c>
@@ -28904,18 +28904,18 @@
       <c r="HR16" s="31"/>
     </row>
     <row r="17" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80">
+      <c r="E17" s="98"/>
+      <c r="F17" s="98">
         <v>1</v>
       </c>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82" t="str">
+      <c r="G17" s="84"/>
+      <c r="H17" s="116" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
       </c>
@@ -28987,12 +28987,12 @@
       <c r="HR17" s="4"/>
     </row>
     <row r="18" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="78"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="82"/>
+      <c r="B18" s="131"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="116"/>
       <c r="I18" s="45" t="s">
         <v>1</v>
       </c>
@@ -29234,20 +29234,20 @@
       <c r="HR18" s="31"/>
     </row>
     <row r="19" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="108" t="s">
+      <c r="D19" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="E19" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="80">
+      <c r="F19" s="98">
         <v>1</v>
       </c>
-      <c r="G19" s="81"/>
-      <c r="H19" s="82" t="str">
+      <c r="G19" s="84"/>
+      <c r="H19" s="116" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
       </c>
@@ -29331,12 +29331,12 @@
       <c r="HR19" s="4"/>
     </row>
     <row r="20" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="78"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="82"/>
+      <c r="B20" s="131"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="116"/>
       <c r="I20" s="45" t="s">
         <v>1</v>
       </c>
@@ -29580,18 +29580,18 @@
       <c r="HR20" s="31"/>
     </row>
     <row r="21" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="108" t="s">
+      <c r="D21" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80">
+      <c r="E21" s="98"/>
+      <c r="F21" s="98">
         <v>1</v>
       </c>
-      <c r="G21" s="81"/>
-      <c r="H21" s="82" t="str">
+      <c r="G21" s="84"/>
+      <c r="H21" s="116" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
       </c>
@@ -29665,12 +29665,12 @@
       <c r="HR21" s="4"/>
     </row>
     <row r="22" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="78"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="82"/>
+      <c r="B22" s="131"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="116"/>
       <c r="I22" s="45" t="s">
         <v>1</v>
       </c>
@@ -29908,18 +29908,18 @@
       <c r="HR22" s="31"/>
     </row>
     <row r="23" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="78" t="s">
+      <c r="B23" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="108" t="s">
+      <c r="D23" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80">
+      <c r="E23" s="98"/>
+      <c r="F23" s="98">
         <v>1</v>
       </c>
-      <c r="G23" s="81"/>
-      <c r="H23" s="82" t="str">
+      <c r="G23" s="84"/>
+      <c r="H23" s="116" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
       </c>
@@ -29996,12 +29996,12 @@
       <c r="HR23" s="4"/>
     </row>
     <row r="24" spans="2:226" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="78"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="82"/>
+      <c r="B24" s="131"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="116"/>
       <c r="I24" s="45" t="s">
         <v>1</v>
       </c>
@@ -30239,18 +30239,18 @@
       <c r="HR24" s="31"/>
     </row>
     <row r="25" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="78" t="s">
+      <c r="B25" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="108" t="s">
+      <c r="D25" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80">
+      <c r="E25" s="98"/>
+      <c r="F25" s="98">
         <v>1</v>
       </c>
-      <c r="G25" s="81"/>
-      <c r="H25" s="82" t="str">
+      <c r="G25" s="84"/>
+      <c r="H25" s="116" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
       </c>
@@ -30323,12 +30323,12 @@
       <c r="HR25" s="4"/>
     </row>
     <row r="26" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="78"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="82"/>
+      <c r="B26" s="131"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="116"/>
       <c r="I26" s="45" t="s">
         <v>1</v>
       </c>
@@ -30566,18 +30566,18 @@
       <c r="HR26" s="31"/>
     </row>
     <row r="27" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="108" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80">
+      <c r="D27" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98">
         <v>2</v>
       </c>
-      <c r="G27" s="81"/>
-      <c r="H27" s="82" t="str">
+      <c r="G27" s="84"/>
+      <c r="H27" s="116" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
       </c>
@@ -30661,12 +30661,12 @@
       <c r="HR27" s="4"/>
     </row>
     <row r="28" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="78"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="82"/>
+      <c r="B28" s="131"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="116"/>
       <c r="I28" s="45" t="s">
         <v>1</v>
       </c>
@@ -30904,20 +30904,20 @@
       <c r="HR28" s="31"/>
     </row>
     <row r="29" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="108" t="s">
+      <c r="D29" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="80" t="s">
+      <c r="E29" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="80">
+      <c r="F29" s="98">
         <v>2</v>
       </c>
-      <c r="G29" s="81"/>
-      <c r="H29" s="82" t="str">
+      <c r="G29" s="84"/>
+      <c r="H29" s="116" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v/>
       </c>
@@ -30946,7 +30946,9 @@
       <c r="Q29" s="5"/>
       <c r="Z29" s="18"/>
       <c r="AA29" s="20"/>
-      <c r="AJ29" s="18"/>
+      <c r="AJ29" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="AK29" s="20"/>
       <c r="AP29" s="71" t="s">
         <v>28</v>
@@ -30997,12 +30999,12 @@
       <c r="HR29" s="4"/>
     </row>
     <row r="30" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="78"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="82"/>
+      <c r="B30" s="131"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="116"/>
       <c r="I30" s="45" t="s">
         <v>1</v>
       </c>
@@ -31240,20 +31242,20 @@
       <c r="HR30" s="31"/>
     </row>
     <row r="31" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="78" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="79" t="s">
+      <c r="B31" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="80" t="s">
+      <c r="E31" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="80">
+      <c r="F31" s="98">
         <v>2</v>
       </c>
-      <c r="G31" s="81"/>
-      <c r="H31" s="82" t="str">
+      <c r="G31" s="84"/>
+      <c r="H31" s="116" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
       </c>
@@ -31325,12 +31327,12 @@
       <c r="HR31" s="4"/>
     </row>
     <row r="32" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="78"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="82"/>
+      <c r="B32" s="131"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="116"/>
       <c r="I32" s="45" t="s">
         <v>1</v>
       </c>
@@ -31568,20 +31570,20 @@
       <c r="HR32" s="31"/>
     </row>
     <row r="33" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="78" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="80" t="s">
+      <c r="B33" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="118" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="80">
+      <c r="F33" s="98">
         <v>2</v>
       </c>
-      <c r="G33" s="81"/>
-      <c r="H33" s="82" t="str">
+      <c r="G33" s="84"/>
+      <c r="H33" s="116" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
       </c>
@@ -31610,12 +31612,7 @@
       <c r="Q33" s="5"/>
       <c r="Z33" s="18"/>
       <c r="AA33" s="20"/>
-      <c r="AI33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ33" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="AJ33" s="18"/>
       <c r="AK33" s="20"/>
       <c r="AU33" s="20"/>
       <c r="AV33" s="71" t="s">
@@ -31662,12 +31659,12 @@
       <c r="HR33" s="4"/>
     </row>
     <row r="34" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="78"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="82"/>
+      <c r="B34" s="131"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="116"/>
       <c r="I34" s="45" t="s">
         <v>1</v>
       </c>
@@ -31905,20 +31902,20 @@
       <c r="HR34" s="31"/>
     </row>
     <row r="35" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="78" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="80" t="s">
+      <c r="B35" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="118" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="80">
+      <c r="F35" s="98">
         <v>2</v>
       </c>
-      <c r="G35" s="81"/>
-      <c r="H35" s="82" t="str">
+      <c r="G35" s="84"/>
+      <c r="H35" s="116" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
       </c>
@@ -31947,6 +31944,9 @@
       <c r="Q35" s="5"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="20"/>
+      <c r="AI35" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="AJ35" s="18"/>
       <c r="AK35" s="20"/>
       <c r="AU35" s="20"/>
@@ -31994,12 +31994,12 @@
       <c r="HR35" s="4"/>
     </row>
     <row r="36" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="78"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="82"/>
+      <c r="B36" s="131"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="116"/>
       <c r="I36" s="45" t="s">
         <v>1</v>
       </c>
@@ -32237,20 +32237,20 @@
       <c r="HR36" s="31"/>
     </row>
     <row r="37" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="78" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="79" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="80" t="s">
+      <c r="B37" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="118" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="80">
+      <c r="F37" s="98">
         <v>2</v>
       </c>
-      <c r="G37" s="81"/>
-      <c r="H37" s="82" t="str">
+      <c r="G37" s="84"/>
+      <c r="H37" s="116" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
       </c>
@@ -32327,12 +32327,12 @@
       <c r="HR37" s="4"/>
     </row>
     <row r="38" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="78"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="82"/>
+      <c r="B38" s="131"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="116"/>
       <c r="I38" s="45" t="s">
         <v>1</v>
       </c>
@@ -32570,18 +32570,18 @@
       <c r="HR38" s="31"/>
     </row>
     <row r="39" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="79" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80">
+      <c r="B39" s="131" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="118" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98">
         <v>3</v>
       </c>
-      <c r="G39" s="81"/>
-      <c r="H39" s="82" t="str">
+      <c r="G39" s="84"/>
+      <c r="H39" s="116" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
       </c>
@@ -32662,12 +32662,12 @@
       <c r="HR39" s="4"/>
     </row>
     <row r="40" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="78"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="82"/>
+      <c r="B40" s="131"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="116"/>
       <c r="I40" s="45" t="s">
         <v>1</v>
       </c>
@@ -32905,18 +32905,18 @@
       <c r="HR40" s="31"/>
     </row>
     <row r="41" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" s="80"/>
-      <c r="F41" s="80">
+      <c r="B41" s="131" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="118" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="98"/>
+      <c r="F41" s="98">
         <v>3</v>
       </c>
-      <c r="G41" s="81"/>
-      <c r="H41" s="82" t="str">
+      <c r="G41" s="84"/>
+      <c r="H41" s="116" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
       </c>
@@ -32990,12 +32990,12 @@
       <c r="HR41" s="4"/>
     </row>
     <row r="42" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="78"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="82"/>
+      <c r="B42" s="131"/>
+      <c r="D42" s="118"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="116"/>
       <c r="I42" s="45" t="s">
         <v>1</v>
       </c>
@@ -33233,18 +33233,18 @@
       <c r="HR42" s="31"/>
     </row>
     <row r="43" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="79" t="s">
-        <v>59</v>
-      </c>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80">
+      <c r="B43" s="131" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="118" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="98"/>
+      <c r="F43" s="98">
         <v>3</v>
       </c>
-      <c r="G43" s="81"/>
-      <c r="H43" s="82" t="str">
+      <c r="G43" s="84"/>
+      <c r="H43" s="116" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
       </c>
@@ -33317,12 +33317,12 @@
       <c r="HR43" s="4"/>
     </row>
     <row r="44" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="78"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="82"/>
+      <c r="B44" s="131"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="116"/>
       <c r="I44" s="45" t="s">
         <v>1</v>
       </c>
@@ -33560,18 +33560,18 @@
       <c r="HR44" s="31"/>
     </row>
     <row r="45" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="80"/>
-      <c r="F45" s="80">
+      <c r="B45" s="131" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="118" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="98"/>
+      <c r="F45" s="98">
         <v>3</v>
       </c>
-      <c r="G45" s="81"/>
-      <c r="H45" s="82" t="str">
+      <c r="G45" s="84"/>
+      <c r="H45" s="116" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
       </c>
@@ -33644,12 +33644,12 @@
       <c r="HR45" s="4"/>
     </row>
     <row r="46" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="78"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="82"/>
+      <c r="B46" s="131"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="116"/>
       <c r="I46" s="45" t="s">
         <v>1</v>
       </c>
@@ -33887,18 +33887,18 @@
       <c r="HR46" s="31"/>
     </row>
     <row r="47" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="78" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" s="79" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80">
+      <c r="B47" s="131" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="118" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="98"/>
+      <c r="F47" s="98">
         <v>3</v>
       </c>
-      <c r="G47" s="81"/>
-      <c r="H47" s="82" t="str">
+      <c r="G47" s="84"/>
+      <c r="H47" s="116" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
       </c>
@@ -33968,12 +33968,12 @@
       <c r="HR47" s="4"/>
     </row>
     <row r="48" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="78"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="81"/>
-      <c r="H48" s="82"/>
+      <c r="B48" s="131"/>
+      <c r="D48" s="118"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="116"/>
       <c r="I48" s="45" t="s">
         <v>1</v>
       </c>
@@ -34211,18 +34211,18 @@
       <c r="HR48" s="31"/>
     </row>
     <row r="49" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="78" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="79" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="80"/>
-      <c r="F49" s="80">
+      <c r="B49" s="131" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="118" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="98"/>
+      <c r="F49" s="98">
         <v>4</v>
       </c>
-      <c r="G49" s="81"/>
-      <c r="H49" s="82" t="str">
+      <c r="G49" s="84"/>
+      <c r="H49" s="116" t="str">
         <f t="shared" ref="H49" si="65">IF(O50&gt;P49,"!","")</f>
         <v/>
       </c>
@@ -34310,12 +34310,12 @@
       <c r="HR49" s="4"/>
     </row>
     <row r="50" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="78"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="81"/>
-      <c r="H50" s="82"/>
+      <c r="B50" s="131"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="98"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="116"/>
       <c r="I50" s="45" t="s">
         <v>1</v>
       </c>
@@ -34553,18 +34553,18 @@
       <c r="HR50" s="31"/>
     </row>
     <row r="51" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="79" t="s">
-        <v>62</v>
-      </c>
-      <c r="E51" s="80"/>
-      <c r="F51" s="80">
+      <c r="B51" s="131" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="98"/>
+      <c r="F51" s="98">
         <v>4</v>
       </c>
-      <c r="G51" s="81"/>
-      <c r="H51" s="82" t="str">
+      <c r="G51" s="84"/>
+      <c r="H51" s="116" t="str">
         <f t="shared" ref="H51" si="71">IF(O52&gt;P51,"!","")</f>
         <v/>
       </c>
@@ -34641,12 +34641,12 @@
       <c r="HR51" s="4"/>
     </row>
     <row r="52" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="78"/>
-      <c r="D52" s="79"/>
-      <c r="E52" s="80"/>
-      <c r="F52" s="80"/>
-      <c r="G52" s="81"/>
-      <c r="H52" s="82"/>
+      <c r="B52" s="131"/>
+      <c r="D52" s="118"/>
+      <c r="E52" s="98"/>
+      <c r="F52" s="98"/>
+      <c r="G52" s="84"/>
+      <c r="H52" s="116"/>
       <c r="I52" s="45" t="s">
         <v>1</v>
       </c>
@@ -34884,18 +34884,18 @@
       <c r="HR52" s="31"/>
     </row>
     <row r="53" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="E53" s="80"/>
-      <c r="F53" s="80">
+      <c r="B53" s="131" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="118" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="98"/>
+      <c r="F53" s="98">
         <v>4</v>
       </c>
-      <c r="G53" s="81"/>
-      <c r="H53" s="82" t="str">
+      <c r="G53" s="84"/>
+      <c r="H53" s="116" t="str">
         <f t="shared" ref="H53" si="77">IF(O54&gt;P53,"!","")</f>
         <v/>
       </c>
@@ -34975,12 +34975,12 @@
       <c r="HR53" s="4"/>
     </row>
     <row r="54" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="78"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="80"/>
-      <c r="G54" s="81"/>
-      <c r="H54" s="82"/>
+      <c r="B54" s="131"/>
+      <c r="D54" s="118"/>
+      <c r="E54" s="98"/>
+      <c r="F54" s="98"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="116"/>
       <c r="I54" s="45" t="s">
         <v>1</v>
       </c>
@@ -35218,20 +35218,20 @@
       <c r="HR54" s="31"/>
     </row>
     <row r="55" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="D55" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="E55" s="80" t="s">
+      <c r="B55" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="F55" s="80">
+      <c r="D55" s="118" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="F55" s="98">
         <v>4</v>
       </c>
-      <c r="G55" s="81"/>
-      <c r="H55" s="82" t="str">
+      <c r="G55" s="84"/>
+      <c r="H55" s="116" t="str">
         <f t="shared" ref="H55" si="83">IF(O56&gt;P55,"!","")</f>
         <v/>
       </c>
@@ -35314,12 +35314,12 @@
       <c r="HR55" s="4"/>
     </row>
     <row r="56" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="78"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="80"/>
-      <c r="F56" s="80"/>
-      <c r="G56" s="81"/>
-      <c r="H56" s="82"/>
+      <c r="B56" s="131"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="98"/>
+      <c r="F56" s="98"/>
+      <c r="G56" s="84"/>
+      <c r="H56" s="116"/>
       <c r="I56" s="45" t="s">
         <v>1</v>
       </c>
@@ -35557,20 +35557,20 @@
       <c r="HR56" s="31"/>
     </row>
     <row r="57" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="E57" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="F57" s="80">
+      <c r="B57" s="131" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="98">
         <v>4</v>
       </c>
-      <c r="G57" s="81"/>
-      <c r="H57" s="82" t="str">
+      <c r="G57" s="84"/>
+      <c r="H57" s="116" t="str">
         <f t="shared" ref="H57" si="89">IF(O58&gt;P57,"!","")</f>
         <v/>
       </c>
@@ -35641,12 +35641,12 @@
       <c r="HR57" s="4"/>
     </row>
     <row r="58" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="78"/>
-      <c r="D58" s="79"/>
-      <c r="E58" s="80"/>
-      <c r="F58" s="80"/>
-      <c r="G58" s="81"/>
-      <c r="H58" s="82"/>
+      <c r="B58" s="131"/>
+      <c r="D58" s="118"/>
+      <c r="E58" s="98"/>
+      <c r="F58" s="98"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="116"/>
       <c r="I58" s="45" t="s">
         <v>1</v>
       </c>
@@ -35884,18 +35884,18 @@
       <c r="HR58" s="31"/>
     </row>
     <row r="59" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="D59" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="E59" s="80"/>
-      <c r="F59" s="80">
+      <c r="B59" s="131" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="118" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" s="98"/>
+      <c r="F59" s="98">
         <v>5</v>
       </c>
-      <c r="G59" s="81"/>
-      <c r="H59" s="82" t="str">
+      <c r="G59" s="84"/>
+      <c r="H59" s="116" t="str">
         <f t="shared" ref="H59" si="95">IF(O60&gt;P59,"!","")</f>
         <v/>
       </c>
@@ -35969,12 +35969,12 @@
       <c r="HR59" s="4"/>
     </row>
     <row r="60" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="78"/>
-      <c r="D60" s="79"/>
-      <c r="E60" s="80"/>
-      <c r="F60" s="80"/>
-      <c r="G60" s="81"/>
-      <c r="H60" s="82"/>
+      <c r="B60" s="131"/>
+      <c r="D60" s="118"/>
+      <c r="E60" s="98"/>
+      <c r="F60" s="98"/>
+      <c r="G60" s="84"/>
+      <c r="H60" s="116"/>
       <c r="I60" s="45" t="s">
         <v>1</v>
       </c>
@@ -36212,18 +36212,18 @@
       <c r="HR60" s="31"/>
     </row>
     <row r="61" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E61" s="80"/>
-      <c r="F61" s="80">
+      <c r="B61" s="131" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="118" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="98"/>
+      <c r="F61" s="98">
         <v>5</v>
       </c>
-      <c r="G61" s="81"/>
-      <c r="H61" s="82" t="str">
+      <c r="G61" s="84"/>
+      <c r="H61" s="116" t="str">
         <f t="shared" ref="H61" si="101">IF(O62&gt;P61,"!","")</f>
         <v/>
       </c>
@@ -36318,12 +36318,12 @@
       <c r="HR61" s="4"/>
     </row>
     <row r="62" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="78"/>
-      <c r="D62" s="79"/>
-      <c r="E62" s="80"/>
-      <c r="F62" s="80"/>
-      <c r="G62" s="81"/>
-      <c r="H62" s="82"/>
+      <c r="B62" s="131"/>
+      <c r="D62" s="118"/>
+      <c r="E62" s="98"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="116"/>
       <c r="I62" s="45" t="s">
         <v>1</v>
       </c>
@@ -36561,18 +36561,18 @@
       <c r="HR62" s="31"/>
     </row>
     <row r="63" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="E63" s="80"/>
-      <c r="F63" s="80">
+      <c r="B63" s="131" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="118" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="98"/>
+      <c r="F63" s="98">
         <v>5</v>
       </c>
-      <c r="G63" s="81"/>
-      <c r="H63" s="82" t="str">
+      <c r="G63" s="84"/>
+      <c r="H63" s="116" t="str">
         <f t="shared" ref="H63" si="107">IF(O64&gt;P63,"!","")</f>
         <v/>
       </c>
@@ -36657,12 +36657,12 @@
       <c r="HR63" s="4"/>
     </row>
     <row r="64" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="78"/>
-      <c r="D64" s="79"/>
-      <c r="E64" s="80"/>
-      <c r="F64" s="80"/>
-      <c r="G64" s="81"/>
-      <c r="H64" s="82"/>
+      <c r="B64" s="131"/>
+      <c r="D64" s="118"/>
+      <c r="E64" s="98"/>
+      <c r="F64" s="98"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="116"/>
       <c r="I64" s="45" t="s">
         <v>1</v>
       </c>
@@ -36900,18 +36900,18 @@
       <c r="HR64" s="31"/>
     </row>
     <row r="65" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="78" t="s">
-        <v>87</v>
-      </c>
-      <c r="D65" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="E65" s="80"/>
-      <c r="F65" s="80">
+      <c r="B65" s="131" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" s="118" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" s="98"/>
+      <c r="F65" s="98">
         <v>6</v>
       </c>
-      <c r="G65" s="81"/>
-      <c r="H65" s="82" t="str">
+      <c r="G65" s="84"/>
+      <c r="H65" s="116" t="str">
         <f t="shared" ref="H65" si="113">IF(O66&gt;P65,"!","")</f>
         <v/>
       </c>
@@ -36989,12 +36989,12 @@
       <c r="HR65" s="4"/>
     </row>
     <row r="66" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="78"/>
-      <c r="D66" s="79"/>
-      <c r="E66" s="80"/>
-      <c r="F66" s="80"/>
-      <c r="G66" s="81"/>
-      <c r="H66" s="82"/>
+      <c r="B66" s="131"/>
+      <c r="D66" s="118"/>
+      <c r="E66" s="98"/>
+      <c r="F66" s="98"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="116"/>
       <c r="I66" s="45" t="s">
         <v>1</v>
       </c>
@@ -37232,20 +37232,20 @@
       <c r="HR66" s="31"/>
     </row>
     <row r="67" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="D67" s="79" t="s">
-        <v>84</v>
-      </c>
-      <c r="E67" s="80" t="s">
+      <c r="B67" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="F67" s="80">
+      <c r="D67" s="118" t="s">
+        <v>83</v>
+      </c>
+      <c r="E67" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="F67" s="98">
         <v>6</v>
       </c>
-      <c r="G67" s="81"/>
-      <c r="H67" s="82" t="str">
+      <c r="G67" s="84"/>
+      <c r="H67" s="116" t="str">
         <f t="shared" ref="H67" si="119">IF(O68&gt;P67,"!","")</f>
         <v/>
       </c>
@@ -37340,12 +37340,12 @@
       <c r="HR67" s="4"/>
     </row>
     <row r="68" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="78"/>
-      <c r="D68" s="79"/>
-      <c r="E68" s="80"/>
-      <c r="F68" s="80"/>
-      <c r="G68" s="81"/>
-      <c r="H68" s="82"/>
+      <c r="B68" s="131"/>
+      <c r="D68" s="118"/>
+      <c r="E68" s="98"/>
+      <c r="F68" s="98"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="116"/>
       <c r="I68" s="45" t="s">
         <v>1</v>
       </c>
@@ -37583,20 +37583,20 @@
       <c r="HR68" s="31"/>
     </row>
     <row r="69" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="78" t="s">
-        <v>89</v>
-      </c>
-      <c r="D69" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="E69" s="80" t="s">
+      <c r="B69" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="F69" s="80">
+      <c r="D69" s="118" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69" s="98">
         <v>6</v>
       </c>
-      <c r="G69" s="81"/>
-      <c r="H69" s="82" t="str">
+      <c r="G69" s="84"/>
+      <c r="H69" s="116" t="str">
         <f t="shared" ref="H69" si="127">IF(O70&gt;P69,"!","")</f>
         <v/>
       </c>
@@ -37673,12 +37673,12 @@
       <c r="HR69" s="4"/>
     </row>
     <row r="70" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="78"/>
-      <c r="D70" s="79"/>
-      <c r="E70" s="80"/>
-      <c r="F70" s="80"/>
-      <c r="G70" s="81"/>
-      <c r="H70" s="82"/>
+      <c r="B70" s="131"/>
+      <c r="D70" s="118"/>
+      <c r="E70" s="98"/>
+      <c r="F70" s="98"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="116"/>
       <c r="I70" s="45" t="s">
         <v>1</v>
       </c>
@@ -37916,20 +37916,20 @@
       <c r="HR70" s="31"/>
     </row>
     <row r="71" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="78" t="s">
-        <v>90</v>
-      </c>
-      <c r="D71" s="79" t="s">
-        <v>86</v>
-      </c>
-      <c r="E71" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="F71" s="80">
+      <c r="B71" s="131" t="s">
+        <v>89</v>
+      </c>
+      <c r="D71" s="118" t="s">
+        <v>85</v>
+      </c>
+      <c r="E71" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="F71" s="98">
         <v>6</v>
       </c>
-      <c r="G71" s="81"/>
-      <c r="H71" s="82" t="str">
+      <c r="G71" s="84"/>
+      <c r="H71" s="116" t="str">
         <f t="shared" ref="H71" si="133">IF(O72&gt;P71,"!","")</f>
         <v/>
       </c>
@@ -38005,12 +38005,12 @@
       <c r="HR71" s="4"/>
     </row>
     <row r="72" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="78"/>
-      <c r="D72" s="79"/>
-      <c r="E72" s="80"/>
-      <c r="F72" s="80"/>
-      <c r="G72" s="81"/>
-      <c r="H72" s="82"/>
+      <c r="B72" s="131"/>
+      <c r="D72" s="118"/>
+      <c r="E72" s="98"/>
+      <c r="F72" s="98"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="116"/>
       <c r="I72" s="45" t="s">
         <v>1</v>
       </c>
@@ -38337,11 +38337,11 @@
     </row>
     <row r="73" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="79"/>
-      <c r="E73" s="80"/>
-      <c r="F73" s="80"/>
-      <c r="G73" s="81"/>
-      <c r="H73" s="82" t="str">
+      <c r="D73" s="118"/>
+      <c r="E73" s="98"/>
+      <c r="F73" s="98"/>
+      <c r="G73" s="84"/>
+      <c r="H73" s="116" t="str">
         <f t="shared" ref="H73" si="139">IF(O74&gt;P73,"!","")</f>
         <v/>
       </c>
@@ -38409,11 +38409,11 @@
     </row>
     <row r="74" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="D74" s="79"/>
-      <c r="E74" s="80"/>
-      <c r="F74" s="80"/>
-      <c r="G74" s="81"/>
-      <c r="H74" s="82"/>
+      <c r="D74" s="118"/>
+      <c r="E74" s="98"/>
+      <c r="F74" s="98"/>
+      <c r="G74" s="84"/>
+      <c r="H74" s="116"/>
       <c r="I74" s="45" t="s">
         <v>1</v>
       </c>
@@ -38652,11 +38652,11 @@
     </row>
     <row r="75" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="79"/>
-      <c r="E75" s="80"/>
-      <c r="F75" s="80"/>
-      <c r="G75" s="81"/>
-      <c r="H75" s="82" t="str">
+      <c r="D75" s="118"/>
+      <c r="E75" s="98"/>
+      <c r="F75" s="98"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="116" t="str">
         <f t="shared" ref="H75" si="145">IF(O76&gt;P75,"!","")</f>
         <v/>
       </c>
@@ -38725,11 +38725,11 @@
     </row>
     <row r="76" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
-      <c r="D76" s="79"/>
-      <c r="E76" s="80"/>
-      <c r="F76" s="80"/>
-      <c r="G76" s="81"/>
-      <c r="H76" s="82"/>
+      <c r="D76" s="118"/>
+      <c r="E76" s="98"/>
+      <c r="F76" s="98"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="116"/>
       <c r="I76" s="45" t="s">
         <v>1</v>
       </c>
@@ -38968,11 +38968,11 @@
     </row>
     <row r="77" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
-      <c r="D77" s="79"/>
-      <c r="E77" s="80"/>
-      <c r="F77" s="80"/>
-      <c r="G77" s="81"/>
-      <c r="H77" s="82" t="str">
+      <c r="D77" s="118"/>
+      <c r="E77" s="98"/>
+      <c r="F77" s="98"/>
+      <c r="G77" s="84"/>
+      <c r="H77" s="116" t="str">
         <f t="shared" ref="H77" si="151">IF(O78&gt;P77,"!","")</f>
         <v/>
       </c>
@@ -39041,11 +39041,11 @@
     </row>
     <row r="78" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="79"/>
-      <c r="E78" s="80"/>
-      <c r="F78" s="80"/>
-      <c r="G78" s="81"/>
-      <c r="H78" s="82"/>
+      <c r="D78" s="118"/>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+      <c r="G78" s="84"/>
+      <c r="H78" s="116"/>
       <c r="I78" s="45" t="s">
         <v>1</v>
       </c>
@@ -39284,11 +39284,11 @@
     </row>
     <row r="79" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="D79" s="79"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="80"/>
-      <c r="G79" s="81"/>
-      <c r="H79" s="82" t="str">
+      <c r="D79" s="118"/>
+      <c r="E79" s="98"/>
+      <c r="F79" s="98"/>
+      <c r="G79" s="84"/>
+      <c r="H79" s="116" t="str">
         <f t="shared" ref="H79" si="157">IF(O80&gt;P79,"!","")</f>
         <v/>
       </c>
@@ -39357,11 +39357,11 @@
     </row>
     <row r="80" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
-      <c r="D80" s="79"/>
-      <c r="E80" s="80"/>
-      <c r="F80" s="80"/>
-      <c r="G80" s="81"/>
-      <c r="H80" s="82"/>
+      <c r="D80" s="118"/>
+      <c r="E80" s="98"/>
+      <c r="F80" s="98"/>
+      <c r="G80" s="84"/>
+      <c r="H80" s="116"/>
       <c r="I80" s="45" t="s">
         <v>1</v>
       </c>
@@ -39600,11 +39600,11 @@
     </row>
     <row r="81" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="D81" s="79"/>
-      <c r="E81" s="80"/>
-      <c r="F81" s="80"/>
-      <c r="G81" s="81"/>
-      <c r="H81" s="82" t="str">
+      <c r="D81" s="118"/>
+      <c r="E81" s="98"/>
+      <c r="F81" s="98"/>
+      <c r="G81" s="84"/>
+      <c r="H81" s="116" t="str">
         <f t="shared" ref="H81" si="163">IF(O82&gt;P81,"!","")</f>
         <v/>
       </c>
@@ -39673,11 +39673,11 @@
     </row>
     <row r="82" spans="2:226" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="70"/>
-      <c r="D82" s="83"/>
-      <c r="E82" s="84"/>
-      <c r="F82" s="84"/>
-      <c r="G82" s="85"/>
-      <c r="H82" s="86"/>
+      <c r="D82" s="127"/>
+      <c r="E82" s="128"/>
+      <c r="F82" s="128"/>
+      <c r="G82" s="129"/>
+      <c r="H82" s="130"/>
       <c r="I82" s="47" t="s">
         <v>1</v>
       </c>
@@ -39916,15 +39916,260 @@
     </row>
   </sheetData>
   <mergeCells count="287">
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="HI7:HR7"/>
+    <mergeCell ref="FA8:FJ8"/>
+    <mergeCell ref="FK8:FT8"/>
+    <mergeCell ref="FU8:GD8"/>
+    <mergeCell ref="GE8:GN8"/>
+    <mergeCell ref="GO8:GX8"/>
+    <mergeCell ref="GY8:HH8"/>
+    <mergeCell ref="HI8:HR8"/>
+    <mergeCell ref="FA9:FJ9"/>
+    <mergeCell ref="FK9:FT9"/>
+    <mergeCell ref="FU9:GD9"/>
+    <mergeCell ref="GE9:GN9"/>
+    <mergeCell ref="GO9:GX9"/>
+    <mergeCell ref="GY9:HH9"/>
+    <mergeCell ref="HI9:HR9"/>
+    <mergeCell ref="EQ7:EZ7"/>
+    <mergeCell ref="EQ8:EZ8"/>
+    <mergeCell ref="EQ9:EZ9"/>
+    <mergeCell ref="FA7:FJ7"/>
+    <mergeCell ref="FK7:FT7"/>
+    <mergeCell ref="FU7:GD7"/>
+    <mergeCell ref="GE7:GN7"/>
+    <mergeCell ref="GO7:GX7"/>
+    <mergeCell ref="GY7:HH7"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="BO7:BX7"/>
+    <mergeCell ref="EG7:EP7"/>
+    <mergeCell ref="AA8:AJ8"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AU8:BD8"/>
+    <mergeCell ref="BE8:BN8"/>
+    <mergeCell ref="BO8:BX8"/>
+    <mergeCell ref="BY8:CH8"/>
+    <mergeCell ref="CI8:CR8"/>
+    <mergeCell ref="CS8:DB8"/>
+    <mergeCell ref="DC8:DL8"/>
+    <mergeCell ref="BY7:CH7"/>
+    <mergeCell ref="CI7:CR7"/>
+    <mergeCell ref="CS7:DB7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="DW7:EF7"/>
+    <mergeCell ref="AA9:AJ9"/>
+    <mergeCell ref="AK9:AT9"/>
+    <mergeCell ref="AU9:BD9"/>
+    <mergeCell ref="BE9:BN9"/>
+    <mergeCell ref="BO9:BX9"/>
+    <mergeCell ref="EG9:EP9"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="BY9:CH9"/>
+    <mergeCell ref="CI9:CR9"/>
+    <mergeCell ref="CS9:DB9"/>
+    <mergeCell ref="DC9:DL9"/>
+    <mergeCell ref="DM9:DV9"/>
+    <mergeCell ref="DW9:EF9"/>
+    <mergeCell ref="DM8:DV8"/>
+    <mergeCell ref="DW8:EF8"/>
+    <mergeCell ref="EG8:EP8"/>
+    <mergeCell ref="AA7:AJ7"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AU7:BD7"/>
+    <mergeCell ref="BE7:BN7"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="DC7:DL7"/>
+    <mergeCell ref="DM7:DV7"/>
+    <mergeCell ref="AJ4:AR4"/>
+    <mergeCell ref="AJ5:AR5"/>
+    <mergeCell ref="AU5:BE5"/>
+    <mergeCell ref="AU4:BE4"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D19:D20"/>
@@ -39949,260 +40194,15 @@
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="AA7:AJ7"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AU7:BD7"/>
-    <mergeCell ref="BE7:BN7"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="DC7:DL7"/>
-    <mergeCell ref="DM7:DV7"/>
-    <mergeCell ref="AJ4:AR4"/>
-    <mergeCell ref="AJ5:AR5"/>
-    <mergeCell ref="AU5:BE5"/>
-    <mergeCell ref="AU4:BE4"/>
-    <mergeCell ref="BY9:CH9"/>
-    <mergeCell ref="CI9:CR9"/>
-    <mergeCell ref="CS9:DB9"/>
-    <mergeCell ref="DC9:DL9"/>
-    <mergeCell ref="DM9:DV9"/>
-    <mergeCell ref="DW9:EF9"/>
-    <mergeCell ref="DM8:DV8"/>
-    <mergeCell ref="DW8:EF8"/>
-    <mergeCell ref="EG8:EP8"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="AK9:AT9"/>
-    <mergeCell ref="AU9:BD9"/>
-    <mergeCell ref="BE9:BN9"/>
-    <mergeCell ref="BO9:BX9"/>
-    <mergeCell ref="EG9:EP9"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="FK7:FT7"/>
-    <mergeCell ref="FU7:GD7"/>
-    <mergeCell ref="GE7:GN7"/>
-    <mergeCell ref="GO7:GX7"/>
-    <mergeCell ref="GY7:HH7"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="BO7:BX7"/>
-    <mergeCell ref="EG7:EP7"/>
-    <mergeCell ref="AA8:AJ8"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AU8:BD8"/>
-    <mergeCell ref="BE8:BN8"/>
-    <mergeCell ref="BO8:BX8"/>
-    <mergeCell ref="BY8:CH8"/>
-    <mergeCell ref="CI8:CR8"/>
-    <mergeCell ref="CS8:DB8"/>
-    <mergeCell ref="DC8:DL8"/>
-    <mergeCell ref="BY7:CH7"/>
-    <mergeCell ref="CI7:CR7"/>
-    <mergeCell ref="CS7:DB7"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="DW7:EF7"/>
-    <mergeCell ref="AA9:AJ9"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="HI7:HR7"/>
-    <mergeCell ref="FA8:FJ8"/>
-    <mergeCell ref="FK8:FT8"/>
-    <mergeCell ref="FU8:GD8"/>
-    <mergeCell ref="GE8:GN8"/>
-    <mergeCell ref="GO8:GX8"/>
-    <mergeCell ref="GY8:HH8"/>
-    <mergeCell ref="HI8:HR8"/>
-    <mergeCell ref="FA9:FJ9"/>
-    <mergeCell ref="FK9:FT9"/>
-    <mergeCell ref="FU9:GD9"/>
-    <mergeCell ref="GE9:GN9"/>
-    <mergeCell ref="GO9:GX9"/>
-    <mergeCell ref="GY9:HH9"/>
-    <mergeCell ref="HI9:HR9"/>
-    <mergeCell ref="EQ7:EZ7"/>
-    <mergeCell ref="EQ8:EZ8"/>
-    <mergeCell ref="EQ9:EZ9"/>
-    <mergeCell ref="FA7:FJ7"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7:HR8">
     <cfRule type="expression" dxfId="2580" priority="3813">
@@ -49144,7 +49144,7 @@
         <v>45042</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -49198,7 +49198,7 @@
         <v>45049</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -49236,7 +49236,7 @@
         <v>45055</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -49274,7 +49274,7 @@
         <v>45057</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -49294,7 +49294,7 @@
         <v>45062</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -49332,7 +49332,7 @@
         <v>45064</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -49913,12 +49913,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50145,15 +50142,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
+    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -50179,18 +50188,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
-    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Affichage des miniatures et info bonus fonctionnel
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F1D7D-622B-4EB0-9105-788AD4C068F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD92784-CE5D-4ABC-A98A-6F862D951F5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="98">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -25864,7 +25864,7 @@
   <dimension ref="A1:HR82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="AH32" sqref="AH32"/>
+      <selection activeCell="AP33" sqref="AP33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25941,7 +25941,7 @@
       <c r="H4" s="3"/>
       <c r="Q4" s="111">
         <f>MAX(L13:L163)-L12</f>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="R4" s="112"/>
       <c r="S4" s="29" t="s">
@@ -30232,12 +30232,6 @@
       <c r="Q23" s="5"/>
       <c r="Z23" s="18"/>
       <c r="AA23" s="20"/>
-      <c r="AD23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE23" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="AI23" s="71" t="s">
         <v>28</v>
       </c>
@@ -30291,12 +30285,12 @@
       </c>
       <c r="J24" s="46">
         <f>IF(D23="","",COUNTIF(Echéancier!$Q24:$EP24,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K24" s="14"/>
       <c r="L24" s="14">
         <f>IFERROR(L22+J24,0)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M24" s="14">
         <f t="shared" si="6"/>
@@ -30308,7 +30302,7 @@
       </c>
       <c r="O24" s="14">
         <f t="shared" ref="O24" si="17">IFERROR(MATCH("ra",$Q24:$EP24,1),0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="23"/>
@@ -30324,8 +30318,12 @@
       <c r="AA24" s="25"/>
       <c r="AB24" s="34"/>
       <c r="AC24" s="34"/>
-      <c r="AD24" s="34"/>
-      <c r="AE24" s="34"/>
+      <c r="AD24" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE24" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="AF24" s="34"/>
       <c r="AG24" s="75"/>
       <c r="AH24" s="34"/>
@@ -30563,9 +30561,6 @@
       <c r="Q25" s="5"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="20"/>
-      <c r="AF25" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="AJ25" s="71" t="s">
         <v>28</v>
       </c>
@@ -30618,12 +30613,12 @@
       </c>
       <c r="J26" s="46">
         <f>IF(D25="","",COUNTIF(Echéancier!$Q26:$EP26,"r"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14">
         <f>IFERROR(L24+J26,0)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M26" s="14">
         <f t="shared" ref="M26" si="20">COUNTIF(Q26:EP26,"a")</f>
@@ -30635,7 +30630,7 @@
       </c>
       <c r="O26" s="14">
         <f t="shared" ref="O26" si="21">IFERROR(MATCH("ra",$Q26:$EP26,1),0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="23"/>
@@ -30653,7 +30648,9 @@
       <c r="AC26" s="34"/>
       <c r="AD26" s="34"/>
       <c r="AE26" s="34"/>
-      <c r="AF26" s="34"/>
+      <c r="AF26" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="AG26" s="34"/>
       <c r="AH26" s="75"/>
       <c r="AI26" s="75"/>
@@ -30890,9 +30887,6 @@
       <c r="Q27" s="5"/>
       <c r="Z27" s="18"/>
       <c r="AA27" s="20"/>
-      <c r="AG27" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="AK27" s="71" t="s">
         <v>28</v>
       </c>
@@ -30956,12 +30950,12 @@
       </c>
       <c r="J28" s="46">
         <f>IF(D27="","",COUNTIF(Echéancier!$Q28:$EP28,"r"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="14"/>
       <c r="L28" s="14">
         <f>IFERROR(L26+J28,0)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="M28" s="14">
         <f t="shared" ref="M28" si="24">COUNTIF(Q28:EP28,"a")</f>
@@ -30973,7 +30967,7 @@
       </c>
       <c r="O28" s="14">
         <f t="shared" ref="O28" si="25">IFERROR(MATCH("ra",$Q28:$EP28,1),0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="23"/>
@@ -30992,7 +30986,9 @@
       <c r="AD28" s="34"/>
       <c r="AE28" s="34"/>
       <c r="AF28" s="34"/>
-      <c r="AG28" s="34"/>
+      <c r="AG28" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="AH28" s="34"/>
       <c r="AI28" s="34"/>
       <c r="AJ28" s="24"/>
@@ -31230,21 +31226,8 @@
       <c r="Q29" s="5"/>
       <c r="Z29" s="18"/>
       <c r="AA29" s="20"/>
-      <c r="AJ29" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK29" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AN29" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="20"/>
       <c r="AP29" s="71" t="s">
         <v>28</v>
       </c>
@@ -31305,12 +31288,12 @@
       </c>
       <c r="J30" s="46">
         <f>IF(D29="","",COUNTIF(Echéancier!$Q30:$EP30,"r"))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="14">
         <f>IFERROR(L28+J30,0)</f>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="M30" s="14">
         <f t="shared" ref="M30" si="28">COUNTIF(Q30:EP30,"a")</f>
@@ -31322,7 +31305,7 @@
       </c>
       <c r="O30" s="14">
         <f t="shared" ref="O30" si="29">IFERROR(MATCH("ra",$Q30:$EP30,1),0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="P30" s="14"/>
       <c r="Q30" s="23"/>
@@ -31344,13 +31327,27 @@
       <c r="AG30" s="34"/>
       <c r="AH30" s="34"/>
       <c r="AI30" s="34"/>
-      <c r="AJ30" s="24"/>
-      <c r="AK30" s="25"/>
-      <c r="AL30" s="34"/>
-      <c r="AM30" s="34"/>
-      <c r="AN30" s="34"/>
-      <c r="AO30" s="34"/>
-      <c r="AP30" s="34"/>
+      <c r="AJ30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK30" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL30" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM30" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN30" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO30" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP30" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="AQ30" s="75"/>
       <c r="AR30" s="75"/>
       <c r="AS30" s="34"/>
@@ -31633,12 +31630,12 @@
       </c>
       <c r="J32" s="46">
         <f>IF(D31="","",COUNTIF(Echéancier!$Q32:$EP32,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="14">
         <f>IFERROR(L30+J32,0)</f>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="M32" s="14">
         <f t="shared" ref="M32" si="32">COUNTIF(Q32:EP32,"a")</f>
@@ -31650,7 +31647,7 @@
       </c>
       <c r="O32" s="14">
         <f t="shared" ref="O32" si="33">IFERROR(MATCH("ra",$Q32:$EP32,1),0)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P32" s="14"/>
       <c r="Q32" s="23"/>
@@ -31679,8 +31676,12 @@
       <c r="AN32" s="34"/>
       <c r="AO32" s="34"/>
       <c r="AP32" s="34"/>
-      <c r="AQ32" s="34"/>
-      <c r="AR32" s="75"/>
+      <c r="AQ32" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR32" s="75" t="s">
+        <v>27</v>
+      </c>
       <c r="AS32" s="75"/>
       <c r="AT32" s="74"/>
       <c r="AU32" s="25"/>
@@ -31970,7 +31971,7 @@
       <c r="K34" s="14"/>
       <c r="L34" s="14">
         <f>IFERROR(L32+J34,0)</f>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="M34" s="14">
         <f t="shared" ref="M34" si="36">COUNTIF(Q34:EP34,"a")</f>
@@ -32305,7 +32306,7 @@
       <c r="K36" s="14"/>
       <c r="L36" s="14">
         <f>IFERROR(L34+J36,0)</f>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="M36" s="14">
         <f t="shared" ref="M36" si="40">COUNTIF(Q36:EP36,"a")</f>
@@ -32574,9 +32575,6 @@
       <c r="Q37" s="5"/>
       <c r="Z37" s="18"/>
       <c r="AA37" s="20"/>
-      <c r="AH37" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="AJ37" s="18"/>
       <c r="AK37" s="20"/>
       <c r="AT37" s="18"/>
@@ -32633,12 +32631,12 @@
       </c>
       <c r="J38" s="46">
         <f>IF(D37="","",COUNTIF(Echéancier!$Q38:$EP38,"r"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="14"/>
       <c r="L38" s="14">
         <f>IFERROR(L36+J38,0)</f>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="M38" s="14">
         <f t="shared" ref="M38" si="44">COUNTIF(Q38:EP38,"a")</f>
@@ -32650,7 +32648,7 @@
       </c>
       <c r="O38" s="14">
         <f t="shared" ref="O38" si="45">IFERROR(MATCH("ra",$Q38:$EP38,1),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="P38" s="14"/>
       <c r="Q38" s="23"/>
@@ -32670,7 +32668,9 @@
       <c r="AE38" s="34"/>
       <c r="AF38" s="34"/>
       <c r="AG38" s="34"/>
-      <c r="AH38" s="34"/>
+      <c r="AH38" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="AI38" s="34"/>
       <c r="AJ38" s="24"/>
       <c r="AK38" s="25"/>
@@ -32973,7 +32973,7 @@
       <c r="K40" s="14"/>
       <c r="L40" s="14">
         <f>IFERROR(L38+J40,0)</f>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="M40" s="14">
         <f t="shared" ref="M40" si="47">COUNTIF(Q40:EP40,"a")</f>

</xml_diff>

<commit_message>
finalisation de la journée.
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A73B563-E722-4D7B-80D9-864AB1ED45F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD5B1C7-7F7F-45F7-ACF1-8F8660668934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25864,7 +25864,7 @@
   <dimension ref="A1:HR82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="AQ35" sqref="AQ35"/>
+      <selection activeCell="BD26" sqref="BD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Début de fonctionement de l'historique des urls
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B06A889-303D-4502-8C52-6D25130AD0E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B212D1D4-95F6-49E9-A9A2-8C886076A07E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="99">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -533,7 +533,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -762,11 +762,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,7 +1092,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26009,8 +26022,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="BG66" sqref="BG66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="BD44" sqref="BD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26087,7 +26100,7 @@
       <c r="H4" s="3"/>
       <c r="Q4" s="108">
         <f>MAX(L13:L163)-L12</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="R4" s="109"/>
       <c r="S4" s="29" t="s">
@@ -33122,12 +33135,12 @@
       </c>
       <c r="J40" s="46">
         <f>IF(D39="","",COUNTIF(Echéancier!$Q40:$EP40,"r"))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K40" s="14"/>
       <c r="L40" s="14">
         <f>IFERROR(L38+J40,0)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="M40" s="14">
         <f t="shared" ref="M40" si="47">COUNTIF(Q40:EP40,"a")</f>
@@ -33139,7 +33152,7 @@
       </c>
       <c r="O40" s="14">
         <f>IFERROR(MATCH("ra",$Q40:$EP40,1),0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P40" s="14"/>
       <c r="Q40" s="23"/>
@@ -33178,10 +33191,18 @@
       <c r="AX40" s="34"/>
       <c r="AY40" s="34"/>
       <c r="AZ40" s="34"/>
-      <c r="BA40" s="34"/>
-      <c r="BB40" s="75"/>
-      <c r="BC40" s="75"/>
-      <c r="BD40" s="24"/>
+      <c r="BA40" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB40" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="BC40" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="BD40" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="BE40" s="25"/>
       <c r="BF40" s="34"/>
       <c r="BG40" s="34"/>
@@ -38265,26 +38286,26 @@
       <c r="DT70" s="75"/>
       <c r="DU70" s="75"/>
       <c r="DV70" s="74"/>
-      <c r="DW70" s="25"/>
-      <c r="DX70" s="34"/>
-      <c r="DY70" s="34"/>
-      <c r="DZ70" s="34"/>
-      <c r="EA70" s="34"/>
-      <c r="EB70" s="34"/>
-      <c r="EC70" s="34"/>
-      <c r="ED70" s="34"/>
-      <c r="EE70" s="34"/>
-      <c r="EF70" s="24"/>
-      <c r="EG70" s="25"/>
-      <c r="EH70" s="34"/>
-      <c r="EI70" s="34"/>
-      <c r="EJ70" s="34"/>
-      <c r="EK70" s="34"/>
-      <c r="EL70" s="34"/>
-      <c r="EM70" s="34"/>
-      <c r="EN70" s="34"/>
-      <c r="EO70" s="34"/>
-      <c r="EP70" s="31"/>
+      <c r="DW70" s="76"/>
+      <c r="DX70" s="75"/>
+      <c r="DY70" s="75"/>
+      <c r="DZ70" s="75"/>
+      <c r="EA70" s="75"/>
+      <c r="EB70" s="75"/>
+      <c r="EC70" s="75"/>
+      <c r="ED70" s="75"/>
+      <c r="EE70" s="75"/>
+      <c r="EF70" s="74"/>
+      <c r="EG70" s="76"/>
+      <c r="EH70" s="75"/>
+      <c r="EI70" s="75"/>
+      <c r="EJ70" s="75"/>
+      <c r="EK70" s="75"/>
+      <c r="EL70" s="75"/>
+      <c r="EM70" s="75"/>
+      <c r="EN70" s="75"/>
+      <c r="EO70" s="75"/>
+      <c r="EP70" s="134"/>
       <c r="EQ70" s="34"/>
       <c r="ER70" s="34"/>
       <c r="ES70" s="34"/>
@@ -38597,26 +38618,26 @@
       <c r="DT72" s="75"/>
       <c r="DU72" s="75"/>
       <c r="DV72" s="74"/>
-      <c r="DW72" s="25"/>
-      <c r="DX72" s="34"/>
-      <c r="DY72" s="34"/>
-      <c r="DZ72" s="34"/>
-      <c r="EA72" s="34"/>
-      <c r="EB72" s="34"/>
-      <c r="EC72" s="34"/>
-      <c r="ED72" s="34"/>
-      <c r="EE72" s="34"/>
-      <c r="EF72" s="24"/>
-      <c r="EG72" s="25"/>
-      <c r="EH72" s="34"/>
-      <c r="EI72" s="34"/>
-      <c r="EJ72" s="34"/>
-      <c r="EK72" s="34"/>
-      <c r="EL72" s="34"/>
-      <c r="EM72" s="34"/>
-      <c r="EN72" s="34"/>
-      <c r="EO72" s="34"/>
-      <c r="EP72" s="31"/>
+      <c r="DW72" s="76"/>
+      <c r="DX72" s="75"/>
+      <c r="DY72" s="75"/>
+      <c r="DZ72" s="75"/>
+      <c r="EA72" s="75"/>
+      <c r="EB72" s="75"/>
+      <c r="EC72" s="75"/>
+      <c r="ED72" s="75"/>
+      <c r="EE72" s="75"/>
+      <c r="EF72" s="74"/>
+      <c r="EG72" s="76"/>
+      <c r="EH72" s="75"/>
+      <c r="EI72" s="75"/>
+      <c r="EJ72" s="75"/>
+      <c r="EK72" s="75"/>
+      <c r="EL72" s="75"/>
+      <c r="EM72" s="75"/>
+      <c r="EN72" s="75"/>
+      <c r="EO72" s="75"/>
+      <c r="EP72" s="134"/>
       <c r="EQ72" s="34" t="s">
         <v>27</v>
       </c>
@@ -38892,136 +38913,136 @@
         <v>0</v>
       </c>
       <c r="P74" s="14"/>
-      <c r="Q74" s="23"/>
-      <c r="R74" s="34"/>
-      <c r="S74" s="34"/>
-      <c r="T74" s="34"/>
-      <c r="U74" s="34"/>
-      <c r="V74" s="34"/>
-      <c r="W74" s="34"/>
-      <c r="X74" s="34"/>
-      <c r="Y74" s="34"/>
-      <c r="Z74" s="24"/>
-      <c r="AA74" s="25"/>
-      <c r="AB74" s="34"/>
-      <c r="AC74" s="34"/>
-      <c r="AD74" s="34"/>
-      <c r="AE74" s="34"/>
-      <c r="AF74" s="34"/>
-      <c r="AG74" s="34"/>
-      <c r="AH74" s="34"/>
-      <c r="AI74" s="34"/>
-      <c r="AJ74" s="24"/>
-      <c r="AK74" s="25"/>
-      <c r="AL74" s="34"/>
-      <c r="AM74" s="34"/>
-      <c r="AN74" s="34"/>
-      <c r="AO74" s="34"/>
-      <c r="AP74" s="34"/>
-      <c r="AQ74" s="34"/>
-      <c r="AR74" s="34"/>
-      <c r="AS74" s="34"/>
-      <c r="AT74" s="24"/>
+      <c r="Q74" s="77"/>
+      <c r="R74" s="75"/>
+      <c r="S74" s="75"/>
+      <c r="T74" s="75"/>
+      <c r="U74" s="75"/>
+      <c r="V74" s="75"/>
+      <c r="W74" s="75"/>
+      <c r="X74" s="75"/>
+      <c r="Y74" s="75"/>
+      <c r="Z74" s="74"/>
+      <c r="AA74" s="76"/>
+      <c r="AB74" s="75"/>
+      <c r="AC74" s="75"/>
+      <c r="AD74" s="75"/>
+      <c r="AE74" s="75"/>
+      <c r="AF74" s="75"/>
+      <c r="AG74" s="75"/>
+      <c r="AH74" s="75"/>
+      <c r="AI74" s="75"/>
+      <c r="AJ74" s="74"/>
+      <c r="AK74" s="76"/>
+      <c r="AL74" s="75"/>
+      <c r="AM74" s="75"/>
+      <c r="AN74" s="75"/>
+      <c r="AO74" s="75"/>
+      <c r="AP74" s="75"/>
+      <c r="AQ74" s="75"/>
+      <c r="AR74" s="75"/>
+      <c r="AS74" s="75"/>
+      <c r="AT74" s="74"/>
       <c r="AU74" s="132"/>
-      <c r="AV74" s="34"/>
-      <c r="AW74" s="34"/>
-      <c r="AX74" s="65"/>
-      <c r="AY74" s="65"/>
-      <c r="AZ74" s="34"/>
-      <c r="BA74" s="34"/>
-      <c r="BB74" s="34"/>
-      <c r="BC74" s="34"/>
-      <c r="BD74" s="24"/>
-      <c r="BE74" s="25"/>
-      <c r="BF74" s="34"/>
-      <c r="BG74" s="34"/>
-      <c r="BH74" s="34"/>
-      <c r="BI74" s="34"/>
-      <c r="BJ74" s="34"/>
-      <c r="BK74" s="34"/>
-      <c r="BL74" s="34"/>
-      <c r="BM74" s="34"/>
-      <c r="BN74" s="24"/>
-      <c r="BO74" s="25"/>
-      <c r="BP74" s="34"/>
-      <c r="BQ74" s="34"/>
-      <c r="BR74" s="34"/>
-      <c r="BS74" s="34"/>
-      <c r="BT74" s="34"/>
-      <c r="BU74" s="34"/>
-      <c r="BV74" s="34"/>
-      <c r="BW74" s="34"/>
-      <c r="BX74" s="24"/>
-      <c r="BY74" s="25"/>
-      <c r="BZ74" s="34"/>
-      <c r="CA74" s="34"/>
-      <c r="CB74" s="34"/>
-      <c r="CC74" s="34"/>
-      <c r="CD74" s="34"/>
-      <c r="CE74" s="34"/>
-      <c r="CF74" s="34"/>
-      <c r="CG74" s="34"/>
-      <c r="CH74" s="24"/>
-      <c r="CI74" s="25"/>
-      <c r="CJ74" s="34"/>
-      <c r="CK74" s="34"/>
-      <c r="CL74" s="34"/>
-      <c r="CM74" s="34"/>
-      <c r="CN74" s="34"/>
-      <c r="CO74" s="34"/>
-      <c r="CP74" s="34"/>
-      <c r="CQ74" s="34"/>
-      <c r="CR74" s="24"/>
-      <c r="CS74" s="25"/>
-      <c r="CT74" s="34"/>
-      <c r="CU74" s="34"/>
-      <c r="CV74" s="34"/>
-      <c r="CW74" s="34"/>
-      <c r="CX74" s="34"/>
-      <c r="CY74" s="34"/>
-      <c r="CZ74" s="34"/>
-      <c r="DA74" s="34"/>
-      <c r="DB74" s="34"/>
-      <c r="DC74" s="25"/>
-      <c r="DD74" s="34"/>
-      <c r="DE74" s="34"/>
-      <c r="DF74" s="34"/>
-      <c r="DG74" s="34"/>
-      <c r="DH74" s="34"/>
-      <c r="DI74" s="34"/>
-      <c r="DJ74" s="34"/>
-      <c r="DK74" s="34"/>
-      <c r="DL74" s="24"/>
-      <c r="DM74" s="25"/>
-      <c r="DN74" s="34"/>
-      <c r="DO74" s="34"/>
-      <c r="DP74" s="34"/>
-      <c r="DQ74" s="34"/>
-      <c r="DR74" s="34"/>
-      <c r="DS74" s="34"/>
-      <c r="DT74" s="34"/>
-      <c r="DU74" s="34"/>
-      <c r="DV74" s="24"/>
-      <c r="DW74" s="25"/>
-      <c r="DX74" s="34"/>
-      <c r="DY74" s="34"/>
-      <c r="DZ74" s="34"/>
-      <c r="EA74" s="34"/>
-      <c r="EB74" s="34"/>
-      <c r="EC74" s="34"/>
-      <c r="ED74" s="34"/>
-      <c r="EE74" s="34"/>
-      <c r="EF74" s="24"/>
-      <c r="EG74" s="25"/>
-      <c r="EH74" s="34"/>
-      <c r="EI74" s="34"/>
-      <c r="EJ74" s="34"/>
-      <c r="EK74" s="34"/>
-      <c r="EL74" s="34"/>
-      <c r="EM74" s="34"/>
-      <c r="EN74" s="34"/>
-      <c r="EO74" s="34"/>
-      <c r="EP74" s="31"/>
+      <c r="AV74" s="75"/>
+      <c r="AW74" s="75"/>
+      <c r="AX74" s="133"/>
+      <c r="AY74" s="133"/>
+      <c r="AZ74" s="75"/>
+      <c r="BA74" s="75"/>
+      <c r="BB74" s="75"/>
+      <c r="BC74" s="75"/>
+      <c r="BD74" s="74"/>
+      <c r="BE74" s="76"/>
+      <c r="BF74" s="75"/>
+      <c r="BG74" s="75"/>
+      <c r="BH74" s="75"/>
+      <c r="BI74" s="75"/>
+      <c r="BJ74" s="75"/>
+      <c r="BK74" s="75"/>
+      <c r="BL74" s="75"/>
+      <c r="BM74" s="75"/>
+      <c r="BN74" s="74"/>
+      <c r="BO74" s="76"/>
+      <c r="BP74" s="75"/>
+      <c r="BQ74" s="75"/>
+      <c r="BR74" s="75"/>
+      <c r="BS74" s="75"/>
+      <c r="BT74" s="75"/>
+      <c r="BU74" s="75"/>
+      <c r="BV74" s="75"/>
+      <c r="BW74" s="75"/>
+      <c r="BX74" s="74"/>
+      <c r="BY74" s="76"/>
+      <c r="BZ74" s="75"/>
+      <c r="CA74" s="75"/>
+      <c r="CB74" s="75"/>
+      <c r="CC74" s="75"/>
+      <c r="CD74" s="75"/>
+      <c r="CE74" s="75"/>
+      <c r="CF74" s="75"/>
+      <c r="CG74" s="75"/>
+      <c r="CH74" s="74"/>
+      <c r="CI74" s="76"/>
+      <c r="CJ74" s="75"/>
+      <c r="CK74" s="75"/>
+      <c r="CL74" s="75"/>
+      <c r="CM74" s="75"/>
+      <c r="CN74" s="75"/>
+      <c r="CO74" s="75"/>
+      <c r="CP74" s="75"/>
+      <c r="CQ74" s="75"/>
+      <c r="CR74" s="74"/>
+      <c r="CS74" s="76"/>
+      <c r="CT74" s="75"/>
+      <c r="CU74" s="75"/>
+      <c r="CV74" s="75"/>
+      <c r="CW74" s="75"/>
+      <c r="CX74" s="75"/>
+      <c r="CY74" s="75"/>
+      <c r="CZ74" s="75"/>
+      <c r="DA74" s="75"/>
+      <c r="DB74" s="75"/>
+      <c r="DC74" s="76"/>
+      <c r="DD74" s="75"/>
+      <c r="DE74" s="75"/>
+      <c r="DF74" s="75"/>
+      <c r="DG74" s="75"/>
+      <c r="DH74" s="75"/>
+      <c r="DI74" s="75"/>
+      <c r="DJ74" s="75"/>
+      <c r="DK74" s="75"/>
+      <c r="DL74" s="74"/>
+      <c r="DM74" s="76"/>
+      <c r="DN74" s="75"/>
+      <c r="DO74" s="75"/>
+      <c r="DP74" s="75"/>
+      <c r="DQ74" s="75"/>
+      <c r="DR74" s="75"/>
+      <c r="DS74" s="75"/>
+      <c r="DT74" s="75"/>
+      <c r="DU74" s="75"/>
+      <c r="DV74" s="74"/>
+      <c r="DW74" s="76"/>
+      <c r="DX74" s="75"/>
+      <c r="DY74" s="75"/>
+      <c r="DZ74" s="75"/>
+      <c r="EA74" s="75"/>
+      <c r="EB74" s="75"/>
+      <c r="EC74" s="75"/>
+      <c r="ED74" s="75"/>
+      <c r="EE74" s="75"/>
+      <c r="EF74" s="74"/>
+      <c r="EG74" s="76"/>
+      <c r="EH74" s="75"/>
+      <c r="EI74" s="75"/>
+      <c r="EJ74" s="75"/>
+      <c r="EK74" s="75"/>
+      <c r="EL74" s="75"/>
+      <c r="EM74" s="75"/>
+      <c r="EN74" s="75"/>
+      <c r="EO74" s="75"/>
+      <c r="EP74" s="134"/>
       <c r="EQ74" s="34"/>
       <c r="ER74" s="34"/>
       <c r="ES74" s="34"/>

</xml_diff>

<commit_message>
Envoi de message professeur -> eleve fonctionel
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A48786-EF83-4175-B79A-3300921AA71A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E96EF9-2193-400C-A6FF-DAF026E1450A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="99">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -25881,7 +25881,7 @@
   <dimension ref="A1:HR82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="CX31" sqref="CX31"/>
+      <selection activeCell="BO22" sqref="BO22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34315,12 +34315,12 @@
       </c>
       <c r="J48" s="46">
         <f>IF(D47="","",COUNTIF(Echéancier!$Q48:$EP48,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K48" s="14"/>
       <c r="L48" s="14">
         <f>IFERROR(L46+J48,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M48" s="14">
         <f t="shared" ref="M48" si="63">COUNTIF(Q48:EP48,"a")</f>
@@ -34332,7 +34332,7 @@
       </c>
       <c r="O48" s="14">
         <f>IFERROR(MATCH("ra",$Q48:$EP48,1),0)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="P48" s="14"/>
       <c r="Q48" s="23"/>
@@ -34378,8 +34378,12 @@
       <c r="BE48" s="25"/>
       <c r="BF48" s="34"/>
       <c r="BG48" s="34"/>
-      <c r="BH48" s="34"/>
-      <c r="BI48" s="75"/>
+      <c r="BH48" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BI48" s="75" t="s">
+        <v>27</v>
+      </c>
       <c r="BJ48" s="75"/>
       <c r="BK48" s="75"/>
       <c r="BL48" s="75"/>
@@ -34662,7 +34666,7 @@
       <c r="K50" s="14"/>
       <c r="L50" s="14">
         <f t="shared" ref="L50" si="68">IFERROR(L48+J50,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M50" s="14">
         <f t="shared" ref="M50" si="69">COUNTIF(Q50:EP50,"a")</f>
@@ -34993,7 +34997,7 @@
       <c r="K52" s="14"/>
       <c r="L52" s="14">
         <f t="shared" ref="L52" si="74">IFERROR(L50+J52,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M52" s="14">
         <f t="shared" ref="M52" si="75">COUNTIF(Q52:EP52,"a")</f>
@@ -35327,7 +35331,7 @@
       <c r="K54" s="14"/>
       <c r="L54" s="14">
         <f t="shared" ref="L54" si="80">IFERROR(L52+J54,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M54" s="14">
         <f t="shared" ref="M54" si="81">COUNTIF(Q54:EP54,"a")</f>
@@ -35666,7 +35670,7 @@
       <c r="K56" s="14"/>
       <c r="L56" s="14">
         <f t="shared" ref="L56" si="86">IFERROR(L54+J56,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M56" s="14">
         <f t="shared" ref="M56" si="87">COUNTIF(Q56:EP56,"a")</f>
@@ -35993,7 +35997,7 @@
       <c r="K58" s="14"/>
       <c r="L58" s="14">
         <f t="shared" ref="L58" si="92">IFERROR(L56+J58,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M58" s="14">
         <f t="shared" ref="M58" si="93">COUNTIF(Q58:EP58,"a")</f>
@@ -36321,7 +36325,7 @@
       <c r="K60" s="14"/>
       <c r="L60" s="14">
         <f t="shared" ref="L60" si="98">IFERROR(L58+J60,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M60" s="14">
         <f t="shared" ref="M60" si="99">COUNTIF(Q60:EP60,"a")</f>
@@ -36670,7 +36674,7 @@
       <c r="K62" s="14"/>
       <c r="L62" s="14">
         <f t="shared" ref="L62" si="104">IFERROR(L60+J62,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M62" s="14">
         <f t="shared" ref="M62" si="105">COUNTIF(Q62:EP62,"a")</f>
@@ -37009,7 +37013,7 @@
       <c r="K64" s="14"/>
       <c r="L64" s="14">
         <f t="shared" ref="L64" si="110">IFERROR(L62+J64,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" ref="M64" si="111">COUNTIF(Q64:EP64,"a")</f>
@@ -37341,7 +37345,7 @@
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -37692,7 +37696,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -38025,7 +38029,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -38357,7 +38361,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -38762,7 +38766,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>

</xml_diff>

<commit_message>
Les processus sont trier avec deux liste alerté et ignoré.
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E96EF9-2193-400C-A6FF-DAF026E1450A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF18F39-5F34-42E0-B73C-26C8BF011966}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="99">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -25880,8 +25880,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="BO22" sqref="BO22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28513,7 +28513,9 @@
         <v>31</v>
       </c>
       <c r="E13" s="83"/>
-      <c r="G13" s="84"/>
+      <c r="G13" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H13" s="85" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
@@ -28888,7 +28890,9 @@
       <c r="F15" s="83">
         <v>1</v>
       </c>
-      <c r="G15" s="84"/>
+      <c r="G15" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H15" s="85" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
@@ -29215,7 +29219,9 @@
       <c r="F17" s="83">
         <v>1</v>
       </c>
-      <c r="G17" s="84"/>
+      <c r="G17" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H17" s="85" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
@@ -29547,7 +29553,9 @@
       <c r="F19" s="83">
         <v>1</v>
       </c>
-      <c r="G19" s="84"/>
+      <c r="G19" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H19" s="85" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
@@ -29891,7 +29899,9 @@
       <c r="F21" s="83">
         <v>1</v>
       </c>
-      <c r="G21" s="84"/>
+      <c r="G21" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H21" s="85" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
@@ -30219,7 +30229,9 @@
       <c r="F23" s="83">
         <v>1</v>
       </c>
-      <c r="G23" s="84"/>
+      <c r="G23" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H23" s="85" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
@@ -30548,7 +30560,9 @@
       <c r="F25" s="83">
         <v>1</v>
       </c>
-      <c r="G25" s="84"/>
+      <c r="G25" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H25" s="85" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
@@ -30874,7 +30888,9 @@
       <c r="F27" s="83">
         <v>2</v>
       </c>
-      <c r="G27" s="84"/>
+      <c r="G27" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H27" s="85" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
@@ -31213,7 +31229,9 @@
       <c r="F29" s="83">
         <v>2</v>
       </c>
-      <c r="G29" s="84"/>
+      <c r="G29" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H29" s="85" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v>!</v>
@@ -31567,7 +31585,9 @@
       <c r="F31" s="83">
         <v>2</v>
       </c>
-      <c r="G31" s="84"/>
+      <c r="G31" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H31" s="85" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
@@ -31899,7 +31919,9 @@
       <c r="F33" s="83">
         <v>2</v>
       </c>
-      <c r="G33" s="84"/>
+      <c r="G33" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H33" s="85" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
@@ -32235,7 +32257,9 @@
       <c r="F35" s="83">
         <v>2</v>
       </c>
-      <c r="G35" s="84"/>
+      <c r="G35" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H35" s="85" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
@@ -32570,7 +32594,9 @@
       <c r="F37" s="83">
         <v>2</v>
       </c>
-      <c r="G37" s="84"/>
+      <c r="G37" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H37" s="85" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
@@ -32900,7 +32926,9 @@
       <c r="F39" s="83">
         <v>3</v>
       </c>
-      <c r="G39" s="84"/>
+      <c r="G39" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H39" s="85" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
@@ -33245,7 +33273,9 @@
       <c r="F41" s="83">
         <v>3</v>
       </c>
-      <c r="G41" s="84"/>
+      <c r="G41" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H41" s="85" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
@@ -33575,7 +33605,9 @@
       <c r="F43" s="83">
         <v>3</v>
       </c>
-      <c r="G43" s="84"/>
+      <c r="G43" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H43" s="85" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
@@ -33906,7 +33938,9 @@
       <c r="F45" s="83">
         <v>3</v>
       </c>
-      <c r="G45" s="84"/>
+      <c r="G45" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H45" s="85" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
@@ -33991,12 +34025,12 @@
       </c>
       <c r="J46" s="46">
         <f>IF(D45="","",COUNTIF(Echéancier!$Q46:$EP46,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46" s="14"/>
       <c r="L46" s="14">
         <f t="shared" ref="L46" si="60">IFERROR(L44+J46,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M46" s="14">
         <f t="shared" ref="M46" si="61">COUNTIF(Q46:EP46,"a")</f>
@@ -34008,7 +34042,7 @@
       </c>
       <c r="O46" s="14">
         <f>IFERROR(MATCH("ra",$Q46:$EP46,1),0)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="P46" s="14"/>
       <c r="Q46" s="23"/>
@@ -34056,8 +34090,12 @@
       <c r="BG46" s="34"/>
       <c r="BH46" s="75"/>
       <c r="BI46" s="34"/>
-      <c r="BJ46" s="34"/>
-      <c r="BK46" s="34"/>
+      <c r="BJ46" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BK46" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="BL46" s="34"/>
       <c r="BM46" s="34"/>
       <c r="BN46" s="24"/>
@@ -34233,7 +34271,9 @@
       <c r="F47" s="83">
         <v>3</v>
       </c>
-      <c r="G47" s="84"/>
+      <c r="G47" s="84" t="s">
+        <v>16</v>
+      </c>
       <c r="H47" s="85" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
@@ -34320,7 +34360,7 @@
       <c r="K48" s="14"/>
       <c r="L48" s="14">
         <f>IFERROR(L46+J48,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M48" s="14">
         <f t="shared" ref="M48" si="63">COUNTIF(Q48:EP48,"a")</f>
@@ -34666,7 +34706,7 @@
       <c r="K50" s="14"/>
       <c r="L50" s="14">
         <f t="shared" ref="L50" si="68">IFERROR(L48+J50,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M50" s="14">
         <f t="shared" ref="M50" si="69">COUNTIF(Q50:EP50,"a")</f>
@@ -34997,7 +35037,7 @@
       <c r="K52" s="14"/>
       <c r="L52" s="14">
         <f t="shared" ref="L52" si="74">IFERROR(L50+J52,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M52" s="14">
         <f t="shared" ref="M52" si="75">COUNTIF(Q52:EP52,"a")</f>
@@ -35331,7 +35371,7 @@
       <c r="K54" s="14"/>
       <c r="L54" s="14">
         <f t="shared" ref="L54" si="80">IFERROR(L52+J54,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M54" s="14">
         <f t="shared" ref="M54" si="81">COUNTIF(Q54:EP54,"a")</f>
@@ -35670,7 +35710,7 @@
       <c r="K56" s="14"/>
       <c r="L56" s="14">
         <f t="shared" ref="L56" si="86">IFERROR(L54+J56,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M56" s="14">
         <f t="shared" ref="M56" si="87">COUNTIF(Q56:EP56,"a")</f>
@@ -35997,7 +36037,7 @@
       <c r="K58" s="14"/>
       <c r="L58" s="14">
         <f t="shared" ref="L58" si="92">IFERROR(L56+J58,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M58" s="14">
         <f t="shared" ref="M58" si="93">COUNTIF(Q58:EP58,"a")</f>
@@ -36325,7 +36365,7 @@
       <c r="K60" s="14"/>
       <c r="L60" s="14">
         <f t="shared" ref="L60" si="98">IFERROR(L58+J60,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M60" s="14">
         <f t="shared" ref="M60" si="99">COUNTIF(Q60:EP60,"a")</f>
@@ -36674,7 +36714,7 @@
       <c r="K62" s="14"/>
       <c r="L62" s="14">
         <f t="shared" ref="L62" si="104">IFERROR(L60+J62,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M62" s="14">
         <f t="shared" ref="M62" si="105">COUNTIF(Q62:EP62,"a")</f>
@@ -37013,7 +37053,7 @@
       <c r="K64" s="14"/>
       <c r="L64" s="14">
         <f t="shared" ref="L64" si="110">IFERROR(L62+J64,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" ref="M64" si="111">COUNTIF(Q64:EP64,"a")</f>
@@ -37345,7 +37385,7 @@
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -37696,7 +37736,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -38029,7 +38069,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -38361,7 +38401,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -38766,7 +38806,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>

</xml_diff>

<commit_message>
Les SplitContainer sont partout dans les rues dans les campagnes
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF18F39-5F34-42E0-B73C-26C8BF011966}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C07AD2-004F-4219-97A4-625449D0322D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="99">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -933,43 +933,70 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -978,10 +1005,7 @@
     <xf numFmtId="14" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -990,41 +1014,8 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1047,53 +1038,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -25880,8 +25880,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49:G50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25927,11 +25927,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="Q3" s="112">
+      <c r="Q3" s="109">
         <f>MAX(K13:K163)</f>
         <v>64</v>
       </c>
-      <c r="R3" s="113"/>
+      <c r="R3" s="110"/>
       <c r="S3" s="28" t="s">
         <v>23</v>
       </c>
@@ -25956,11 +25956,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="Q4" s="114">
+      <c r="Q4" s="111">
         <f>MAX(L13:L163)-L12</f>
         <v>36</v>
       </c>
-      <c r="R4" s="115"/>
+      <c r="R4" s="112"/>
       <c r="S4" s="29" t="s">
         <v>24</v>
       </c>
@@ -25977,31 +25977,31 @@
       <c r="AD4" s="26"/>
       <c r="AE4" s="27"/>
       <c r="AI4" s="66"/>
-      <c r="AJ4" s="118" t="s">
+      <c r="AJ4" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="AK4" s="118"/>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="118"/>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118"/>
+      <c r="AK4" s="115"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="118" t="s">
+      <c r="AU4" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118"/>
-      <c r="AZ4" s="118"/>
-      <c r="BA4" s="118"/>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="115"/>
+      <c r="BC4" s="115"/>
+      <c r="BD4" s="115"/>
+      <c r="BE4" s="115"/>
       <c r="BG4" s="8"/>
       <c r="BH4" s="3" t="s">
         <v>2</v>
@@ -26013,11 +26013,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="Q5" s="116">
+      <c r="Q5" s="113">
         <f>MAX(M13:M163)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="117"/>
+      <c r="R5" s="114"/>
       <c r="S5" s="30" t="s">
         <v>25</v>
       </c>
@@ -26034,31 +26034,31 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="12"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="118" t="s">
+      <c r="AJ5" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="118"/>
-      <c r="AM5" s="118"/>
-      <c r="AN5" s="118"/>
-      <c r="AO5" s="118"/>
-      <c r="AP5" s="118"/>
-      <c r="AQ5" s="118"/>
-      <c r="AR5" s="118"/>
+      <c r="AK5" s="115"/>
+      <c r="AL5" s="115"/>
+      <c r="AM5" s="115"/>
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="115"/>
       <c r="AT5" s="65"/>
-      <c r="AU5" s="118" t="s">
+      <c r="AU5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="118"/>
-      <c r="AZ5" s="118"/>
-      <c r="BA5" s="118"/>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="115"/>
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="115"/>
+      <c r="BA5" s="115"/>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="115"/>
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="115"/>
     </row>
     <row r="6" spans="1:226" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -26069,889 +26069,889 @@
     </row>
     <row r="7" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B7" s="69"/>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="108" t="s">
+      <c r="F7" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="108" t="s">
+      <c r="G7" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="108" t="s">
+      <c r="H7" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="105" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="132" t="s">
+      <c r="K7" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="127" t="s">
+      <c r="L7" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="127" t="s">
+      <c r="M7" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="127" t="s">
+      <c r="N7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="127" t="s">
+      <c r="O7" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="124" t="s">
+      <c r="P7" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="123">
+      <c r="Q7" s="95">
         <v>1</v>
       </c>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="91"/>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="101"/>
-      <c r="AA7" s="90">
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="96"/>
+      <c r="V7" s="96"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="97"/>
+      <c r="AA7" s="108">
         <v>2</v>
       </c>
-      <c r="AB7" s="91"/>
-      <c r="AC7" s="91"/>
-      <c r="AD7" s="91"/>
-      <c r="AE7" s="91"/>
-      <c r="AF7" s="91"/>
-      <c r="AG7" s="91"/>
-      <c r="AH7" s="91"/>
-      <c r="AI7" s="91"/>
-      <c r="AJ7" s="101"/>
-      <c r="AK7" s="90">
+      <c r="AB7" s="96"/>
+      <c r="AC7" s="96"/>
+      <c r="AD7" s="96"/>
+      <c r="AE7" s="96"/>
+      <c r="AF7" s="96"/>
+      <c r="AG7" s="96"/>
+      <c r="AH7" s="96"/>
+      <c r="AI7" s="96"/>
+      <c r="AJ7" s="97"/>
+      <c r="AK7" s="108">
         <v>3</v>
       </c>
-      <c r="AL7" s="91"/>
-      <c r="AM7" s="91"/>
-      <c r="AN7" s="91"/>
-      <c r="AO7" s="91"/>
-      <c r="AP7" s="91"/>
-      <c r="AQ7" s="91"/>
-      <c r="AR7" s="91"/>
-      <c r="AS7" s="91"/>
-      <c r="AT7" s="101"/>
-      <c r="AU7" s="90">
+      <c r="AL7" s="96"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="96"/>
+      <c r="AO7" s="96"/>
+      <c r="AP7" s="96"/>
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="96"/>
+      <c r="AS7" s="96"/>
+      <c r="AT7" s="97"/>
+      <c r="AU7" s="108">
         <v>4</v>
       </c>
-      <c r="AV7" s="91"/>
-      <c r="AW7" s="91"/>
-      <c r="AX7" s="91"/>
-      <c r="AY7" s="91"/>
-      <c r="AZ7" s="91"/>
-      <c r="BA7" s="91"/>
-      <c r="BB7" s="91"/>
-      <c r="BC7" s="91"/>
-      <c r="BD7" s="101"/>
-      <c r="BE7" s="90">
+      <c r="AV7" s="96"/>
+      <c r="AW7" s="96"/>
+      <c r="AX7" s="96"/>
+      <c r="AY7" s="96"/>
+      <c r="AZ7" s="96"/>
+      <c r="BA7" s="96"/>
+      <c r="BB7" s="96"/>
+      <c r="BC7" s="96"/>
+      <c r="BD7" s="97"/>
+      <c r="BE7" s="108">
         <v>5</v>
       </c>
-      <c r="BF7" s="91"/>
-      <c r="BG7" s="91"/>
-      <c r="BH7" s="91"/>
-      <c r="BI7" s="91"/>
-      <c r="BJ7" s="91"/>
-      <c r="BK7" s="91"/>
-      <c r="BL7" s="91"/>
-      <c r="BM7" s="91"/>
-      <c r="BN7" s="101"/>
-      <c r="BO7" s="90">
+      <c r="BF7" s="96"/>
+      <c r="BG7" s="96"/>
+      <c r="BH7" s="96"/>
+      <c r="BI7" s="96"/>
+      <c r="BJ7" s="96"/>
+      <c r="BK7" s="96"/>
+      <c r="BL7" s="96"/>
+      <c r="BM7" s="96"/>
+      <c r="BN7" s="97"/>
+      <c r="BO7" s="108">
         <v>6</v>
       </c>
-      <c r="BP7" s="91"/>
-      <c r="BQ7" s="91"/>
-      <c r="BR7" s="91"/>
-      <c r="BS7" s="91"/>
-      <c r="BT7" s="91"/>
-      <c r="BU7" s="91"/>
-      <c r="BV7" s="91"/>
-      <c r="BW7" s="91"/>
-      <c r="BX7" s="101"/>
-      <c r="BY7" s="90">
+      <c r="BP7" s="96"/>
+      <c r="BQ7" s="96"/>
+      <c r="BR7" s="96"/>
+      <c r="BS7" s="96"/>
+      <c r="BT7" s="96"/>
+      <c r="BU7" s="96"/>
+      <c r="BV7" s="96"/>
+      <c r="BW7" s="96"/>
+      <c r="BX7" s="97"/>
+      <c r="BY7" s="108">
         <v>7</v>
       </c>
-      <c r="BZ7" s="91"/>
-      <c r="CA7" s="91"/>
-      <c r="CB7" s="91"/>
-      <c r="CC7" s="91"/>
-      <c r="CD7" s="91"/>
-      <c r="CE7" s="91"/>
-      <c r="CF7" s="91"/>
-      <c r="CG7" s="91"/>
-      <c r="CH7" s="101"/>
-      <c r="CI7" s="90">
+      <c r="BZ7" s="96"/>
+      <c r="CA7" s="96"/>
+      <c r="CB7" s="96"/>
+      <c r="CC7" s="96"/>
+      <c r="CD7" s="96"/>
+      <c r="CE7" s="96"/>
+      <c r="CF7" s="96"/>
+      <c r="CG7" s="96"/>
+      <c r="CH7" s="97"/>
+      <c r="CI7" s="108">
         <v>8</v>
       </c>
-      <c r="CJ7" s="91"/>
-      <c r="CK7" s="91"/>
-      <c r="CL7" s="91"/>
-      <c r="CM7" s="91"/>
-      <c r="CN7" s="91"/>
-      <c r="CO7" s="91"/>
-      <c r="CP7" s="91"/>
-      <c r="CQ7" s="91"/>
-      <c r="CR7" s="101"/>
-      <c r="CS7" s="90">
+      <c r="CJ7" s="96"/>
+      <c r="CK7" s="96"/>
+      <c r="CL7" s="96"/>
+      <c r="CM7" s="96"/>
+      <c r="CN7" s="96"/>
+      <c r="CO7" s="96"/>
+      <c r="CP7" s="96"/>
+      <c r="CQ7" s="96"/>
+      <c r="CR7" s="97"/>
+      <c r="CS7" s="108">
         <v>9</v>
       </c>
-      <c r="CT7" s="91"/>
-      <c r="CU7" s="91"/>
-      <c r="CV7" s="91"/>
-      <c r="CW7" s="91"/>
-      <c r="CX7" s="91"/>
-      <c r="CY7" s="91"/>
-      <c r="CZ7" s="91"/>
-      <c r="DA7" s="91"/>
-      <c r="DB7" s="91"/>
-      <c r="DC7" s="90">
+      <c r="CT7" s="96"/>
+      <c r="CU7" s="96"/>
+      <c r="CV7" s="96"/>
+      <c r="CW7" s="96"/>
+      <c r="CX7" s="96"/>
+      <c r="CY7" s="96"/>
+      <c r="CZ7" s="96"/>
+      <c r="DA7" s="96"/>
+      <c r="DB7" s="96"/>
+      <c r="DC7" s="108">
         <v>10</v>
       </c>
-      <c r="DD7" s="91"/>
-      <c r="DE7" s="91"/>
-      <c r="DF7" s="91"/>
-      <c r="DG7" s="91"/>
-      <c r="DH7" s="91"/>
-      <c r="DI7" s="91"/>
-      <c r="DJ7" s="91"/>
-      <c r="DK7" s="91"/>
-      <c r="DL7" s="101"/>
-      <c r="DM7" s="90">
+      <c r="DD7" s="96"/>
+      <c r="DE7" s="96"/>
+      <c r="DF7" s="96"/>
+      <c r="DG7" s="96"/>
+      <c r="DH7" s="96"/>
+      <c r="DI7" s="96"/>
+      <c r="DJ7" s="96"/>
+      <c r="DK7" s="96"/>
+      <c r="DL7" s="97"/>
+      <c r="DM7" s="108">
         <v>11</v>
       </c>
-      <c r="DN7" s="91"/>
-      <c r="DO7" s="91"/>
-      <c r="DP7" s="91"/>
-      <c r="DQ7" s="91"/>
-      <c r="DR7" s="91"/>
-      <c r="DS7" s="91"/>
-      <c r="DT7" s="91"/>
-      <c r="DU7" s="91"/>
-      <c r="DV7" s="101"/>
-      <c r="DW7" s="90">
+      <c r="DN7" s="96"/>
+      <c r="DO7" s="96"/>
+      <c r="DP7" s="96"/>
+      <c r="DQ7" s="96"/>
+      <c r="DR7" s="96"/>
+      <c r="DS7" s="96"/>
+      <c r="DT7" s="96"/>
+      <c r="DU7" s="96"/>
+      <c r="DV7" s="97"/>
+      <c r="DW7" s="108">
         <v>12</v>
       </c>
-      <c r="DX7" s="91"/>
-      <c r="DY7" s="91"/>
-      <c r="DZ7" s="91"/>
-      <c r="EA7" s="91"/>
-      <c r="EB7" s="91"/>
-      <c r="EC7" s="91"/>
-      <c r="ED7" s="91"/>
-      <c r="EE7" s="91"/>
-      <c r="EF7" s="101"/>
-      <c r="EG7" s="90">
+      <c r="DX7" s="96"/>
+      <c r="DY7" s="96"/>
+      <c r="DZ7" s="96"/>
+      <c r="EA7" s="96"/>
+      <c r="EB7" s="96"/>
+      <c r="EC7" s="96"/>
+      <c r="ED7" s="96"/>
+      <c r="EE7" s="96"/>
+      <c r="EF7" s="97"/>
+      <c r="EG7" s="108">
         <v>13</v>
       </c>
-      <c r="EH7" s="91"/>
-      <c r="EI7" s="91"/>
-      <c r="EJ7" s="91"/>
-      <c r="EK7" s="91"/>
-      <c r="EL7" s="91"/>
-      <c r="EM7" s="91"/>
-      <c r="EN7" s="91"/>
-      <c r="EO7" s="91"/>
-      <c r="EP7" s="92"/>
-      <c r="EQ7" s="91">
+      <c r="EH7" s="96"/>
+      <c r="EI7" s="96"/>
+      <c r="EJ7" s="96"/>
+      <c r="EK7" s="96"/>
+      <c r="EL7" s="96"/>
+      <c r="EM7" s="96"/>
+      <c r="EN7" s="96"/>
+      <c r="EO7" s="96"/>
+      <c r="EP7" s="126"/>
+      <c r="EQ7" s="96">
         <v>14</v>
       </c>
-      <c r="ER7" s="91"/>
-      <c r="ES7" s="91"/>
-      <c r="ET7" s="91"/>
-      <c r="EU7" s="91"/>
-      <c r="EV7" s="91"/>
-      <c r="EW7" s="91"/>
-      <c r="EX7" s="91"/>
-      <c r="EY7" s="91"/>
-      <c r="EZ7" s="101"/>
-      <c r="FA7" s="90">
+      <c r="ER7" s="96"/>
+      <c r="ES7" s="96"/>
+      <c r="ET7" s="96"/>
+      <c r="EU7" s="96"/>
+      <c r="EV7" s="96"/>
+      <c r="EW7" s="96"/>
+      <c r="EX7" s="96"/>
+      <c r="EY7" s="96"/>
+      <c r="EZ7" s="97"/>
+      <c r="FA7" s="108">
         <v>15</v>
       </c>
-      <c r="FB7" s="91"/>
-      <c r="FC7" s="91"/>
-      <c r="FD7" s="91"/>
-      <c r="FE7" s="91"/>
-      <c r="FF7" s="91"/>
-      <c r="FG7" s="91"/>
-      <c r="FH7" s="91"/>
-      <c r="FI7" s="91"/>
-      <c r="FJ7" s="101"/>
-      <c r="FK7" s="90">
+      <c r="FB7" s="96"/>
+      <c r="FC7" s="96"/>
+      <c r="FD7" s="96"/>
+      <c r="FE7" s="96"/>
+      <c r="FF7" s="96"/>
+      <c r="FG7" s="96"/>
+      <c r="FH7" s="96"/>
+      <c r="FI7" s="96"/>
+      <c r="FJ7" s="97"/>
+      <c r="FK7" s="108">
         <v>16</v>
       </c>
-      <c r="FL7" s="91"/>
-      <c r="FM7" s="91"/>
-      <c r="FN7" s="91"/>
-      <c r="FO7" s="91"/>
-      <c r="FP7" s="91"/>
-      <c r="FQ7" s="91"/>
-      <c r="FR7" s="91"/>
-      <c r="FS7" s="91"/>
-      <c r="FT7" s="101"/>
-      <c r="FU7" s="90">
+      <c r="FL7" s="96"/>
+      <c r="FM7" s="96"/>
+      <c r="FN7" s="96"/>
+      <c r="FO7" s="96"/>
+      <c r="FP7" s="96"/>
+      <c r="FQ7" s="96"/>
+      <c r="FR7" s="96"/>
+      <c r="FS7" s="96"/>
+      <c r="FT7" s="97"/>
+      <c r="FU7" s="108">
         <v>17</v>
       </c>
-      <c r="FV7" s="91"/>
-      <c r="FW7" s="91"/>
-      <c r="FX7" s="91"/>
-      <c r="FY7" s="91"/>
-      <c r="FZ7" s="91"/>
-      <c r="GA7" s="91"/>
-      <c r="GB7" s="91"/>
-      <c r="GC7" s="91"/>
-      <c r="GD7" s="101"/>
-      <c r="GE7" s="90">
+      <c r="FV7" s="96"/>
+      <c r="FW7" s="96"/>
+      <c r="FX7" s="96"/>
+      <c r="FY7" s="96"/>
+      <c r="FZ7" s="96"/>
+      <c r="GA7" s="96"/>
+      <c r="GB7" s="96"/>
+      <c r="GC7" s="96"/>
+      <c r="GD7" s="97"/>
+      <c r="GE7" s="108">
         <v>18</v>
       </c>
-      <c r="GF7" s="91"/>
-      <c r="GG7" s="91"/>
-      <c r="GH7" s="91"/>
-      <c r="GI7" s="91"/>
-      <c r="GJ7" s="91"/>
-      <c r="GK7" s="91"/>
-      <c r="GL7" s="91"/>
-      <c r="GM7" s="91"/>
-      <c r="GN7" s="101"/>
-      <c r="GO7" s="90">
+      <c r="GF7" s="96"/>
+      <c r="GG7" s="96"/>
+      <c r="GH7" s="96"/>
+      <c r="GI7" s="96"/>
+      <c r="GJ7" s="96"/>
+      <c r="GK7" s="96"/>
+      <c r="GL7" s="96"/>
+      <c r="GM7" s="96"/>
+      <c r="GN7" s="97"/>
+      <c r="GO7" s="108">
         <v>19</v>
       </c>
-      <c r="GP7" s="91"/>
-      <c r="GQ7" s="91"/>
-      <c r="GR7" s="91"/>
-      <c r="GS7" s="91"/>
-      <c r="GT7" s="91"/>
-      <c r="GU7" s="91"/>
-      <c r="GV7" s="91"/>
-      <c r="GW7" s="91"/>
-      <c r="GX7" s="101"/>
-      <c r="GY7" s="90">
+      <c r="GP7" s="96"/>
+      <c r="GQ7" s="96"/>
+      <c r="GR7" s="96"/>
+      <c r="GS7" s="96"/>
+      <c r="GT7" s="96"/>
+      <c r="GU7" s="96"/>
+      <c r="GV7" s="96"/>
+      <c r="GW7" s="96"/>
+      <c r="GX7" s="97"/>
+      <c r="GY7" s="108">
         <v>20</v>
       </c>
-      <c r="GZ7" s="91"/>
-      <c r="HA7" s="91"/>
-      <c r="HB7" s="91"/>
-      <c r="HC7" s="91"/>
-      <c r="HD7" s="91"/>
-      <c r="HE7" s="91"/>
-      <c r="HF7" s="91"/>
-      <c r="HG7" s="91"/>
-      <c r="HH7" s="101"/>
-      <c r="HI7" s="90">
+      <c r="GZ7" s="96"/>
+      <c r="HA7" s="96"/>
+      <c r="HB7" s="96"/>
+      <c r="HC7" s="96"/>
+      <c r="HD7" s="96"/>
+      <c r="HE7" s="96"/>
+      <c r="HF7" s="96"/>
+      <c r="HG7" s="96"/>
+      <c r="HH7" s="97"/>
+      <c r="HI7" s="108">
         <v>21</v>
       </c>
-      <c r="HJ7" s="91"/>
-      <c r="HK7" s="91"/>
-      <c r="HL7" s="91"/>
-      <c r="HM7" s="91"/>
-      <c r="HN7" s="91"/>
-      <c r="HO7" s="91"/>
-      <c r="HP7" s="91"/>
-      <c r="HQ7" s="91"/>
-      <c r="HR7" s="92"/>
+      <c r="HJ7" s="96"/>
+      <c r="HK7" s="96"/>
+      <c r="HL7" s="96"/>
+      <c r="HM7" s="96"/>
+      <c r="HN7" s="96"/>
+      <c r="HO7" s="96"/>
+      <c r="HP7" s="96"/>
+      <c r="HQ7" s="96"/>
+      <c r="HR7" s="126"/>
     </row>
     <row r="8" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="128"/>
-      <c r="M8" s="128"/>
-      <c r="N8" s="128"/>
-      <c r="O8" s="128"/>
-      <c r="P8" s="125"/>
-      <c r="Q8" s="130">
+      <c r="D8" s="124"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="102">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],Q7),"")</f>
         <v>45040</v>
       </c>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
-      <c r="U8" s="94"/>
-      <c r="V8" s="94"/>
-      <c r="W8" s="94"/>
-      <c r="X8" s="94"/>
-      <c r="Y8" s="94"/>
-      <c r="Z8" s="95"/>
-      <c r="AA8" s="93">
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="103"/>
+      <c r="Z8" s="104"/>
+      <c r="AA8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AA7),"")</f>
         <v>45041</v>
       </c>
-      <c r="AB8" s="94"/>
-      <c r="AC8" s="94"/>
-      <c r="AD8" s="94"/>
-      <c r="AE8" s="94"/>
-      <c r="AF8" s="94"/>
-      <c r="AG8" s="94"/>
-      <c r="AH8" s="94"/>
-      <c r="AI8" s="94"/>
-      <c r="AJ8" s="95"/>
-      <c r="AK8" s="93">
+      <c r="AB8" s="103"/>
+      <c r="AC8" s="103"/>
+      <c r="AD8" s="103"/>
+      <c r="AE8" s="103"/>
+      <c r="AF8" s="103"/>
+      <c r="AG8" s="103"/>
+      <c r="AH8" s="103"/>
+      <c r="AI8" s="103"/>
+      <c r="AJ8" s="104"/>
+      <c r="AK8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AK7),"")</f>
         <v>45042</v>
       </c>
-      <c r="AL8" s="94"/>
-      <c r="AM8" s="94"/>
-      <c r="AN8" s="94"/>
-      <c r="AO8" s="94"/>
-      <c r="AP8" s="94"/>
-      <c r="AQ8" s="94"/>
-      <c r="AR8" s="94"/>
-      <c r="AS8" s="94"/>
-      <c r="AT8" s="95"/>
-      <c r="AU8" s="93">
+      <c r="AL8" s="103"/>
+      <c r="AM8" s="103"/>
+      <c r="AN8" s="103"/>
+      <c r="AO8" s="103"/>
+      <c r="AP8" s="103"/>
+      <c r="AQ8" s="103"/>
+      <c r="AR8" s="103"/>
+      <c r="AS8" s="103"/>
+      <c r="AT8" s="104"/>
+      <c r="AU8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AU7),"")</f>
         <v>45048</v>
       </c>
-      <c r="AV8" s="94"/>
-      <c r="AW8" s="94"/>
-      <c r="AX8" s="94"/>
-      <c r="AY8" s="94"/>
-      <c r="AZ8" s="94"/>
-      <c r="BA8" s="94"/>
-      <c r="BB8" s="94"/>
-      <c r="BC8" s="94"/>
-      <c r="BD8" s="95"/>
-      <c r="BE8" s="93">
+      <c r="AV8" s="103"/>
+      <c r="AW8" s="103"/>
+      <c r="AX8" s="103"/>
+      <c r="AY8" s="103"/>
+      <c r="AZ8" s="103"/>
+      <c r="BA8" s="103"/>
+      <c r="BB8" s="103"/>
+      <c r="BC8" s="103"/>
+      <c r="BD8" s="104"/>
+      <c r="BE8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BE7),"")</f>
         <v>45049</v>
       </c>
-      <c r="BF8" s="94"/>
-      <c r="BG8" s="94"/>
-      <c r="BH8" s="94"/>
-      <c r="BI8" s="94"/>
-      <c r="BJ8" s="94"/>
-      <c r="BK8" s="94"/>
-      <c r="BL8" s="94"/>
-      <c r="BM8" s="94"/>
-      <c r="BN8" s="95"/>
-      <c r="BO8" s="93">
+      <c r="BF8" s="103"/>
+      <c r="BG8" s="103"/>
+      <c r="BH8" s="103"/>
+      <c r="BI8" s="103"/>
+      <c r="BJ8" s="103"/>
+      <c r="BK8" s="103"/>
+      <c r="BL8" s="103"/>
+      <c r="BM8" s="103"/>
+      <c r="BN8" s="104"/>
+      <c r="BO8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BO7),"")</f>
         <v>45054</v>
       </c>
-      <c r="BP8" s="94"/>
-      <c r="BQ8" s="94"/>
-      <c r="BR8" s="94"/>
-      <c r="BS8" s="94"/>
-      <c r="BT8" s="94"/>
-      <c r="BU8" s="94"/>
-      <c r="BV8" s="94"/>
-      <c r="BW8" s="94"/>
-      <c r="BX8" s="95"/>
-      <c r="BY8" s="93">
+      <c r="BP8" s="103"/>
+      <c r="BQ8" s="103"/>
+      <c r="BR8" s="103"/>
+      <c r="BS8" s="103"/>
+      <c r="BT8" s="103"/>
+      <c r="BU8" s="103"/>
+      <c r="BV8" s="103"/>
+      <c r="BW8" s="103"/>
+      <c r="BX8" s="104"/>
+      <c r="BY8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BY7),"")</f>
         <v>45055</v>
       </c>
-      <c r="BZ8" s="94"/>
-      <c r="CA8" s="94"/>
-      <c r="CB8" s="94"/>
-      <c r="CC8" s="94"/>
-      <c r="CD8" s="94"/>
-      <c r="CE8" s="94"/>
-      <c r="CF8" s="94"/>
-      <c r="CG8" s="94"/>
-      <c r="CH8" s="95"/>
-      <c r="CI8" s="93">
+      <c r="BZ8" s="103"/>
+      <c r="CA8" s="103"/>
+      <c r="CB8" s="103"/>
+      <c r="CC8" s="103"/>
+      <c r="CD8" s="103"/>
+      <c r="CE8" s="103"/>
+      <c r="CF8" s="103"/>
+      <c r="CG8" s="103"/>
+      <c r="CH8" s="104"/>
+      <c r="CI8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CI7),"")</f>
         <v>45056</v>
       </c>
-      <c r="CJ8" s="94"/>
-      <c r="CK8" s="94"/>
-      <c r="CL8" s="94"/>
-      <c r="CM8" s="94"/>
-      <c r="CN8" s="94"/>
-      <c r="CO8" s="94"/>
-      <c r="CP8" s="94"/>
-      <c r="CQ8" s="94"/>
-      <c r="CR8" s="95"/>
-      <c r="CS8" s="93">
+      <c r="CJ8" s="103"/>
+      <c r="CK8" s="103"/>
+      <c r="CL8" s="103"/>
+      <c r="CM8" s="103"/>
+      <c r="CN8" s="103"/>
+      <c r="CO8" s="103"/>
+      <c r="CP8" s="103"/>
+      <c r="CQ8" s="103"/>
+      <c r="CR8" s="104"/>
+      <c r="CS8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CS7),"")</f>
         <v>45061</v>
       </c>
-      <c r="CT8" s="94"/>
-      <c r="CU8" s="94"/>
-      <c r="CV8" s="94"/>
-      <c r="CW8" s="94"/>
-      <c r="CX8" s="94"/>
-      <c r="CY8" s="94"/>
-      <c r="CZ8" s="94"/>
-      <c r="DA8" s="94"/>
-      <c r="DB8" s="94"/>
-      <c r="DC8" s="93">
+      <c r="CT8" s="103"/>
+      <c r="CU8" s="103"/>
+      <c r="CV8" s="103"/>
+      <c r="CW8" s="103"/>
+      <c r="CX8" s="103"/>
+      <c r="CY8" s="103"/>
+      <c r="CZ8" s="103"/>
+      <c r="DA8" s="103"/>
+      <c r="DB8" s="103"/>
+      <c r="DC8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DC7),"")</f>
         <v>45062</v>
       </c>
-      <c r="DD8" s="94"/>
-      <c r="DE8" s="94"/>
-      <c r="DF8" s="94"/>
-      <c r="DG8" s="94"/>
-      <c r="DH8" s="94"/>
-      <c r="DI8" s="94"/>
-      <c r="DJ8" s="94"/>
-      <c r="DK8" s="94"/>
-      <c r="DL8" s="95"/>
-      <c r="DM8" s="93">
+      <c r="DD8" s="103"/>
+      <c r="DE8" s="103"/>
+      <c r="DF8" s="103"/>
+      <c r="DG8" s="103"/>
+      <c r="DH8" s="103"/>
+      <c r="DI8" s="103"/>
+      <c r="DJ8" s="103"/>
+      <c r="DK8" s="103"/>
+      <c r="DL8" s="104"/>
+      <c r="DM8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DM7),"")</f>
         <v>45063</v>
       </c>
-      <c r="DN8" s="94"/>
-      <c r="DO8" s="94"/>
-      <c r="DP8" s="94"/>
-      <c r="DQ8" s="94"/>
-      <c r="DR8" s="94"/>
-      <c r="DS8" s="94"/>
-      <c r="DT8" s="94"/>
-      <c r="DU8" s="94"/>
-      <c r="DV8" s="95"/>
-      <c r="DW8" s="93" t="str">
+      <c r="DN8" s="103"/>
+      <c r="DO8" s="103"/>
+      <c r="DP8" s="103"/>
+      <c r="DQ8" s="103"/>
+      <c r="DR8" s="103"/>
+      <c r="DS8" s="103"/>
+      <c r="DT8" s="103"/>
+      <c r="DU8" s="103"/>
+      <c r="DV8" s="104"/>
+      <c r="DW8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DW7),"")</f>
         <v/>
       </c>
-      <c r="DX8" s="94"/>
-      <c r="DY8" s="94"/>
-      <c r="DZ8" s="94"/>
-      <c r="EA8" s="94"/>
-      <c r="EB8" s="94"/>
-      <c r="EC8" s="94"/>
-      <c r="ED8" s="94"/>
-      <c r="EE8" s="94"/>
-      <c r="EF8" s="95"/>
-      <c r="EG8" s="93" t="str">
+      <c r="DX8" s="103"/>
+      <c r="DY8" s="103"/>
+      <c r="DZ8" s="103"/>
+      <c r="EA8" s="103"/>
+      <c r="EB8" s="103"/>
+      <c r="EC8" s="103"/>
+      <c r="ED8" s="103"/>
+      <c r="EE8" s="103"/>
+      <c r="EF8" s="104"/>
+      <c r="EG8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EG7),"")</f>
         <v/>
       </c>
-      <c r="EH8" s="94"/>
-      <c r="EI8" s="94"/>
-      <c r="EJ8" s="94"/>
-      <c r="EK8" s="94"/>
-      <c r="EL8" s="94"/>
-      <c r="EM8" s="94"/>
-      <c r="EN8" s="94"/>
-      <c r="EO8" s="94"/>
-      <c r="EP8" s="96"/>
-      <c r="EQ8" s="94" t="str">
+      <c r="EH8" s="103"/>
+      <c r="EI8" s="103"/>
+      <c r="EJ8" s="103"/>
+      <c r="EK8" s="103"/>
+      <c r="EL8" s="103"/>
+      <c r="EM8" s="103"/>
+      <c r="EN8" s="103"/>
+      <c r="EO8" s="103"/>
+      <c r="EP8" s="118"/>
+      <c r="EQ8" s="103" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EQ7),"")</f>
         <v/>
       </c>
-      <c r="ER8" s="94"/>
-      <c r="ES8" s="94"/>
-      <c r="ET8" s="94"/>
-      <c r="EU8" s="94"/>
-      <c r="EV8" s="94"/>
-      <c r="EW8" s="94"/>
-      <c r="EX8" s="94"/>
-      <c r="EY8" s="94"/>
-      <c r="EZ8" s="95"/>
-      <c r="FA8" s="93" t="str">
+      <c r="ER8" s="103"/>
+      <c r="ES8" s="103"/>
+      <c r="ET8" s="103"/>
+      <c r="EU8" s="103"/>
+      <c r="EV8" s="103"/>
+      <c r="EW8" s="103"/>
+      <c r="EX8" s="103"/>
+      <c r="EY8" s="103"/>
+      <c r="EZ8" s="104"/>
+      <c r="FA8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FA7),"")</f>
         <v/>
       </c>
-      <c r="FB8" s="94"/>
-      <c r="FC8" s="94"/>
-      <c r="FD8" s="94"/>
-      <c r="FE8" s="94"/>
-      <c r="FF8" s="94"/>
-      <c r="FG8" s="94"/>
-      <c r="FH8" s="94"/>
-      <c r="FI8" s="94"/>
-      <c r="FJ8" s="95"/>
-      <c r="FK8" s="93" t="str">
+      <c r="FB8" s="103"/>
+      <c r="FC8" s="103"/>
+      <c r="FD8" s="103"/>
+      <c r="FE8" s="103"/>
+      <c r="FF8" s="103"/>
+      <c r="FG8" s="103"/>
+      <c r="FH8" s="103"/>
+      <c r="FI8" s="103"/>
+      <c r="FJ8" s="104"/>
+      <c r="FK8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FK7),"")</f>
         <v/>
       </c>
-      <c r="FL8" s="94"/>
-      <c r="FM8" s="94"/>
-      <c r="FN8" s="94"/>
-      <c r="FO8" s="94"/>
-      <c r="FP8" s="94"/>
-      <c r="FQ8" s="94"/>
-      <c r="FR8" s="94"/>
-      <c r="FS8" s="94"/>
-      <c r="FT8" s="95"/>
-      <c r="FU8" s="93" t="str">
+      <c r="FL8" s="103"/>
+      <c r="FM8" s="103"/>
+      <c r="FN8" s="103"/>
+      <c r="FO8" s="103"/>
+      <c r="FP8" s="103"/>
+      <c r="FQ8" s="103"/>
+      <c r="FR8" s="103"/>
+      <c r="FS8" s="103"/>
+      <c r="FT8" s="104"/>
+      <c r="FU8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FU7),"")</f>
         <v/>
       </c>
-      <c r="FV8" s="94"/>
-      <c r="FW8" s="94"/>
-      <c r="FX8" s="94"/>
-      <c r="FY8" s="94"/>
-      <c r="FZ8" s="94"/>
-      <c r="GA8" s="94"/>
-      <c r="GB8" s="94"/>
-      <c r="GC8" s="94"/>
-      <c r="GD8" s="95"/>
-      <c r="GE8" s="93" t="str">
+      <c r="FV8" s="103"/>
+      <c r="FW8" s="103"/>
+      <c r="FX8" s="103"/>
+      <c r="FY8" s="103"/>
+      <c r="FZ8" s="103"/>
+      <c r="GA8" s="103"/>
+      <c r="GB8" s="103"/>
+      <c r="GC8" s="103"/>
+      <c r="GD8" s="104"/>
+      <c r="GE8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GE7),"")</f>
         <v/>
       </c>
-      <c r="GF8" s="94"/>
-      <c r="GG8" s="94"/>
-      <c r="GH8" s="94"/>
-      <c r="GI8" s="94"/>
-      <c r="GJ8" s="94"/>
-      <c r="GK8" s="94"/>
-      <c r="GL8" s="94"/>
-      <c r="GM8" s="94"/>
-      <c r="GN8" s="95"/>
-      <c r="GO8" s="93" t="str">
+      <c r="GF8" s="103"/>
+      <c r="GG8" s="103"/>
+      <c r="GH8" s="103"/>
+      <c r="GI8" s="103"/>
+      <c r="GJ8" s="103"/>
+      <c r="GK8" s="103"/>
+      <c r="GL8" s="103"/>
+      <c r="GM8" s="103"/>
+      <c r="GN8" s="104"/>
+      <c r="GO8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GO7),"")</f>
         <v/>
       </c>
-      <c r="GP8" s="94"/>
-      <c r="GQ8" s="94"/>
-      <c r="GR8" s="94"/>
-      <c r="GS8" s="94"/>
-      <c r="GT8" s="94"/>
-      <c r="GU8" s="94"/>
-      <c r="GV8" s="94"/>
-      <c r="GW8" s="94"/>
-      <c r="GX8" s="95"/>
-      <c r="GY8" s="93" t="str">
+      <c r="GP8" s="103"/>
+      <c r="GQ8" s="103"/>
+      <c r="GR8" s="103"/>
+      <c r="GS8" s="103"/>
+      <c r="GT8" s="103"/>
+      <c r="GU8" s="103"/>
+      <c r="GV8" s="103"/>
+      <c r="GW8" s="103"/>
+      <c r="GX8" s="104"/>
+      <c r="GY8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GY7),"")</f>
         <v/>
       </c>
-      <c r="GZ8" s="94"/>
-      <c r="HA8" s="94"/>
-      <c r="HB8" s="94"/>
-      <c r="HC8" s="94"/>
-      <c r="HD8" s="94"/>
-      <c r="HE8" s="94"/>
-      <c r="HF8" s="94"/>
-      <c r="HG8" s="94"/>
-      <c r="HH8" s="95"/>
-      <c r="HI8" s="93" t="str">
+      <c r="GZ8" s="103"/>
+      <c r="HA8" s="103"/>
+      <c r="HB8" s="103"/>
+      <c r="HC8" s="103"/>
+      <c r="HD8" s="103"/>
+      <c r="HE8" s="103"/>
+      <c r="HF8" s="103"/>
+      <c r="HG8" s="103"/>
+      <c r="HH8" s="104"/>
+      <c r="HI8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],HI7),"")</f>
         <v/>
       </c>
-      <c r="HJ8" s="94"/>
-      <c r="HK8" s="94"/>
-      <c r="HL8" s="94"/>
-      <c r="HM8" s="94"/>
-      <c r="HN8" s="94"/>
-      <c r="HO8" s="94"/>
-      <c r="HP8" s="94"/>
-      <c r="HQ8" s="94"/>
-      <c r="HR8" s="96"/>
+      <c r="HJ8" s="103"/>
+      <c r="HK8" s="103"/>
+      <c r="HL8" s="103"/>
+      <c r="HM8" s="103"/>
+      <c r="HN8" s="103"/>
+      <c r="HO8" s="103"/>
+      <c r="HP8" s="103"/>
+      <c r="HQ8" s="103"/>
+      <c r="HR8" s="118"/>
     </row>
     <row r="9" spans="1:226" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="133"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="131">
+      <c r="D9" s="124"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="99"/>
+      <c r="Q9" s="105">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(Q8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="98"/>
-      <c r="Z9" s="99"/>
-      <c r="AA9" s="97" t="str">
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="106"/>
+      <c r="V9" s="106"/>
+      <c r="W9" s="106"/>
+      <c r="X9" s="106"/>
+      <c r="Y9" s="106"/>
+      <c r="Z9" s="107"/>
+      <c r="AA9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L1] Connexion</v>
       </c>
-      <c r="AB9" s="98"/>
-      <c r="AC9" s="98"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="98"/>
-      <c r="AF9" s="98"/>
-      <c r="AG9" s="98"/>
-      <c r="AH9" s="98"/>
-      <c r="AI9" s="98"/>
-      <c r="AJ9" s="99"/>
-      <c r="AK9" s="97">
+      <c r="AB9" s="106"/>
+      <c r="AC9" s="106"/>
+      <c r="AD9" s="106"/>
+      <c r="AE9" s="106"/>
+      <c r="AF9" s="106"/>
+      <c r="AG9" s="106"/>
+      <c r="AH9" s="106"/>
+      <c r="AI9" s="106"/>
+      <c r="AJ9" s="107"/>
+      <c r="AK9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="98"/>
-      <c r="AM9" s="98"/>
-      <c r="AN9" s="98"/>
-      <c r="AO9" s="98"/>
-      <c r="AP9" s="98"/>
-      <c r="AQ9" s="98"/>
-      <c r="AR9" s="98"/>
-      <c r="AS9" s="98"/>
-      <c r="AT9" s="99"/>
-      <c r="AU9" s="97" t="str">
+      <c r="AL9" s="106"/>
+      <c r="AM9" s="106"/>
+      <c r="AN9" s="106"/>
+      <c r="AO9" s="106"/>
+      <c r="AP9" s="106"/>
+      <c r="AQ9" s="106"/>
+      <c r="AR9" s="106"/>
+      <c r="AS9" s="106"/>
+      <c r="AT9" s="107"/>
+      <c r="AU9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L2] Affichage Professeur</v>
       </c>
-      <c r="AV9" s="98"/>
-      <c r="AW9" s="98"/>
-      <c r="AX9" s="98"/>
-      <c r="AY9" s="98"/>
-      <c r="AZ9" s="98"/>
-      <c r="BA9" s="98"/>
-      <c r="BB9" s="98"/>
-      <c r="BC9" s="98"/>
-      <c r="BD9" s="99"/>
-      <c r="BE9" s="97">
+      <c r="AV9" s="106"/>
+      <c r="AW9" s="106"/>
+      <c r="AX9" s="106"/>
+      <c r="AY9" s="106"/>
+      <c r="AZ9" s="106"/>
+      <c r="BA9" s="106"/>
+      <c r="BB9" s="106"/>
+      <c r="BC9" s="106"/>
+      <c r="BD9" s="107"/>
+      <c r="BE9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BF9" s="98"/>
-      <c r="BG9" s="98"/>
-      <c r="BH9" s="98"/>
-      <c r="BI9" s="98"/>
-      <c r="BJ9" s="98"/>
-      <c r="BK9" s="98"/>
-      <c r="BL9" s="98"/>
-      <c r="BM9" s="98"/>
-      <c r="BN9" s="99"/>
-      <c r="BO9" s="97" t="str">
+      <c r="BF9" s="106"/>
+      <c r="BG9" s="106"/>
+      <c r="BH9" s="106"/>
+      <c r="BI9" s="106"/>
+      <c r="BJ9" s="106"/>
+      <c r="BK9" s="106"/>
+      <c r="BL9" s="106"/>
+      <c r="BM9" s="106"/>
+      <c r="BN9" s="107"/>
+      <c r="BO9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L3] Historique</v>
       </c>
-      <c r="BP9" s="98"/>
-      <c r="BQ9" s="98"/>
-      <c r="BR9" s="98"/>
-      <c r="BS9" s="98"/>
-      <c r="BT9" s="98"/>
-      <c r="BU9" s="98"/>
-      <c r="BV9" s="98"/>
-      <c r="BW9" s="98"/>
-      <c r="BX9" s="99"/>
-      <c r="BY9" s="97">
+      <c r="BP9" s="106"/>
+      <c r="BQ9" s="106"/>
+      <c r="BR9" s="106"/>
+      <c r="BS9" s="106"/>
+      <c r="BT9" s="106"/>
+      <c r="BU9" s="106"/>
+      <c r="BV9" s="106"/>
+      <c r="BW9" s="106"/>
+      <c r="BX9" s="107"/>
+      <c r="BY9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BZ9" s="98"/>
-      <c r="CA9" s="98"/>
-      <c r="CB9" s="98"/>
-      <c r="CC9" s="98"/>
-      <c r="CD9" s="98"/>
-      <c r="CE9" s="98"/>
-      <c r="CF9" s="98"/>
-      <c r="CG9" s="98"/>
-      <c r="CH9" s="99"/>
-      <c r="CI9" s="97" t="str">
+      <c r="BZ9" s="106"/>
+      <c r="CA9" s="106"/>
+      <c r="CB9" s="106"/>
+      <c r="CC9" s="106"/>
+      <c r="CD9" s="106"/>
+      <c r="CE9" s="106"/>
+      <c r="CF9" s="106"/>
+      <c r="CG9" s="106"/>
+      <c r="CH9" s="107"/>
+      <c r="CI9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L4] Filtrage</v>
       </c>
-      <c r="CJ9" s="98"/>
-      <c r="CK9" s="98"/>
-      <c r="CL9" s="98"/>
-      <c r="CM9" s="98"/>
-      <c r="CN9" s="98"/>
-      <c r="CO9" s="98"/>
-      <c r="CP9" s="98"/>
-      <c r="CQ9" s="98"/>
-      <c r="CR9" s="99"/>
-      <c r="CS9" s="97" t="str">
+      <c r="CJ9" s="106"/>
+      <c r="CK9" s="106"/>
+      <c r="CL9" s="106"/>
+      <c r="CM9" s="106"/>
+      <c r="CN9" s="106"/>
+      <c r="CO9" s="106"/>
+      <c r="CP9" s="106"/>
+      <c r="CQ9" s="106"/>
+      <c r="CR9" s="107"/>
+      <c r="CS9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CS8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L5] Streaming multicast</v>
       </c>
-      <c r="CT9" s="98"/>
-      <c r="CU9" s="98"/>
-      <c r="CV9" s="98"/>
-      <c r="CW9" s="98"/>
-      <c r="CX9" s="98"/>
-      <c r="CY9" s="98"/>
-      <c r="CZ9" s="98"/>
-      <c r="DA9" s="98"/>
-      <c r="DB9" s="98"/>
-      <c r="DC9" s="97">
+      <c r="CT9" s="106"/>
+      <c r="CU9" s="106"/>
+      <c r="CV9" s="106"/>
+      <c r="CW9" s="106"/>
+      <c r="CX9" s="106"/>
+      <c r="CY9" s="106"/>
+      <c r="CZ9" s="106"/>
+      <c r="DA9" s="106"/>
+      <c r="DB9" s="106"/>
+      <c r="DC9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DC8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DD9" s="98"/>
-      <c r="DE9" s="98"/>
-      <c r="DF9" s="98"/>
-      <c r="DG9" s="98"/>
-      <c r="DH9" s="98"/>
-      <c r="DI9" s="98"/>
-      <c r="DJ9" s="98"/>
-      <c r="DK9" s="98"/>
-      <c r="DL9" s="99"/>
-      <c r="DM9" s="97" t="str">
+      <c r="DD9" s="106"/>
+      <c r="DE9" s="106"/>
+      <c r="DF9" s="106"/>
+      <c r="DG9" s="106"/>
+      <c r="DH9" s="106"/>
+      <c r="DI9" s="106"/>
+      <c r="DJ9" s="106"/>
+      <c r="DK9" s="106"/>
+      <c r="DL9" s="107"/>
+      <c r="DM9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DM8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L6] Contrôle à distance</v>
       </c>
-      <c r="DN9" s="98"/>
-      <c r="DO9" s="98"/>
-      <c r="DP9" s="98"/>
-      <c r="DQ9" s="98"/>
-      <c r="DR9" s="98"/>
-      <c r="DS9" s="98"/>
-      <c r="DT9" s="98"/>
-      <c r="DU9" s="98"/>
-      <c r="DV9" s="99"/>
-      <c r="DW9" s="97">
+      <c r="DN9" s="106"/>
+      <c r="DO9" s="106"/>
+      <c r="DP9" s="106"/>
+      <c r="DQ9" s="106"/>
+      <c r="DR9" s="106"/>
+      <c r="DS9" s="106"/>
+      <c r="DT9" s="106"/>
+      <c r="DU9" s="106"/>
+      <c r="DV9" s="107"/>
+      <c r="DW9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DW8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DX9" s="98"/>
-      <c r="DY9" s="98"/>
-      <c r="DZ9" s="98"/>
-      <c r="EA9" s="98"/>
-      <c r="EB9" s="98"/>
-      <c r="EC9" s="98"/>
-      <c r="ED9" s="98"/>
-      <c r="EE9" s="98"/>
-      <c r="EF9" s="99"/>
-      <c r="EG9" s="97">
+      <c r="DX9" s="106"/>
+      <c r="DY9" s="106"/>
+      <c r="DZ9" s="106"/>
+      <c r="EA9" s="106"/>
+      <c r="EB9" s="106"/>
+      <c r="EC9" s="106"/>
+      <c r="ED9" s="106"/>
+      <c r="EE9" s="106"/>
+      <c r="EF9" s="107"/>
+      <c r="EG9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EG8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="EH9" s="98"/>
-      <c r="EI9" s="98"/>
-      <c r="EJ9" s="98"/>
-      <c r="EK9" s="98"/>
-      <c r="EL9" s="98"/>
-      <c r="EM9" s="98"/>
-      <c r="EN9" s="98"/>
-      <c r="EO9" s="98"/>
-      <c r="EP9" s="100"/>
-      <c r="EQ9" s="98">
+      <c r="EH9" s="106"/>
+      <c r="EI9" s="106"/>
+      <c r="EJ9" s="106"/>
+      <c r="EK9" s="106"/>
+      <c r="EL9" s="106"/>
+      <c r="EM9" s="106"/>
+      <c r="EN9" s="106"/>
+      <c r="EO9" s="106"/>
+      <c r="EP9" s="122"/>
+      <c r="EQ9" s="106">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EQ8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="ER9" s="98"/>
-      <c r="ES9" s="98"/>
-      <c r="ET9" s="98"/>
-      <c r="EU9" s="98"/>
-      <c r="EV9" s="98"/>
-      <c r="EW9" s="98"/>
-      <c r="EX9" s="98"/>
-      <c r="EY9" s="98"/>
-      <c r="EZ9" s="99"/>
-      <c r="FA9" s="97">
+      <c r="ER9" s="106"/>
+      <c r="ES9" s="106"/>
+      <c r="ET9" s="106"/>
+      <c r="EU9" s="106"/>
+      <c r="EV9" s="106"/>
+      <c r="EW9" s="106"/>
+      <c r="EX9" s="106"/>
+      <c r="EY9" s="106"/>
+      <c r="EZ9" s="107"/>
+      <c r="FA9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FB9" s="98"/>
-      <c r="FC9" s="98"/>
-      <c r="FD9" s="98"/>
-      <c r="FE9" s="98"/>
-      <c r="FF9" s="98"/>
-      <c r="FG9" s="98"/>
-      <c r="FH9" s="98"/>
-      <c r="FI9" s="98"/>
-      <c r="FJ9" s="99"/>
-      <c r="FK9" s="97">
+      <c r="FB9" s="106"/>
+      <c r="FC9" s="106"/>
+      <c r="FD9" s="106"/>
+      <c r="FE9" s="106"/>
+      <c r="FF9" s="106"/>
+      <c r="FG9" s="106"/>
+      <c r="FH9" s="106"/>
+      <c r="FI9" s="106"/>
+      <c r="FJ9" s="107"/>
+      <c r="FK9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FL9" s="98"/>
-      <c r="FM9" s="98"/>
-      <c r="FN9" s="98"/>
-      <c r="FO9" s="98"/>
-      <c r="FP9" s="98"/>
-      <c r="FQ9" s="98"/>
-      <c r="FR9" s="98"/>
-      <c r="FS9" s="98"/>
-      <c r="FT9" s="99"/>
-      <c r="FU9" s="97">
+      <c r="FL9" s="106"/>
+      <c r="FM9" s="106"/>
+      <c r="FN9" s="106"/>
+      <c r="FO9" s="106"/>
+      <c r="FP9" s="106"/>
+      <c r="FQ9" s="106"/>
+      <c r="FR9" s="106"/>
+      <c r="FS9" s="106"/>
+      <c r="FT9" s="107"/>
+      <c r="FU9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FV9" s="98"/>
-      <c r="FW9" s="98"/>
-      <c r="FX9" s="98"/>
-      <c r="FY9" s="98"/>
-      <c r="FZ9" s="98"/>
-      <c r="GA9" s="98"/>
-      <c r="GB9" s="98"/>
-      <c r="GC9" s="98"/>
-      <c r="GD9" s="99"/>
-      <c r="GE9" s="97">
+      <c r="FV9" s="106"/>
+      <c r="FW9" s="106"/>
+      <c r="FX9" s="106"/>
+      <c r="FY9" s="106"/>
+      <c r="FZ9" s="106"/>
+      <c r="GA9" s="106"/>
+      <c r="GB9" s="106"/>
+      <c r="GC9" s="106"/>
+      <c r="GD9" s="107"/>
+      <c r="GE9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GF9" s="98"/>
-      <c r="GG9" s="98"/>
-      <c r="GH9" s="98"/>
-      <c r="GI9" s="98"/>
-      <c r="GJ9" s="98"/>
-      <c r="GK9" s="98"/>
-      <c r="GL9" s="98"/>
-      <c r="GM9" s="98"/>
-      <c r="GN9" s="99"/>
-      <c r="GO9" s="97">
+      <c r="GF9" s="106"/>
+      <c r="GG9" s="106"/>
+      <c r="GH9" s="106"/>
+      <c r="GI9" s="106"/>
+      <c r="GJ9" s="106"/>
+      <c r="GK9" s="106"/>
+      <c r="GL9" s="106"/>
+      <c r="GM9" s="106"/>
+      <c r="GN9" s="107"/>
+      <c r="GO9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GP9" s="98"/>
-      <c r="GQ9" s="98"/>
-      <c r="GR9" s="98"/>
-      <c r="GS9" s="98"/>
-      <c r="GT9" s="98"/>
-      <c r="GU9" s="98"/>
-      <c r="GV9" s="98"/>
-      <c r="GW9" s="98"/>
-      <c r="GX9" s="99"/>
-      <c r="GY9" s="97">
+      <c r="GP9" s="106"/>
+      <c r="GQ9" s="106"/>
+      <c r="GR9" s="106"/>
+      <c r="GS9" s="106"/>
+      <c r="GT9" s="106"/>
+      <c r="GU9" s="106"/>
+      <c r="GV9" s="106"/>
+      <c r="GW9" s="106"/>
+      <c r="GX9" s="107"/>
+      <c r="GY9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GZ9" s="98"/>
-      <c r="HA9" s="98"/>
-      <c r="HB9" s="98"/>
-      <c r="HC9" s="98"/>
-      <c r="HD9" s="98"/>
-      <c r="HE9" s="98"/>
-      <c r="HF9" s="98"/>
-      <c r="HG9" s="98"/>
-      <c r="HH9" s="99"/>
-      <c r="HI9" s="97">
+      <c r="GZ9" s="106"/>
+      <c r="HA9" s="106"/>
+      <c r="HB9" s="106"/>
+      <c r="HC9" s="106"/>
+      <c r="HD9" s="106"/>
+      <c r="HE9" s="106"/>
+      <c r="HF9" s="106"/>
+      <c r="HG9" s="106"/>
+      <c r="HH9" s="107"/>
+      <c r="HI9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(HI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="HJ9" s="98"/>
-      <c r="HK9" s="98"/>
-      <c r="HL9" s="98"/>
-      <c r="HM9" s="98"/>
-      <c r="HN9" s="98"/>
-      <c r="HO9" s="98"/>
-      <c r="HP9" s="98"/>
-      <c r="HQ9" s="98"/>
-      <c r="HR9" s="100"/>
+      <c r="HJ9" s="106"/>
+      <c r="HK9" s="106"/>
+      <c r="HL9" s="106"/>
+      <c r="HM9" s="106"/>
+      <c r="HN9" s="106"/>
+      <c r="HO9" s="106"/>
+      <c r="HP9" s="106"/>
+      <c r="HQ9" s="106"/>
+      <c r="HR9" s="122"/>
     </row>
     <row r="10" spans="1:226" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="133"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="125"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="99"/>
       <c r="Q10" s="5"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="20"/>
@@ -26997,19 +26997,19 @@
       <c r="A11" s="68"/>
       <c r="B11" s="5"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
-      <c r="O11" s="129"/>
-      <c r="P11" s="126"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="100"/>
       <c r="Q11" s="51">
         <v>0</v>
       </c>
@@ -28506,17 +28506,17 @@
       </c>
     </row>
     <row r="13" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="111" t="s">
+      <c r="D13" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="83"/>
-      <c r="G13" s="84" t="s">
+      <c r="E13" s="101"/>
+      <c r="G13" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="85" t="str">
+      <c r="H13" s="119" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
       </c>
@@ -28622,11 +28622,11 @@
       <c r="HR13" s="4"/>
     </row>
     <row r="14" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="83"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="85"/>
+      <c r="B14" s="134"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="101"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="119"/>
       <c r="I14" s="45" t="s">
         <v>1</v>
       </c>
@@ -28878,22 +28878,22 @@
       <c r="HR14" s="31"/>
     </row>
     <row r="15" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="83" t="s">
+      <c r="E15" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="83">
+      <c r="F15" s="101">
         <v>1</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="85" t="str">
+      <c r="H15" s="119" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
       </c>
@@ -28964,12 +28964,12 @@
       <c r="HR15" s="4"/>
     </row>
     <row r="16" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="81"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="85"/>
+      <c r="B16" s="134"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="119"/>
       <c r="I16" s="45" t="s">
         <v>1</v>
       </c>
@@ -29209,20 +29209,20 @@
       <c r="HR16" s="31"/>
     </row>
     <row r="17" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83">
+      <c r="E17" s="101"/>
+      <c r="F17" s="101">
         <v>1</v>
       </c>
-      <c r="G17" s="84" t="s">
+      <c r="G17" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="85" t="str">
+      <c r="H17" s="119" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
       </c>
@@ -29294,12 +29294,12 @@
       <c r="HR17" s="4"/>
     </row>
     <row r="18" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="85"/>
+      <c r="B18" s="134"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="119"/>
       <c r="I18" s="45" t="s">
         <v>1</v>
       </c>
@@ -29541,22 +29541,22 @@
       <c r="HR18" s="31"/>
     </row>
     <row r="19" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="111" t="s">
+      <c r="D19" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E19" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="83">
+      <c r="F19" s="101">
         <v>1</v>
       </c>
-      <c r="G19" s="84" t="s">
+      <c r="G19" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="85" t="str">
+      <c r="H19" s="119" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
       </c>
@@ -29640,12 +29640,12 @@
       <c r="HR19" s="4"/>
     </row>
     <row r="20" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="81"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="85"/>
+      <c r="B20" s="134"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="119"/>
       <c r="I20" s="45" t="s">
         <v>1</v>
       </c>
@@ -29889,20 +29889,20 @@
       <c r="HR20" s="31"/>
     </row>
     <row r="21" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83">
+      <c r="E21" s="101"/>
+      <c r="F21" s="101">
         <v>1</v>
       </c>
-      <c r="G21" s="84" t="s">
+      <c r="G21" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="85" t="str">
+      <c r="H21" s="119" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
       </c>
@@ -29976,12 +29976,12 @@
       <c r="HR21" s="4"/>
     </row>
     <row r="22" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="81"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="85"/>
+      <c r="B22" s="134"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="119"/>
       <c r="I22" s="45" t="s">
         <v>1</v>
       </c>
@@ -30219,20 +30219,20 @@
       <c r="HR22" s="31"/>
     </row>
     <row r="23" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="111" t="s">
+      <c r="D23" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83">
+      <c r="E23" s="101"/>
+      <c r="F23" s="101">
         <v>1</v>
       </c>
-      <c r="G23" s="84" t="s">
+      <c r="G23" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="85" t="str">
+      <c r="H23" s="119" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
       </c>
@@ -30303,12 +30303,12 @@
       <c r="HR23" s="4"/>
     </row>
     <row r="24" spans="2:226" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="81"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="85"/>
+      <c r="B24" s="134"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="119"/>
       <c r="I24" s="45" t="s">
         <v>1</v>
       </c>
@@ -30550,20 +30550,20 @@
       <c r="HR24" s="31"/>
     </row>
     <row r="25" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83">
+      <c r="E25" s="101"/>
+      <c r="F25" s="101">
         <v>1</v>
       </c>
-      <c r="G25" s="84" t="s">
+      <c r="G25" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="85" t="str">
+      <c r="H25" s="119" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
       </c>
@@ -30633,12 +30633,12 @@
       <c r="HR25" s="4"/>
     </row>
     <row r="26" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="81"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="85"/>
+      <c r="B26" s="134"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="119"/>
       <c r="I26" s="45" t="s">
         <v>1</v>
       </c>
@@ -30878,20 +30878,20 @@
       <c r="HR26" s="31"/>
     </row>
     <row r="27" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="111" t="s">
+      <c r="D27" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83">
+      <c r="E27" s="101"/>
+      <c r="F27" s="101">
         <v>2</v>
       </c>
-      <c r="G27" s="84" t="s">
+      <c r="G27" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="85" t="str">
+      <c r="H27" s="119" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
       </c>
@@ -30972,12 +30972,12 @@
       <c r="HR27" s="4"/>
     </row>
     <row r="28" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="81"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="85"/>
+      <c r="B28" s="134"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="119"/>
       <c r="I28" s="45" t="s">
         <v>1</v>
       </c>
@@ -31217,22 +31217,22 @@
       <c r="HR28" s="31"/>
     </row>
     <row r="29" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="83" t="s">
+      <c r="E29" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="83">
+      <c r="F29" s="101">
         <v>2</v>
       </c>
-      <c r="G29" s="84" t="s">
+      <c r="G29" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="85" t="str">
+      <c r="H29" s="119" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v>!</v>
       </c>
@@ -31312,12 +31312,12 @@
       <c r="HR29" s="4"/>
     </row>
     <row r="30" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="81"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="B30" s="134"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="119"/>
       <c r="I30" s="45" t="s">
         <v>1</v>
       </c>
@@ -31573,22 +31573,22 @@
       <c r="HR30" s="31"/>
     </row>
     <row r="31" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="82" t="s">
+      <c r="D31" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="83" t="s">
+      <c r="E31" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="83">
+      <c r="F31" s="101">
         <v>2</v>
       </c>
-      <c r="G31" s="84" t="s">
+      <c r="G31" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="85" t="str">
+      <c r="H31" s="119" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
       </c>
@@ -31660,12 +31660,12 @@
       <c r="HR31" s="4"/>
     </row>
     <row r="32" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="81"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="85"/>
+      <c r="B32" s="134"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="45" t="s">
         <v>1</v>
       </c>
@@ -31907,22 +31907,22 @@
       <c r="HR32" s="31"/>
     </row>
     <row r="33" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="134" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="82" t="s">
+      <c r="D33" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="83" t="s">
+      <c r="E33" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="83">
+      <c r="F33" s="101">
         <v>2</v>
       </c>
-      <c r="G33" s="84" t="s">
+      <c r="G33" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="85" t="str">
+      <c r="H33" s="119" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
       </c>
@@ -31998,12 +31998,12 @@
       <c r="HR33" s="4"/>
     </row>
     <row r="34" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="81"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="84"/>
-      <c r="H34" s="85"/>
+      <c r="B34" s="134"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="45" t="s">
         <v>1</v>
       </c>
@@ -32245,22 +32245,22 @@
       <c r="HR34" s="31"/>
     </row>
     <row r="35" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="81" t="s">
+      <c r="B35" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="83" t="s">
+      <c r="E35" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="83">
+      <c r="F35" s="101">
         <v>2</v>
       </c>
-      <c r="G35" s="84" t="s">
+      <c r="G35" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="85" t="str">
+      <c r="H35" s="119" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
       </c>
@@ -32339,12 +32339,12 @@
       <c r="HR35" s="4"/>
     </row>
     <row r="36" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="81"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="85"/>
+      <c r="B36" s="134"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="45" t="s">
         <v>1</v>
       </c>
@@ -32582,22 +32582,22 @@
       <c r="HR36" s="31"/>
     </row>
     <row r="37" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="81" t="s">
+      <c r="B37" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="121" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="83">
+      <c r="F37" s="101">
         <v>2</v>
       </c>
-      <c r="G37" s="84" t="s">
+      <c r="G37" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="85" t="str">
+      <c r="H37" s="119" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
       </c>
@@ -32671,12 +32671,12 @@
       <c r="HR37" s="4"/>
     </row>
     <row r="38" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="81"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="84"/>
-      <c r="H38" s="85"/>
+      <c r="B38" s="134"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="119"/>
       <c r="I38" s="45" t="s">
         <v>1</v>
       </c>
@@ -32916,20 +32916,20 @@
       <c r="HR38" s="31"/>
     </row>
     <row r="39" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="81" t="s">
+      <c r="B39" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="82" t="s">
+      <c r="D39" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83">
+      <c r="E39" s="101"/>
+      <c r="F39" s="101">
         <v>3</v>
       </c>
-      <c r="G39" s="84" t="s">
+      <c r="G39" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="85" t="str">
+      <c r="H39" s="119" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
       </c>
@@ -33010,12 +33010,12 @@
       <c r="HR39" s="4"/>
     </row>
     <row r="40" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="81"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="85"/>
+      <c r="B40" s="134"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="119"/>
       <c r="I40" s="45" t="s">
         <v>1</v>
       </c>
@@ -33263,20 +33263,20 @@
       <c r="HR40" s="31"/>
     </row>
     <row r="41" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="81" t="s">
+      <c r="B41" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="82" t="s">
+      <c r="D41" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83">
+      <c r="E41" s="101"/>
+      <c r="F41" s="101">
         <v>3</v>
       </c>
-      <c r="G41" s="84" t="s">
+      <c r="G41" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="85" t="str">
+      <c r="H41" s="119" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
       </c>
@@ -33350,12 +33350,12 @@
       <c r="HR41" s="4"/>
     </row>
     <row r="42" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="81"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="83"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="84"/>
-      <c r="H42" s="85"/>
+      <c r="B42" s="134"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="101"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="119"/>
       <c r="I42" s="45" t="s">
         <v>1</v>
       </c>
@@ -33595,20 +33595,20 @@
       <c r="HR42" s="31"/>
     </row>
     <row r="43" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="81" t="s">
+      <c r="B43" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="83"/>
-      <c r="F43" s="83">
+      <c r="E43" s="101"/>
+      <c r="F43" s="101">
         <v>3</v>
       </c>
-      <c r="G43" s="84" t="s">
+      <c r="G43" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="85" t="str">
+      <c r="H43" s="119" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
       </c>
@@ -33681,12 +33681,12 @@
       <c r="HR43" s="4"/>
     </row>
     <row r="44" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="81"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="83"/>
-      <c r="F44" s="83"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="85"/>
+      <c r="B44" s="134"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="101"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="45" t="s">
         <v>1</v>
       </c>
@@ -33928,20 +33928,20 @@
       <c r="HR44" s="31"/>
     </row>
     <row r="45" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="81" t="s">
+      <c r="B45" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="82" t="s">
+      <c r="D45" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="83"/>
-      <c r="F45" s="83">
+      <c r="E45" s="101"/>
+      <c r="F45" s="101">
         <v>3</v>
       </c>
-      <c r="G45" s="84" t="s">
+      <c r="G45" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="85" t="str">
+      <c r="H45" s="119" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
       </c>
@@ -34014,12 +34014,12 @@
       <c r="HR45" s="4"/>
     </row>
     <row r="46" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="81"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="85"/>
+      <c r="B46" s="134"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="101"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="45" t="s">
         <v>1</v>
       </c>
@@ -34261,20 +34261,20 @@
       <c r="HR46" s="31"/>
     </row>
     <row r="47" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="81" t="s">
+      <c r="B47" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="82" t="s">
+      <c r="D47" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83">
+      <c r="E47" s="101"/>
+      <c r="F47" s="101">
         <v>3</v>
       </c>
-      <c r="G47" s="84" t="s">
+      <c r="G47" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="85" t="str">
+      <c r="H47" s="119" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
       </c>
@@ -34344,12 +34344,12 @@
       <c r="HR47" s="4"/>
     </row>
     <row r="48" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="81"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="84"/>
-      <c r="H48" s="85"/>
+      <c r="B48" s="134"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="101"/>
+      <c r="F48" s="101"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="119"/>
       <c r="I48" s="45" t="s">
         <v>1</v>
       </c>
@@ -34591,18 +34591,20 @@
       <c r="HR48" s="31"/>
     </row>
     <row r="49" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="82" t="s">
+      <c r="D49" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83">
+      <c r="E49" s="101"/>
+      <c r="F49" s="101">
         <v>4</v>
       </c>
-      <c r="G49" s="84"/>
-      <c r="H49" s="85" t="str">
+      <c r="G49" s="87" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="119" t="str">
         <f t="shared" ref="H49" si="65">IF(O50&gt;P49,"!","")</f>
         <v/>
       </c>
@@ -34690,23 +34692,23 @@
       <c r="HR49" s="4"/>
     </row>
     <row r="50" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="81"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="85"/>
+      <c r="B50" s="134"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="101"/>
+      <c r="F50" s="101"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="119"/>
       <c r="I50" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J50" s="46">
         <f>IF(D49="","",COUNTIF(Echéancier!$Q50:$EP50,"r"))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K50" s="14"/>
       <c r="L50" s="14">
         <f t="shared" ref="L50" si="68">IFERROR(L48+J50,0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M50" s="14">
         <f t="shared" ref="M50" si="69">COUNTIF(Q50:EP50,"a")</f>
@@ -34718,7 +34720,7 @@
       </c>
       <c r="O50" s="14">
         <f>IFERROR(MATCH("ra",$Q50:$EP50,1),0)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P50" s="14"/>
       <c r="Q50" s="23"/>
@@ -34768,9 +34770,15 @@
       <c r="BI50" s="34"/>
       <c r="BJ50" s="34"/>
       <c r="BK50" s="34"/>
-      <c r="BL50" s="34"/>
-      <c r="BM50" s="34"/>
-      <c r="BN50" s="24"/>
+      <c r="BL50" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BM50" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BN50" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="BO50" s="76"/>
       <c r="BP50" s="75"/>
       <c r="BQ50" s="75"/>
@@ -34933,18 +34941,20 @@
       <c r="HR50" s="31"/>
     </row>
     <row r="51" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="81" t="s">
+      <c r="B51" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="82" t="s">
+      <c r="D51" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83">
+      <c r="E51" s="101"/>
+      <c r="F51" s="101">
         <v>4</v>
       </c>
-      <c r="G51" s="84"/>
-      <c r="H51" s="85" t="str">
+      <c r="G51" s="87" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="119" t="str">
         <f t="shared" ref="H51" si="71">IF(O52&gt;P51,"!","")</f>
         <v/>
       </c>
@@ -35021,23 +35031,23 @@
       <c r="HR51" s="4"/>
     </row>
     <row r="52" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="81"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="84"/>
-      <c r="H52" s="85"/>
+      <c r="B52" s="134"/>
+      <c r="D52" s="121"/>
+      <c r="E52" s="101"/>
+      <c r="F52" s="101"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="119"/>
       <c r="I52" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J52" s="46">
         <f>IF(D51="","",COUNTIF(Echéancier!$Q52:$EP52,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K52" s="14"/>
       <c r="L52" s="14">
         <f t="shared" ref="L52" si="74">IFERROR(L50+J52,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M52" s="14">
         <f t="shared" ref="M52" si="75">COUNTIF(Q52:EP52,"a")</f>
@@ -35049,7 +35059,7 @@
       </c>
       <c r="O52" s="14">
         <f>IFERROR(MATCH("ra",$Q52:$EP52,1),0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="P52" s="14"/>
       <c r="Q52" s="23"/>
@@ -35102,8 +35112,12 @@
       <c r="BL52" s="34"/>
       <c r="BM52" s="34"/>
       <c r="BN52" s="24"/>
-      <c r="BO52" s="25"/>
-      <c r="BP52" s="34"/>
+      <c r="BO52" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="BP52" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="BQ52" s="34"/>
       <c r="BR52" s="75"/>
       <c r="BS52" s="75"/>
@@ -35264,18 +35278,18 @@
       <c r="HR52" s="31"/>
     </row>
     <row r="53" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="81" t="s">
+      <c r="B53" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="82" t="s">
+      <c r="D53" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="83"/>
-      <c r="F53" s="83">
+      <c r="E53" s="101"/>
+      <c r="F53" s="101">
         <v>4</v>
       </c>
-      <c r="G53" s="84"/>
-      <c r="H53" s="85" t="str">
+      <c r="G53" s="87"/>
+      <c r="H53" s="119" t="str">
         <f t="shared" ref="H53" si="77">IF(O54&gt;P53,"!","")</f>
         <v/>
       </c>
@@ -35355,12 +35369,12 @@
       <c r="HR53" s="4"/>
     </row>
     <row r="54" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="81"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="85"/>
+      <c r="B54" s="134"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="87"/>
+      <c r="H54" s="119"/>
       <c r="I54" s="45" t="s">
         <v>1</v>
       </c>
@@ -35371,7 +35385,7 @@
       <c r="K54" s="14"/>
       <c r="L54" s="14">
         <f t="shared" ref="L54" si="80">IFERROR(L52+J54,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M54" s="14">
         <f t="shared" ref="M54" si="81">COUNTIF(Q54:EP54,"a")</f>
@@ -35598,20 +35612,20 @@
       <c r="HR54" s="31"/>
     </row>
     <row r="55" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="81" t="s">
+      <c r="B55" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="82" t="s">
+      <c r="D55" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="83" t="s">
+      <c r="E55" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="83">
+      <c r="F55" s="101">
         <v>4</v>
       </c>
-      <c r="G55" s="84"/>
-      <c r="H55" s="85" t="str">
+      <c r="G55" s="87"/>
+      <c r="H55" s="119" t="str">
         <f t="shared" ref="H55" si="83">IF(O56&gt;P55,"!","")</f>
         <v/>
       </c>
@@ -35694,12 +35708,12 @@
       <c r="HR55" s="4"/>
     </row>
     <row r="56" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="81"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="83"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="85"/>
+      <c r="B56" s="134"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="87"/>
+      <c r="H56" s="119"/>
       <c r="I56" s="45" t="s">
         <v>1</v>
       </c>
@@ -35710,7 +35724,7 @@
       <c r="K56" s="14"/>
       <c r="L56" s="14">
         <f t="shared" ref="L56" si="86">IFERROR(L54+J56,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M56" s="14">
         <f t="shared" ref="M56" si="87">COUNTIF(Q56:EP56,"a")</f>
@@ -35937,20 +35951,20 @@
       <c r="HR56" s="31"/>
     </row>
     <row r="57" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="81" t="s">
+      <c r="B57" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="82" t="s">
+      <c r="D57" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="83" t="s">
+      <c r="E57" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="83">
+      <c r="F57" s="101">
         <v>4</v>
       </c>
-      <c r="G57" s="84"/>
-      <c r="H57" s="85" t="str">
+      <c r="G57" s="87"/>
+      <c r="H57" s="119" t="str">
         <f t="shared" ref="H57" si="89">IF(O58&gt;P57,"!","")</f>
         <v/>
       </c>
@@ -36021,12 +36035,12 @@
       <c r="HR57" s="4"/>
     </row>
     <row r="58" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="81"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="83"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="85"/>
+      <c r="B58" s="134"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="101"/>
+      <c r="F58" s="101"/>
+      <c r="G58" s="87"/>
+      <c r="H58" s="119"/>
       <c r="I58" s="45" t="s">
         <v>1</v>
       </c>
@@ -36037,7 +36051,7 @@
       <c r="K58" s="14"/>
       <c r="L58" s="14">
         <f t="shared" ref="L58" si="92">IFERROR(L56+J58,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M58" s="14">
         <f t="shared" ref="M58" si="93">COUNTIF(Q58:EP58,"a")</f>
@@ -36264,18 +36278,18 @@
       <c r="HR58" s="31"/>
     </row>
     <row r="59" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="81" t="s">
+      <c r="B59" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="82" t="s">
+      <c r="D59" s="121" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="83"/>
-      <c r="F59" s="83">
+      <c r="E59" s="101"/>
+      <c r="F59" s="101">
         <v>5</v>
       </c>
-      <c r="G59" s="84"/>
-      <c r="H59" s="85" t="str">
+      <c r="G59" s="87"/>
+      <c r="H59" s="119" t="str">
         <f t="shared" ref="H59" si="95">IF(O60&gt;P59,"!","")</f>
         <v/>
       </c>
@@ -36349,12 +36363,12 @@
       <c r="HR59" s="4"/>
     </row>
     <row r="60" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="81"/>
-      <c r="D60" s="82"/>
-      <c r="E60" s="83"/>
-      <c r="F60" s="83"/>
-      <c r="G60" s="84"/>
-      <c r="H60" s="85"/>
+      <c r="B60" s="134"/>
+      <c r="D60" s="121"/>
+      <c r="E60" s="101"/>
+      <c r="F60" s="101"/>
+      <c r="G60" s="87"/>
+      <c r="H60" s="119"/>
       <c r="I60" s="45" t="s">
         <v>1</v>
       </c>
@@ -36365,7 +36379,7 @@
       <c r="K60" s="14"/>
       <c r="L60" s="14">
         <f t="shared" ref="L60" si="98">IFERROR(L58+J60,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M60" s="14">
         <f t="shared" ref="M60" si="99">COUNTIF(Q60:EP60,"a")</f>
@@ -36592,18 +36606,18 @@
       <c r="HR60" s="31"/>
     </row>
     <row r="61" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="81" t="s">
+      <c r="B61" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="82" t="s">
+      <c r="D61" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="E61" s="83"/>
-      <c r="F61" s="83">
+      <c r="E61" s="101"/>
+      <c r="F61" s="101">
         <v>5</v>
       </c>
-      <c r="G61" s="84"/>
-      <c r="H61" s="85" t="str">
+      <c r="G61" s="87"/>
+      <c r="H61" s="119" t="str">
         <f t="shared" ref="H61" si="101">IF(O62&gt;P61,"!","")</f>
         <v/>
       </c>
@@ -36698,12 +36712,12 @@
       <c r="HR61" s="4"/>
     </row>
     <row r="62" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="81"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="84"/>
-      <c r="H62" s="85"/>
+      <c r="B62" s="134"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="101"/>
+      <c r="F62" s="101"/>
+      <c r="G62" s="87"/>
+      <c r="H62" s="119"/>
       <c r="I62" s="45" t="s">
         <v>1</v>
       </c>
@@ -36714,7 +36728,7 @@
       <c r="K62" s="14"/>
       <c r="L62" s="14">
         <f t="shared" ref="L62" si="104">IFERROR(L60+J62,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M62" s="14">
         <f t="shared" ref="M62" si="105">COUNTIF(Q62:EP62,"a")</f>
@@ -36941,18 +36955,18 @@
       <c r="HR62" s="31"/>
     </row>
     <row r="63" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="81" t="s">
+      <c r="B63" s="134" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="82" t="s">
+      <c r="D63" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="83"/>
-      <c r="F63" s="83">
+      <c r="E63" s="101"/>
+      <c r="F63" s="101">
         <v>5</v>
       </c>
-      <c r="G63" s="84"/>
-      <c r="H63" s="85" t="str">
+      <c r="G63" s="87"/>
+      <c r="H63" s="119" t="str">
         <f t="shared" ref="H63" si="107">IF(O64&gt;P63,"!","")</f>
         <v/>
       </c>
@@ -37037,12 +37051,12 @@
       <c r="HR63" s="4"/>
     </row>
     <row r="64" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="81"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="83"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="85"/>
+      <c r="B64" s="134"/>
+      <c r="D64" s="121"/>
+      <c r="E64" s="101"/>
+      <c r="F64" s="101"/>
+      <c r="G64" s="87"/>
+      <c r="H64" s="119"/>
       <c r="I64" s="45" t="s">
         <v>1</v>
       </c>
@@ -37053,7 +37067,7 @@
       <c r="K64" s="14"/>
       <c r="L64" s="14">
         <f t="shared" ref="L64" si="110">IFERROR(L62+J64,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" ref="M64" si="111">COUNTIF(Q64:EP64,"a")</f>
@@ -37280,18 +37294,18 @@
       <c r="HR64" s="31"/>
     </row>
     <row r="65" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="81" t="s">
+      <c r="B65" s="134" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="82" t="s">
+      <c r="D65" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="83"/>
-      <c r="F65" s="83">
+      <c r="E65" s="101"/>
+      <c r="F65" s="101">
         <v>6</v>
       </c>
-      <c r="G65" s="84"/>
-      <c r="H65" s="85" t="str">
+      <c r="G65" s="87"/>
+      <c r="H65" s="119" t="str">
         <f t="shared" ref="H65" si="113">IF(O66&gt;P65,"!","")</f>
         <v/>
       </c>
@@ -37369,12 +37383,12 @@
       <c r="HR65" s="4"/>
     </row>
     <row r="66" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="81"/>
-      <c r="D66" s="82"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="84"/>
-      <c r="H66" s="85"/>
+      <c r="B66" s="134"/>
+      <c r="D66" s="121"/>
+      <c r="E66" s="101"/>
+      <c r="F66" s="101"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="119"/>
       <c r="I66" s="45" t="s">
         <v>1</v>
       </c>
@@ -37385,7 +37399,7 @@
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -37612,20 +37626,20 @@
       <c r="HR66" s="31"/>
     </row>
     <row r="67" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="81" t="s">
+      <c r="B67" s="134" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="82" t="s">
+      <c r="D67" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="83" t="s">
+      <c r="E67" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="F67" s="83">
+      <c r="F67" s="101">
         <v>6</v>
       </c>
-      <c r="G67" s="84"/>
-      <c r="H67" s="85" t="str">
+      <c r="G67" s="87"/>
+      <c r="H67" s="119" t="str">
         <f t="shared" ref="H67" si="119">IF(O68&gt;P67,"!","")</f>
         <v/>
       </c>
@@ -37720,12 +37734,12 @@
       <c r="HR67" s="4"/>
     </row>
     <row r="68" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="81"/>
-      <c r="D68" s="82"/>
-      <c r="E68" s="83"/>
-      <c r="F68" s="83"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="85"/>
+      <c r="B68" s="134"/>
+      <c r="D68" s="121"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="87"/>
+      <c r="H68" s="119"/>
       <c r="I68" s="45" t="s">
         <v>1</v>
       </c>
@@ -37736,7 +37750,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -37963,20 +37977,20 @@
       <c r="HR68" s="31"/>
     </row>
     <row r="69" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="81" t="s">
+      <c r="B69" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="82" t="s">
+      <c r="D69" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="83" t="s">
+      <c r="E69" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F69" s="83">
+      <c r="F69" s="101">
         <v>6</v>
       </c>
-      <c r="G69" s="84"/>
-      <c r="H69" s="85" t="str">
+      <c r="G69" s="87"/>
+      <c r="H69" s="119" t="str">
         <f t="shared" ref="H69" si="127">IF(O70&gt;P69,"!","")</f>
         <v/>
       </c>
@@ -38053,12 +38067,12 @@
       <c r="HR69" s="4"/>
     </row>
     <row r="70" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="81"/>
-      <c r="D70" s="82"/>
-      <c r="E70" s="83"/>
-      <c r="F70" s="83"/>
-      <c r="G70" s="84"/>
-      <c r="H70" s="85"/>
+      <c r="B70" s="134"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="101"/>
+      <c r="F70" s="101"/>
+      <c r="G70" s="87"/>
+      <c r="H70" s="119"/>
       <c r="I70" s="45" t="s">
         <v>1</v>
       </c>
@@ -38069,7 +38083,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -38296,20 +38310,20 @@
       <c r="HR70" s="31"/>
     </row>
     <row r="71" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="81" t="s">
+      <c r="B71" s="134" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="82" t="s">
+      <c r="D71" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="E71" s="83" t="s">
+      <c r="E71" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F71" s="83">
+      <c r="F71" s="101">
         <v>6</v>
       </c>
-      <c r="G71" s="84"/>
-      <c r="H71" s="85" t="str">
+      <c r="G71" s="87"/>
+      <c r="H71" s="119" t="str">
         <f t="shared" ref="H71" si="133">IF(O72&gt;P71,"!","")</f>
         <v/>
       </c>
@@ -38385,12 +38399,12 @@
       <c r="HR71" s="4"/>
     </row>
     <row r="72" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="81"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="83"/>
-      <c r="F72" s="83"/>
-      <c r="G72" s="84"/>
-      <c r="H72" s="85"/>
+      <c r="B72" s="134"/>
+      <c r="D72" s="121"/>
+      <c r="E72" s="101"/>
+      <c r="F72" s="101"/>
+      <c r="G72" s="87"/>
+      <c r="H72" s="119"/>
       <c r="I72" s="45" t="s">
         <v>1</v>
       </c>
@@ -38401,7 +38415,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -38717,13 +38731,13 @@
     </row>
     <row r="73" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="82" t="s">
+      <c r="D73" s="121" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="83"/>
-      <c r="F73" s="83"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="85" t="str">
+      <c r="E73" s="101"/>
+      <c r="F73" s="101"/>
+      <c r="G73" s="87"/>
+      <c r="H73" s="119" t="str">
         <f t="shared" ref="H73" si="139">IF(O74&gt;P73,"!","")</f>
         <v/>
       </c>
@@ -38791,11 +38805,11 @@
     </row>
     <row r="74" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="D74" s="82"/>
-      <c r="E74" s="83"/>
-      <c r="F74" s="83"/>
-      <c r="G74" s="84"/>
-      <c r="H74" s="85"/>
+      <c r="D74" s="121"/>
+      <c r="E74" s="101"/>
+      <c r="F74" s="101"/>
+      <c r="G74" s="87"/>
+      <c r="H74" s="119"/>
       <c r="I74" s="45" t="s">
         <v>1</v>
       </c>
@@ -38806,7 +38820,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>
@@ -39034,11 +39048,11 @@
     </row>
     <row r="75" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="82"/>
-      <c r="E75" s="83"/>
-      <c r="F75" s="83"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="85" t="str">
+      <c r="D75" s="121"/>
+      <c r="E75" s="101"/>
+      <c r="F75" s="101"/>
+      <c r="G75" s="87"/>
+      <c r="H75" s="119" t="str">
         <f t="shared" ref="H75" si="145">IF(O76&gt;P75,"!","")</f>
         <v/>
       </c>
@@ -39107,11 +39121,11 @@
     </row>
     <row r="76" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
-      <c r="D76" s="82"/>
-      <c r="E76" s="83"/>
-      <c r="F76" s="83"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="85"/>
+      <c r="D76" s="121"/>
+      <c r="E76" s="101"/>
+      <c r="F76" s="101"/>
+      <c r="G76" s="87"/>
+      <c r="H76" s="119"/>
       <c r="I76" s="45" t="s">
         <v>1</v>
       </c>
@@ -39350,11 +39364,11 @@
     </row>
     <row r="77" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
-      <c r="D77" s="82"/>
-      <c r="E77" s="83"/>
-      <c r="F77" s="83"/>
-      <c r="G77" s="84"/>
-      <c r="H77" s="85" t="str">
+      <c r="D77" s="121"/>
+      <c r="E77" s="101"/>
+      <c r="F77" s="101"/>
+      <c r="G77" s="87"/>
+      <c r="H77" s="119" t="str">
         <f t="shared" ref="H77" si="151">IF(O78&gt;P77,"!","")</f>
         <v/>
       </c>
@@ -39423,11 +39437,11 @@
     </row>
     <row r="78" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="82"/>
-      <c r="E78" s="83"/>
-      <c r="F78" s="83"/>
-      <c r="G78" s="84"/>
-      <c r="H78" s="85"/>
+      <c r="D78" s="121"/>
+      <c r="E78" s="101"/>
+      <c r="F78" s="101"/>
+      <c r="G78" s="87"/>
+      <c r="H78" s="119"/>
       <c r="I78" s="45" t="s">
         <v>1</v>
       </c>
@@ -39666,11 +39680,11 @@
     </row>
     <row r="79" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="D79" s="82"/>
-      <c r="E79" s="83"/>
-      <c r="F79" s="83"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="85" t="str">
+      <c r="D79" s="121"/>
+      <c r="E79" s="101"/>
+      <c r="F79" s="101"/>
+      <c r="G79" s="87"/>
+      <c r="H79" s="119" t="str">
         <f t="shared" ref="H79" si="157">IF(O80&gt;P79,"!","")</f>
         <v/>
       </c>
@@ -39739,11 +39753,11 @@
     </row>
     <row r="80" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
-      <c r="D80" s="82"/>
-      <c r="E80" s="83"/>
-      <c r="F80" s="83"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="85"/>
+      <c r="D80" s="121"/>
+      <c r="E80" s="101"/>
+      <c r="F80" s="101"/>
+      <c r="G80" s="87"/>
+      <c r="H80" s="119"/>
       <c r="I80" s="45" t="s">
         <v>1</v>
       </c>
@@ -39982,11 +39996,11 @@
     </row>
     <row r="81" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="D81" s="82"/>
-      <c r="E81" s="83"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="85" t="str">
+      <c r="D81" s="121"/>
+      <c r="E81" s="101"/>
+      <c r="F81" s="101"/>
+      <c r="G81" s="87"/>
+      <c r="H81" s="119" t="str">
         <f t="shared" ref="H81" si="163">IF(O82&gt;P81,"!","")</f>
         <v/>
       </c>
@@ -40055,11 +40069,11 @@
     </row>
     <row r="82" spans="2:226" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="70"/>
-      <c r="D82" s="86"/>
-      <c r="E82" s="87"/>
-      <c r="F82" s="87"/>
-      <c r="G82" s="88"/>
-      <c r="H82" s="89"/>
+      <c r="D82" s="130"/>
+      <c r="E82" s="131"/>
+      <c r="F82" s="131"/>
+      <c r="G82" s="132"/>
+      <c r="H82" s="133"/>
       <c r="I82" s="47" t="s">
         <v>1</v>
       </c>
@@ -40298,15 +40312,260 @@
     </row>
   </sheetData>
   <mergeCells count="287">
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="HI7:HR7"/>
+    <mergeCell ref="FA8:FJ8"/>
+    <mergeCell ref="FK8:FT8"/>
+    <mergeCell ref="FU8:GD8"/>
+    <mergeCell ref="GE8:GN8"/>
+    <mergeCell ref="GO8:GX8"/>
+    <mergeCell ref="GY8:HH8"/>
+    <mergeCell ref="HI8:HR8"/>
+    <mergeCell ref="FA9:FJ9"/>
+    <mergeCell ref="FK9:FT9"/>
+    <mergeCell ref="FU9:GD9"/>
+    <mergeCell ref="GE9:GN9"/>
+    <mergeCell ref="GO9:GX9"/>
+    <mergeCell ref="GY9:HH9"/>
+    <mergeCell ref="HI9:HR9"/>
+    <mergeCell ref="EQ7:EZ7"/>
+    <mergeCell ref="EQ8:EZ8"/>
+    <mergeCell ref="EQ9:EZ9"/>
+    <mergeCell ref="FA7:FJ7"/>
+    <mergeCell ref="FK7:FT7"/>
+    <mergeCell ref="FU7:GD7"/>
+    <mergeCell ref="GE7:GN7"/>
+    <mergeCell ref="GO7:GX7"/>
+    <mergeCell ref="GY7:HH7"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="BO7:BX7"/>
+    <mergeCell ref="EG7:EP7"/>
+    <mergeCell ref="AA8:AJ8"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AU8:BD8"/>
+    <mergeCell ref="BE8:BN8"/>
+    <mergeCell ref="BO8:BX8"/>
+    <mergeCell ref="BY8:CH8"/>
+    <mergeCell ref="CI8:CR8"/>
+    <mergeCell ref="CS8:DB8"/>
+    <mergeCell ref="DC8:DL8"/>
+    <mergeCell ref="BY7:CH7"/>
+    <mergeCell ref="CI7:CR7"/>
+    <mergeCell ref="CS7:DB7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="DW7:EF7"/>
+    <mergeCell ref="AA9:AJ9"/>
+    <mergeCell ref="AK9:AT9"/>
+    <mergeCell ref="AU9:BD9"/>
+    <mergeCell ref="BE9:BN9"/>
+    <mergeCell ref="BO9:BX9"/>
+    <mergeCell ref="EG9:EP9"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="BY9:CH9"/>
+    <mergeCell ref="CI9:CR9"/>
+    <mergeCell ref="CS9:DB9"/>
+    <mergeCell ref="DC9:DL9"/>
+    <mergeCell ref="DM9:DV9"/>
+    <mergeCell ref="DW9:EF9"/>
+    <mergeCell ref="DM8:DV8"/>
+    <mergeCell ref="DW8:EF8"/>
+    <mergeCell ref="EG8:EP8"/>
+    <mergeCell ref="AA7:AJ7"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AU7:BD7"/>
+    <mergeCell ref="BE7:BN7"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="DC7:DL7"/>
+    <mergeCell ref="DM7:DV7"/>
+    <mergeCell ref="AJ4:AR4"/>
+    <mergeCell ref="AJ5:AR5"/>
+    <mergeCell ref="AU5:BE5"/>
+    <mergeCell ref="AU4:BE4"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D19:D20"/>
@@ -40331,260 +40590,15 @@
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="AA7:AJ7"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AU7:BD7"/>
-    <mergeCell ref="BE7:BN7"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="DC7:DL7"/>
-    <mergeCell ref="DM7:DV7"/>
-    <mergeCell ref="AJ4:AR4"/>
-    <mergeCell ref="AJ5:AR5"/>
-    <mergeCell ref="AU5:BE5"/>
-    <mergeCell ref="AU4:BE4"/>
-    <mergeCell ref="BY9:CH9"/>
-    <mergeCell ref="CI9:CR9"/>
-    <mergeCell ref="CS9:DB9"/>
-    <mergeCell ref="DC9:DL9"/>
-    <mergeCell ref="DM9:DV9"/>
-    <mergeCell ref="DW9:EF9"/>
-    <mergeCell ref="DM8:DV8"/>
-    <mergeCell ref="DW8:EF8"/>
-    <mergeCell ref="EG8:EP8"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="AK9:AT9"/>
-    <mergeCell ref="AU9:BD9"/>
-    <mergeCell ref="BE9:BN9"/>
-    <mergeCell ref="BO9:BX9"/>
-    <mergeCell ref="EG9:EP9"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="FK7:FT7"/>
-    <mergeCell ref="FU7:GD7"/>
-    <mergeCell ref="GE7:GN7"/>
-    <mergeCell ref="GO7:GX7"/>
-    <mergeCell ref="GY7:HH7"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="BO7:BX7"/>
-    <mergeCell ref="EG7:EP7"/>
-    <mergeCell ref="AA8:AJ8"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AU8:BD8"/>
-    <mergeCell ref="BE8:BN8"/>
-    <mergeCell ref="BO8:BX8"/>
-    <mergeCell ref="BY8:CH8"/>
-    <mergeCell ref="CI8:CR8"/>
-    <mergeCell ref="CS8:DB8"/>
-    <mergeCell ref="DC8:DL8"/>
-    <mergeCell ref="BY7:CH7"/>
-    <mergeCell ref="CI7:CR7"/>
-    <mergeCell ref="CS7:DB7"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="DW7:EF7"/>
-    <mergeCell ref="AA9:AJ9"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="HI7:HR7"/>
-    <mergeCell ref="FA8:FJ8"/>
-    <mergeCell ref="FK8:FT8"/>
-    <mergeCell ref="FU8:GD8"/>
-    <mergeCell ref="GE8:GN8"/>
-    <mergeCell ref="GO8:GX8"/>
-    <mergeCell ref="GY8:HH8"/>
-    <mergeCell ref="HI8:HR8"/>
-    <mergeCell ref="FA9:FJ9"/>
-    <mergeCell ref="FK9:FT9"/>
-    <mergeCell ref="FU9:GD9"/>
-    <mergeCell ref="GE9:GN9"/>
-    <mergeCell ref="GO9:GX9"/>
-    <mergeCell ref="GY9:HH9"/>
-    <mergeCell ref="HI9:HR9"/>
-    <mergeCell ref="EQ7:EZ7"/>
-    <mergeCell ref="EQ8:EZ8"/>
-    <mergeCell ref="EQ9:EZ9"/>
-    <mergeCell ref="FA7:FJ7"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7:HR8">
     <cfRule type="expression" dxfId="2610" priority="3843">
@@ -50396,12 +50410,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50628,15 +50639,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
+    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -50662,18 +50685,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
-    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modification du WPF en Forms et urls bloqués correctement
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72167C62-7324-497D-9E6D-D3F361AA9892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C4B893-C118-4539-886E-08049455BF7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="100">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -1104,148 +1104,6 @@
   </cellStyles>
   <dxfs count="2626">
     <dxf>
-      <border>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dashDot">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="hair">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dashDot">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1349,6 +1207,148 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dashDot">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="hair">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dashDot">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -25708,16 +25708,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TabDates" displayName="TabDates" ref="A1:E47" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TabDates" displayName="TabDates" ref="A1:E47" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E47" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Jours" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Jours TPI" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date TPI" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Jours" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Jours TPI" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date TPI" dataDxfId="1">
       <calculatedColumnFormula>IF(TabDates[[#This Row],[Jours TPI]]&lt;&gt;"",TabDates[[#This Row],[Jours]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Livrables / infos" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Livrables / infos" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -26025,8 +26025,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="BK36" sqref="BK36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="CD57" sqref="CD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35527,12 +35527,12 @@
       </c>
       <c r="J54" s="46">
         <f>IF(D53="","",COUNTIF(Echéancier!$Q54:$EP54,"r"))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K54" s="14"/>
       <c r="L54" s="14">
         <f t="shared" ref="L54" si="80">IFERROR(L52+J54,0)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M54" s="14">
         <f t="shared" ref="M54" si="81">COUNTIF(Q54:EP54,"a")</f>
@@ -35544,7 +35544,7 @@
       </c>
       <c r="O54" s="14">
         <f>IFERROR(MATCH("ra",$Q54:$EP54,1),0)</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="P54" s="14"/>
       <c r="Q54" s="23"/>
@@ -35602,12 +35602,24 @@
       <c r="BQ54" s="34"/>
       <c r="BR54" s="34"/>
       <c r="BS54" s="34"/>
-      <c r="BT54" s="34"/>
-      <c r="BU54" s="75"/>
-      <c r="BV54" s="75"/>
-      <c r="BW54" s="75"/>
-      <c r="BX54" s="74"/>
-      <c r="BY54" s="76"/>
+      <c r="BT54" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="BU54" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="BV54" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="BW54" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="BX54" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="BY54" s="76" t="s">
+        <v>27</v>
+      </c>
       <c r="BZ54" s="75"/>
       <c r="CA54" s="34"/>
       <c r="CB54" s="34"/>
@@ -35866,12 +35878,12 @@
       </c>
       <c r="J56" s="46">
         <f>IF(D55="","",COUNTIF(Echéancier!$Q56:$EP56,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K56" s="14"/>
       <c r="L56" s="14">
         <f t="shared" ref="L56" si="86">IFERROR(L54+J56,0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M56" s="14">
         <f t="shared" ref="M56" si="87">COUNTIF(Q56:EP56,"a")</f>
@@ -35883,7 +35895,7 @@
       </c>
       <c r="O56" s="14">
         <f>IFERROR(MATCH("ra",$Q56:$EP56,1),0)</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="P56" s="14"/>
       <c r="Q56" s="23"/>
@@ -35947,8 +35959,12 @@
       <c r="BW56" s="34"/>
       <c r="BX56" s="24"/>
       <c r="BY56" s="25"/>
-      <c r="BZ56" s="75"/>
-      <c r="CA56" s="34"/>
+      <c r="BZ56" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="CA56" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="CB56" s="34"/>
       <c r="CC56" s="34"/>
       <c r="CD56" s="34"/>
@@ -36198,7 +36214,7 @@
       <c r="K58" s="14"/>
       <c r="L58" s="14">
         <f t="shared" ref="L58" si="92">IFERROR(L56+J58,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M58" s="14">
         <f t="shared" ref="M58" si="93">COUNTIF(Q58:EP58,"a")</f>
@@ -36528,7 +36544,7 @@
       <c r="K60" s="14"/>
       <c r="L60" s="14">
         <f t="shared" ref="L60" si="98">IFERROR(L58+J60,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M60" s="14">
         <f t="shared" ref="M60" si="99">COUNTIF(Q60:EP60,"a")</f>
@@ -36877,7 +36893,7 @@
       <c r="K62" s="14"/>
       <c r="L62" s="14">
         <f t="shared" ref="L62" si="104">IFERROR(L60+J62,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M62" s="14">
         <f t="shared" ref="M62" si="105">COUNTIF(Q62:EP62,"a")</f>
@@ -37216,7 +37232,7 @@
       <c r="K64" s="14"/>
       <c r="L64" s="14">
         <f t="shared" ref="L64" si="110">IFERROR(L62+J64,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" ref="M64" si="111">COUNTIF(Q64:EP64,"a")</f>
@@ -37548,7 +37564,7 @@
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -37899,7 +37915,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -38232,7 +38248,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -38564,7 +38580,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -38969,7 +38985,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>
@@ -39290,7 +39306,7 @@
       <c r="K76" s="14"/>
       <c r="L76" s="14">
         <f t="shared" ref="L76" si="148">IFERROR(L74+J76,0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M76" s="14">
         <f t="shared" ref="M76" si="149">COUNTIF(Q76:EP76,"a")</f>
@@ -49603,53 +49619,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR75">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>AND(BR75="p",$G75="x")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>AND(BR75="r",BR74&lt;&gt;"p")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"r"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"a"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR75">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$D74="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(ISBLANK($D76),$I75="Réalisé",$D74&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND($N75="f",$F76="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>$D75&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>AND($N74="f",$N75="d")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>AND($N75="d",$N74="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR75">
-    <cfRule type="expression" dxfId="3" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>AND(ISBLANK($D76),$I75="Réalisé",$D74&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>AND($N75="d",$N74="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>AND($N74="f",$N75="d")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>$D75&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50583,7 +50599,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A1:E47">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>WEEKDAY($B1,2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Blocage du clavier fonctionnel.
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C330F5C-C0E4-4042-9149-25C65AA99501}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD1407-82AE-4E06-A806-50EEE5F4908E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -939,70 +939,43 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1011,7 +984,10 @@
     <xf numFmtId="14" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1020,8 +996,41 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1044,352 +1053,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2731">
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dashDot">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="hair">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dashDot">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dashDot">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="hair">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dashDot">
-          <color rgb="FFFF0000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1494,6 +1210,290 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dashDot">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="hair">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dashDot">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dashDot">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="hair">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dashDot">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FFFF0000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -26705,16 +26705,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TabDates" displayName="TabDates" ref="A1:E47" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TabDates" displayName="TabDates" ref="A1:E47" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E47" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Jours" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Jours TPI" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date TPI" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Jours" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Jours TPI" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date TPI" dataDxfId="1">
       <calculatedColumnFormula>IF(TabDates[[#This Row],[Jours TPI]]&lt;&gt;"",TabDates[[#This Row],[Jours]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Livrables / infos" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Livrables / infos" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27023,7 +27023,7 @@
   <dimension ref="A1:HR82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="CF68" sqref="CF68"/>
+      <selection activeCell="D41" sqref="D41:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27069,11 +27069,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="Q3" s="109">
+      <c r="Q3" s="112">
         <f>MAX(K13:K163)</f>
         <v>64</v>
       </c>
-      <c r="R3" s="110"/>
+      <c r="R3" s="113"/>
       <c r="S3" s="28" t="s">
         <v>23</v>
       </c>
@@ -27098,11 +27098,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="Q4" s="111">
+      <c r="Q4" s="114">
         <f>MAX(L13:L163)-L12</f>
         <v>36</v>
       </c>
-      <c r="R4" s="112"/>
+      <c r="R4" s="115"/>
       <c r="S4" s="29" t="s">
         <v>24</v>
       </c>
@@ -27119,31 +27119,31 @@
       <c r="AD4" s="26"/>
       <c r="AE4" s="27"/>
       <c r="AI4" s="66"/>
-      <c r="AJ4" s="115" t="s">
+      <c r="AJ4" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="AK4" s="115"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="115"/>
-      <c r="AN4" s="115"/>
-      <c r="AO4" s="115"/>
-      <c r="AP4" s="115"/>
-      <c r="AQ4" s="115"/>
-      <c r="AR4" s="115"/>
+      <c r="AK4" s="118"/>
+      <c r="AL4" s="118"/>
+      <c r="AM4" s="118"/>
+      <c r="AN4" s="118"/>
+      <c r="AO4" s="118"/>
+      <c r="AP4" s="118"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="118"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="115" t="s">
+      <c r="AU4" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="AV4" s="115"/>
-      <c r="AW4" s="115"/>
-      <c r="AX4" s="115"/>
-      <c r="AY4" s="115"/>
-      <c r="AZ4" s="115"/>
-      <c r="BA4" s="115"/>
-      <c r="BB4" s="115"/>
-      <c r="BC4" s="115"/>
-      <c r="BD4" s="115"/>
-      <c r="BE4" s="115"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+      <c r="AY4" s="118"/>
+      <c r="AZ4" s="118"/>
+      <c r="BA4" s="118"/>
+      <c r="BB4" s="118"/>
+      <c r="BC4" s="118"/>
+      <c r="BD4" s="118"/>
+      <c r="BE4" s="118"/>
       <c r="BG4" s="8"/>
       <c r="BH4" s="3" t="s">
         <v>2</v>
@@ -27155,11 +27155,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="Q5" s="113">
+      <c r="Q5" s="116">
         <f>MAX(M13:M163)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="114"/>
+      <c r="R5" s="117"/>
       <c r="S5" s="30" t="s">
         <v>25</v>
       </c>
@@ -27176,31 +27176,31 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="12"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="115" t="s">
+      <c r="AJ5" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="115"/>
-      <c r="AM5" s="115"/>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="118"/>
+      <c r="AM5" s="118"/>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
       <c r="AT5" s="65"/>
-      <c r="AU5" s="115" t="s">
+      <c r="AU5" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="115"/>
-      <c r="BA5" s="115"/>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="118"/>
+      <c r="AZ5" s="118"/>
+      <c r="BA5" s="118"/>
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
     </row>
     <row r="6" spans="1:226" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -27211,889 +27211,889 @@
     </row>
     <row r="7" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B7" s="69"/>
-      <c r="D7" s="123" t="s">
+      <c r="D7" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="89" t="s">
+      <c r="E7" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="127" t="s">
+      <c r="I7" s="108"/>
+      <c r="J7" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="81" t="s">
+      <c r="M7" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="81" t="s">
+      <c r="O7" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="98" t="s">
+      <c r="P7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="95">
+      <c r="Q7" s="123">
         <v>1</v>
       </c>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="96"/>
-      <c r="U7" s="96"/>
-      <c r="V7" s="96"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="96"/>
-      <c r="Y7" s="96"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="108">
+      <c r="R7" s="91"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="91"/>
+      <c r="U7" s="91"/>
+      <c r="V7" s="91"/>
+      <c r="W7" s="91"/>
+      <c r="X7" s="91"/>
+      <c r="Y7" s="91"/>
+      <c r="Z7" s="101"/>
+      <c r="AA7" s="90">
         <v>2</v>
       </c>
-      <c r="AB7" s="96"/>
-      <c r="AC7" s="96"/>
-      <c r="AD7" s="96"/>
-      <c r="AE7" s="96"/>
-      <c r="AF7" s="96"/>
-      <c r="AG7" s="96"/>
-      <c r="AH7" s="96"/>
-      <c r="AI7" s="96"/>
-      <c r="AJ7" s="97"/>
-      <c r="AK7" s="108">
+      <c r="AB7" s="91"/>
+      <c r="AC7" s="91"/>
+      <c r="AD7" s="91"/>
+      <c r="AE7" s="91"/>
+      <c r="AF7" s="91"/>
+      <c r="AG7" s="91"/>
+      <c r="AH7" s="91"/>
+      <c r="AI7" s="91"/>
+      <c r="AJ7" s="101"/>
+      <c r="AK7" s="90">
         <v>3</v>
       </c>
-      <c r="AL7" s="96"/>
-      <c r="AM7" s="96"/>
-      <c r="AN7" s="96"/>
-      <c r="AO7" s="96"/>
-      <c r="AP7" s="96"/>
-      <c r="AQ7" s="96"/>
-      <c r="AR7" s="96"/>
-      <c r="AS7" s="96"/>
-      <c r="AT7" s="97"/>
-      <c r="AU7" s="108">
+      <c r="AL7" s="91"/>
+      <c r="AM7" s="91"/>
+      <c r="AN7" s="91"/>
+      <c r="AO7" s="91"/>
+      <c r="AP7" s="91"/>
+      <c r="AQ7" s="91"/>
+      <c r="AR7" s="91"/>
+      <c r="AS7" s="91"/>
+      <c r="AT7" s="101"/>
+      <c r="AU7" s="90">
         <v>4</v>
       </c>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="96"/>
-      <c r="AX7" s="96"/>
-      <c r="AY7" s="96"/>
-      <c r="AZ7" s="96"/>
-      <c r="BA7" s="96"/>
-      <c r="BB7" s="96"/>
-      <c r="BC7" s="96"/>
-      <c r="BD7" s="97"/>
-      <c r="BE7" s="108">
+      <c r="AV7" s="91"/>
+      <c r="AW7" s="91"/>
+      <c r="AX7" s="91"/>
+      <c r="AY7" s="91"/>
+      <c r="AZ7" s="91"/>
+      <c r="BA7" s="91"/>
+      <c r="BB7" s="91"/>
+      <c r="BC7" s="91"/>
+      <c r="BD7" s="101"/>
+      <c r="BE7" s="90">
         <v>5</v>
       </c>
-      <c r="BF7" s="96"/>
-      <c r="BG7" s="96"/>
-      <c r="BH7" s="96"/>
-      <c r="BI7" s="96"/>
-      <c r="BJ7" s="96"/>
-      <c r="BK7" s="96"/>
-      <c r="BL7" s="96"/>
-      <c r="BM7" s="96"/>
-      <c r="BN7" s="97"/>
-      <c r="BO7" s="108">
+      <c r="BF7" s="91"/>
+      <c r="BG7" s="91"/>
+      <c r="BH7" s="91"/>
+      <c r="BI7" s="91"/>
+      <c r="BJ7" s="91"/>
+      <c r="BK7" s="91"/>
+      <c r="BL7" s="91"/>
+      <c r="BM7" s="91"/>
+      <c r="BN7" s="101"/>
+      <c r="BO7" s="90">
         <v>6</v>
       </c>
-      <c r="BP7" s="96"/>
-      <c r="BQ7" s="96"/>
-      <c r="BR7" s="96"/>
-      <c r="BS7" s="96"/>
-      <c r="BT7" s="96"/>
-      <c r="BU7" s="96"/>
-      <c r="BV7" s="96"/>
-      <c r="BW7" s="96"/>
-      <c r="BX7" s="97"/>
-      <c r="BY7" s="108">
+      <c r="BP7" s="91"/>
+      <c r="BQ7" s="91"/>
+      <c r="BR7" s="91"/>
+      <c r="BS7" s="91"/>
+      <c r="BT7" s="91"/>
+      <c r="BU7" s="91"/>
+      <c r="BV7" s="91"/>
+      <c r="BW7" s="91"/>
+      <c r="BX7" s="101"/>
+      <c r="BY7" s="90">
         <v>7</v>
       </c>
-      <c r="BZ7" s="96"/>
-      <c r="CA7" s="96"/>
-      <c r="CB7" s="96"/>
-      <c r="CC7" s="96"/>
-      <c r="CD7" s="96"/>
-      <c r="CE7" s="96"/>
-      <c r="CF7" s="96"/>
-      <c r="CG7" s="96"/>
-      <c r="CH7" s="97"/>
-      <c r="CI7" s="108">
+      <c r="BZ7" s="91"/>
+      <c r="CA7" s="91"/>
+      <c r="CB7" s="91"/>
+      <c r="CC7" s="91"/>
+      <c r="CD7" s="91"/>
+      <c r="CE7" s="91"/>
+      <c r="CF7" s="91"/>
+      <c r="CG7" s="91"/>
+      <c r="CH7" s="101"/>
+      <c r="CI7" s="90">
         <v>8</v>
       </c>
-      <c r="CJ7" s="96"/>
-      <c r="CK7" s="96"/>
-      <c r="CL7" s="96"/>
-      <c r="CM7" s="96"/>
-      <c r="CN7" s="96"/>
-      <c r="CO7" s="96"/>
-      <c r="CP7" s="96"/>
-      <c r="CQ7" s="96"/>
-      <c r="CR7" s="97"/>
-      <c r="CS7" s="108">
+      <c r="CJ7" s="91"/>
+      <c r="CK7" s="91"/>
+      <c r="CL7" s="91"/>
+      <c r="CM7" s="91"/>
+      <c r="CN7" s="91"/>
+      <c r="CO7" s="91"/>
+      <c r="CP7" s="91"/>
+      <c r="CQ7" s="91"/>
+      <c r="CR7" s="101"/>
+      <c r="CS7" s="90">
         <v>9</v>
       </c>
-      <c r="CT7" s="96"/>
-      <c r="CU7" s="96"/>
-      <c r="CV7" s="96"/>
-      <c r="CW7" s="96"/>
-      <c r="CX7" s="96"/>
-      <c r="CY7" s="96"/>
-      <c r="CZ7" s="96"/>
-      <c r="DA7" s="96"/>
-      <c r="DB7" s="96"/>
-      <c r="DC7" s="108">
+      <c r="CT7" s="91"/>
+      <c r="CU7" s="91"/>
+      <c r="CV7" s="91"/>
+      <c r="CW7" s="91"/>
+      <c r="CX7" s="91"/>
+      <c r="CY7" s="91"/>
+      <c r="CZ7" s="91"/>
+      <c r="DA7" s="91"/>
+      <c r="DB7" s="91"/>
+      <c r="DC7" s="90">
         <v>10</v>
       </c>
-      <c r="DD7" s="96"/>
-      <c r="DE7" s="96"/>
-      <c r="DF7" s="96"/>
-      <c r="DG7" s="96"/>
-      <c r="DH7" s="96"/>
-      <c r="DI7" s="96"/>
-      <c r="DJ7" s="96"/>
-      <c r="DK7" s="96"/>
-      <c r="DL7" s="97"/>
-      <c r="DM7" s="108">
+      <c r="DD7" s="91"/>
+      <c r="DE7" s="91"/>
+      <c r="DF7" s="91"/>
+      <c r="DG7" s="91"/>
+      <c r="DH7" s="91"/>
+      <c r="DI7" s="91"/>
+      <c r="DJ7" s="91"/>
+      <c r="DK7" s="91"/>
+      <c r="DL7" s="101"/>
+      <c r="DM7" s="90">
         <v>11</v>
       </c>
-      <c r="DN7" s="96"/>
-      <c r="DO7" s="96"/>
-      <c r="DP7" s="96"/>
-      <c r="DQ7" s="96"/>
-      <c r="DR7" s="96"/>
-      <c r="DS7" s="96"/>
-      <c r="DT7" s="96"/>
-      <c r="DU7" s="96"/>
-      <c r="DV7" s="97"/>
-      <c r="DW7" s="108">
+      <c r="DN7" s="91"/>
+      <c r="DO7" s="91"/>
+      <c r="DP7" s="91"/>
+      <c r="DQ7" s="91"/>
+      <c r="DR7" s="91"/>
+      <c r="DS7" s="91"/>
+      <c r="DT7" s="91"/>
+      <c r="DU7" s="91"/>
+      <c r="DV7" s="101"/>
+      <c r="DW7" s="90">
         <v>12</v>
       </c>
-      <c r="DX7" s="96"/>
-      <c r="DY7" s="96"/>
-      <c r="DZ7" s="96"/>
-      <c r="EA7" s="96"/>
-      <c r="EB7" s="96"/>
-      <c r="EC7" s="96"/>
-      <c r="ED7" s="96"/>
-      <c r="EE7" s="96"/>
-      <c r="EF7" s="97"/>
-      <c r="EG7" s="108">
+      <c r="DX7" s="91"/>
+      <c r="DY7" s="91"/>
+      <c r="DZ7" s="91"/>
+      <c r="EA7" s="91"/>
+      <c r="EB7" s="91"/>
+      <c r="EC7" s="91"/>
+      <c r="ED7" s="91"/>
+      <c r="EE7" s="91"/>
+      <c r="EF7" s="101"/>
+      <c r="EG7" s="90">
         <v>13</v>
       </c>
-      <c r="EH7" s="96"/>
-      <c r="EI7" s="96"/>
-      <c r="EJ7" s="96"/>
-      <c r="EK7" s="96"/>
-      <c r="EL7" s="96"/>
-      <c r="EM7" s="96"/>
-      <c r="EN7" s="96"/>
-      <c r="EO7" s="96"/>
-      <c r="EP7" s="126"/>
-      <c r="EQ7" s="96">
+      <c r="EH7" s="91"/>
+      <c r="EI7" s="91"/>
+      <c r="EJ7" s="91"/>
+      <c r="EK7" s="91"/>
+      <c r="EL7" s="91"/>
+      <c r="EM7" s="91"/>
+      <c r="EN7" s="91"/>
+      <c r="EO7" s="91"/>
+      <c r="EP7" s="92"/>
+      <c r="EQ7" s="91">
         <v>14</v>
       </c>
-      <c r="ER7" s="96"/>
-      <c r="ES7" s="96"/>
-      <c r="ET7" s="96"/>
-      <c r="EU7" s="96"/>
-      <c r="EV7" s="96"/>
-      <c r="EW7" s="96"/>
-      <c r="EX7" s="96"/>
-      <c r="EY7" s="96"/>
-      <c r="EZ7" s="97"/>
-      <c r="FA7" s="108">
+      <c r="ER7" s="91"/>
+      <c r="ES7" s="91"/>
+      <c r="ET7" s="91"/>
+      <c r="EU7" s="91"/>
+      <c r="EV7" s="91"/>
+      <c r="EW7" s="91"/>
+      <c r="EX7" s="91"/>
+      <c r="EY7" s="91"/>
+      <c r="EZ7" s="101"/>
+      <c r="FA7" s="90">
         <v>15</v>
       </c>
-      <c r="FB7" s="96"/>
-      <c r="FC7" s="96"/>
-      <c r="FD7" s="96"/>
-      <c r="FE7" s="96"/>
-      <c r="FF7" s="96"/>
-      <c r="FG7" s="96"/>
-      <c r="FH7" s="96"/>
-      <c r="FI7" s="96"/>
-      <c r="FJ7" s="97"/>
-      <c r="FK7" s="108">
+      <c r="FB7" s="91"/>
+      <c r="FC7" s="91"/>
+      <c r="FD7" s="91"/>
+      <c r="FE7" s="91"/>
+      <c r="FF7" s="91"/>
+      <c r="FG7" s="91"/>
+      <c r="FH7" s="91"/>
+      <c r="FI7" s="91"/>
+      <c r="FJ7" s="101"/>
+      <c r="FK7" s="90">
         <v>16</v>
       </c>
-      <c r="FL7" s="96"/>
-      <c r="FM7" s="96"/>
-      <c r="FN7" s="96"/>
-      <c r="FO7" s="96"/>
-      <c r="FP7" s="96"/>
-      <c r="FQ7" s="96"/>
-      <c r="FR7" s="96"/>
-      <c r="FS7" s="96"/>
-      <c r="FT7" s="97"/>
-      <c r="FU7" s="108">
+      <c r="FL7" s="91"/>
+      <c r="FM7" s="91"/>
+      <c r="FN7" s="91"/>
+      <c r="FO7" s="91"/>
+      <c r="FP7" s="91"/>
+      <c r="FQ7" s="91"/>
+      <c r="FR7" s="91"/>
+      <c r="FS7" s="91"/>
+      <c r="FT7" s="101"/>
+      <c r="FU7" s="90">
         <v>17</v>
       </c>
-      <c r="FV7" s="96"/>
-      <c r="FW7" s="96"/>
-      <c r="FX7" s="96"/>
-      <c r="FY7" s="96"/>
-      <c r="FZ7" s="96"/>
-      <c r="GA7" s="96"/>
-      <c r="GB7" s="96"/>
-      <c r="GC7" s="96"/>
-      <c r="GD7" s="97"/>
-      <c r="GE7" s="108">
+      <c r="FV7" s="91"/>
+      <c r="FW7" s="91"/>
+      <c r="FX7" s="91"/>
+      <c r="FY7" s="91"/>
+      <c r="FZ7" s="91"/>
+      <c r="GA7" s="91"/>
+      <c r="GB7" s="91"/>
+      <c r="GC7" s="91"/>
+      <c r="GD7" s="101"/>
+      <c r="GE7" s="90">
         <v>18</v>
       </c>
-      <c r="GF7" s="96"/>
-      <c r="GG7" s="96"/>
-      <c r="GH7" s="96"/>
-      <c r="GI7" s="96"/>
-      <c r="GJ7" s="96"/>
-      <c r="GK7" s="96"/>
-      <c r="GL7" s="96"/>
-      <c r="GM7" s="96"/>
-      <c r="GN7" s="97"/>
-      <c r="GO7" s="108">
+      <c r="GF7" s="91"/>
+      <c r="GG7" s="91"/>
+      <c r="GH7" s="91"/>
+      <c r="GI7" s="91"/>
+      <c r="GJ7" s="91"/>
+      <c r="GK7" s="91"/>
+      <c r="GL7" s="91"/>
+      <c r="GM7" s="91"/>
+      <c r="GN7" s="101"/>
+      <c r="GO7" s="90">
         <v>19</v>
       </c>
-      <c r="GP7" s="96"/>
-      <c r="GQ7" s="96"/>
-      <c r="GR7" s="96"/>
-      <c r="GS7" s="96"/>
-      <c r="GT7" s="96"/>
-      <c r="GU7" s="96"/>
-      <c r="GV7" s="96"/>
-      <c r="GW7" s="96"/>
-      <c r="GX7" s="97"/>
-      <c r="GY7" s="108">
+      <c r="GP7" s="91"/>
+      <c r="GQ7" s="91"/>
+      <c r="GR7" s="91"/>
+      <c r="GS7" s="91"/>
+      <c r="GT7" s="91"/>
+      <c r="GU7" s="91"/>
+      <c r="GV7" s="91"/>
+      <c r="GW7" s="91"/>
+      <c r="GX7" s="101"/>
+      <c r="GY7" s="90">
         <v>20</v>
       </c>
-      <c r="GZ7" s="96"/>
-      <c r="HA7" s="96"/>
-      <c r="HB7" s="96"/>
-      <c r="HC7" s="96"/>
-      <c r="HD7" s="96"/>
-      <c r="HE7" s="96"/>
-      <c r="HF7" s="96"/>
-      <c r="HG7" s="96"/>
-      <c r="HH7" s="97"/>
-      <c r="HI7" s="108">
+      <c r="GZ7" s="91"/>
+      <c r="HA7" s="91"/>
+      <c r="HB7" s="91"/>
+      <c r="HC7" s="91"/>
+      <c r="HD7" s="91"/>
+      <c r="HE7" s="91"/>
+      <c r="HF7" s="91"/>
+      <c r="HG7" s="91"/>
+      <c r="HH7" s="101"/>
+      <c r="HI7" s="90">
         <v>21</v>
       </c>
-      <c r="HJ7" s="96"/>
-      <c r="HK7" s="96"/>
-      <c r="HL7" s="96"/>
-      <c r="HM7" s="96"/>
-      <c r="HN7" s="96"/>
-      <c r="HO7" s="96"/>
-      <c r="HP7" s="96"/>
-      <c r="HQ7" s="96"/>
-      <c r="HR7" s="126"/>
+      <c r="HJ7" s="91"/>
+      <c r="HK7" s="91"/>
+      <c r="HL7" s="91"/>
+      <c r="HM7" s="91"/>
+      <c r="HN7" s="91"/>
+      <c r="HO7" s="91"/>
+      <c r="HP7" s="91"/>
+      <c r="HQ7" s="91"/>
+      <c r="HR7" s="92"/>
     </row>
     <row r="8" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="128"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="102">
+      <c r="D8" s="103"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="128"/>
+      <c r="N8" s="128"/>
+      <c r="O8" s="128"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="130">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],Q7),"")</f>
         <v>45040</v>
       </c>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="103"/>
-      <c r="Z8" s="104"/>
-      <c r="AA8" s="117">
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="94"/>
+      <c r="U8" s="94"/>
+      <c r="V8" s="94"/>
+      <c r="W8" s="94"/>
+      <c r="X8" s="94"/>
+      <c r="Y8" s="94"/>
+      <c r="Z8" s="95"/>
+      <c r="AA8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AA7),"")</f>
         <v>45041</v>
       </c>
-      <c r="AB8" s="103"/>
-      <c r="AC8" s="103"/>
-      <c r="AD8" s="103"/>
-      <c r="AE8" s="103"/>
-      <c r="AF8" s="103"/>
-      <c r="AG8" s="103"/>
-      <c r="AH8" s="103"/>
-      <c r="AI8" s="103"/>
-      <c r="AJ8" s="104"/>
-      <c r="AK8" s="117">
+      <c r="AB8" s="94"/>
+      <c r="AC8" s="94"/>
+      <c r="AD8" s="94"/>
+      <c r="AE8" s="94"/>
+      <c r="AF8" s="94"/>
+      <c r="AG8" s="94"/>
+      <c r="AH8" s="94"/>
+      <c r="AI8" s="94"/>
+      <c r="AJ8" s="95"/>
+      <c r="AK8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AK7),"")</f>
         <v>45042</v>
       </c>
-      <c r="AL8" s="103"/>
-      <c r="AM8" s="103"/>
-      <c r="AN8" s="103"/>
-      <c r="AO8" s="103"/>
-      <c r="AP8" s="103"/>
-      <c r="AQ8" s="103"/>
-      <c r="AR8" s="103"/>
-      <c r="AS8" s="103"/>
-      <c r="AT8" s="104"/>
-      <c r="AU8" s="117">
+      <c r="AL8" s="94"/>
+      <c r="AM8" s="94"/>
+      <c r="AN8" s="94"/>
+      <c r="AO8" s="94"/>
+      <c r="AP8" s="94"/>
+      <c r="AQ8" s="94"/>
+      <c r="AR8" s="94"/>
+      <c r="AS8" s="94"/>
+      <c r="AT8" s="95"/>
+      <c r="AU8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AU7),"")</f>
         <v>45048</v>
       </c>
-      <c r="AV8" s="103"/>
-      <c r="AW8" s="103"/>
-      <c r="AX8" s="103"/>
-      <c r="AY8" s="103"/>
-      <c r="AZ8" s="103"/>
-      <c r="BA8" s="103"/>
-      <c r="BB8" s="103"/>
-      <c r="BC8" s="103"/>
-      <c r="BD8" s="104"/>
-      <c r="BE8" s="117">
+      <c r="AV8" s="94"/>
+      <c r="AW8" s="94"/>
+      <c r="AX8" s="94"/>
+      <c r="AY8" s="94"/>
+      <c r="AZ8" s="94"/>
+      <c r="BA8" s="94"/>
+      <c r="BB8" s="94"/>
+      <c r="BC8" s="94"/>
+      <c r="BD8" s="95"/>
+      <c r="BE8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BE7),"")</f>
         <v>45049</v>
       </c>
-      <c r="BF8" s="103"/>
-      <c r="BG8" s="103"/>
-      <c r="BH8" s="103"/>
-      <c r="BI8" s="103"/>
-      <c r="BJ8" s="103"/>
-      <c r="BK8" s="103"/>
-      <c r="BL8" s="103"/>
-      <c r="BM8" s="103"/>
-      <c r="BN8" s="104"/>
-      <c r="BO8" s="117">
+      <c r="BF8" s="94"/>
+      <c r="BG8" s="94"/>
+      <c r="BH8" s="94"/>
+      <c r="BI8" s="94"/>
+      <c r="BJ8" s="94"/>
+      <c r="BK8" s="94"/>
+      <c r="BL8" s="94"/>
+      <c r="BM8" s="94"/>
+      <c r="BN8" s="95"/>
+      <c r="BO8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BO7),"")</f>
         <v>45054</v>
       </c>
-      <c r="BP8" s="103"/>
-      <c r="BQ8" s="103"/>
-      <c r="BR8" s="103"/>
-      <c r="BS8" s="103"/>
-      <c r="BT8" s="103"/>
-      <c r="BU8" s="103"/>
-      <c r="BV8" s="103"/>
-      <c r="BW8" s="103"/>
-      <c r="BX8" s="104"/>
-      <c r="BY8" s="117">
+      <c r="BP8" s="94"/>
+      <c r="BQ8" s="94"/>
+      <c r="BR8" s="94"/>
+      <c r="BS8" s="94"/>
+      <c r="BT8" s="94"/>
+      <c r="BU8" s="94"/>
+      <c r="BV8" s="94"/>
+      <c r="BW8" s="94"/>
+      <c r="BX8" s="95"/>
+      <c r="BY8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BY7),"")</f>
         <v>45055</v>
       </c>
-      <c r="BZ8" s="103"/>
-      <c r="CA8" s="103"/>
-      <c r="CB8" s="103"/>
-      <c r="CC8" s="103"/>
-      <c r="CD8" s="103"/>
-      <c r="CE8" s="103"/>
-      <c r="CF8" s="103"/>
-      <c r="CG8" s="103"/>
-      <c r="CH8" s="104"/>
-      <c r="CI8" s="117">
+      <c r="BZ8" s="94"/>
+      <c r="CA8" s="94"/>
+      <c r="CB8" s="94"/>
+      <c r="CC8" s="94"/>
+      <c r="CD8" s="94"/>
+      <c r="CE8" s="94"/>
+      <c r="CF8" s="94"/>
+      <c r="CG8" s="94"/>
+      <c r="CH8" s="95"/>
+      <c r="CI8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CI7),"")</f>
         <v>45056</v>
       </c>
-      <c r="CJ8" s="103"/>
-      <c r="CK8" s="103"/>
-      <c r="CL8" s="103"/>
-      <c r="CM8" s="103"/>
-      <c r="CN8" s="103"/>
-      <c r="CO8" s="103"/>
-      <c r="CP8" s="103"/>
-      <c r="CQ8" s="103"/>
-      <c r="CR8" s="104"/>
-      <c r="CS8" s="117">
+      <c r="CJ8" s="94"/>
+      <c r="CK8" s="94"/>
+      <c r="CL8" s="94"/>
+      <c r="CM8" s="94"/>
+      <c r="CN8" s="94"/>
+      <c r="CO8" s="94"/>
+      <c r="CP8" s="94"/>
+      <c r="CQ8" s="94"/>
+      <c r="CR8" s="95"/>
+      <c r="CS8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CS7),"")</f>
         <v>45061</v>
       </c>
-      <c r="CT8" s="103"/>
-      <c r="CU8" s="103"/>
-      <c r="CV8" s="103"/>
-      <c r="CW8" s="103"/>
-      <c r="CX8" s="103"/>
-      <c r="CY8" s="103"/>
-      <c r="CZ8" s="103"/>
-      <c r="DA8" s="103"/>
-      <c r="DB8" s="103"/>
-      <c r="DC8" s="117">
+      <c r="CT8" s="94"/>
+      <c r="CU8" s="94"/>
+      <c r="CV8" s="94"/>
+      <c r="CW8" s="94"/>
+      <c r="CX8" s="94"/>
+      <c r="CY8" s="94"/>
+      <c r="CZ8" s="94"/>
+      <c r="DA8" s="94"/>
+      <c r="DB8" s="94"/>
+      <c r="DC8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DC7),"")</f>
         <v>45062</v>
       </c>
-      <c r="DD8" s="103"/>
-      <c r="DE8" s="103"/>
-      <c r="DF8" s="103"/>
-      <c r="DG8" s="103"/>
-      <c r="DH8" s="103"/>
-      <c r="DI8" s="103"/>
-      <c r="DJ8" s="103"/>
-      <c r="DK8" s="103"/>
-      <c r="DL8" s="104"/>
-      <c r="DM8" s="117">
+      <c r="DD8" s="94"/>
+      <c r="DE8" s="94"/>
+      <c r="DF8" s="94"/>
+      <c r="DG8" s="94"/>
+      <c r="DH8" s="94"/>
+      <c r="DI8" s="94"/>
+      <c r="DJ8" s="94"/>
+      <c r="DK8" s="94"/>
+      <c r="DL8" s="95"/>
+      <c r="DM8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DM7),"")</f>
         <v>45063</v>
       </c>
-      <c r="DN8" s="103"/>
-      <c r="DO8" s="103"/>
-      <c r="DP8" s="103"/>
-      <c r="DQ8" s="103"/>
-      <c r="DR8" s="103"/>
-      <c r="DS8" s="103"/>
-      <c r="DT8" s="103"/>
-      <c r="DU8" s="103"/>
-      <c r="DV8" s="104"/>
-      <c r="DW8" s="117" t="str">
+      <c r="DN8" s="94"/>
+      <c r="DO8" s="94"/>
+      <c r="DP8" s="94"/>
+      <c r="DQ8" s="94"/>
+      <c r="DR8" s="94"/>
+      <c r="DS8" s="94"/>
+      <c r="DT8" s="94"/>
+      <c r="DU8" s="94"/>
+      <c r="DV8" s="95"/>
+      <c r="DW8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DW7),"")</f>
         <v/>
       </c>
-      <c r="DX8" s="103"/>
-      <c r="DY8" s="103"/>
-      <c r="DZ8" s="103"/>
-      <c r="EA8" s="103"/>
-      <c r="EB8" s="103"/>
-      <c r="EC8" s="103"/>
-      <c r="ED8" s="103"/>
-      <c r="EE8" s="103"/>
-      <c r="EF8" s="104"/>
-      <c r="EG8" s="117" t="str">
+      <c r="DX8" s="94"/>
+      <c r="DY8" s="94"/>
+      <c r="DZ8" s="94"/>
+      <c r="EA8" s="94"/>
+      <c r="EB8" s="94"/>
+      <c r="EC8" s="94"/>
+      <c r="ED8" s="94"/>
+      <c r="EE8" s="94"/>
+      <c r="EF8" s="95"/>
+      <c r="EG8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EG7),"")</f>
         <v/>
       </c>
-      <c r="EH8" s="103"/>
-      <c r="EI8" s="103"/>
-      <c r="EJ8" s="103"/>
-      <c r="EK8" s="103"/>
-      <c r="EL8" s="103"/>
-      <c r="EM8" s="103"/>
-      <c r="EN8" s="103"/>
-      <c r="EO8" s="103"/>
-      <c r="EP8" s="118"/>
-      <c r="EQ8" s="103" t="str">
+      <c r="EH8" s="94"/>
+      <c r="EI8" s="94"/>
+      <c r="EJ8" s="94"/>
+      <c r="EK8" s="94"/>
+      <c r="EL8" s="94"/>
+      <c r="EM8" s="94"/>
+      <c r="EN8" s="94"/>
+      <c r="EO8" s="94"/>
+      <c r="EP8" s="96"/>
+      <c r="EQ8" s="94" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EQ7),"")</f>
         <v/>
       </c>
-      <c r="ER8" s="103"/>
-      <c r="ES8" s="103"/>
-      <c r="ET8" s="103"/>
-      <c r="EU8" s="103"/>
-      <c r="EV8" s="103"/>
-      <c r="EW8" s="103"/>
-      <c r="EX8" s="103"/>
-      <c r="EY8" s="103"/>
-      <c r="EZ8" s="104"/>
-      <c r="FA8" s="117" t="str">
+      <c r="ER8" s="94"/>
+      <c r="ES8" s="94"/>
+      <c r="ET8" s="94"/>
+      <c r="EU8" s="94"/>
+      <c r="EV8" s="94"/>
+      <c r="EW8" s="94"/>
+      <c r="EX8" s="94"/>
+      <c r="EY8" s="94"/>
+      <c r="EZ8" s="95"/>
+      <c r="FA8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FA7),"")</f>
         <v/>
       </c>
-      <c r="FB8" s="103"/>
-      <c r="FC8" s="103"/>
-      <c r="FD8" s="103"/>
-      <c r="FE8" s="103"/>
-      <c r="FF8" s="103"/>
-      <c r="FG8" s="103"/>
-      <c r="FH8" s="103"/>
-      <c r="FI8" s="103"/>
-      <c r="FJ8" s="104"/>
-      <c r="FK8" s="117" t="str">
+      <c r="FB8" s="94"/>
+      <c r="FC8" s="94"/>
+      <c r="FD8" s="94"/>
+      <c r="FE8" s="94"/>
+      <c r="FF8" s="94"/>
+      <c r="FG8" s="94"/>
+      <c r="FH8" s="94"/>
+      <c r="FI8" s="94"/>
+      <c r="FJ8" s="95"/>
+      <c r="FK8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FK7),"")</f>
         <v/>
       </c>
-      <c r="FL8" s="103"/>
-      <c r="FM8" s="103"/>
-      <c r="FN8" s="103"/>
-      <c r="FO8" s="103"/>
-      <c r="FP8" s="103"/>
-      <c r="FQ8" s="103"/>
-      <c r="FR8" s="103"/>
-      <c r="FS8" s="103"/>
-      <c r="FT8" s="104"/>
-      <c r="FU8" s="117" t="str">
+      <c r="FL8" s="94"/>
+      <c r="FM8" s="94"/>
+      <c r="FN8" s="94"/>
+      <c r="FO8" s="94"/>
+      <c r="FP8" s="94"/>
+      <c r="FQ8" s="94"/>
+      <c r="FR8" s="94"/>
+      <c r="FS8" s="94"/>
+      <c r="FT8" s="95"/>
+      <c r="FU8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FU7),"")</f>
         <v/>
       </c>
-      <c r="FV8" s="103"/>
-      <c r="FW8" s="103"/>
-      <c r="FX8" s="103"/>
-      <c r="FY8" s="103"/>
-      <c r="FZ8" s="103"/>
-      <c r="GA8" s="103"/>
-      <c r="GB8" s="103"/>
-      <c r="GC8" s="103"/>
-      <c r="GD8" s="104"/>
-      <c r="GE8" s="117" t="str">
+      <c r="FV8" s="94"/>
+      <c r="FW8" s="94"/>
+      <c r="FX8" s="94"/>
+      <c r="FY8" s="94"/>
+      <c r="FZ8" s="94"/>
+      <c r="GA8" s="94"/>
+      <c r="GB8" s="94"/>
+      <c r="GC8" s="94"/>
+      <c r="GD8" s="95"/>
+      <c r="GE8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GE7),"")</f>
         <v/>
       </c>
-      <c r="GF8" s="103"/>
-      <c r="GG8" s="103"/>
-      <c r="GH8" s="103"/>
-      <c r="GI8" s="103"/>
-      <c r="GJ8" s="103"/>
-      <c r="GK8" s="103"/>
-      <c r="GL8" s="103"/>
-      <c r="GM8" s="103"/>
-      <c r="GN8" s="104"/>
-      <c r="GO8" s="117" t="str">
+      <c r="GF8" s="94"/>
+      <c r="GG8" s="94"/>
+      <c r="GH8" s="94"/>
+      <c r="GI8" s="94"/>
+      <c r="GJ8" s="94"/>
+      <c r="GK8" s="94"/>
+      <c r="GL8" s="94"/>
+      <c r="GM8" s="94"/>
+      <c r="GN8" s="95"/>
+      <c r="GO8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GO7),"")</f>
         <v/>
       </c>
-      <c r="GP8" s="103"/>
-      <c r="GQ8" s="103"/>
-      <c r="GR8" s="103"/>
-      <c r="GS8" s="103"/>
-      <c r="GT8" s="103"/>
-      <c r="GU8" s="103"/>
-      <c r="GV8" s="103"/>
-      <c r="GW8" s="103"/>
-      <c r="GX8" s="104"/>
-      <c r="GY8" s="117" t="str">
+      <c r="GP8" s="94"/>
+      <c r="GQ8" s="94"/>
+      <c r="GR8" s="94"/>
+      <c r="GS8" s="94"/>
+      <c r="GT8" s="94"/>
+      <c r="GU8" s="94"/>
+      <c r="GV8" s="94"/>
+      <c r="GW8" s="94"/>
+      <c r="GX8" s="95"/>
+      <c r="GY8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GY7),"")</f>
         <v/>
       </c>
-      <c r="GZ8" s="103"/>
-      <c r="HA8" s="103"/>
-      <c r="HB8" s="103"/>
-      <c r="HC8" s="103"/>
-      <c r="HD8" s="103"/>
-      <c r="HE8" s="103"/>
-      <c r="HF8" s="103"/>
-      <c r="HG8" s="103"/>
-      <c r="HH8" s="104"/>
-      <c r="HI8" s="117" t="str">
+      <c r="GZ8" s="94"/>
+      <c r="HA8" s="94"/>
+      <c r="HB8" s="94"/>
+      <c r="HC8" s="94"/>
+      <c r="HD8" s="94"/>
+      <c r="HE8" s="94"/>
+      <c r="HF8" s="94"/>
+      <c r="HG8" s="94"/>
+      <c r="HH8" s="95"/>
+      <c r="HI8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],HI7),"")</f>
         <v/>
       </c>
-      <c r="HJ8" s="103"/>
-      <c r="HK8" s="103"/>
-      <c r="HL8" s="103"/>
-      <c r="HM8" s="103"/>
-      <c r="HN8" s="103"/>
-      <c r="HO8" s="103"/>
-      <c r="HP8" s="103"/>
-      <c r="HQ8" s="103"/>
-      <c r="HR8" s="118"/>
+      <c r="HJ8" s="94"/>
+      <c r="HK8" s="94"/>
+      <c r="HL8" s="94"/>
+      <c r="HM8" s="94"/>
+      <c r="HN8" s="94"/>
+      <c r="HO8" s="94"/>
+      <c r="HP8" s="94"/>
+      <c r="HQ8" s="94"/>
+      <c r="HR8" s="96"/>
     </row>
     <row r="9" spans="1:226" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="128"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="105">
+      <c r="D9" s="103"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
+      <c r="O9" s="128"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="131">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(Q8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="107"/>
-      <c r="AA9" s="116" t="str">
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="98"/>
+      <c r="U9" s="98"/>
+      <c r="V9" s="98"/>
+      <c r="W9" s="98"/>
+      <c r="X9" s="98"/>
+      <c r="Y9" s="98"/>
+      <c r="Z9" s="99"/>
+      <c r="AA9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L1] Connexion</v>
       </c>
-      <c r="AB9" s="106"/>
-      <c r="AC9" s="106"/>
-      <c r="AD9" s="106"/>
-      <c r="AE9" s="106"/>
-      <c r="AF9" s="106"/>
-      <c r="AG9" s="106"/>
-      <c r="AH9" s="106"/>
-      <c r="AI9" s="106"/>
-      <c r="AJ9" s="107"/>
-      <c r="AK9" s="116">
+      <c r="AB9" s="98"/>
+      <c r="AC9" s="98"/>
+      <c r="AD9" s="98"/>
+      <c r="AE9" s="98"/>
+      <c r="AF9" s="98"/>
+      <c r="AG9" s="98"/>
+      <c r="AH9" s="98"/>
+      <c r="AI9" s="98"/>
+      <c r="AJ9" s="99"/>
+      <c r="AK9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="106"/>
-      <c r="AM9" s="106"/>
-      <c r="AN9" s="106"/>
-      <c r="AO9" s="106"/>
-      <c r="AP9" s="106"/>
-      <c r="AQ9" s="106"/>
-      <c r="AR9" s="106"/>
-      <c r="AS9" s="106"/>
-      <c r="AT9" s="107"/>
-      <c r="AU9" s="116" t="str">
+      <c r="AL9" s="98"/>
+      <c r="AM9" s="98"/>
+      <c r="AN9" s="98"/>
+      <c r="AO9" s="98"/>
+      <c r="AP9" s="98"/>
+      <c r="AQ9" s="98"/>
+      <c r="AR9" s="98"/>
+      <c r="AS9" s="98"/>
+      <c r="AT9" s="99"/>
+      <c r="AU9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L2] Affichage Professeur</v>
       </c>
-      <c r="AV9" s="106"/>
-      <c r="AW9" s="106"/>
-      <c r="AX9" s="106"/>
-      <c r="AY9" s="106"/>
-      <c r="AZ9" s="106"/>
-      <c r="BA9" s="106"/>
-      <c r="BB9" s="106"/>
-      <c r="BC9" s="106"/>
-      <c r="BD9" s="107"/>
-      <c r="BE9" s="116">
+      <c r="AV9" s="98"/>
+      <c r="AW9" s="98"/>
+      <c r="AX9" s="98"/>
+      <c r="AY9" s="98"/>
+      <c r="AZ9" s="98"/>
+      <c r="BA9" s="98"/>
+      <c r="BB9" s="98"/>
+      <c r="BC9" s="98"/>
+      <c r="BD9" s="99"/>
+      <c r="BE9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BF9" s="106"/>
-      <c r="BG9" s="106"/>
-      <c r="BH9" s="106"/>
-      <c r="BI9" s="106"/>
-      <c r="BJ9" s="106"/>
-      <c r="BK9" s="106"/>
-      <c r="BL9" s="106"/>
-      <c r="BM9" s="106"/>
-      <c r="BN9" s="107"/>
-      <c r="BO9" s="116" t="str">
+      <c r="BF9" s="98"/>
+      <c r="BG9" s="98"/>
+      <c r="BH9" s="98"/>
+      <c r="BI9" s="98"/>
+      <c r="BJ9" s="98"/>
+      <c r="BK9" s="98"/>
+      <c r="BL9" s="98"/>
+      <c r="BM9" s="98"/>
+      <c r="BN9" s="99"/>
+      <c r="BO9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L3] Historique</v>
       </c>
-      <c r="BP9" s="106"/>
-      <c r="BQ9" s="106"/>
-      <c r="BR9" s="106"/>
-      <c r="BS9" s="106"/>
-      <c r="BT9" s="106"/>
-      <c r="BU9" s="106"/>
-      <c r="BV9" s="106"/>
-      <c r="BW9" s="106"/>
-      <c r="BX9" s="107"/>
-      <c r="BY9" s="116">
+      <c r="BP9" s="98"/>
+      <c r="BQ9" s="98"/>
+      <c r="BR9" s="98"/>
+      <c r="BS9" s="98"/>
+      <c r="BT9" s="98"/>
+      <c r="BU9" s="98"/>
+      <c r="BV9" s="98"/>
+      <c r="BW9" s="98"/>
+      <c r="BX9" s="99"/>
+      <c r="BY9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BZ9" s="106"/>
-      <c r="CA9" s="106"/>
-      <c r="CB9" s="106"/>
-      <c r="CC9" s="106"/>
-      <c r="CD9" s="106"/>
-      <c r="CE9" s="106"/>
-      <c r="CF9" s="106"/>
-      <c r="CG9" s="106"/>
-      <c r="CH9" s="107"/>
-      <c r="CI9" s="116" t="str">
+      <c r="BZ9" s="98"/>
+      <c r="CA9" s="98"/>
+      <c r="CB9" s="98"/>
+      <c r="CC9" s="98"/>
+      <c r="CD9" s="98"/>
+      <c r="CE9" s="98"/>
+      <c r="CF9" s="98"/>
+      <c r="CG9" s="98"/>
+      <c r="CH9" s="99"/>
+      <c r="CI9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L4] Filtrage</v>
       </c>
-      <c r="CJ9" s="106"/>
-      <c r="CK9" s="106"/>
-      <c r="CL9" s="106"/>
-      <c r="CM9" s="106"/>
-      <c r="CN9" s="106"/>
-      <c r="CO9" s="106"/>
-      <c r="CP9" s="106"/>
-      <c r="CQ9" s="106"/>
-      <c r="CR9" s="107"/>
-      <c r="CS9" s="116" t="str">
+      <c r="CJ9" s="98"/>
+      <c r="CK9" s="98"/>
+      <c r="CL9" s="98"/>
+      <c r="CM9" s="98"/>
+      <c r="CN9" s="98"/>
+      <c r="CO9" s="98"/>
+      <c r="CP9" s="98"/>
+      <c r="CQ9" s="98"/>
+      <c r="CR9" s="99"/>
+      <c r="CS9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CS8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L5] Streaming multicast</v>
       </c>
-      <c r="CT9" s="106"/>
-      <c r="CU9" s="106"/>
-      <c r="CV9" s="106"/>
-      <c r="CW9" s="106"/>
-      <c r="CX9" s="106"/>
-      <c r="CY9" s="106"/>
-      <c r="CZ9" s="106"/>
-      <c r="DA9" s="106"/>
-      <c r="DB9" s="106"/>
-      <c r="DC9" s="116">
+      <c r="CT9" s="98"/>
+      <c r="CU9" s="98"/>
+      <c r="CV9" s="98"/>
+      <c r="CW9" s="98"/>
+      <c r="CX9" s="98"/>
+      <c r="CY9" s="98"/>
+      <c r="CZ9" s="98"/>
+      <c r="DA9" s="98"/>
+      <c r="DB9" s="98"/>
+      <c r="DC9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DC8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DD9" s="106"/>
-      <c r="DE9" s="106"/>
-      <c r="DF9" s="106"/>
-      <c r="DG9" s="106"/>
-      <c r="DH9" s="106"/>
-      <c r="DI9" s="106"/>
-      <c r="DJ9" s="106"/>
-      <c r="DK9" s="106"/>
-      <c r="DL9" s="107"/>
-      <c r="DM9" s="116" t="str">
+      <c r="DD9" s="98"/>
+      <c r="DE9" s="98"/>
+      <c r="DF9" s="98"/>
+      <c r="DG9" s="98"/>
+      <c r="DH9" s="98"/>
+      <c r="DI9" s="98"/>
+      <c r="DJ9" s="98"/>
+      <c r="DK9" s="98"/>
+      <c r="DL9" s="99"/>
+      <c r="DM9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DM8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L6] Contrôle à distance</v>
       </c>
-      <c r="DN9" s="106"/>
-      <c r="DO9" s="106"/>
-      <c r="DP9" s="106"/>
-      <c r="DQ9" s="106"/>
-      <c r="DR9" s="106"/>
-      <c r="DS9" s="106"/>
-      <c r="DT9" s="106"/>
-      <c r="DU9" s="106"/>
-      <c r="DV9" s="107"/>
-      <c r="DW9" s="116">
+      <c r="DN9" s="98"/>
+      <c r="DO9" s="98"/>
+      <c r="DP9" s="98"/>
+      <c r="DQ9" s="98"/>
+      <c r="DR9" s="98"/>
+      <c r="DS9" s="98"/>
+      <c r="DT9" s="98"/>
+      <c r="DU9" s="98"/>
+      <c r="DV9" s="99"/>
+      <c r="DW9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DW8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DX9" s="106"/>
-      <c r="DY9" s="106"/>
-      <c r="DZ9" s="106"/>
-      <c r="EA9" s="106"/>
-      <c r="EB9" s="106"/>
-      <c r="EC9" s="106"/>
-      <c r="ED9" s="106"/>
-      <c r="EE9" s="106"/>
-      <c r="EF9" s="107"/>
-      <c r="EG9" s="116">
+      <c r="DX9" s="98"/>
+      <c r="DY9" s="98"/>
+      <c r="DZ9" s="98"/>
+      <c r="EA9" s="98"/>
+      <c r="EB9" s="98"/>
+      <c r="EC9" s="98"/>
+      <c r="ED9" s="98"/>
+      <c r="EE9" s="98"/>
+      <c r="EF9" s="99"/>
+      <c r="EG9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EG8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="EH9" s="106"/>
-      <c r="EI9" s="106"/>
-      <c r="EJ9" s="106"/>
-      <c r="EK9" s="106"/>
-      <c r="EL9" s="106"/>
-      <c r="EM9" s="106"/>
-      <c r="EN9" s="106"/>
-      <c r="EO9" s="106"/>
-      <c r="EP9" s="122"/>
-      <c r="EQ9" s="106">
+      <c r="EH9" s="98"/>
+      <c r="EI9" s="98"/>
+      <c r="EJ9" s="98"/>
+      <c r="EK9" s="98"/>
+      <c r="EL9" s="98"/>
+      <c r="EM9" s="98"/>
+      <c r="EN9" s="98"/>
+      <c r="EO9" s="98"/>
+      <c r="EP9" s="100"/>
+      <c r="EQ9" s="98">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EQ8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="ER9" s="106"/>
-      <c r="ES9" s="106"/>
-      <c r="ET9" s="106"/>
-      <c r="EU9" s="106"/>
-      <c r="EV9" s="106"/>
-      <c r="EW9" s="106"/>
-      <c r="EX9" s="106"/>
-      <c r="EY9" s="106"/>
-      <c r="EZ9" s="107"/>
-      <c r="FA9" s="116">
+      <c r="ER9" s="98"/>
+      <c r="ES9" s="98"/>
+      <c r="ET9" s="98"/>
+      <c r="EU9" s="98"/>
+      <c r="EV9" s="98"/>
+      <c r="EW9" s="98"/>
+      <c r="EX9" s="98"/>
+      <c r="EY9" s="98"/>
+      <c r="EZ9" s="99"/>
+      <c r="FA9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FB9" s="106"/>
-      <c r="FC9" s="106"/>
-      <c r="FD9" s="106"/>
-      <c r="FE9" s="106"/>
-      <c r="FF9" s="106"/>
-      <c r="FG9" s="106"/>
-      <c r="FH9" s="106"/>
-      <c r="FI9" s="106"/>
-      <c r="FJ9" s="107"/>
-      <c r="FK9" s="116">
+      <c r="FB9" s="98"/>
+      <c r="FC9" s="98"/>
+      <c r="FD9" s="98"/>
+      <c r="FE9" s="98"/>
+      <c r="FF9" s="98"/>
+      <c r="FG9" s="98"/>
+      <c r="FH9" s="98"/>
+      <c r="FI9" s="98"/>
+      <c r="FJ9" s="99"/>
+      <c r="FK9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FL9" s="106"/>
-      <c r="FM9" s="106"/>
-      <c r="FN9" s="106"/>
-      <c r="FO9" s="106"/>
-      <c r="FP9" s="106"/>
-      <c r="FQ9" s="106"/>
-      <c r="FR9" s="106"/>
-      <c r="FS9" s="106"/>
-      <c r="FT9" s="107"/>
-      <c r="FU9" s="116">
+      <c r="FL9" s="98"/>
+      <c r="FM9" s="98"/>
+      <c r="FN9" s="98"/>
+      <c r="FO9" s="98"/>
+      <c r="FP9" s="98"/>
+      <c r="FQ9" s="98"/>
+      <c r="FR9" s="98"/>
+      <c r="FS9" s="98"/>
+      <c r="FT9" s="99"/>
+      <c r="FU9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FV9" s="106"/>
-      <c r="FW9" s="106"/>
-      <c r="FX9" s="106"/>
-      <c r="FY9" s="106"/>
-      <c r="FZ9" s="106"/>
-      <c r="GA9" s="106"/>
-      <c r="GB9" s="106"/>
-      <c r="GC9" s="106"/>
-      <c r="GD9" s="107"/>
-      <c r="GE9" s="116">
+      <c r="FV9" s="98"/>
+      <c r="FW9" s="98"/>
+      <c r="FX9" s="98"/>
+      <c r="FY9" s="98"/>
+      <c r="FZ9" s="98"/>
+      <c r="GA9" s="98"/>
+      <c r="GB9" s="98"/>
+      <c r="GC9" s="98"/>
+      <c r="GD9" s="99"/>
+      <c r="GE9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GF9" s="106"/>
-      <c r="GG9" s="106"/>
-      <c r="GH9" s="106"/>
-      <c r="GI9" s="106"/>
-      <c r="GJ9" s="106"/>
-      <c r="GK9" s="106"/>
-      <c r="GL9" s="106"/>
-      <c r="GM9" s="106"/>
-      <c r="GN9" s="107"/>
-      <c r="GO9" s="116">
+      <c r="GF9" s="98"/>
+      <c r="GG9" s="98"/>
+      <c r="GH9" s="98"/>
+      <c r="GI9" s="98"/>
+      <c r="GJ9" s="98"/>
+      <c r="GK9" s="98"/>
+      <c r="GL9" s="98"/>
+      <c r="GM9" s="98"/>
+      <c r="GN9" s="99"/>
+      <c r="GO9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GP9" s="106"/>
-      <c r="GQ9" s="106"/>
-      <c r="GR9" s="106"/>
-      <c r="GS9" s="106"/>
-      <c r="GT9" s="106"/>
-      <c r="GU9" s="106"/>
-      <c r="GV9" s="106"/>
-      <c r="GW9" s="106"/>
-      <c r="GX9" s="107"/>
-      <c r="GY9" s="116">
+      <c r="GP9" s="98"/>
+      <c r="GQ9" s="98"/>
+      <c r="GR9" s="98"/>
+      <c r="GS9" s="98"/>
+      <c r="GT9" s="98"/>
+      <c r="GU9" s="98"/>
+      <c r="GV9" s="98"/>
+      <c r="GW9" s="98"/>
+      <c r="GX9" s="99"/>
+      <c r="GY9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GZ9" s="106"/>
-      <c r="HA9" s="106"/>
-      <c r="HB9" s="106"/>
-      <c r="HC9" s="106"/>
-      <c r="HD9" s="106"/>
-      <c r="HE9" s="106"/>
-      <c r="HF9" s="106"/>
-      <c r="HG9" s="106"/>
-      <c r="HH9" s="107"/>
-      <c r="HI9" s="116">
+      <c r="GZ9" s="98"/>
+      <c r="HA9" s="98"/>
+      <c r="HB9" s="98"/>
+      <c r="HC9" s="98"/>
+      <c r="HD9" s="98"/>
+      <c r="HE9" s="98"/>
+      <c r="HF9" s="98"/>
+      <c r="HG9" s="98"/>
+      <c r="HH9" s="99"/>
+      <c r="HI9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(HI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="HJ9" s="106"/>
-      <c r="HK9" s="106"/>
-      <c r="HL9" s="106"/>
-      <c r="HM9" s="106"/>
-      <c r="HN9" s="106"/>
-      <c r="HO9" s="106"/>
-      <c r="HP9" s="106"/>
-      <c r="HQ9" s="106"/>
-      <c r="HR9" s="122"/>
+      <c r="HJ9" s="98"/>
+      <c r="HK9" s="98"/>
+      <c r="HL9" s="98"/>
+      <c r="HM9" s="98"/>
+      <c r="HN9" s="98"/>
+      <c r="HO9" s="98"/>
+      <c r="HP9" s="98"/>
+      <c r="HQ9" s="98"/>
+      <c r="HR9" s="100"/>
     </row>
     <row r="10" spans="1:226" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="99"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
+      <c r="N10" s="128"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="125"/>
       <c r="Q10" s="5"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="20"/>
@@ -28139,19 +28139,19 @@
       <c r="A11" s="68"/>
       <c r="B11" s="5"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="100"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="134"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
+      <c r="O11" s="129"/>
+      <c r="P11" s="126"/>
       <c r="Q11" s="51">
         <v>0</v>
       </c>
@@ -29648,17 +29648,17 @@
       </c>
     </row>
     <row r="13" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="G13" s="87" t="s">
+      <c r="E13" s="83"/>
+      <c r="G13" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="119" t="str">
+      <c r="H13" s="85" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
       </c>
@@ -29764,11 +29764,11 @@
       <c r="HR13" s="4"/>
     </row>
     <row r="14" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="134"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="101"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="119"/>
+      <c r="B14" s="81"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="83"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="85"/>
       <c r="I14" s="45" t="s">
         <v>1</v>
       </c>
@@ -30020,22 +30020,22 @@
       <c r="HR14" s="31"/>
     </row>
     <row r="15" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="134" t="s">
+      <c r="B15" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="101">
+      <c r="F15" s="83">
         <v>1</v>
       </c>
-      <c r="G15" s="87" t="s">
+      <c r="G15" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="119" t="str">
+      <c r="H15" s="85" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
       </c>
@@ -30106,12 +30106,12 @@
       <c r="HR15" s="4"/>
     </row>
     <row r="16" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="134"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="119"/>
+      <c r="B16" s="81"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="85"/>
       <c r="I16" s="45" t="s">
         <v>1</v>
       </c>
@@ -30351,20 +30351,20 @@
       <c r="HR16" s="31"/>
     </row>
     <row r="17" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="88" t="s">
+      <c r="D17" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101">
+      <c r="E17" s="83"/>
+      <c r="F17" s="83">
         <v>1</v>
       </c>
-      <c r="G17" s="87" t="s">
+      <c r="G17" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="119" t="str">
+      <c r="H17" s="85" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
       </c>
@@ -30436,12 +30436,12 @@
       <c r="HR17" s="4"/>
     </row>
     <row r="18" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="134"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="119"/>
+      <c r="B18" s="81"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="85"/>
       <c r="I18" s="45" t="s">
         <v>1</v>
       </c>
@@ -30683,22 +30683,22 @@
       <c r="HR18" s="31"/>
     </row>
     <row r="19" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="88" t="s">
+      <c r="D19" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="101" t="s">
+      <c r="E19" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="101">
+      <c r="F19" s="83">
         <v>1</v>
       </c>
-      <c r="G19" s="87" t="s">
+      <c r="G19" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="119" t="str">
+      <c r="H19" s="85" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
       </c>
@@ -30782,12 +30782,12 @@
       <c r="HR19" s="4"/>
     </row>
     <row r="20" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="134"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="119"/>
+      <c r="B20" s="81"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="85"/>
       <c r="I20" s="45" t="s">
         <v>1</v>
       </c>
@@ -31031,20 +31031,20 @@
       <c r="HR20" s="31"/>
     </row>
     <row r="21" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="134" t="s">
+      <c r="B21" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="88" t="s">
+      <c r="D21" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101">
+      <c r="E21" s="83"/>
+      <c r="F21" s="83">
         <v>1</v>
       </c>
-      <c r="G21" s="87" t="s">
+      <c r="G21" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="119" t="str">
+      <c r="H21" s="85" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
       </c>
@@ -31118,12 +31118,12 @@
       <c r="HR21" s="4"/>
     </row>
     <row r="22" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="134"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="119"/>
+      <c r="B22" s="81"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="85"/>
       <c r="I22" s="45" t="s">
         <v>1</v>
       </c>
@@ -31361,20 +31361,20 @@
       <c r="HR22" s="31"/>
     </row>
     <row r="23" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="134" t="s">
+      <c r="B23" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101">
+      <c r="E23" s="83"/>
+      <c r="F23" s="83">
         <v>1</v>
       </c>
-      <c r="G23" s="87" t="s">
+      <c r="G23" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="119" t="str">
+      <c r="H23" s="85" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
       </c>
@@ -31445,12 +31445,12 @@
       <c r="HR23" s="4"/>
     </row>
     <row r="24" spans="2:226" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="134"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="119"/>
+      <c r="B24" s="81"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
       <c r="I24" s="45" t="s">
         <v>1</v>
       </c>
@@ -31692,20 +31692,20 @@
       <c r="HR24" s="31"/>
     </row>
     <row r="25" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="134" t="s">
+      <c r="B25" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="88" t="s">
+      <c r="D25" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101">
+      <c r="E25" s="83"/>
+      <c r="F25" s="83">
         <v>1</v>
       </c>
-      <c r="G25" s="87" t="s">
+      <c r="G25" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="119" t="str">
+      <c r="H25" s="85" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
       </c>
@@ -31775,12 +31775,12 @@
       <c r="HR25" s="4"/>
     </row>
     <row r="26" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="134"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="119"/>
+      <c r="B26" s="81"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="85"/>
       <c r="I26" s="45" t="s">
         <v>1</v>
       </c>
@@ -32020,20 +32020,20 @@
       <c r="HR26" s="31"/>
     </row>
     <row r="27" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="134" t="s">
+      <c r="B27" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="88" t="s">
+      <c r="D27" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101">
+      <c r="E27" s="83"/>
+      <c r="F27" s="83">
         <v>2</v>
       </c>
-      <c r="G27" s="87" t="s">
+      <c r="G27" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="119" t="str">
+      <c r="H27" s="85" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
       </c>
@@ -32114,12 +32114,12 @@
       <c r="HR27" s="4"/>
     </row>
     <row r="28" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="134"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="119"/>
+      <c r="B28" s="81"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="85"/>
       <c r="I28" s="45" t="s">
         <v>1</v>
       </c>
@@ -32359,22 +32359,22 @@
       <c r="HR28" s="31"/>
     </row>
     <row r="29" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="134" t="s">
+      <c r="B29" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="88" t="s">
+      <c r="D29" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="101" t="s">
+      <c r="E29" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="101">
+      <c r="F29" s="83">
         <v>2</v>
       </c>
-      <c r="G29" s="87" t="s">
+      <c r="G29" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="119" t="str">
+      <c r="H29" s="85" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v>!</v>
       </c>
@@ -32454,12 +32454,12 @@
       <c r="HR29" s="4"/>
     </row>
     <row r="30" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="134"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="119"/>
+      <c r="B30" s="81"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="45" t="s">
         <v>1</v>
       </c>
@@ -32715,22 +32715,22 @@
       <c r="HR30" s="31"/>
     </row>
     <row r="31" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="134" t="s">
+      <c r="B31" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="121" t="s">
+      <c r="D31" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="101" t="s">
+      <c r="E31" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="101">
+      <c r="F31" s="83">
         <v>2</v>
       </c>
-      <c r="G31" s="87" t="s">
+      <c r="G31" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="119" t="str">
+      <c r="H31" s="85" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
       </c>
@@ -32802,12 +32802,12 @@
       <c r="HR31" s="4"/>
     </row>
     <row r="32" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="134"/>
-      <c r="D32" s="121"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="119"/>
+      <c r="B32" s="81"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="85"/>
       <c r="I32" s="45" t="s">
         <v>1</v>
       </c>
@@ -33049,22 +33049,22 @@
       <c r="HR32" s="31"/>
     </row>
     <row r="33" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="134" t="s">
+      <c r="B33" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="121" t="s">
+      <c r="D33" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="101" t="s">
+      <c r="E33" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="101">
+      <c r="F33" s="83">
         <v>2</v>
       </c>
-      <c r="G33" s="87" t="s">
+      <c r="G33" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="119" t="str">
+      <c r="H33" s="85" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
       </c>
@@ -33140,12 +33140,12 @@
       <c r="HR33" s="4"/>
     </row>
     <row r="34" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="134"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="119"/>
+      <c r="B34" s="81"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="45" t="s">
         <v>1</v>
       </c>
@@ -33387,22 +33387,22 @@
       <c r="HR34" s="31"/>
     </row>
     <row r="35" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="134" t="s">
+      <c r="B35" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="121" t="s">
+      <c r="D35" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="101" t="s">
+      <c r="E35" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="101">
+      <c r="F35" s="83">
         <v>2</v>
       </c>
-      <c r="G35" s="87" t="s">
+      <c r="G35" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="119" t="str">
+      <c r="H35" s="85" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
       </c>
@@ -33481,12 +33481,12 @@
       <c r="HR35" s="4"/>
     </row>
     <row r="36" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="134"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="101"/>
-      <c r="F36" s="101"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="119"/>
+      <c r="B36" s="81"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="45" t="s">
         <v>1</v>
       </c>
@@ -33724,22 +33724,22 @@
       <c r="HR36" s="31"/>
     </row>
     <row r="37" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="134" t="s">
+      <c r="B37" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="121" t="s">
+      <c r="D37" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="101" t="s">
+      <c r="E37" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="101">
+      <c r="F37" s="83">
         <v>2</v>
       </c>
-      <c r="G37" s="87" t="s">
+      <c r="G37" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="119" t="str">
+      <c r="H37" s="85" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
       </c>
@@ -33813,12 +33813,12 @@
       <c r="HR37" s="4"/>
     </row>
     <row r="38" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="134"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="119"/>
+      <c r="B38" s="81"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="45" t="s">
         <v>1</v>
       </c>
@@ -34058,20 +34058,20 @@
       <c r="HR38" s="31"/>
     </row>
     <row r="39" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="121" t="s">
+      <c r="D39" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101">
+      <c r="E39" s="83"/>
+      <c r="F39" s="83">
         <v>3</v>
       </c>
-      <c r="G39" s="87" t="s">
+      <c r="G39" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="119" t="str">
+      <c r="H39" s="85" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
       </c>
@@ -34152,12 +34152,12 @@
       <c r="HR39" s="4"/>
     </row>
     <row r="40" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="134"/>
-      <c r="D40" s="121"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="119"/>
+      <c r="B40" s="81"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="85"/>
       <c r="I40" s="45" t="s">
         <v>1</v>
       </c>
@@ -34405,20 +34405,20 @@
       <c r="HR40" s="31"/>
     </row>
     <row r="41" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="134" t="s">
+      <c r="B41" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="121" t="s">
+      <c r="D41" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="101"/>
-      <c r="F41" s="101">
+      <c r="E41" s="83"/>
+      <c r="F41" s="83">
         <v>3</v>
       </c>
-      <c r="G41" s="87" t="s">
+      <c r="G41" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="119" t="str">
+      <c r="H41" s="85" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
       </c>
@@ -34492,12 +34492,12 @@
       <c r="HR41" s="4"/>
     </row>
     <row r="42" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="134"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="101"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="119"/>
+      <c r="B42" s="81"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="83"/>
+      <c r="F42" s="83"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="85"/>
       <c r="I42" s="45" t="s">
         <v>1</v>
       </c>
@@ -34737,20 +34737,20 @@
       <c r="HR42" s="31"/>
     </row>
     <row r="43" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="134" t="s">
+      <c r="B43" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="121" t="s">
+      <c r="D43" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="101"/>
-      <c r="F43" s="101">
+      <c r="E43" s="83"/>
+      <c r="F43" s="83">
         <v>3</v>
       </c>
-      <c r="G43" s="87" t="s">
+      <c r="G43" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="119" t="str">
+      <c r="H43" s="85" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
       </c>
@@ -34823,12 +34823,12 @@
       <c r="HR43" s="4"/>
     </row>
     <row r="44" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="134"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="101"/>
-      <c r="F44" s="101"/>
-      <c r="G44" s="87"/>
-      <c r="H44" s="119"/>
+      <c r="B44" s="81"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="85"/>
       <c r="I44" s="45" t="s">
         <v>1</v>
       </c>
@@ -35070,20 +35070,20 @@
       <c r="HR44" s="31"/>
     </row>
     <row r="45" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="134" t="s">
+      <c r="B45" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="121" t="s">
+      <c r="D45" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="101"/>
-      <c r="F45" s="101">
+      <c r="E45" s="83"/>
+      <c r="F45" s="83">
         <v>3</v>
       </c>
-      <c r="G45" s="87" t="s">
+      <c r="G45" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="119" t="str">
+      <c r="H45" s="85" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
       </c>
@@ -35156,12 +35156,12 @@
       <c r="HR45" s="4"/>
     </row>
     <row r="46" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="134"/>
-      <c r="D46" s="121"/>
-      <c r="E46" s="101"/>
-      <c r="F46" s="101"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="119"/>
+      <c r="B46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="85"/>
       <c r="I46" s="45" t="s">
         <v>1</v>
       </c>
@@ -35403,20 +35403,20 @@
       <c r="HR46" s="31"/>
     </row>
     <row r="47" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="134" t="s">
+      <c r="B47" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="121" t="s">
+      <c r="D47" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="101"/>
-      <c r="F47" s="101">
+      <c r="E47" s="83"/>
+      <c r="F47" s="83">
         <v>3</v>
       </c>
-      <c r="G47" s="87" t="s">
+      <c r="G47" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="119" t="str">
+      <c r="H47" s="85" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
       </c>
@@ -35486,12 +35486,12 @@
       <c r="HR47" s="4"/>
     </row>
     <row r="48" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="134"/>
-      <c r="D48" s="121"/>
-      <c r="E48" s="101"/>
-      <c r="F48" s="101"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="119"/>
+      <c r="B48" s="81"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="85"/>
       <c r="I48" s="45" t="s">
         <v>1</v>
       </c>
@@ -35733,20 +35733,20 @@
       <c r="HR48" s="31"/>
     </row>
     <row r="49" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="134" t="s">
+      <c r="B49" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="121" t="s">
+      <c r="D49" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="101"/>
-      <c r="F49" s="101">
+      <c r="E49" s="83"/>
+      <c r="F49" s="83">
         <v>4</v>
       </c>
-      <c r="G49" s="87" t="s">
+      <c r="G49" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="119" t="str">
+      <c r="H49" s="85" t="str">
         <f t="shared" ref="H49" si="65">IF(O50&gt;P49,"!","")</f>
         <v/>
       </c>
@@ -35834,12 +35834,12 @@
       <c r="HR49" s="4"/>
     </row>
     <row r="50" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="134"/>
-      <c r="D50" s="121"/>
-      <c r="E50" s="101"/>
-      <c r="F50" s="101"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="119"/>
+      <c r="B50" s="81"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="85"/>
       <c r="I50" s="45" t="s">
         <v>1</v>
       </c>
@@ -36083,20 +36083,20 @@
       <c r="HR50" s="31"/>
     </row>
     <row r="51" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="134" t="s">
+      <c r="B51" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="121" t="s">
+      <c r="D51" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="101"/>
-      <c r="F51" s="101">
+      <c r="E51" s="83"/>
+      <c r="F51" s="83">
         <v>4</v>
       </c>
-      <c r="G51" s="87" t="s">
+      <c r="G51" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="119" t="str">
+      <c r="H51" s="85" t="str">
         <f t="shared" ref="H51" si="71">IF(O52&gt;P51,"!","")</f>
         <v/>
       </c>
@@ -36173,12 +36173,12 @@
       <c r="HR51" s="4"/>
     </row>
     <row r="52" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="134"/>
-      <c r="D52" s="121"/>
-      <c r="E52" s="101"/>
-      <c r="F52" s="101"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="119"/>
+      <c r="B52" s="81"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="84"/>
+      <c r="H52" s="85"/>
       <c r="I52" s="45" t="s">
         <v>1</v>
       </c>
@@ -36422,20 +36422,20 @@
       <c r="HR52" s="31"/>
     </row>
     <row r="53" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="134" t="s">
+      <c r="B53" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="121" t="s">
+      <c r="D53" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101">
+      <c r="E53" s="83"/>
+      <c r="F53" s="83">
         <v>4</v>
       </c>
-      <c r="G53" s="87" t="s">
+      <c r="G53" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H53" s="119" t="str">
+      <c r="H53" s="85" t="str">
         <f t="shared" ref="H53" si="77">IF(O54&gt;P53,"!","")</f>
         <v/>
       </c>
@@ -36515,12 +36515,12 @@
       <c r="HR53" s="4"/>
     </row>
     <row r="54" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="134"/>
-      <c r="D54" s="121"/>
-      <c r="E54" s="101"/>
-      <c r="F54" s="101"/>
-      <c r="G54" s="87"/>
-      <c r="H54" s="119"/>
+      <c r="B54" s="81"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="83"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="85"/>
       <c r="I54" s="45" t="s">
         <v>1</v>
       </c>
@@ -36760,22 +36760,22 @@
       <c r="HR54" s="31"/>
     </row>
     <row r="55" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="134" t="s">
+      <c r="B55" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="121" t="s">
+      <c r="D55" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="101" t="s">
+      <c r="E55" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="101">
+      <c r="F55" s="83">
         <v>4</v>
       </c>
-      <c r="G55" s="87" t="s">
+      <c r="G55" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H55" s="119" t="str">
+      <c r="H55" s="85" t="str">
         <f t="shared" ref="H55" si="83">IF(O56&gt;P55,"!","")</f>
         <v/>
       </c>
@@ -36858,12 +36858,12 @@
       <c r="HR55" s="4"/>
     </row>
     <row r="56" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="134"/>
-      <c r="D56" s="121"/>
-      <c r="E56" s="101"/>
-      <c r="F56" s="101"/>
-      <c r="G56" s="87"/>
-      <c r="H56" s="119"/>
+      <c r="B56" s="81"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="83"/>
+      <c r="F56" s="83"/>
+      <c r="G56" s="84"/>
+      <c r="H56" s="85"/>
       <c r="I56" s="45" t="s">
         <v>1</v>
       </c>
@@ -37105,22 +37105,22 @@
       <c r="HR56" s="31"/>
     </row>
     <row r="57" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="134" t="s">
+      <c r="B57" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="121" t="s">
+      <c r="D57" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="101" t="s">
+      <c r="E57" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="101">
+      <c r="F57" s="83">
         <v>4</v>
       </c>
-      <c r="G57" s="87" t="s">
+      <c r="G57" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H57" s="119" t="str">
+      <c r="H57" s="85" t="str">
         <f t="shared" ref="H57" si="89">IF(O58&gt;P57,"!","")</f>
         <v/>
       </c>
@@ -37191,12 +37191,12 @@
       <c r="HR57" s="4"/>
     </row>
     <row r="58" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="134"/>
-      <c r="D58" s="121"/>
-      <c r="E58" s="101"/>
-      <c r="F58" s="101"/>
-      <c r="G58" s="87"/>
-      <c r="H58" s="119"/>
+      <c r="B58" s="81"/>
+      <c r="D58" s="82"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="85"/>
       <c r="I58" s="45" t="s">
         <v>1</v>
       </c>
@@ -37440,20 +37440,20 @@
       <c r="HR58" s="31"/>
     </row>
     <row r="59" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="134" t="s">
+      <c r="B59" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="121" t="s">
+      <c r="D59" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="101"/>
-      <c r="F59" s="101">
+      <c r="E59" s="83"/>
+      <c r="F59" s="83">
         <v>5</v>
       </c>
-      <c r="G59" s="87" t="s">
+      <c r="G59" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="119" t="str">
+      <c r="H59" s="85" t="str">
         <f t="shared" ref="H59" si="95">IF(O60&gt;P59,"!","")</f>
         <v/>
       </c>
@@ -37527,12 +37527,12 @@
       <c r="HR59" s="4"/>
     </row>
     <row r="60" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="134"/>
-      <c r="D60" s="121"/>
-      <c r="E60" s="101"/>
-      <c r="F60" s="101"/>
-      <c r="G60" s="87"/>
-      <c r="H60" s="119"/>
+      <c r="B60" s="81"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="83"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="84"/>
+      <c r="H60" s="85"/>
       <c r="I60" s="45" t="s">
         <v>1</v>
       </c>
@@ -37772,18 +37772,18 @@
       <c r="HR60" s="31"/>
     </row>
     <row r="61" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="134" t="s">
+      <c r="B61" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="121" t="s">
+      <c r="D61" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E61" s="101"/>
-      <c r="F61" s="101">
+      <c r="E61" s="83"/>
+      <c r="F61" s="83">
         <v>5</v>
       </c>
-      <c r="G61" s="87"/>
-      <c r="H61" s="119" t="str">
+      <c r="G61" s="84"/>
+      <c r="H61" s="85" t="str">
         <f t="shared" ref="H61" si="101">IF(O62&gt;P61,"!","")</f>
         <v/>
       </c>
@@ -37878,12 +37878,12 @@
       <c r="HR61" s="4"/>
     </row>
     <row r="62" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="134"/>
-      <c r="D62" s="121"/>
-      <c r="E62" s="101"/>
-      <c r="F62" s="101"/>
-      <c r="G62" s="87"/>
-      <c r="H62" s="119"/>
+      <c r="B62" s="81"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="83"/>
+      <c r="F62" s="83"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="85"/>
       <c r="I62" s="45" t="s">
         <v>1</v>
       </c>
@@ -38125,18 +38125,18 @@
       <c r="HR62" s="31"/>
     </row>
     <row r="63" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="134" t="s">
+      <c r="B63" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="121" t="s">
+      <c r="D63" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="101"/>
-      <c r="F63" s="101">
+      <c r="E63" s="83"/>
+      <c r="F63" s="83">
         <v>5</v>
       </c>
-      <c r="G63" s="87"/>
-      <c r="H63" s="119" t="str">
+      <c r="G63" s="84"/>
+      <c r="H63" s="85" t="str">
         <f t="shared" ref="H63" si="107">IF(O64&gt;P63,"!","")</f>
         <v/>
       </c>
@@ -38221,12 +38221,12 @@
       <c r="HR63" s="4"/>
     </row>
     <row r="64" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="134"/>
-      <c r="D64" s="121"/>
-      <c r="E64" s="101"/>
-      <c r="F64" s="101"/>
-      <c r="G64" s="87"/>
-      <c r="H64" s="119"/>
+      <c r="B64" s="81"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="83"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="85"/>
       <c r="I64" s="45" t="s">
         <v>1</v>
       </c>
@@ -38464,18 +38464,18 @@
       <c r="HR64" s="31"/>
     </row>
     <row r="65" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="134" t="s">
+      <c r="B65" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="121" t="s">
+      <c r="D65" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="101"/>
-      <c r="F65" s="101">
+      <c r="E65" s="83"/>
+      <c r="F65" s="83">
         <v>6</v>
       </c>
-      <c r="G65" s="87"/>
-      <c r="H65" s="119" t="str">
+      <c r="G65" s="84"/>
+      <c r="H65" s="85" t="str">
         <f t="shared" ref="H65" si="113">IF(O66&gt;P65,"!","")</f>
         <v/>
       </c>
@@ -38553,12 +38553,12 @@
       <c r="HR65" s="4"/>
     </row>
     <row r="66" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="134"/>
-      <c r="D66" s="121"/>
-      <c r="E66" s="101"/>
-      <c r="F66" s="101"/>
-      <c r="G66" s="87"/>
-      <c r="H66" s="119"/>
+      <c r="B66" s="81"/>
+      <c r="D66" s="82"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="85"/>
       <c r="I66" s="45" t="s">
         <v>1</v>
       </c>
@@ -38796,20 +38796,20 @@
       <c r="HR66" s="31"/>
     </row>
     <row r="67" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="134" t="s">
+      <c r="B67" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="121" t="s">
+      <c r="D67" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="101" t="s">
+      <c r="E67" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="F67" s="101">
+      <c r="F67" s="83">
         <v>6</v>
       </c>
-      <c r="G67" s="87"/>
-      <c r="H67" s="119" t="str">
+      <c r="G67" s="84"/>
+      <c r="H67" s="85" t="str">
         <f t="shared" ref="H67" si="119">IF(O68&gt;P67,"!","")</f>
         <v/>
       </c>
@@ -38904,12 +38904,12 @@
       <c r="HR67" s="4"/>
     </row>
     <row r="68" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="134"/>
-      <c r="D68" s="121"/>
-      <c r="E68" s="101"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="87"/>
-      <c r="H68" s="119"/>
+      <c r="B68" s="81"/>
+      <c r="D68" s="82"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="85"/>
       <c r="I68" s="45" t="s">
         <v>1</v>
       </c>
@@ -39147,20 +39147,20 @@
       <c r="HR68" s="31"/>
     </row>
     <row r="69" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="134" t="s">
+      <c r="B69" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="121" t="s">
+      <c r="D69" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="101" t="s">
+      <c r="E69" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="F69" s="101">
+      <c r="F69" s="83">
         <v>6</v>
       </c>
-      <c r="G69" s="87"/>
-      <c r="H69" s="119" t="str">
+      <c r="G69" s="84"/>
+      <c r="H69" s="85" t="str">
         <f t="shared" ref="H69" si="127">IF(O70&gt;P69,"!","")</f>
         <v/>
       </c>
@@ -39237,12 +39237,12 @@
       <c r="HR69" s="4"/>
     </row>
     <row r="70" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="134"/>
-      <c r="D70" s="121"/>
-      <c r="E70" s="101"/>
-      <c r="F70" s="101"/>
-      <c r="G70" s="87"/>
-      <c r="H70" s="119"/>
+      <c r="B70" s="81"/>
+      <c r="D70" s="82"/>
+      <c r="E70" s="83"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="85"/>
       <c r="I70" s="45" t="s">
         <v>1</v>
       </c>
@@ -39480,20 +39480,20 @@
       <c r="HR70" s="31"/>
     </row>
     <row r="71" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="134" t="s">
+      <c r="B71" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="121" t="s">
+      <c r="D71" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="E71" s="101" t="s">
+      <c r="E71" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="F71" s="101">
+      <c r="F71" s="83">
         <v>6</v>
       </c>
-      <c r="G71" s="87"/>
-      <c r="H71" s="119" t="str">
+      <c r="G71" s="84"/>
+      <c r="H71" s="85" t="str">
         <f t="shared" ref="H71" si="133">IF(O72&gt;P71,"!","")</f>
         <v/>
       </c>
@@ -39569,12 +39569,12 @@
       <c r="HR71" s="4"/>
     </row>
     <row r="72" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="134"/>
-      <c r="D72" s="121"/>
-      <c r="E72" s="101"/>
-      <c r="F72" s="101"/>
-      <c r="G72" s="87"/>
-      <c r="H72" s="119"/>
+      <c r="B72" s="81"/>
+      <c r="D72" s="82"/>
+      <c r="E72" s="83"/>
+      <c r="F72" s="83"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="85"/>
       <c r="I72" s="45" t="s">
         <v>1</v>
       </c>
@@ -39901,13 +39901,13 @@
     </row>
     <row r="73" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="121" t="s">
+      <c r="D73" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="101"/>
-      <c r="F73" s="101"/>
-      <c r="G73" s="87"/>
-      <c r="H73" s="119" t="str">
+      <c r="E73" s="83"/>
+      <c r="F73" s="83"/>
+      <c r="G73" s="84"/>
+      <c r="H73" s="85" t="str">
         <f t="shared" ref="H73" si="139">IF(O74&gt;P73,"!","")</f>
         <v/>
       </c>
@@ -39975,11 +39975,11 @@
     </row>
     <row r="74" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="D74" s="121"/>
-      <c r="E74" s="101"/>
-      <c r="F74" s="101"/>
-      <c r="G74" s="87"/>
-      <c r="H74" s="119"/>
+      <c r="D74" s="82"/>
+      <c r="E74" s="83"/>
+      <c r="F74" s="83"/>
+      <c r="G74" s="84"/>
+      <c r="H74" s="85"/>
       <c r="I74" s="45" t="s">
         <v>1</v>
       </c>
@@ -40218,13 +40218,13 @@
     </row>
     <row r="75" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="121" t="s">
+      <c r="D75" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="101"/>
-      <c r="F75" s="101"/>
-      <c r="G75" s="87"/>
-      <c r="H75" s="119" t="str">
+      <c r="E75" s="83"/>
+      <c r="F75" s="83"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="85" t="str">
         <f t="shared" ref="H75" si="145">IF(O76&gt;P75,"!","")</f>
         <v/>
       </c>
@@ -40296,11 +40296,11 @@
     </row>
     <row r="76" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
-      <c r="D76" s="121"/>
-      <c r="E76" s="101"/>
-      <c r="F76" s="101"/>
-      <c r="G76" s="87"/>
-      <c r="H76" s="119"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="83"/>
+      <c r="F76" s="83"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="85"/>
       <c r="I76" s="45" t="s">
         <v>1</v>
       </c>
@@ -40539,13 +40539,13 @@
     </row>
     <row r="77" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
-      <c r="D77" s="121" t="s">
+      <c r="D77" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="E77" s="101"/>
-      <c r="F77" s="101"/>
-      <c r="G77" s="87"/>
-      <c r="H77" s="119" t="str">
+      <c r="E77" s="83"/>
+      <c r="F77" s="83"/>
+      <c r="G77" s="84"/>
+      <c r="H77" s="85" t="str">
         <f t="shared" ref="H77" si="151">IF(O78&gt;P77,"!","")</f>
         <v/>
       </c>
@@ -40634,11 +40634,11 @@
     </row>
     <row r="78" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="121"/>
-      <c r="E78" s="101"/>
-      <c r="F78" s="101"/>
-      <c r="G78" s="87"/>
-      <c r="H78" s="119"/>
+      <c r="D78" s="82"/>
+      <c r="E78" s="83"/>
+      <c r="F78" s="83"/>
+      <c r="G78" s="84"/>
+      <c r="H78" s="85"/>
       <c r="I78" s="45" t="s">
         <v>1</v>
       </c>
@@ -40877,11 +40877,11 @@
     </row>
     <row r="79" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="D79" s="121"/>
-      <c r="E79" s="101"/>
-      <c r="F79" s="101"/>
-      <c r="G79" s="87"/>
-      <c r="H79" s="119" t="str">
+      <c r="D79" s="82"/>
+      <c r="E79" s="83"/>
+      <c r="F79" s="83"/>
+      <c r="G79" s="84"/>
+      <c r="H79" s="85" t="str">
         <f t="shared" ref="H79" si="157">IF(O80&gt;P79,"!","")</f>
         <v/>
       </c>
@@ -40950,11 +40950,11 @@
     </row>
     <row r="80" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
-      <c r="D80" s="121"/>
-      <c r="E80" s="101"/>
-      <c r="F80" s="101"/>
-      <c r="G80" s="87"/>
-      <c r="H80" s="119"/>
+      <c r="D80" s="82"/>
+      <c r="E80" s="83"/>
+      <c r="F80" s="83"/>
+      <c r="G80" s="84"/>
+      <c r="H80" s="85"/>
       <c r="I80" s="45" t="s">
         <v>1</v>
       </c>
@@ -41193,11 +41193,11 @@
     </row>
     <row r="81" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="D81" s="121"/>
-      <c r="E81" s="101"/>
-      <c r="F81" s="101"/>
-      <c r="G81" s="87"/>
-      <c r="H81" s="119" t="str">
+      <c r="D81" s="82"/>
+      <c r="E81" s="83"/>
+      <c r="F81" s="83"/>
+      <c r="G81" s="84"/>
+      <c r="H81" s="85" t="str">
         <f t="shared" ref="H81" si="163">IF(O82&gt;P81,"!","")</f>
         <v/>
       </c>
@@ -41266,11 +41266,11 @@
     </row>
     <row r="82" spans="2:226" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="70"/>
-      <c r="D82" s="130"/>
-      <c r="E82" s="131"/>
-      <c r="F82" s="131"/>
-      <c r="G82" s="132"/>
-      <c r="H82" s="133"/>
+      <c r="D82" s="86"/>
+      <c r="E82" s="87"/>
+      <c r="F82" s="87"/>
+      <c r="G82" s="88"/>
+      <c r="H82" s="89"/>
       <c r="I82" s="47" t="s">
         <v>1</v>
       </c>
@@ -41509,136 +41509,139 @@
     </row>
   </sheetData>
   <mergeCells count="287">
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="Q7:Z7"/>
+    <mergeCell ref="P7:P11"/>
+    <mergeCell ref="O7:O11"/>
+    <mergeCell ref="N7:N11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="Q8:Z8"/>
+    <mergeCell ref="Q9:Z9"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="AA7:AJ7"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AU7:BD7"/>
+    <mergeCell ref="BE7:BN7"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="DC7:DL7"/>
+    <mergeCell ref="DM7:DV7"/>
+    <mergeCell ref="AJ4:AR4"/>
+    <mergeCell ref="AJ5:AR5"/>
+    <mergeCell ref="AU5:BE5"/>
+    <mergeCell ref="AU4:BE4"/>
+    <mergeCell ref="BY9:CH9"/>
+    <mergeCell ref="CI9:CR9"/>
+    <mergeCell ref="CS9:DB9"/>
+    <mergeCell ref="DC9:DL9"/>
+    <mergeCell ref="DM9:DV9"/>
+    <mergeCell ref="DW9:EF9"/>
+    <mergeCell ref="DM8:DV8"/>
+    <mergeCell ref="DW8:EF8"/>
+    <mergeCell ref="EG8:EP8"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="AK9:AT9"/>
+    <mergeCell ref="AU9:BD9"/>
+    <mergeCell ref="BE9:BN9"/>
+    <mergeCell ref="BO9:BX9"/>
+    <mergeCell ref="EG9:EP9"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="FK7:FT7"/>
+    <mergeCell ref="FU7:GD7"/>
+    <mergeCell ref="GE7:GN7"/>
+    <mergeCell ref="GO7:GX7"/>
+    <mergeCell ref="GY7:HH7"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="BO7:BX7"/>
+    <mergeCell ref="EG7:EP7"/>
+    <mergeCell ref="AA8:AJ8"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AU8:BD8"/>
+    <mergeCell ref="BE8:BN8"/>
+    <mergeCell ref="BO8:BX8"/>
+    <mergeCell ref="BY8:CH8"/>
+    <mergeCell ref="CI8:CR8"/>
+    <mergeCell ref="CS8:DB8"/>
+    <mergeCell ref="DC8:DL8"/>
+    <mergeCell ref="BY7:CH7"/>
+    <mergeCell ref="CI7:CR7"/>
+    <mergeCell ref="CS7:DB7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="DW7:EF7"/>
+    <mergeCell ref="AA9:AJ9"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="F41:F42"/>
@@ -41663,139 +41666,136 @@
     <mergeCell ref="EQ8:EZ8"/>
     <mergeCell ref="EQ9:EZ9"/>
     <mergeCell ref="FA7:FJ7"/>
-    <mergeCell ref="FK7:FT7"/>
-    <mergeCell ref="FU7:GD7"/>
-    <mergeCell ref="GE7:GN7"/>
-    <mergeCell ref="GO7:GX7"/>
-    <mergeCell ref="GY7:HH7"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="BO7:BX7"/>
-    <mergeCell ref="EG7:EP7"/>
-    <mergeCell ref="AA8:AJ8"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AU8:BD8"/>
-    <mergeCell ref="BE8:BN8"/>
-    <mergeCell ref="BO8:BX8"/>
-    <mergeCell ref="BY8:CH8"/>
-    <mergeCell ref="CI8:CR8"/>
-    <mergeCell ref="CS8:DB8"/>
-    <mergeCell ref="DC8:DL8"/>
-    <mergeCell ref="BY7:CH7"/>
-    <mergeCell ref="CI7:CR7"/>
-    <mergeCell ref="CS7:DB7"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="DW7:EF7"/>
-    <mergeCell ref="AA9:AJ9"/>
-    <mergeCell ref="AK9:AT9"/>
-    <mergeCell ref="AU9:BD9"/>
-    <mergeCell ref="BE9:BN9"/>
-    <mergeCell ref="BO9:BX9"/>
-    <mergeCell ref="EG9:EP9"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="BY9:CH9"/>
-    <mergeCell ref="CI9:CR9"/>
-    <mergeCell ref="CS9:DB9"/>
-    <mergeCell ref="DC9:DL9"/>
-    <mergeCell ref="DM9:DV9"/>
-    <mergeCell ref="DW9:EF9"/>
-    <mergeCell ref="DM8:DV8"/>
-    <mergeCell ref="DW8:EF8"/>
-    <mergeCell ref="EG8:EP8"/>
-    <mergeCell ref="AA7:AJ7"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AU7:BD7"/>
-    <mergeCell ref="BE7:BN7"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="DC7:DL7"/>
-    <mergeCell ref="DM7:DV7"/>
-    <mergeCell ref="AJ4:AR4"/>
-    <mergeCell ref="AJ5:AR5"/>
-    <mergeCell ref="AU5:BE5"/>
-    <mergeCell ref="AU4:BE4"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="Q7:Z7"/>
-    <mergeCell ref="P7:P11"/>
-    <mergeCell ref="O7:O11"/>
-    <mergeCell ref="N7:N11"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="Q8:Z8"/>
-    <mergeCell ref="Q9:Z9"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7:HR8">
     <cfRule type="expression" dxfId="2730" priority="3963">
@@ -50952,104 +50952,104 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF77">
-    <cfRule type="expression" dxfId="29" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>AND(CF77="p",$G77="x")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="24">
+    <cfRule type="expression" dxfId="36" priority="24">
       <formula>AND(CF77="r",CF76&lt;&gt;"p")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
       <formula>"r"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
       <formula>"a"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF77">
-    <cfRule type="expression" dxfId="24" priority="16">
+    <cfRule type="expression" dxfId="33" priority="16">
       <formula>$D76="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="32" priority="17">
       <formula>AND(ISBLANK($D78),$I77="Réalisé",$D76&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="31" priority="18">
       <formula>AND($N77="f",$F78="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="30" priority="19">
       <formula>$D77&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="29" priority="20">
       <formula>AND($N76="f",$N77="d")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="28" priority="21">
       <formula>AND($N77="d",$N76="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF77">
-    <cfRule type="expression" dxfId="18" priority="27">
+    <cfRule type="expression" dxfId="27" priority="27">
       <formula>AND(ISBLANK($D78),$I77="Réalisé",$D76&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="28">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>AND($N77="d",$N76="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="29">
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>AND($N76="f",$N77="d")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="30">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>$D77&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE77">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>AND(CE77="p",$G77="x")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>AND(CE77="r",CE76&lt;&gt;"p")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"r"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"a"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE77">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$D76="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(ISBLANK($D78),$I77="Réalisé",$D76&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND($N77="f",$F78="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>$D77&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>AND($N76="f",$N77="d")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>AND($N77="d",$N76="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE77">
-    <cfRule type="expression" dxfId="3" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>AND(ISBLANK($D78),$I77="Réalisé",$D76&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>AND($N77="d",$N76="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>AND($N76="f",$N77="d")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>$D77&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51983,7 +51983,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A1:E47">
-    <cfRule type="expression" dxfId="37" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>WEEKDAY($B1,2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52015,9 +52015,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52244,27 +52247,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
-    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -52290,9 +52281,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
+    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Début du chois du focus autorisé
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD1407-82AE-4E06-A806-50EEE5F4908E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E94D9C0-67EE-4552-9E48-9205DE967600}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="101">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -939,43 +939,70 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -984,10 +1011,7 @@
     <xf numFmtId="14" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -996,41 +1020,8 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1053,53 +1044,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -27023,7 +27023,7 @@
   <dimension ref="A1:HR82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:D42"/>
+      <selection activeCell="CN63" sqref="CN63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27069,11 +27069,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="Q3" s="112">
+      <c r="Q3" s="109">
         <f>MAX(K13:K163)</f>
         <v>64</v>
       </c>
-      <c r="R3" s="113"/>
+      <c r="R3" s="110"/>
       <c r="S3" s="28" t="s">
         <v>23</v>
       </c>
@@ -27098,11 +27098,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="Q4" s="114">
+      <c r="Q4" s="111">
         <f>MAX(L13:L163)-L12</f>
         <v>36</v>
       </c>
-      <c r="R4" s="115"/>
+      <c r="R4" s="112"/>
       <c r="S4" s="29" t="s">
         <v>24</v>
       </c>
@@ -27119,31 +27119,31 @@
       <c r="AD4" s="26"/>
       <c r="AE4" s="27"/>
       <c r="AI4" s="66"/>
-      <c r="AJ4" s="118" t="s">
+      <c r="AJ4" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="AK4" s="118"/>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="118"/>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118"/>
+      <c r="AK4" s="115"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="118" t="s">
+      <c r="AU4" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118"/>
-      <c r="AZ4" s="118"/>
-      <c r="BA4" s="118"/>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="115"/>
+      <c r="BC4" s="115"/>
+      <c r="BD4" s="115"/>
+      <c r="BE4" s="115"/>
       <c r="BG4" s="8"/>
       <c r="BH4" s="3" t="s">
         <v>2</v>
@@ -27155,11 +27155,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="Q5" s="116">
+      <c r="Q5" s="113">
         <f>MAX(M13:M163)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="117"/>
+      <c r="R5" s="114"/>
       <c r="S5" s="30" t="s">
         <v>25</v>
       </c>
@@ -27176,31 +27176,31 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="12"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="118" t="s">
+      <c r="AJ5" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="118"/>
-      <c r="AM5" s="118"/>
-      <c r="AN5" s="118"/>
-      <c r="AO5" s="118"/>
-      <c r="AP5" s="118"/>
-      <c r="AQ5" s="118"/>
-      <c r="AR5" s="118"/>
+      <c r="AK5" s="115"/>
+      <c r="AL5" s="115"/>
+      <c r="AM5" s="115"/>
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="115"/>
       <c r="AT5" s="65"/>
-      <c r="AU5" s="118" t="s">
+      <c r="AU5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="118"/>
-      <c r="AZ5" s="118"/>
-      <c r="BA5" s="118"/>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="115"/>
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="115"/>
+      <c r="BA5" s="115"/>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="115"/>
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="115"/>
     </row>
     <row r="6" spans="1:226" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -27211,889 +27211,889 @@
     </row>
     <row r="7" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B7" s="69"/>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="108" t="s">
+      <c r="F7" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="108" t="s">
+      <c r="G7" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="108" t="s">
+      <c r="H7" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="105" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="132" t="s">
+      <c r="K7" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="127" t="s">
+      <c r="L7" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="127" t="s">
+      <c r="M7" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="127" t="s">
+      <c r="N7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="127" t="s">
+      <c r="O7" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="124" t="s">
+      <c r="P7" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="123">
+      <c r="Q7" s="95">
         <v>1</v>
       </c>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="91"/>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="101"/>
-      <c r="AA7" s="90">
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="96"/>
+      <c r="V7" s="96"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="97"/>
+      <c r="AA7" s="108">
         <v>2</v>
       </c>
-      <c r="AB7" s="91"/>
-      <c r="AC7" s="91"/>
-      <c r="AD7" s="91"/>
-      <c r="AE7" s="91"/>
-      <c r="AF7" s="91"/>
-      <c r="AG7" s="91"/>
-      <c r="AH7" s="91"/>
-      <c r="AI7" s="91"/>
-      <c r="AJ7" s="101"/>
-      <c r="AK7" s="90">
+      <c r="AB7" s="96"/>
+      <c r="AC7" s="96"/>
+      <c r="AD7" s="96"/>
+      <c r="AE7" s="96"/>
+      <c r="AF7" s="96"/>
+      <c r="AG7" s="96"/>
+      <c r="AH7" s="96"/>
+      <c r="AI7" s="96"/>
+      <c r="AJ7" s="97"/>
+      <c r="AK7" s="108">
         <v>3</v>
       </c>
-      <c r="AL7" s="91"/>
-      <c r="AM7" s="91"/>
-      <c r="AN7" s="91"/>
-      <c r="AO7" s="91"/>
-      <c r="AP7" s="91"/>
-      <c r="AQ7" s="91"/>
-      <c r="AR7" s="91"/>
-      <c r="AS7" s="91"/>
-      <c r="AT7" s="101"/>
-      <c r="AU7" s="90">
+      <c r="AL7" s="96"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="96"/>
+      <c r="AO7" s="96"/>
+      <c r="AP7" s="96"/>
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="96"/>
+      <c r="AS7" s="96"/>
+      <c r="AT7" s="97"/>
+      <c r="AU7" s="108">
         <v>4</v>
       </c>
-      <c r="AV7" s="91"/>
-      <c r="AW7" s="91"/>
-      <c r="AX7" s="91"/>
-      <c r="AY7" s="91"/>
-      <c r="AZ7" s="91"/>
-      <c r="BA7" s="91"/>
-      <c r="BB7" s="91"/>
-      <c r="BC7" s="91"/>
-      <c r="BD7" s="101"/>
-      <c r="BE7" s="90">
+      <c r="AV7" s="96"/>
+      <c r="AW7" s="96"/>
+      <c r="AX7" s="96"/>
+      <c r="AY7" s="96"/>
+      <c r="AZ7" s="96"/>
+      <c r="BA7" s="96"/>
+      <c r="BB7" s="96"/>
+      <c r="BC7" s="96"/>
+      <c r="BD7" s="97"/>
+      <c r="BE7" s="108">
         <v>5</v>
       </c>
-      <c r="BF7" s="91"/>
-      <c r="BG7" s="91"/>
-      <c r="BH7" s="91"/>
-      <c r="BI7" s="91"/>
-      <c r="BJ7" s="91"/>
-      <c r="BK7" s="91"/>
-      <c r="BL7" s="91"/>
-      <c r="BM7" s="91"/>
-      <c r="BN7" s="101"/>
-      <c r="BO7" s="90">
+      <c r="BF7" s="96"/>
+      <c r="BG7" s="96"/>
+      <c r="BH7" s="96"/>
+      <c r="BI7" s="96"/>
+      <c r="BJ7" s="96"/>
+      <c r="BK7" s="96"/>
+      <c r="BL7" s="96"/>
+      <c r="BM7" s="96"/>
+      <c r="BN7" s="97"/>
+      <c r="BO7" s="108">
         <v>6</v>
       </c>
-      <c r="BP7" s="91"/>
-      <c r="BQ7" s="91"/>
-      <c r="BR7" s="91"/>
-      <c r="BS7" s="91"/>
-      <c r="BT7" s="91"/>
-      <c r="BU7" s="91"/>
-      <c r="BV7" s="91"/>
-      <c r="BW7" s="91"/>
-      <c r="BX7" s="101"/>
-      <c r="BY7" s="90">
+      <c r="BP7" s="96"/>
+      <c r="BQ7" s="96"/>
+      <c r="BR7" s="96"/>
+      <c r="BS7" s="96"/>
+      <c r="BT7" s="96"/>
+      <c r="BU7" s="96"/>
+      <c r="BV7" s="96"/>
+      <c r="BW7" s="96"/>
+      <c r="BX7" s="97"/>
+      <c r="BY7" s="108">
         <v>7</v>
       </c>
-      <c r="BZ7" s="91"/>
-      <c r="CA7" s="91"/>
-      <c r="CB7" s="91"/>
-      <c r="CC7" s="91"/>
-      <c r="CD7" s="91"/>
-      <c r="CE7" s="91"/>
-      <c r="CF7" s="91"/>
-      <c r="CG7" s="91"/>
-      <c r="CH7" s="101"/>
-      <c r="CI7" s="90">
+      <c r="BZ7" s="96"/>
+      <c r="CA7" s="96"/>
+      <c r="CB7" s="96"/>
+      <c r="CC7" s="96"/>
+      <c r="CD7" s="96"/>
+      <c r="CE7" s="96"/>
+      <c r="CF7" s="96"/>
+      <c r="CG7" s="96"/>
+      <c r="CH7" s="97"/>
+      <c r="CI7" s="108">
         <v>8</v>
       </c>
-      <c r="CJ7" s="91"/>
-      <c r="CK7" s="91"/>
-      <c r="CL7" s="91"/>
-      <c r="CM7" s="91"/>
-      <c r="CN7" s="91"/>
-      <c r="CO7" s="91"/>
-      <c r="CP7" s="91"/>
-      <c r="CQ7" s="91"/>
-      <c r="CR7" s="101"/>
-      <c r="CS7" s="90">
+      <c r="CJ7" s="96"/>
+      <c r="CK7" s="96"/>
+      <c r="CL7" s="96"/>
+      <c r="CM7" s="96"/>
+      <c r="CN7" s="96"/>
+      <c r="CO7" s="96"/>
+      <c r="CP7" s="96"/>
+      <c r="CQ7" s="96"/>
+      <c r="CR7" s="97"/>
+      <c r="CS7" s="108">
         <v>9</v>
       </c>
-      <c r="CT7" s="91"/>
-      <c r="CU7" s="91"/>
-      <c r="CV7" s="91"/>
-      <c r="CW7" s="91"/>
-      <c r="CX7" s="91"/>
-      <c r="CY7" s="91"/>
-      <c r="CZ7" s="91"/>
-      <c r="DA7" s="91"/>
-      <c r="DB7" s="91"/>
-      <c r="DC7" s="90">
+      <c r="CT7" s="96"/>
+      <c r="CU7" s="96"/>
+      <c r="CV7" s="96"/>
+      <c r="CW7" s="96"/>
+      <c r="CX7" s="96"/>
+      <c r="CY7" s="96"/>
+      <c r="CZ7" s="96"/>
+      <c r="DA7" s="96"/>
+      <c r="DB7" s="96"/>
+      <c r="DC7" s="108">
         <v>10</v>
       </c>
-      <c r="DD7" s="91"/>
-      <c r="DE7" s="91"/>
-      <c r="DF7" s="91"/>
-      <c r="DG7" s="91"/>
-      <c r="DH7" s="91"/>
-      <c r="DI7" s="91"/>
-      <c r="DJ7" s="91"/>
-      <c r="DK7" s="91"/>
-      <c r="DL7" s="101"/>
-      <c r="DM7" s="90">
+      <c r="DD7" s="96"/>
+      <c r="DE7" s="96"/>
+      <c r="DF7" s="96"/>
+      <c r="DG7" s="96"/>
+      <c r="DH7" s="96"/>
+      <c r="DI7" s="96"/>
+      <c r="DJ7" s="96"/>
+      <c r="DK7" s="96"/>
+      <c r="DL7" s="97"/>
+      <c r="DM7" s="108">
         <v>11</v>
       </c>
-      <c r="DN7" s="91"/>
-      <c r="DO7" s="91"/>
-      <c r="DP7" s="91"/>
-      <c r="DQ7" s="91"/>
-      <c r="DR7" s="91"/>
-      <c r="DS7" s="91"/>
-      <c r="DT7" s="91"/>
-      <c r="DU7" s="91"/>
-      <c r="DV7" s="101"/>
-      <c r="DW7" s="90">
+      <c r="DN7" s="96"/>
+      <c r="DO7" s="96"/>
+      <c r="DP7" s="96"/>
+      <c r="DQ7" s="96"/>
+      <c r="DR7" s="96"/>
+      <c r="DS7" s="96"/>
+      <c r="DT7" s="96"/>
+      <c r="DU7" s="96"/>
+      <c r="DV7" s="97"/>
+      <c r="DW7" s="108">
         <v>12</v>
       </c>
-      <c r="DX7" s="91"/>
-      <c r="DY7" s="91"/>
-      <c r="DZ7" s="91"/>
-      <c r="EA7" s="91"/>
-      <c r="EB7" s="91"/>
-      <c r="EC7" s="91"/>
-      <c r="ED7" s="91"/>
-      <c r="EE7" s="91"/>
-      <c r="EF7" s="101"/>
-      <c r="EG7" s="90">
+      <c r="DX7" s="96"/>
+      <c r="DY7" s="96"/>
+      <c r="DZ7" s="96"/>
+      <c r="EA7" s="96"/>
+      <c r="EB7" s="96"/>
+      <c r="EC7" s="96"/>
+      <c r="ED7" s="96"/>
+      <c r="EE7" s="96"/>
+      <c r="EF7" s="97"/>
+      <c r="EG7" s="108">
         <v>13</v>
       </c>
-      <c r="EH7" s="91"/>
-      <c r="EI7" s="91"/>
-      <c r="EJ7" s="91"/>
-      <c r="EK7" s="91"/>
-      <c r="EL7" s="91"/>
-      <c r="EM7" s="91"/>
-      <c r="EN7" s="91"/>
-      <c r="EO7" s="91"/>
-      <c r="EP7" s="92"/>
-      <c r="EQ7" s="91">
+      <c r="EH7" s="96"/>
+      <c r="EI7" s="96"/>
+      <c r="EJ7" s="96"/>
+      <c r="EK7" s="96"/>
+      <c r="EL7" s="96"/>
+      <c r="EM7" s="96"/>
+      <c r="EN7" s="96"/>
+      <c r="EO7" s="96"/>
+      <c r="EP7" s="126"/>
+      <c r="EQ7" s="96">
         <v>14</v>
       </c>
-      <c r="ER7" s="91"/>
-      <c r="ES7" s="91"/>
-      <c r="ET7" s="91"/>
-      <c r="EU7" s="91"/>
-      <c r="EV7" s="91"/>
-      <c r="EW7" s="91"/>
-      <c r="EX7" s="91"/>
-      <c r="EY7" s="91"/>
-      <c r="EZ7" s="101"/>
-      <c r="FA7" s="90">
+      <c r="ER7" s="96"/>
+      <c r="ES7" s="96"/>
+      <c r="ET7" s="96"/>
+      <c r="EU7" s="96"/>
+      <c r="EV7" s="96"/>
+      <c r="EW7" s="96"/>
+      <c r="EX7" s="96"/>
+      <c r="EY7" s="96"/>
+      <c r="EZ7" s="97"/>
+      <c r="FA7" s="108">
         <v>15</v>
       </c>
-      <c r="FB7" s="91"/>
-      <c r="FC7" s="91"/>
-      <c r="FD7" s="91"/>
-      <c r="FE7" s="91"/>
-      <c r="FF7" s="91"/>
-      <c r="FG7" s="91"/>
-      <c r="FH7" s="91"/>
-      <c r="FI7" s="91"/>
-      <c r="FJ7" s="101"/>
-      <c r="FK7" s="90">
+      <c r="FB7" s="96"/>
+      <c r="FC7" s="96"/>
+      <c r="FD7" s="96"/>
+      <c r="FE7" s="96"/>
+      <c r="FF7" s="96"/>
+      <c r="FG7" s="96"/>
+      <c r="FH7" s="96"/>
+      <c r="FI7" s="96"/>
+      <c r="FJ7" s="97"/>
+      <c r="FK7" s="108">
         <v>16</v>
       </c>
-      <c r="FL7" s="91"/>
-      <c r="FM7" s="91"/>
-      <c r="FN7" s="91"/>
-      <c r="FO7" s="91"/>
-      <c r="FP7" s="91"/>
-      <c r="FQ7" s="91"/>
-      <c r="FR7" s="91"/>
-      <c r="FS7" s="91"/>
-      <c r="FT7" s="101"/>
-      <c r="FU7" s="90">
+      <c r="FL7" s="96"/>
+      <c r="FM7" s="96"/>
+      <c r="FN7" s="96"/>
+      <c r="FO7" s="96"/>
+      <c r="FP7" s="96"/>
+      <c r="FQ7" s="96"/>
+      <c r="FR7" s="96"/>
+      <c r="FS7" s="96"/>
+      <c r="FT7" s="97"/>
+      <c r="FU7" s="108">
         <v>17</v>
       </c>
-      <c r="FV7" s="91"/>
-      <c r="FW7" s="91"/>
-      <c r="FX7" s="91"/>
-      <c r="FY7" s="91"/>
-      <c r="FZ7" s="91"/>
-      <c r="GA7" s="91"/>
-      <c r="GB7" s="91"/>
-      <c r="GC7" s="91"/>
-      <c r="GD7" s="101"/>
-      <c r="GE7" s="90">
+      <c r="FV7" s="96"/>
+      <c r="FW7" s="96"/>
+      <c r="FX7" s="96"/>
+      <c r="FY7" s="96"/>
+      <c r="FZ7" s="96"/>
+      <c r="GA7" s="96"/>
+      <c r="GB7" s="96"/>
+      <c r="GC7" s="96"/>
+      <c r="GD7" s="97"/>
+      <c r="GE7" s="108">
         <v>18</v>
       </c>
-      <c r="GF7" s="91"/>
-      <c r="GG7" s="91"/>
-      <c r="GH7" s="91"/>
-      <c r="GI7" s="91"/>
-      <c r="GJ7" s="91"/>
-      <c r="GK7" s="91"/>
-      <c r="GL7" s="91"/>
-      <c r="GM7" s="91"/>
-      <c r="GN7" s="101"/>
-      <c r="GO7" s="90">
+      <c r="GF7" s="96"/>
+      <c r="GG7" s="96"/>
+      <c r="GH7" s="96"/>
+      <c r="GI7" s="96"/>
+      <c r="GJ7" s="96"/>
+      <c r="GK7" s="96"/>
+      <c r="GL7" s="96"/>
+      <c r="GM7" s="96"/>
+      <c r="GN7" s="97"/>
+      <c r="GO7" s="108">
         <v>19</v>
       </c>
-      <c r="GP7" s="91"/>
-      <c r="GQ7" s="91"/>
-      <c r="GR7" s="91"/>
-      <c r="GS7" s="91"/>
-      <c r="GT7" s="91"/>
-      <c r="GU7" s="91"/>
-      <c r="GV7" s="91"/>
-      <c r="GW7" s="91"/>
-      <c r="GX7" s="101"/>
-      <c r="GY7" s="90">
+      <c r="GP7" s="96"/>
+      <c r="GQ7" s="96"/>
+      <c r="GR7" s="96"/>
+      <c r="GS7" s="96"/>
+      <c r="GT7" s="96"/>
+      <c r="GU7" s="96"/>
+      <c r="GV7" s="96"/>
+      <c r="GW7" s="96"/>
+      <c r="GX7" s="97"/>
+      <c r="GY7" s="108">
         <v>20</v>
       </c>
-      <c r="GZ7" s="91"/>
-      <c r="HA7" s="91"/>
-      <c r="HB7" s="91"/>
-      <c r="HC7" s="91"/>
-      <c r="HD7" s="91"/>
-      <c r="HE7" s="91"/>
-      <c r="HF7" s="91"/>
-      <c r="HG7" s="91"/>
-      <c r="HH7" s="101"/>
-      <c r="HI7" s="90">
+      <c r="GZ7" s="96"/>
+      <c r="HA7" s="96"/>
+      <c r="HB7" s="96"/>
+      <c r="HC7" s="96"/>
+      <c r="HD7" s="96"/>
+      <c r="HE7" s="96"/>
+      <c r="HF7" s="96"/>
+      <c r="HG7" s="96"/>
+      <c r="HH7" s="97"/>
+      <c r="HI7" s="108">
         <v>21</v>
       </c>
-      <c r="HJ7" s="91"/>
-      <c r="HK7" s="91"/>
-      <c r="HL7" s="91"/>
-      <c r="HM7" s="91"/>
-      <c r="HN7" s="91"/>
-      <c r="HO7" s="91"/>
-      <c r="HP7" s="91"/>
-      <c r="HQ7" s="91"/>
-      <c r="HR7" s="92"/>
+      <c r="HJ7" s="96"/>
+      <c r="HK7" s="96"/>
+      <c r="HL7" s="96"/>
+      <c r="HM7" s="96"/>
+      <c r="HN7" s="96"/>
+      <c r="HO7" s="96"/>
+      <c r="HP7" s="96"/>
+      <c r="HQ7" s="96"/>
+      <c r="HR7" s="126"/>
     </row>
     <row r="8" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="128"/>
-      <c r="M8" s="128"/>
-      <c r="N8" s="128"/>
-      <c r="O8" s="128"/>
-      <c r="P8" s="125"/>
-      <c r="Q8" s="130">
+      <c r="D8" s="124"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="102">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],Q7),"")</f>
         <v>45040</v>
       </c>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
-      <c r="U8" s="94"/>
-      <c r="V8" s="94"/>
-      <c r="W8" s="94"/>
-      <c r="X8" s="94"/>
-      <c r="Y8" s="94"/>
-      <c r="Z8" s="95"/>
-      <c r="AA8" s="93">
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="103"/>
+      <c r="Z8" s="104"/>
+      <c r="AA8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AA7),"")</f>
         <v>45041</v>
       </c>
-      <c r="AB8" s="94"/>
-      <c r="AC8" s="94"/>
-      <c r="AD8" s="94"/>
-      <c r="AE8" s="94"/>
-      <c r="AF8" s="94"/>
-      <c r="AG8" s="94"/>
-      <c r="AH8" s="94"/>
-      <c r="AI8" s="94"/>
-      <c r="AJ8" s="95"/>
-      <c r="AK8" s="93">
+      <c r="AB8" s="103"/>
+      <c r="AC8" s="103"/>
+      <c r="AD8" s="103"/>
+      <c r="AE8" s="103"/>
+      <c r="AF8" s="103"/>
+      <c r="AG8" s="103"/>
+      <c r="AH8" s="103"/>
+      <c r="AI8" s="103"/>
+      <c r="AJ8" s="104"/>
+      <c r="AK8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AK7),"")</f>
         <v>45042</v>
       </c>
-      <c r="AL8" s="94"/>
-      <c r="AM8" s="94"/>
-      <c r="AN8" s="94"/>
-      <c r="AO8" s="94"/>
-      <c r="AP8" s="94"/>
-      <c r="AQ8" s="94"/>
-      <c r="AR8" s="94"/>
-      <c r="AS8" s="94"/>
-      <c r="AT8" s="95"/>
-      <c r="AU8" s="93">
+      <c r="AL8" s="103"/>
+      <c r="AM8" s="103"/>
+      <c r="AN8" s="103"/>
+      <c r="AO8" s="103"/>
+      <c r="AP8" s="103"/>
+      <c r="AQ8" s="103"/>
+      <c r="AR8" s="103"/>
+      <c r="AS8" s="103"/>
+      <c r="AT8" s="104"/>
+      <c r="AU8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AU7),"")</f>
         <v>45048</v>
       </c>
-      <c r="AV8" s="94"/>
-      <c r="AW8" s="94"/>
-      <c r="AX8" s="94"/>
-      <c r="AY8" s="94"/>
-      <c r="AZ8" s="94"/>
-      <c r="BA8" s="94"/>
-      <c r="BB8" s="94"/>
-      <c r="BC8" s="94"/>
-      <c r="BD8" s="95"/>
-      <c r="BE8" s="93">
+      <c r="AV8" s="103"/>
+      <c r="AW8" s="103"/>
+      <c r="AX8" s="103"/>
+      <c r="AY8" s="103"/>
+      <c r="AZ8" s="103"/>
+      <c r="BA8" s="103"/>
+      <c r="BB8" s="103"/>
+      <c r="BC8" s="103"/>
+      <c r="BD8" s="104"/>
+      <c r="BE8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BE7),"")</f>
         <v>45049</v>
       </c>
-      <c r="BF8" s="94"/>
-      <c r="BG8" s="94"/>
-      <c r="BH8" s="94"/>
-      <c r="BI8" s="94"/>
-      <c r="BJ8" s="94"/>
-      <c r="BK8" s="94"/>
-      <c r="BL8" s="94"/>
-      <c r="BM8" s="94"/>
-      <c r="BN8" s="95"/>
-      <c r="BO8" s="93">
+      <c r="BF8" s="103"/>
+      <c r="BG8" s="103"/>
+      <c r="BH8" s="103"/>
+      <c r="BI8" s="103"/>
+      <c r="BJ8" s="103"/>
+      <c r="BK8" s="103"/>
+      <c r="BL8" s="103"/>
+      <c r="BM8" s="103"/>
+      <c r="BN8" s="104"/>
+      <c r="BO8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BO7),"")</f>
         <v>45054</v>
       </c>
-      <c r="BP8" s="94"/>
-      <c r="BQ8" s="94"/>
-      <c r="BR8" s="94"/>
-      <c r="BS8" s="94"/>
-      <c r="BT8" s="94"/>
-      <c r="BU8" s="94"/>
-      <c r="BV8" s="94"/>
-      <c r="BW8" s="94"/>
-      <c r="BX8" s="95"/>
-      <c r="BY8" s="93">
+      <c r="BP8" s="103"/>
+      <c r="BQ8" s="103"/>
+      <c r="BR8" s="103"/>
+      <c r="BS8" s="103"/>
+      <c r="BT8" s="103"/>
+      <c r="BU8" s="103"/>
+      <c r="BV8" s="103"/>
+      <c r="BW8" s="103"/>
+      <c r="BX8" s="104"/>
+      <c r="BY8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BY7),"")</f>
         <v>45055</v>
       </c>
-      <c r="BZ8" s="94"/>
-      <c r="CA8" s="94"/>
-      <c r="CB8" s="94"/>
-      <c r="CC8" s="94"/>
-      <c r="CD8" s="94"/>
-      <c r="CE8" s="94"/>
-      <c r="CF8" s="94"/>
-      <c r="CG8" s="94"/>
-      <c r="CH8" s="95"/>
-      <c r="CI8" s="93">
+      <c r="BZ8" s="103"/>
+      <c r="CA8" s="103"/>
+      <c r="CB8" s="103"/>
+      <c r="CC8" s="103"/>
+      <c r="CD8" s="103"/>
+      <c r="CE8" s="103"/>
+      <c r="CF8" s="103"/>
+      <c r="CG8" s="103"/>
+      <c r="CH8" s="104"/>
+      <c r="CI8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CI7),"")</f>
         <v>45056</v>
       </c>
-      <c r="CJ8" s="94"/>
-      <c r="CK8" s="94"/>
-      <c r="CL8" s="94"/>
-      <c r="CM8" s="94"/>
-      <c r="CN8" s="94"/>
-      <c r="CO8" s="94"/>
-      <c r="CP8" s="94"/>
-      <c r="CQ8" s="94"/>
-      <c r="CR8" s="95"/>
-      <c r="CS8" s="93">
+      <c r="CJ8" s="103"/>
+      <c r="CK8" s="103"/>
+      <c r="CL8" s="103"/>
+      <c r="CM8" s="103"/>
+      <c r="CN8" s="103"/>
+      <c r="CO8" s="103"/>
+      <c r="CP8" s="103"/>
+      <c r="CQ8" s="103"/>
+      <c r="CR8" s="104"/>
+      <c r="CS8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CS7),"")</f>
         <v>45061</v>
       </c>
-      <c r="CT8" s="94"/>
-      <c r="CU8" s="94"/>
-      <c r="CV8" s="94"/>
-      <c r="CW8" s="94"/>
-      <c r="CX8" s="94"/>
-      <c r="CY8" s="94"/>
-      <c r="CZ8" s="94"/>
-      <c r="DA8" s="94"/>
-      <c r="DB8" s="94"/>
-      <c r="DC8" s="93">
+      <c r="CT8" s="103"/>
+      <c r="CU8" s="103"/>
+      <c r="CV8" s="103"/>
+      <c r="CW8" s="103"/>
+      <c r="CX8" s="103"/>
+      <c r="CY8" s="103"/>
+      <c r="CZ8" s="103"/>
+      <c r="DA8" s="103"/>
+      <c r="DB8" s="103"/>
+      <c r="DC8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DC7),"")</f>
         <v>45062</v>
       </c>
-      <c r="DD8" s="94"/>
-      <c r="DE8" s="94"/>
-      <c r="DF8" s="94"/>
-      <c r="DG8" s="94"/>
-      <c r="DH8" s="94"/>
-      <c r="DI8" s="94"/>
-      <c r="DJ8" s="94"/>
-      <c r="DK8" s="94"/>
-      <c r="DL8" s="95"/>
-      <c r="DM8" s="93">
+      <c r="DD8" s="103"/>
+      <c r="DE8" s="103"/>
+      <c r="DF8" s="103"/>
+      <c r="DG8" s="103"/>
+      <c r="DH8" s="103"/>
+      <c r="DI8" s="103"/>
+      <c r="DJ8" s="103"/>
+      <c r="DK8" s="103"/>
+      <c r="DL8" s="104"/>
+      <c r="DM8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DM7),"")</f>
         <v>45063</v>
       </c>
-      <c r="DN8" s="94"/>
-      <c r="DO8" s="94"/>
-      <c r="DP8" s="94"/>
-      <c r="DQ8" s="94"/>
-      <c r="DR8" s="94"/>
-      <c r="DS8" s="94"/>
-      <c r="DT8" s="94"/>
-      <c r="DU8" s="94"/>
-      <c r="DV8" s="95"/>
-      <c r="DW8" s="93" t="str">
+      <c r="DN8" s="103"/>
+      <c r="DO8" s="103"/>
+      <c r="DP8" s="103"/>
+      <c r="DQ8" s="103"/>
+      <c r="DR8" s="103"/>
+      <c r="DS8" s="103"/>
+      <c r="DT8" s="103"/>
+      <c r="DU8" s="103"/>
+      <c r="DV8" s="104"/>
+      <c r="DW8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DW7),"")</f>
         <v/>
       </c>
-      <c r="DX8" s="94"/>
-      <c r="DY8" s="94"/>
-      <c r="DZ8" s="94"/>
-      <c r="EA8" s="94"/>
-      <c r="EB8" s="94"/>
-      <c r="EC8" s="94"/>
-      <c r="ED8" s="94"/>
-      <c r="EE8" s="94"/>
-      <c r="EF8" s="95"/>
-      <c r="EG8" s="93" t="str">
+      <c r="DX8" s="103"/>
+      <c r="DY8" s="103"/>
+      <c r="DZ8" s="103"/>
+      <c r="EA8" s="103"/>
+      <c r="EB8" s="103"/>
+      <c r="EC8" s="103"/>
+      <c r="ED8" s="103"/>
+      <c r="EE8" s="103"/>
+      <c r="EF8" s="104"/>
+      <c r="EG8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EG7),"")</f>
         <v/>
       </c>
-      <c r="EH8" s="94"/>
-      <c r="EI8" s="94"/>
-      <c r="EJ8" s="94"/>
-      <c r="EK8" s="94"/>
-      <c r="EL8" s="94"/>
-      <c r="EM8" s="94"/>
-      <c r="EN8" s="94"/>
-      <c r="EO8" s="94"/>
-      <c r="EP8" s="96"/>
-      <c r="EQ8" s="94" t="str">
+      <c r="EH8" s="103"/>
+      <c r="EI8" s="103"/>
+      <c r="EJ8" s="103"/>
+      <c r="EK8" s="103"/>
+      <c r="EL8" s="103"/>
+      <c r="EM8" s="103"/>
+      <c r="EN8" s="103"/>
+      <c r="EO8" s="103"/>
+      <c r="EP8" s="118"/>
+      <c r="EQ8" s="103" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EQ7),"")</f>
         <v/>
       </c>
-      <c r="ER8" s="94"/>
-      <c r="ES8" s="94"/>
-      <c r="ET8" s="94"/>
-      <c r="EU8" s="94"/>
-      <c r="EV8" s="94"/>
-      <c r="EW8" s="94"/>
-      <c r="EX8" s="94"/>
-      <c r="EY8" s="94"/>
-      <c r="EZ8" s="95"/>
-      <c r="FA8" s="93" t="str">
+      <c r="ER8" s="103"/>
+      <c r="ES8" s="103"/>
+      <c r="ET8" s="103"/>
+      <c r="EU8" s="103"/>
+      <c r="EV8" s="103"/>
+      <c r="EW8" s="103"/>
+      <c r="EX8" s="103"/>
+      <c r="EY8" s="103"/>
+      <c r="EZ8" s="104"/>
+      <c r="FA8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FA7),"")</f>
         <v/>
       </c>
-      <c r="FB8" s="94"/>
-      <c r="FC8" s="94"/>
-      <c r="FD8" s="94"/>
-      <c r="FE8" s="94"/>
-      <c r="FF8" s="94"/>
-      <c r="FG8" s="94"/>
-      <c r="FH8" s="94"/>
-      <c r="FI8" s="94"/>
-      <c r="FJ8" s="95"/>
-      <c r="FK8" s="93" t="str">
+      <c r="FB8" s="103"/>
+      <c r="FC8" s="103"/>
+      <c r="FD8" s="103"/>
+      <c r="FE8" s="103"/>
+      <c r="FF8" s="103"/>
+      <c r="FG8" s="103"/>
+      <c r="FH8" s="103"/>
+      <c r="FI8" s="103"/>
+      <c r="FJ8" s="104"/>
+      <c r="FK8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FK7),"")</f>
         <v/>
       </c>
-      <c r="FL8" s="94"/>
-      <c r="FM8" s="94"/>
-      <c r="FN8" s="94"/>
-      <c r="FO8" s="94"/>
-      <c r="FP8" s="94"/>
-      <c r="FQ8" s="94"/>
-      <c r="FR8" s="94"/>
-      <c r="FS8" s="94"/>
-      <c r="FT8" s="95"/>
-      <c r="FU8" s="93" t="str">
+      <c r="FL8" s="103"/>
+      <c r="FM8" s="103"/>
+      <c r="FN8" s="103"/>
+      <c r="FO8" s="103"/>
+      <c r="FP8" s="103"/>
+      <c r="FQ8" s="103"/>
+      <c r="FR8" s="103"/>
+      <c r="FS8" s="103"/>
+      <c r="FT8" s="104"/>
+      <c r="FU8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FU7),"")</f>
         <v/>
       </c>
-      <c r="FV8" s="94"/>
-      <c r="FW8" s="94"/>
-      <c r="FX8" s="94"/>
-      <c r="FY8" s="94"/>
-      <c r="FZ8" s="94"/>
-      <c r="GA8" s="94"/>
-      <c r="GB8" s="94"/>
-      <c r="GC8" s="94"/>
-      <c r="GD8" s="95"/>
-      <c r="GE8" s="93" t="str">
+      <c r="FV8" s="103"/>
+      <c r="FW8" s="103"/>
+      <c r="FX8" s="103"/>
+      <c r="FY8" s="103"/>
+      <c r="FZ8" s="103"/>
+      <c r="GA8" s="103"/>
+      <c r="GB8" s="103"/>
+      <c r="GC8" s="103"/>
+      <c r="GD8" s="104"/>
+      <c r="GE8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GE7),"")</f>
         <v/>
       </c>
-      <c r="GF8" s="94"/>
-      <c r="GG8" s="94"/>
-      <c r="GH8" s="94"/>
-      <c r="GI8" s="94"/>
-      <c r="GJ8" s="94"/>
-      <c r="GK8" s="94"/>
-      <c r="GL8" s="94"/>
-      <c r="GM8" s="94"/>
-      <c r="GN8" s="95"/>
-      <c r="GO8" s="93" t="str">
+      <c r="GF8" s="103"/>
+      <c r="GG8" s="103"/>
+      <c r="GH8" s="103"/>
+      <c r="GI8" s="103"/>
+      <c r="GJ8" s="103"/>
+      <c r="GK8" s="103"/>
+      <c r="GL8" s="103"/>
+      <c r="GM8" s="103"/>
+      <c r="GN8" s="104"/>
+      <c r="GO8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GO7),"")</f>
         <v/>
       </c>
-      <c r="GP8" s="94"/>
-      <c r="GQ8" s="94"/>
-      <c r="GR8" s="94"/>
-      <c r="GS8" s="94"/>
-      <c r="GT8" s="94"/>
-      <c r="GU8" s="94"/>
-      <c r="GV8" s="94"/>
-      <c r="GW8" s="94"/>
-      <c r="GX8" s="95"/>
-      <c r="GY8" s="93" t="str">
+      <c r="GP8" s="103"/>
+      <c r="GQ8" s="103"/>
+      <c r="GR8" s="103"/>
+      <c r="GS8" s="103"/>
+      <c r="GT8" s="103"/>
+      <c r="GU8" s="103"/>
+      <c r="GV8" s="103"/>
+      <c r="GW8" s="103"/>
+      <c r="GX8" s="104"/>
+      <c r="GY8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GY7),"")</f>
         <v/>
       </c>
-      <c r="GZ8" s="94"/>
-      <c r="HA8" s="94"/>
-      <c r="HB8" s="94"/>
-      <c r="HC8" s="94"/>
-      <c r="HD8" s="94"/>
-      <c r="HE8" s="94"/>
-      <c r="HF8" s="94"/>
-      <c r="HG8" s="94"/>
-      <c r="HH8" s="95"/>
-      <c r="HI8" s="93" t="str">
+      <c r="GZ8" s="103"/>
+      <c r="HA8" s="103"/>
+      <c r="HB8" s="103"/>
+      <c r="HC8" s="103"/>
+      <c r="HD8" s="103"/>
+      <c r="HE8" s="103"/>
+      <c r="HF8" s="103"/>
+      <c r="HG8" s="103"/>
+      <c r="HH8" s="104"/>
+      <c r="HI8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],HI7),"")</f>
         <v/>
       </c>
-      <c r="HJ8" s="94"/>
-      <c r="HK8" s="94"/>
-      <c r="HL8" s="94"/>
-      <c r="HM8" s="94"/>
-      <c r="HN8" s="94"/>
-      <c r="HO8" s="94"/>
-      <c r="HP8" s="94"/>
-      <c r="HQ8" s="94"/>
-      <c r="HR8" s="96"/>
+      <c r="HJ8" s="103"/>
+      <c r="HK8" s="103"/>
+      <c r="HL8" s="103"/>
+      <c r="HM8" s="103"/>
+      <c r="HN8" s="103"/>
+      <c r="HO8" s="103"/>
+      <c r="HP8" s="103"/>
+      <c r="HQ8" s="103"/>
+      <c r="HR8" s="118"/>
     </row>
     <row r="9" spans="1:226" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="133"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="131">
+      <c r="D9" s="124"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="99"/>
+      <c r="Q9" s="105">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(Q8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="98"/>
-      <c r="Z9" s="99"/>
-      <c r="AA9" s="97" t="str">
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="106"/>
+      <c r="V9" s="106"/>
+      <c r="W9" s="106"/>
+      <c r="X9" s="106"/>
+      <c r="Y9" s="106"/>
+      <c r="Z9" s="107"/>
+      <c r="AA9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L1] Connexion</v>
       </c>
-      <c r="AB9" s="98"/>
-      <c r="AC9" s="98"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="98"/>
-      <c r="AF9" s="98"/>
-      <c r="AG9" s="98"/>
-      <c r="AH9" s="98"/>
-      <c r="AI9" s="98"/>
-      <c r="AJ9" s="99"/>
-      <c r="AK9" s="97">
+      <c r="AB9" s="106"/>
+      <c r="AC9" s="106"/>
+      <c r="AD9" s="106"/>
+      <c r="AE9" s="106"/>
+      <c r="AF9" s="106"/>
+      <c r="AG9" s="106"/>
+      <c r="AH9" s="106"/>
+      <c r="AI9" s="106"/>
+      <c r="AJ9" s="107"/>
+      <c r="AK9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="98"/>
-      <c r="AM9" s="98"/>
-      <c r="AN9" s="98"/>
-      <c r="AO9" s="98"/>
-      <c r="AP9" s="98"/>
-      <c r="AQ9" s="98"/>
-      <c r="AR9" s="98"/>
-      <c r="AS9" s="98"/>
-      <c r="AT9" s="99"/>
-      <c r="AU9" s="97" t="str">
+      <c r="AL9" s="106"/>
+      <c r="AM9" s="106"/>
+      <c r="AN9" s="106"/>
+      <c r="AO9" s="106"/>
+      <c r="AP9" s="106"/>
+      <c r="AQ9" s="106"/>
+      <c r="AR9" s="106"/>
+      <c r="AS9" s="106"/>
+      <c r="AT9" s="107"/>
+      <c r="AU9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L2] Affichage Professeur</v>
       </c>
-      <c r="AV9" s="98"/>
-      <c r="AW9" s="98"/>
-      <c r="AX9" s="98"/>
-      <c r="AY9" s="98"/>
-      <c r="AZ9" s="98"/>
-      <c r="BA9" s="98"/>
-      <c r="BB9" s="98"/>
-      <c r="BC9" s="98"/>
-      <c r="BD9" s="99"/>
-      <c r="BE9" s="97">
+      <c r="AV9" s="106"/>
+      <c r="AW9" s="106"/>
+      <c r="AX9" s="106"/>
+      <c r="AY9" s="106"/>
+      <c r="AZ9" s="106"/>
+      <c r="BA9" s="106"/>
+      <c r="BB9" s="106"/>
+      <c r="BC9" s="106"/>
+      <c r="BD9" s="107"/>
+      <c r="BE9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BF9" s="98"/>
-      <c r="BG9" s="98"/>
-      <c r="BH9" s="98"/>
-      <c r="BI9" s="98"/>
-      <c r="BJ9" s="98"/>
-      <c r="BK9" s="98"/>
-      <c r="BL9" s="98"/>
-      <c r="BM9" s="98"/>
-      <c r="BN9" s="99"/>
-      <c r="BO9" s="97" t="str">
+      <c r="BF9" s="106"/>
+      <c r="BG9" s="106"/>
+      <c r="BH9" s="106"/>
+      <c r="BI9" s="106"/>
+      <c r="BJ9" s="106"/>
+      <c r="BK9" s="106"/>
+      <c r="BL9" s="106"/>
+      <c r="BM9" s="106"/>
+      <c r="BN9" s="107"/>
+      <c r="BO9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L3] Historique</v>
       </c>
-      <c r="BP9" s="98"/>
-      <c r="BQ9" s="98"/>
-      <c r="BR9" s="98"/>
-      <c r="BS9" s="98"/>
-      <c r="BT9" s="98"/>
-      <c r="BU9" s="98"/>
-      <c r="BV9" s="98"/>
-      <c r="BW9" s="98"/>
-      <c r="BX9" s="99"/>
-      <c r="BY9" s="97">
+      <c r="BP9" s="106"/>
+      <c r="BQ9" s="106"/>
+      <c r="BR9" s="106"/>
+      <c r="BS9" s="106"/>
+      <c r="BT9" s="106"/>
+      <c r="BU9" s="106"/>
+      <c r="BV9" s="106"/>
+      <c r="BW9" s="106"/>
+      <c r="BX9" s="107"/>
+      <c r="BY9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BZ9" s="98"/>
-      <c r="CA9" s="98"/>
-      <c r="CB9" s="98"/>
-      <c r="CC9" s="98"/>
-      <c r="CD9" s="98"/>
-      <c r="CE9" s="98"/>
-      <c r="CF9" s="98"/>
-      <c r="CG9" s="98"/>
-      <c r="CH9" s="99"/>
-      <c r="CI9" s="97" t="str">
+      <c r="BZ9" s="106"/>
+      <c r="CA9" s="106"/>
+      <c r="CB9" s="106"/>
+      <c r="CC9" s="106"/>
+      <c r="CD9" s="106"/>
+      <c r="CE9" s="106"/>
+      <c r="CF9" s="106"/>
+      <c r="CG9" s="106"/>
+      <c r="CH9" s="107"/>
+      <c r="CI9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L4] Filtrage</v>
       </c>
-      <c r="CJ9" s="98"/>
-      <c r="CK9" s="98"/>
-      <c r="CL9" s="98"/>
-      <c r="CM9" s="98"/>
-      <c r="CN9" s="98"/>
-      <c r="CO9" s="98"/>
-      <c r="CP9" s="98"/>
-      <c r="CQ9" s="98"/>
-      <c r="CR9" s="99"/>
-      <c r="CS9" s="97" t="str">
+      <c r="CJ9" s="106"/>
+      <c r="CK9" s="106"/>
+      <c r="CL9" s="106"/>
+      <c r="CM9" s="106"/>
+      <c r="CN9" s="106"/>
+      <c r="CO9" s="106"/>
+      <c r="CP9" s="106"/>
+      <c r="CQ9" s="106"/>
+      <c r="CR9" s="107"/>
+      <c r="CS9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CS8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L5] Streaming multicast</v>
       </c>
-      <c r="CT9" s="98"/>
-      <c r="CU9" s="98"/>
-      <c r="CV9" s="98"/>
-      <c r="CW9" s="98"/>
-      <c r="CX9" s="98"/>
-      <c r="CY9" s="98"/>
-      <c r="CZ9" s="98"/>
-      <c r="DA9" s="98"/>
-      <c r="DB9" s="98"/>
-      <c r="DC9" s="97">
+      <c r="CT9" s="106"/>
+      <c r="CU9" s="106"/>
+      <c r="CV9" s="106"/>
+      <c r="CW9" s="106"/>
+      <c r="CX9" s="106"/>
+      <c r="CY9" s="106"/>
+      <c r="CZ9" s="106"/>
+      <c r="DA9" s="106"/>
+      <c r="DB9" s="106"/>
+      <c r="DC9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DC8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DD9" s="98"/>
-      <c r="DE9" s="98"/>
-      <c r="DF9" s="98"/>
-      <c r="DG9" s="98"/>
-      <c r="DH9" s="98"/>
-      <c r="DI9" s="98"/>
-      <c r="DJ9" s="98"/>
-      <c r="DK9" s="98"/>
-      <c r="DL9" s="99"/>
-      <c r="DM9" s="97" t="str">
+      <c r="DD9" s="106"/>
+      <c r="DE9" s="106"/>
+      <c r="DF9" s="106"/>
+      <c r="DG9" s="106"/>
+      <c r="DH9" s="106"/>
+      <c r="DI9" s="106"/>
+      <c r="DJ9" s="106"/>
+      <c r="DK9" s="106"/>
+      <c r="DL9" s="107"/>
+      <c r="DM9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DM8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L6] Contrôle à distance</v>
       </c>
-      <c r="DN9" s="98"/>
-      <c r="DO9" s="98"/>
-      <c r="DP9" s="98"/>
-      <c r="DQ9" s="98"/>
-      <c r="DR9" s="98"/>
-      <c r="DS9" s="98"/>
-      <c r="DT9" s="98"/>
-      <c r="DU9" s="98"/>
-      <c r="DV9" s="99"/>
-      <c r="DW9" s="97">
+      <c r="DN9" s="106"/>
+      <c r="DO9" s="106"/>
+      <c r="DP9" s="106"/>
+      <c r="DQ9" s="106"/>
+      <c r="DR9" s="106"/>
+      <c r="DS9" s="106"/>
+      <c r="DT9" s="106"/>
+      <c r="DU9" s="106"/>
+      <c r="DV9" s="107"/>
+      <c r="DW9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DW8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DX9" s="98"/>
-      <c r="DY9" s="98"/>
-      <c r="DZ9" s="98"/>
-      <c r="EA9" s="98"/>
-      <c r="EB9" s="98"/>
-      <c r="EC9" s="98"/>
-      <c r="ED9" s="98"/>
-      <c r="EE9" s="98"/>
-      <c r="EF9" s="99"/>
-      <c r="EG9" s="97">
+      <c r="DX9" s="106"/>
+      <c r="DY9" s="106"/>
+      <c r="DZ9" s="106"/>
+      <c r="EA9" s="106"/>
+      <c r="EB9" s="106"/>
+      <c r="EC9" s="106"/>
+      <c r="ED9" s="106"/>
+      <c r="EE9" s="106"/>
+      <c r="EF9" s="107"/>
+      <c r="EG9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EG8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="EH9" s="98"/>
-      <c r="EI9" s="98"/>
-      <c r="EJ9" s="98"/>
-      <c r="EK9" s="98"/>
-      <c r="EL9" s="98"/>
-      <c r="EM9" s="98"/>
-      <c r="EN9" s="98"/>
-      <c r="EO9" s="98"/>
-      <c r="EP9" s="100"/>
-      <c r="EQ9" s="98">
+      <c r="EH9" s="106"/>
+      <c r="EI9" s="106"/>
+      <c r="EJ9" s="106"/>
+      <c r="EK9" s="106"/>
+      <c r="EL9" s="106"/>
+      <c r="EM9" s="106"/>
+      <c r="EN9" s="106"/>
+      <c r="EO9" s="106"/>
+      <c r="EP9" s="122"/>
+      <c r="EQ9" s="106">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EQ8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="ER9" s="98"/>
-      <c r="ES9" s="98"/>
-      <c r="ET9" s="98"/>
-      <c r="EU9" s="98"/>
-      <c r="EV9" s="98"/>
-      <c r="EW9" s="98"/>
-      <c r="EX9" s="98"/>
-      <c r="EY9" s="98"/>
-      <c r="EZ9" s="99"/>
-      <c r="FA9" s="97">
+      <c r="ER9" s="106"/>
+      <c r="ES9" s="106"/>
+      <c r="ET9" s="106"/>
+      <c r="EU9" s="106"/>
+      <c r="EV9" s="106"/>
+      <c r="EW9" s="106"/>
+      <c r="EX9" s="106"/>
+      <c r="EY9" s="106"/>
+      <c r="EZ9" s="107"/>
+      <c r="FA9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FB9" s="98"/>
-      <c r="FC9" s="98"/>
-      <c r="FD9" s="98"/>
-      <c r="FE9" s="98"/>
-      <c r="FF9" s="98"/>
-      <c r="FG9" s="98"/>
-      <c r="FH9" s="98"/>
-      <c r="FI9" s="98"/>
-      <c r="FJ9" s="99"/>
-      <c r="FK9" s="97">
+      <c r="FB9" s="106"/>
+      <c r="FC9" s="106"/>
+      <c r="FD9" s="106"/>
+      <c r="FE9" s="106"/>
+      <c r="FF9" s="106"/>
+      <c r="FG9" s="106"/>
+      <c r="FH9" s="106"/>
+      <c r="FI9" s="106"/>
+      <c r="FJ9" s="107"/>
+      <c r="FK9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FL9" s="98"/>
-      <c r="FM9" s="98"/>
-      <c r="FN9" s="98"/>
-      <c r="FO9" s="98"/>
-      <c r="FP9" s="98"/>
-      <c r="FQ9" s="98"/>
-      <c r="FR9" s="98"/>
-      <c r="FS9" s="98"/>
-      <c r="FT9" s="99"/>
-      <c r="FU9" s="97">
+      <c r="FL9" s="106"/>
+      <c r="FM9" s="106"/>
+      <c r="FN9" s="106"/>
+      <c r="FO9" s="106"/>
+      <c r="FP9" s="106"/>
+      <c r="FQ9" s="106"/>
+      <c r="FR9" s="106"/>
+      <c r="FS9" s="106"/>
+      <c r="FT9" s="107"/>
+      <c r="FU9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FV9" s="98"/>
-      <c r="FW9" s="98"/>
-      <c r="FX9" s="98"/>
-      <c r="FY9" s="98"/>
-      <c r="FZ9" s="98"/>
-      <c r="GA9" s="98"/>
-      <c r="GB9" s="98"/>
-      <c r="GC9" s="98"/>
-      <c r="GD9" s="99"/>
-      <c r="GE9" s="97">
+      <c r="FV9" s="106"/>
+      <c r="FW9" s="106"/>
+      <c r="FX9" s="106"/>
+      <c r="FY9" s="106"/>
+      <c r="FZ9" s="106"/>
+      <c r="GA9" s="106"/>
+      <c r="GB9" s="106"/>
+      <c r="GC9" s="106"/>
+      <c r="GD9" s="107"/>
+      <c r="GE9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GF9" s="98"/>
-      <c r="GG9" s="98"/>
-      <c r="GH9" s="98"/>
-      <c r="GI9" s="98"/>
-      <c r="GJ9" s="98"/>
-      <c r="GK9" s="98"/>
-      <c r="GL9" s="98"/>
-      <c r="GM9" s="98"/>
-      <c r="GN9" s="99"/>
-      <c r="GO9" s="97">
+      <c r="GF9" s="106"/>
+      <c r="GG9" s="106"/>
+      <c r="GH9" s="106"/>
+      <c r="GI9" s="106"/>
+      <c r="GJ9" s="106"/>
+      <c r="GK9" s="106"/>
+      <c r="GL9" s="106"/>
+      <c r="GM9" s="106"/>
+      <c r="GN9" s="107"/>
+      <c r="GO9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GP9" s="98"/>
-      <c r="GQ9" s="98"/>
-      <c r="GR9" s="98"/>
-      <c r="GS9" s="98"/>
-      <c r="GT9" s="98"/>
-      <c r="GU9" s="98"/>
-      <c r="GV9" s="98"/>
-      <c r="GW9" s="98"/>
-      <c r="GX9" s="99"/>
-      <c r="GY9" s="97">
+      <c r="GP9" s="106"/>
+      <c r="GQ9" s="106"/>
+      <c r="GR9" s="106"/>
+      <c r="GS9" s="106"/>
+      <c r="GT9" s="106"/>
+      <c r="GU9" s="106"/>
+      <c r="GV9" s="106"/>
+      <c r="GW9" s="106"/>
+      <c r="GX9" s="107"/>
+      <c r="GY9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GZ9" s="98"/>
-      <c r="HA9" s="98"/>
-      <c r="HB9" s="98"/>
-      <c r="HC9" s="98"/>
-      <c r="HD9" s="98"/>
-      <c r="HE9" s="98"/>
-      <c r="HF9" s="98"/>
-      <c r="HG9" s="98"/>
-      <c r="HH9" s="99"/>
-      <c r="HI9" s="97">
+      <c r="GZ9" s="106"/>
+      <c r="HA9" s="106"/>
+      <c r="HB9" s="106"/>
+      <c r="HC9" s="106"/>
+      <c r="HD9" s="106"/>
+      <c r="HE9" s="106"/>
+      <c r="HF9" s="106"/>
+      <c r="HG9" s="106"/>
+      <c r="HH9" s="107"/>
+      <c r="HI9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(HI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="HJ9" s="98"/>
-      <c r="HK9" s="98"/>
-      <c r="HL9" s="98"/>
-      <c r="HM9" s="98"/>
-      <c r="HN9" s="98"/>
-      <c r="HO9" s="98"/>
-      <c r="HP9" s="98"/>
-      <c r="HQ9" s="98"/>
-      <c r="HR9" s="100"/>
+      <c r="HJ9" s="106"/>
+      <c r="HK9" s="106"/>
+      <c r="HL9" s="106"/>
+      <c r="HM9" s="106"/>
+      <c r="HN9" s="106"/>
+      <c r="HO9" s="106"/>
+      <c r="HP9" s="106"/>
+      <c r="HQ9" s="106"/>
+      <c r="HR9" s="122"/>
     </row>
     <row r="10" spans="1:226" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="133"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="125"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="99"/>
       <c r="Q10" s="5"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="20"/>
@@ -28139,19 +28139,19 @@
       <c r="A11" s="68"/>
       <c r="B11" s="5"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
-      <c r="O11" s="129"/>
-      <c r="P11" s="126"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="100"/>
       <c r="Q11" s="51">
         <v>0</v>
       </c>
@@ -29648,17 +29648,17 @@
       </c>
     </row>
     <row r="13" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="111" t="s">
+      <c r="D13" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="83"/>
-      <c r="G13" s="84" t="s">
+      <c r="E13" s="101"/>
+      <c r="G13" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="85" t="str">
+      <c r="H13" s="119" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
       </c>
@@ -29764,11 +29764,11 @@
       <c r="HR13" s="4"/>
     </row>
     <row r="14" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="83"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="85"/>
+      <c r="B14" s="134"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="101"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="119"/>
       <c r="I14" s="45" t="s">
         <v>1</v>
       </c>
@@ -30020,22 +30020,22 @@
       <c r="HR14" s="31"/>
     </row>
     <row r="15" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="83" t="s">
+      <c r="E15" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="83">
+      <c r="F15" s="101">
         <v>1</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="85" t="str">
+      <c r="H15" s="119" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
       </c>
@@ -30106,12 +30106,12 @@
       <c r="HR15" s="4"/>
     </row>
     <row r="16" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="81"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="85"/>
+      <c r="B16" s="134"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="119"/>
       <c r="I16" s="45" t="s">
         <v>1</v>
       </c>
@@ -30351,20 +30351,20 @@
       <c r="HR16" s="31"/>
     </row>
     <row r="17" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83">
+      <c r="E17" s="101"/>
+      <c r="F17" s="101">
         <v>1</v>
       </c>
-      <c r="G17" s="84" t="s">
+      <c r="G17" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="85" t="str">
+      <c r="H17" s="119" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
       </c>
@@ -30436,12 +30436,12 @@
       <c r="HR17" s="4"/>
     </row>
     <row r="18" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="85"/>
+      <c r="B18" s="134"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="119"/>
       <c r="I18" s="45" t="s">
         <v>1</v>
       </c>
@@ -30683,22 +30683,22 @@
       <c r="HR18" s="31"/>
     </row>
     <row r="19" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="111" t="s">
+      <c r="D19" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E19" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="83">
+      <c r="F19" s="101">
         <v>1</v>
       </c>
-      <c r="G19" s="84" t="s">
+      <c r="G19" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="85" t="str">
+      <c r="H19" s="119" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
       </c>
@@ -30782,12 +30782,12 @@
       <c r="HR19" s="4"/>
     </row>
     <row r="20" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="81"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="85"/>
+      <c r="B20" s="134"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="119"/>
       <c r="I20" s="45" t="s">
         <v>1</v>
       </c>
@@ -31031,20 +31031,20 @@
       <c r="HR20" s="31"/>
     </row>
     <row r="21" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83">
+      <c r="E21" s="101"/>
+      <c r="F21" s="101">
         <v>1</v>
       </c>
-      <c r="G21" s="84" t="s">
+      <c r="G21" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="85" t="str">
+      <c r="H21" s="119" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
       </c>
@@ -31118,12 +31118,12 @@
       <c r="HR21" s="4"/>
     </row>
     <row r="22" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="81"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="85"/>
+      <c r="B22" s="134"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="119"/>
       <c r="I22" s="45" t="s">
         <v>1</v>
       </c>
@@ -31361,20 +31361,20 @@
       <c r="HR22" s="31"/>
     </row>
     <row r="23" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="111" t="s">
+      <c r="D23" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83">
+      <c r="E23" s="101"/>
+      <c r="F23" s="101">
         <v>1</v>
       </c>
-      <c r="G23" s="84" t="s">
+      <c r="G23" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="85" t="str">
+      <c r="H23" s="119" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
       </c>
@@ -31445,12 +31445,12 @@
       <c r="HR23" s="4"/>
     </row>
     <row r="24" spans="2:226" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="81"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="85"/>
+      <c r="B24" s="134"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="119"/>
       <c r="I24" s="45" t="s">
         <v>1</v>
       </c>
@@ -31692,20 +31692,20 @@
       <c r="HR24" s="31"/>
     </row>
     <row r="25" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83">
+      <c r="E25" s="101"/>
+      <c r="F25" s="101">
         <v>1</v>
       </c>
-      <c r="G25" s="84" t="s">
+      <c r="G25" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="85" t="str">
+      <c r="H25" s="119" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
       </c>
@@ -31775,12 +31775,12 @@
       <c r="HR25" s="4"/>
     </row>
     <row r="26" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="81"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="85"/>
+      <c r="B26" s="134"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="119"/>
       <c r="I26" s="45" t="s">
         <v>1</v>
       </c>
@@ -32020,20 +32020,20 @@
       <c r="HR26" s="31"/>
     </row>
     <row r="27" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="111" t="s">
+      <c r="D27" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83">
+      <c r="E27" s="101"/>
+      <c r="F27" s="101">
         <v>2</v>
       </c>
-      <c r="G27" s="84" t="s">
+      <c r="G27" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="85" t="str">
+      <c r="H27" s="119" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
       </c>
@@ -32114,12 +32114,12 @@
       <c r="HR27" s="4"/>
     </row>
     <row r="28" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="81"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="85"/>
+      <c r="B28" s="134"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="119"/>
       <c r="I28" s="45" t="s">
         <v>1</v>
       </c>
@@ -32359,22 +32359,22 @@
       <c r="HR28" s="31"/>
     </row>
     <row r="29" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="83" t="s">
+      <c r="E29" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="83">
+      <c r="F29" s="101">
         <v>2</v>
       </c>
-      <c r="G29" s="84" t="s">
+      <c r="G29" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="85" t="str">
+      <c r="H29" s="119" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v>!</v>
       </c>
@@ -32454,12 +32454,12 @@
       <c r="HR29" s="4"/>
     </row>
     <row r="30" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="81"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="B30" s="134"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="119"/>
       <c r="I30" s="45" t="s">
         <v>1</v>
       </c>
@@ -32715,22 +32715,22 @@
       <c r="HR30" s="31"/>
     </row>
     <row r="31" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="82" t="s">
+      <c r="D31" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="83" t="s">
+      <c r="E31" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="83">
+      <c r="F31" s="101">
         <v>2</v>
       </c>
-      <c r="G31" s="84" t="s">
+      <c r="G31" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="85" t="str">
+      <c r="H31" s="119" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
       </c>
@@ -32802,12 +32802,12 @@
       <c r="HR31" s="4"/>
     </row>
     <row r="32" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="81"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="85"/>
+      <c r="B32" s="134"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="45" t="s">
         <v>1</v>
       </c>
@@ -33049,22 +33049,22 @@
       <c r="HR32" s="31"/>
     </row>
     <row r="33" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="134" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="82" t="s">
+      <c r="D33" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="83" t="s">
+      <c r="E33" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="83">
+      <c r="F33" s="101">
         <v>2</v>
       </c>
-      <c r="G33" s="84" t="s">
+      <c r="G33" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="85" t="str">
+      <c r="H33" s="119" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
       </c>
@@ -33140,12 +33140,12 @@
       <c r="HR33" s="4"/>
     </row>
     <row r="34" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="81"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="84"/>
-      <c r="H34" s="85"/>
+      <c r="B34" s="134"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="45" t="s">
         <v>1</v>
       </c>
@@ -33387,22 +33387,22 @@
       <c r="HR34" s="31"/>
     </row>
     <row r="35" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="81" t="s">
+      <c r="B35" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="83" t="s">
+      <c r="E35" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="83">
+      <c r="F35" s="101">
         <v>2</v>
       </c>
-      <c r="G35" s="84" t="s">
+      <c r="G35" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="85" t="str">
+      <c r="H35" s="119" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
       </c>
@@ -33481,12 +33481,12 @@
       <c r="HR35" s="4"/>
     </row>
     <row r="36" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="81"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="85"/>
+      <c r="B36" s="134"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="45" t="s">
         <v>1</v>
       </c>
@@ -33724,22 +33724,22 @@
       <c r="HR36" s="31"/>
     </row>
     <row r="37" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="81" t="s">
+      <c r="B37" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="121" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="83">
+      <c r="F37" s="101">
         <v>2</v>
       </c>
-      <c r="G37" s="84" t="s">
+      <c r="G37" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="85" t="str">
+      <c r="H37" s="119" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
       </c>
@@ -33813,12 +33813,12 @@
       <c r="HR37" s="4"/>
     </row>
     <row r="38" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="81"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="84"/>
-      <c r="H38" s="85"/>
+      <c r="B38" s="134"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="119"/>
       <c r="I38" s="45" t="s">
         <v>1</v>
       </c>
@@ -34058,20 +34058,20 @@
       <c r="HR38" s="31"/>
     </row>
     <row r="39" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="81" t="s">
+      <c r="B39" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="82" t="s">
+      <c r="D39" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83">
+      <c r="E39" s="101"/>
+      <c r="F39" s="101">
         <v>3</v>
       </c>
-      <c r="G39" s="84" t="s">
+      <c r="G39" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="85" t="str">
+      <c r="H39" s="119" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
       </c>
@@ -34152,12 +34152,12 @@
       <c r="HR39" s="4"/>
     </row>
     <row r="40" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="81"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="85"/>
+      <c r="B40" s="134"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="119"/>
       <c r="I40" s="45" t="s">
         <v>1</v>
       </c>
@@ -34405,20 +34405,20 @@
       <c r="HR40" s="31"/>
     </row>
     <row r="41" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="81" t="s">
+      <c r="B41" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="82" t="s">
+      <c r="D41" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83">
+      <c r="E41" s="101"/>
+      <c r="F41" s="101">
         <v>3</v>
       </c>
-      <c r="G41" s="84" t="s">
+      <c r="G41" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="85" t="str">
+      <c r="H41" s="119" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
       </c>
@@ -34492,12 +34492,12 @@
       <c r="HR41" s="4"/>
     </row>
     <row r="42" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="81"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="83"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="84"/>
-      <c r="H42" s="85"/>
+      <c r="B42" s="134"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="101"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="119"/>
       <c r="I42" s="45" t="s">
         <v>1</v>
       </c>
@@ -34737,20 +34737,20 @@
       <c r="HR42" s="31"/>
     </row>
     <row r="43" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="81" t="s">
+      <c r="B43" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="83"/>
-      <c r="F43" s="83">
+      <c r="E43" s="101"/>
+      <c r="F43" s="101">
         <v>3</v>
       </c>
-      <c r="G43" s="84" t="s">
+      <c r="G43" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="85" t="str">
+      <c r="H43" s="119" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
       </c>
@@ -34823,12 +34823,12 @@
       <c r="HR43" s="4"/>
     </row>
     <row r="44" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="81"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="83"/>
-      <c r="F44" s="83"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="85"/>
+      <c r="B44" s="134"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="101"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="45" t="s">
         <v>1</v>
       </c>
@@ -35070,20 +35070,20 @@
       <c r="HR44" s="31"/>
     </row>
     <row r="45" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="81" t="s">
+      <c r="B45" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="82" t="s">
+      <c r="D45" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="83"/>
-      <c r="F45" s="83">
+      <c r="E45" s="101"/>
+      <c r="F45" s="101">
         <v>3</v>
       </c>
-      <c r="G45" s="84" t="s">
+      <c r="G45" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="85" t="str">
+      <c r="H45" s="119" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
       </c>
@@ -35156,12 +35156,12 @@
       <c r="HR45" s="4"/>
     </row>
     <row r="46" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="81"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="85"/>
+      <c r="B46" s="134"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="101"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="45" t="s">
         <v>1</v>
       </c>
@@ -35403,20 +35403,20 @@
       <c r="HR46" s="31"/>
     </row>
     <row r="47" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="81" t="s">
+      <c r="B47" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="82" t="s">
+      <c r="D47" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83">
+      <c r="E47" s="101"/>
+      <c r="F47" s="101">
         <v>3</v>
       </c>
-      <c r="G47" s="84" t="s">
+      <c r="G47" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="85" t="str">
+      <c r="H47" s="119" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
       </c>
@@ -35486,12 +35486,12 @@
       <c r="HR47" s="4"/>
     </row>
     <row r="48" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="81"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="84"/>
-      <c r="H48" s="85"/>
+      <c r="B48" s="134"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="101"/>
+      <c r="F48" s="101"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="119"/>
       <c r="I48" s="45" t="s">
         <v>1</v>
       </c>
@@ -35733,20 +35733,20 @@
       <c r="HR48" s="31"/>
     </row>
     <row r="49" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="82" t="s">
+      <c r="D49" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83">
+      <c r="E49" s="101"/>
+      <c r="F49" s="101">
         <v>4</v>
       </c>
-      <c r="G49" s="84" t="s">
+      <c r="G49" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="85" t="str">
+      <c r="H49" s="119" t="str">
         <f t="shared" ref="H49" si="65">IF(O50&gt;P49,"!","")</f>
         <v/>
       </c>
@@ -35834,12 +35834,12 @@
       <c r="HR49" s="4"/>
     </row>
     <row r="50" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="81"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="85"/>
+      <c r="B50" s="134"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="101"/>
+      <c r="F50" s="101"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="119"/>
       <c r="I50" s="45" t="s">
         <v>1</v>
       </c>
@@ -36083,20 +36083,20 @@
       <c r="HR50" s="31"/>
     </row>
     <row r="51" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="81" t="s">
+      <c r="B51" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="82" t="s">
+      <c r="D51" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83">
+      <c r="E51" s="101"/>
+      <c r="F51" s="101">
         <v>4</v>
       </c>
-      <c r="G51" s="84" t="s">
+      <c r="G51" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="85" t="str">
+      <c r="H51" s="119" t="str">
         <f t="shared" ref="H51" si="71">IF(O52&gt;P51,"!","")</f>
         <v/>
       </c>
@@ -36173,12 +36173,12 @@
       <c r="HR51" s="4"/>
     </row>
     <row r="52" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="81"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="84"/>
-      <c r="H52" s="85"/>
+      <c r="B52" s="134"/>
+      <c r="D52" s="121"/>
+      <c r="E52" s="101"/>
+      <c r="F52" s="101"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="119"/>
       <c r="I52" s="45" t="s">
         <v>1</v>
       </c>
@@ -36422,20 +36422,20 @@
       <c r="HR52" s="31"/>
     </row>
     <row r="53" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="81" t="s">
+      <c r="B53" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="82" t="s">
+      <c r="D53" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="83"/>
-      <c r="F53" s="83">
+      <c r="E53" s="101"/>
+      <c r="F53" s="101">
         <v>4</v>
       </c>
-      <c r="G53" s="84" t="s">
+      <c r="G53" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H53" s="85" t="str">
+      <c r="H53" s="119" t="str">
         <f t="shared" ref="H53" si="77">IF(O54&gt;P53,"!","")</f>
         <v/>
       </c>
@@ -36515,12 +36515,12 @@
       <c r="HR53" s="4"/>
     </row>
     <row r="54" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="81"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="85"/>
+      <c r="B54" s="134"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="87"/>
+      <c r="H54" s="119"/>
       <c r="I54" s="45" t="s">
         <v>1</v>
       </c>
@@ -36760,22 +36760,22 @@
       <c r="HR54" s="31"/>
     </row>
     <row r="55" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="81" t="s">
+      <c r="B55" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="82" t="s">
+      <c r="D55" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="83" t="s">
+      <c r="E55" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="83">
+      <c r="F55" s="101">
         <v>4</v>
       </c>
-      <c r="G55" s="84" t="s">
+      <c r="G55" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H55" s="85" t="str">
+      <c r="H55" s="119" t="str">
         <f t="shared" ref="H55" si="83">IF(O56&gt;P55,"!","")</f>
         <v/>
       </c>
@@ -36858,12 +36858,12 @@
       <c r="HR55" s="4"/>
     </row>
     <row r="56" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="81"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="83"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="85"/>
+      <c r="B56" s="134"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="87"/>
+      <c r="H56" s="119"/>
       <c r="I56" s="45" t="s">
         <v>1</v>
       </c>
@@ -37105,22 +37105,22 @@
       <c r="HR56" s="31"/>
     </row>
     <row r="57" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="81" t="s">
+      <c r="B57" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="82" t="s">
+      <c r="D57" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="83" t="s">
+      <c r="E57" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="83">
+      <c r="F57" s="101">
         <v>4</v>
       </c>
-      <c r="G57" s="84" t="s">
+      <c r="G57" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H57" s="85" t="str">
+      <c r="H57" s="119" t="str">
         <f t="shared" ref="H57" si="89">IF(O58&gt;P57,"!","")</f>
         <v/>
       </c>
@@ -37191,12 +37191,12 @@
       <c r="HR57" s="4"/>
     </row>
     <row r="58" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="81"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="83"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="85"/>
+      <c r="B58" s="134"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="101"/>
+      <c r="F58" s="101"/>
+      <c r="G58" s="87"/>
+      <c r="H58" s="119"/>
       <c r="I58" s="45" t="s">
         <v>1</v>
       </c>
@@ -37440,20 +37440,20 @@
       <c r="HR58" s="31"/>
     </row>
     <row r="59" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="81" t="s">
+      <c r="B59" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="82" t="s">
+      <c r="D59" s="121" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="83"/>
-      <c r="F59" s="83">
+      <c r="E59" s="101"/>
+      <c r="F59" s="101">
         <v>5</v>
       </c>
-      <c r="G59" s="84" t="s">
+      <c r="G59" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="85" t="str">
+      <c r="H59" s="119" t="str">
         <f t="shared" ref="H59" si="95">IF(O60&gt;P59,"!","")</f>
         <v/>
       </c>
@@ -37527,12 +37527,12 @@
       <c r="HR59" s="4"/>
     </row>
     <row r="60" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="81"/>
-      <c r="D60" s="82"/>
-      <c r="E60" s="83"/>
-      <c r="F60" s="83"/>
-      <c r="G60" s="84"/>
-      <c r="H60" s="85"/>
+      <c r="B60" s="134"/>
+      <c r="D60" s="121"/>
+      <c r="E60" s="101"/>
+      <c r="F60" s="101"/>
+      <c r="G60" s="87"/>
+      <c r="H60" s="119"/>
       <c r="I60" s="45" t="s">
         <v>1</v>
       </c>
@@ -37772,18 +37772,18 @@
       <c r="HR60" s="31"/>
     </row>
     <row r="61" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="81" t="s">
+      <c r="B61" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="82" t="s">
+      <c r="D61" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="E61" s="83"/>
-      <c r="F61" s="83">
+      <c r="E61" s="101"/>
+      <c r="F61" s="101">
         <v>5</v>
       </c>
-      <c r="G61" s="84"/>
-      <c r="H61" s="85" t="str">
+      <c r="G61" s="87"/>
+      <c r="H61" s="119" t="str">
         <f t="shared" ref="H61" si="101">IF(O62&gt;P61,"!","")</f>
         <v/>
       </c>
@@ -37878,23 +37878,23 @@
       <c r="HR61" s="4"/>
     </row>
     <row r="62" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="81"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="84"/>
-      <c r="H62" s="85"/>
+      <c r="B62" s="134"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="101"/>
+      <c r="F62" s="101"/>
+      <c r="G62" s="87"/>
+      <c r="H62" s="119"/>
       <c r="I62" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J62" s="46">
         <f>IF(D61="","",COUNTIF(Echéancier!$Q62:$EP62,"r"))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K62" s="14"/>
       <c r="L62" s="14">
         <f t="shared" ref="L62" si="104">IFERROR(L60+J62,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M62" s="14">
         <f t="shared" ref="M62" si="105">COUNTIF(Q62:EP62,"a")</f>
@@ -37906,7 +37906,7 @@
       </c>
       <c r="O62" s="14">
         <f>IFERROR(MATCH("ra",$Q62:$EP62,1),0)</f>
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P62" s="14"/>
       <c r="Q62" s="23"/>
@@ -37983,13 +37983,27 @@
       <c r="CH62" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="CI62" s="25"/>
-      <c r="CJ62" s="34"/>
-      <c r="CK62" s="34"/>
-      <c r="CL62" s="75"/>
-      <c r="CM62" s="75"/>
-      <c r="CN62" s="75"/>
-      <c r="CO62" s="75"/>
+      <c r="CI62" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="CJ62" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="CK62" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="CL62" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="CM62" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="CN62" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="CO62" s="75" t="s">
+        <v>27</v>
+      </c>
       <c r="CP62" s="75"/>
       <c r="CQ62" s="34"/>
       <c r="CR62" s="24"/>
@@ -38125,18 +38139,18 @@
       <c r="HR62" s="31"/>
     </row>
     <row r="63" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="81" t="s">
+      <c r="B63" s="134" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="82" t="s">
+      <c r="D63" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="83"/>
-      <c r="F63" s="83">
+      <c r="E63" s="101"/>
+      <c r="F63" s="101">
         <v>5</v>
       </c>
-      <c r="G63" s="84"/>
-      <c r="H63" s="85" t="str">
+      <c r="G63" s="87"/>
+      <c r="H63" s="119" t="str">
         <f t="shared" ref="H63" si="107">IF(O64&gt;P63,"!","")</f>
         <v/>
       </c>
@@ -38221,12 +38235,12 @@
       <c r="HR63" s="4"/>
     </row>
     <row r="64" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="81"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="83"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="85"/>
+      <c r="B64" s="134"/>
+      <c r="D64" s="121"/>
+      <c r="E64" s="101"/>
+      <c r="F64" s="101"/>
+      <c r="G64" s="87"/>
+      <c r="H64" s="119"/>
       <c r="I64" s="45" t="s">
         <v>1</v>
       </c>
@@ -38237,7 +38251,7 @@
       <c r="K64" s="14"/>
       <c r="L64" s="14">
         <f t="shared" ref="L64" si="110">IFERROR(L62+J64,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" ref="M64" si="111">COUNTIF(Q64:EP64,"a")</f>
@@ -38464,18 +38478,18 @@
       <c r="HR64" s="31"/>
     </row>
     <row r="65" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="81" t="s">
+      <c r="B65" s="134" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="82" t="s">
+      <c r="D65" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="83"/>
-      <c r="F65" s="83">
+      <c r="E65" s="101"/>
+      <c r="F65" s="101">
         <v>6</v>
       </c>
-      <c r="G65" s="84"/>
-      <c r="H65" s="85" t="str">
+      <c r="G65" s="87"/>
+      <c r="H65" s="119" t="str">
         <f t="shared" ref="H65" si="113">IF(O66&gt;P65,"!","")</f>
         <v/>
       </c>
@@ -38553,12 +38567,12 @@
       <c r="HR65" s="4"/>
     </row>
     <row r="66" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="81"/>
-      <c r="D66" s="82"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="84"/>
-      <c r="H66" s="85"/>
+      <c r="B66" s="134"/>
+      <c r="D66" s="121"/>
+      <c r="E66" s="101"/>
+      <c r="F66" s="101"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="119"/>
       <c r="I66" s="45" t="s">
         <v>1</v>
       </c>
@@ -38569,7 +38583,7 @@
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -38796,20 +38810,20 @@
       <c r="HR66" s="31"/>
     </row>
     <row r="67" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="81" t="s">
+      <c r="B67" s="134" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="82" t="s">
+      <c r="D67" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="83" t="s">
+      <c r="E67" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="F67" s="83">
+      <c r="F67" s="101">
         <v>6</v>
       </c>
-      <c r="G67" s="84"/>
-      <c r="H67" s="85" t="str">
+      <c r="G67" s="87"/>
+      <c r="H67" s="119" t="str">
         <f t="shared" ref="H67" si="119">IF(O68&gt;P67,"!","")</f>
         <v/>
       </c>
@@ -38904,12 +38918,12 @@
       <c r="HR67" s="4"/>
     </row>
     <row r="68" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="81"/>
-      <c r="D68" s="82"/>
-      <c r="E68" s="83"/>
-      <c r="F68" s="83"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="85"/>
+      <c r="B68" s="134"/>
+      <c r="D68" s="121"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="87"/>
+      <c r="H68" s="119"/>
       <c r="I68" s="45" t="s">
         <v>1</v>
       </c>
@@ -38920,7 +38934,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -39147,20 +39161,20 @@
       <c r="HR68" s="31"/>
     </row>
     <row r="69" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="81" t="s">
+      <c r="B69" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="82" t="s">
+      <c r="D69" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="83" t="s">
+      <c r="E69" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F69" s="83">
+      <c r="F69" s="101">
         <v>6</v>
       </c>
-      <c r="G69" s="84"/>
-      <c r="H69" s="85" t="str">
+      <c r="G69" s="87"/>
+      <c r="H69" s="119" t="str">
         <f t="shared" ref="H69" si="127">IF(O70&gt;P69,"!","")</f>
         <v/>
       </c>
@@ -39237,12 +39251,12 @@
       <c r="HR69" s="4"/>
     </row>
     <row r="70" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="81"/>
-      <c r="D70" s="82"/>
-      <c r="E70" s="83"/>
-      <c r="F70" s="83"/>
-      <c r="G70" s="84"/>
-      <c r="H70" s="85"/>
+      <c r="B70" s="134"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="101"/>
+      <c r="F70" s="101"/>
+      <c r="G70" s="87"/>
+      <c r="H70" s="119"/>
       <c r="I70" s="45" t="s">
         <v>1</v>
       </c>
@@ -39253,7 +39267,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -39480,20 +39494,20 @@
       <c r="HR70" s="31"/>
     </row>
     <row r="71" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="81" t="s">
+      <c r="B71" s="134" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="82" t="s">
+      <c r="D71" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="E71" s="83" t="s">
+      <c r="E71" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F71" s="83">
+      <c r="F71" s="101">
         <v>6</v>
       </c>
-      <c r="G71" s="84"/>
-      <c r="H71" s="85" t="str">
+      <c r="G71" s="87"/>
+      <c r="H71" s="119" t="str">
         <f t="shared" ref="H71" si="133">IF(O72&gt;P71,"!","")</f>
         <v/>
       </c>
@@ -39569,12 +39583,12 @@
       <c r="HR71" s="4"/>
     </row>
     <row r="72" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="81"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="83"/>
-      <c r="F72" s="83"/>
-      <c r="G72" s="84"/>
-      <c r="H72" s="85"/>
+      <c r="B72" s="134"/>
+      <c r="D72" s="121"/>
+      <c r="E72" s="101"/>
+      <c r="F72" s="101"/>
+      <c r="G72" s="87"/>
+      <c r="H72" s="119"/>
       <c r="I72" s="45" t="s">
         <v>1</v>
       </c>
@@ -39585,7 +39599,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -39901,13 +39915,13 @@
     </row>
     <row r="73" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="82" t="s">
+      <c r="D73" s="121" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="83"/>
-      <c r="F73" s="83"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="85" t="str">
+      <c r="E73" s="101"/>
+      <c r="F73" s="101"/>
+      <c r="G73" s="87"/>
+      <c r="H73" s="119" t="str">
         <f t="shared" ref="H73" si="139">IF(O74&gt;P73,"!","")</f>
         <v/>
       </c>
@@ -39975,11 +39989,11 @@
     </row>
     <row r="74" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="D74" s="82"/>
-      <c r="E74" s="83"/>
-      <c r="F74" s="83"/>
-      <c r="G74" s="84"/>
-      <c r="H74" s="85"/>
+      <c r="D74" s="121"/>
+      <c r="E74" s="101"/>
+      <c r="F74" s="101"/>
+      <c r="G74" s="87"/>
+      <c r="H74" s="119"/>
       <c r="I74" s="45" t="s">
         <v>1</v>
       </c>
@@ -39990,7 +40004,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>
@@ -40218,13 +40232,13 @@
     </row>
     <row r="75" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="82" t="s">
+      <c r="D75" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="83"/>
-      <c r="F75" s="83"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="85" t="str">
+      <c r="E75" s="101"/>
+      <c r="F75" s="101"/>
+      <c r="G75" s="87"/>
+      <c r="H75" s="119" t="str">
         <f t="shared" ref="H75" si="145">IF(O76&gt;P75,"!","")</f>
         <v/>
       </c>
@@ -40296,11 +40310,11 @@
     </row>
     <row r="76" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
-      <c r="D76" s="82"/>
-      <c r="E76" s="83"/>
-      <c r="F76" s="83"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="85"/>
+      <c r="D76" s="121"/>
+      <c r="E76" s="101"/>
+      <c r="F76" s="101"/>
+      <c r="G76" s="87"/>
+      <c r="H76" s="119"/>
       <c r="I76" s="45" t="s">
         <v>1</v>
       </c>
@@ -40311,7 +40325,7 @@
       <c r="K76" s="14"/>
       <c r="L76" s="14">
         <f t="shared" ref="L76" si="148">IFERROR(L74+J76,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M76" s="14">
         <f t="shared" ref="M76" si="149">COUNTIF(Q76:EP76,"a")</f>
@@ -40539,13 +40553,13 @@
     </row>
     <row r="77" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
-      <c r="D77" s="82" t="s">
+      <c r="D77" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="E77" s="83"/>
-      <c r="F77" s="83"/>
-      <c r="G77" s="84"/>
-      <c r="H77" s="85" t="str">
+      <c r="E77" s="101"/>
+      <c r="F77" s="101"/>
+      <c r="G77" s="87"/>
+      <c r="H77" s="119" t="str">
         <f t="shared" ref="H77" si="151">IF(O78&gt;P77,"!","")</f>
         <v/>
       </c>
@@ -40634,11 +40648,11 @@
     </row>
     <row r="78" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="82"/>
-      <c r="E78" s="83"/>
-      <c r="F78" s="83"/>
-      <c r="G78" s="84"/>
-      <c r="H78" s="85"/>
+      <c r="D78" s="121"/>
+      <c r="E78" s="101"/>
+      <c r="F78" s="101"/>
+      <c r="G78" s="87"/>
+      <c r="H78" s="119"/>
       <c r="I78" s="45" t="s">
         <v>1</v>
       </c>
@@ -40649,7 +40663,7 @@
       <c r="K78" s="14"/>
       <c r="L78" s="14">
         <f t="shared" ref="L78" si="154">IFERROR(L76+J78,0)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M78" s="14">
         <f t="shared" ref="M78" si="155">COUNTIF(Q78:EP78,"a")</f>
@@ -40877,11 +40891,11 @@
     </row>
     <row r="79" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="D79" s="82"/>
-      <c r="E79" s="83"/>
-      <c r="F79" s="83"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="85" t="str">
+      <c r="D79" s="121"/>
+      <c r="E79" s="101"/>
+      <c r="F79" s="101"/>
+      <c r="G79" s="87"/>
+      <c r="H79" s="119" t="str">
         <f t="shared" ref="H79" si="157">IF(O80&gt;P79,"!","")</f>
         <v/>
       </c>
@@ -40950,11 +40964,11 @@
     </row>
     <row r="80" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
-      <c r="D80" s="82"/>
-      <c r="E80" s="83"/>
-      <c r="F80" s="83"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="85"/>
+      <c r="D80" s="121"/>
+      <c r="E80" s="101"/>
+      <c r="F80" s="101"/>
+      <c r="G80" s="87"/>
+      <c r="H80" s="119"/>
       <c r="I80" s="45" t="s">
         <v>1</v>
       </c>
@@ -41193,11 +41207,11 @@
     </row>
     <row r="81" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="D81" s="82"/>
-      <c r="E81" s="83"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="85" t="str">
+      <c r="D81" s="121"/>
+      <c r="E81" s="101"/>
+      <c r="F81" s="101"/>
+      <c r="G81" s="87"/>
+      <c r="H81" s="119" t="str">
         <f t="shared" ref="H81" si="163">IF(O82&gt;P81,"!","")</f>
         <v/>
       </c>
@@ -41266,11 +41280,11 @@
     </row>
     <row r="82" spans="2:226" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="70"/>
-      <c r="D82" s="86"/>
-      <c r="E82" s="87"/>
-      <c r="F82" s="87"/>
-      <c r="G82" s="88"/>
-      <c r="H82" s="89"/>
+      <c r="D82" s="130"/>
+      <c r="E82" s="131"/>
+      <c r="F82" s="131"/>
+      <c r="G82" s="132"/>
+      <c r="H82" s="133"/>
       <c r="I82" s="47" t="s">
         <v>1</v>
       </c>
@@ -41509,15 +41523,260 @@
     </row>
   </sheetData>
   <mergeCells count="287">
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="HI7:HR7"/>
+    <mergeCell ref="FA8:FJ8"/>
+    <mergeCell ref="FK8:FT8"/>
+    <mergeCell ref="FU8:GD8"/>
+    <mergeCell ref="GE8:GN8"/>
+    <mergeCell ref="GO8:GX8"/>
+    <mergeCell ref="GY8:HH8"/>
+    <mergeCell ref="HI8:HR8"/>
+    <mergeCell ref="FA9:FJ9"/>
+    <mergeCell ref="FK9:FT9"/>
+    <mergeCell ref="FU9:GD9"/>
+    <mergeCell ref="GE9:GN9"/>
+    <mergeCell ref="GO9:GX9"/>
+    <mergeCell ref="GY9:HH9"/>
+    <mergeCell ref="HI9:HR9"/>
+    <mergeCell ref="EQ7:EZ7"/>
+    <mergeCell ref="EQ8:EZ8"/>
+    <mergeCell ref="EQ9:EZ9"/>
+    <mergeCell ref="FA7:FJ7"/>
+    <mergeCell ref="FK7:FT7"/>
+    <mergeCell ref="FU7:GD7"/>
+    <mergeCell ref="GE7:GN7"/>
+    <mergeCell ref="GO7:GX7"/>
+    <mergeCell ref="GY7:HH7"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="BO7:BX7"/>
+    <mergeCell ref="EG7:EP7"/>
+    <mergeCell ref="AA8:AJ8"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AU8:BD8"/>
+    <mergeCell ref="BE8:BN8"/>
+    <mergeCell ref="BO8:BX8"/>
+    <mergeCell ref="BY8:CH8"/>
+    <mergeCell ref="CI8:CR8"/>
+    <mergeCell ref="CS8:DB8"/>
+    <mergeCell ref="DC8:DL8"/>
+    <mergeCell ref="BY7:CH7"/>
+    <mergeCell ref="CI7:CR7"/>
+    <mergeCell ref="CS7:DB7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="DW7:EF7"/>
+    <mergeCell ref="AA9:AJ9"/>
+    <mergeCell ref="AK9:AT9"/>
+    <mergeCell ref="AU9:BD9"/>
+    <mergeCell ref="BE9:BN9"/>
+    <mergeCell ref="BO9:BX9"/>
+    <mergeCell ref="EG9:EP9"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="BY9:CH9"/>
+    <mergeCell ref="CI9:CR9"/>
+    <mergeCell ref="CS9:DB9"/>
+    <mergeCell ref="DC9:DL9"/>
+    <mergeCell ref="DM9:DV9"/>
+    <mergeCell ref="DW9:EF9"/>
+    <mergeCell ref="DM8:DV8"/>
+    <mergeCell ref="DW8:EF8"/>
+    <mergeCell ref="EG8:EP8"/>
+    <mergeCell ref="AA7:AJ7"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AU7:BD7"/>
+    <mergeCell ref="BE7:BN7"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="DC7:DL7"/>
+    <mergeCell ref="DM7:DV7"/>
+    <mergeCell ref="AJ4:AR4"/>
+    <mergeCell ref="AJ5:AR5"/>
+    <mergeCell ref="AU5:BE5"/>
+    <mergeCell ref="AU4:BE4"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D19:D20"/>
@@ -41542,260 +41801,15 @@
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="AA7:AJ7"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AU7:BD7"/>
-    <mergeCell ref="BE7:BN7"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="DC7:DL7"/>
-    <mergeCell ref="DM7:DV7"/>
-    <mergeCell ref="AJ4:AR4"/>
-    <mergeCell ref="AJ5:AR5"/>
-    <mergeCell ref="AU5:BE5"/>
-    <mergeCell ref="AU4:BE4"/>
-    <mergeCell ref="BY9:CH9"/>
-    <mergeCell ref="CI9:CR9"/>
-    <mergeCell ref="CS9:DB9"/>
-    <mergeCell ref="DC9:DL9"/>
-    <mergeCell ref="DM9:DV9"/>
-    <mergeCell ref="DW9:EF9"/>
-    <mergeCell ref="DM8:DV8"/>
-    <mergeCell ref="DW8:EF8"/>
-    <mergeCell ref="EG8:EP8"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="AK9:AT9"/>
-    <mergeCell ref="AU9:BD9"/>
-    <mergeCell ref="BE9:BN9"/>
-    <mergeCell ref="BO9:BX9"/>
-    <mergeCell ref="EG9:EP9"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="FK7:FT7"/>
-    <mergeCell ref="FU7:GD7"/>
-    <mergeCell ref="GE7:GN7"/>
-    <mergeCell ref="GO7:GX7"/>
-    <mergeCell ref="GY7:HH7"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="BO7:BX7"/>
-    <mergeCell ref="EG7:EP7"/>
-    <mergeCell ref="AA8:AJ8"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AU8:BD8"/>
-    <mergeCell ref="BE8:BN8"/>
-    <mergeCell ref="BO8:BX8"/>
-    <mergeCell ref="BY8:CH8"/>
-    <mergeCell ref="CI8:CR8"/>
-    <mergeCell ref="CS8:DB8"/>
-    <mergeCell ref="DC8:DL8"/>
-    <mergeCell ref="BY7:CH7"/>
-    <mergeCell ref="CI7:CR7"/>
-    <mergeCell ref="CS7:DB7"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="DW7:EF7"/>
-    <mergeCell ref="AA9:AJ9"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="HI7:HR7"/>
-    <mergeCell ref="FA8:FJ8"/>
-    <mergeCell ref="FK8:FT8"/>
-    <mergeCell ref="FU8:GD8"/>
-    <mergeCell ref="GE8:GN8"/>
-    <mergeCell ref="GO8:GX8"/>
-    <mergeCell ref="GY8:HH8"/>
-    <mergeCell ref="HI8:HR8"/>
-    <mergeCell ref="FA9:FJ9"/>
-    <mergeCell ref="FK9:FT9"/>
-    <mergeCell ref="FU9:GD9"/>
-    <mergeCell ref="GE9:GN9"/>
-    <mergeCell ref="GO9:GX9"/>
-    <mergeCell ref="GY9:HH9"/>
-    <mergeCell ref="HI9:HR9"/>
-    <mergeCell ref="EQ7:EZ7"/>
-    <mergeCell ref="EQ8:EZ8"/>
-    <mergeCell ref="EQ9:EZ9"/>
-    <mergeCell ref="FA7:FJ7"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7:HR8">
     <cfRule type="expression" dxfId="2730" priority="3963">
@@ -52015,12 +52029,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52247,15 +52258,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
+    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -52281,18 +52304,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
-    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Focus pendant le stream fonctionnel
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E94D9C0-67EE-4552-9E48-9205DE967600}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0C9D97-86BD-4875-97DE-8688B652270B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="101">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -939,70 +939,43 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1011,7 +984,10 @@
     <xf numFmtId="14" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1020,8 +996,41 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1044,62 +1053,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -27023,7 +27023,7 @@
   <dimension ref="A1:HR82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="CN63" sqref="CN63"/>
+      <selection activeCell="CS63" sqref="CS63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27069,11 +27069,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="Q3" s="109">
+      <c r="Q3" s="112">
         <f>MAX(K13:K163)</f>
         <v>64</v>
       </c>
-      <c r="R3" s="110"/>
+      <c r="R3" s="113"/>
       <c r="S3" s="28" t="s">
         <v>23</v>
       </c>
@@ -27098,11 +27098,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="Q4" s="111">
+      <c r="Q4" s="114">
         <f>MAX(L13:L163)-L12</f>
         <v>36</v>
       </c>
-      <c r="R4" s="112"/>
+      <c r="R4" s="115"/>
       <c r="S4" s="29" t="s">
         <v>24</v>
       </c>
@@ -27119,31 +27119,31 @@
       <c r="AD4" s="26"/>
       <c r="AE4" s="27"/>
       <c r="AI4" s="66"/>
-      <c r="AJ4" s="115" t="s">
+      <c r="AJ4" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="AK4" s="115"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="115"/>
-      <c r="AN4" s="115"/>
-      <c r="AO4" s="115"/>
-      <c r="AP4" s="115"/>
-      <c r="AQ4" s="115"/>
-      <c r="AR4" s="115"/>
+      <c r="AK4" s="118"/>
+      <c r="AL4" s="118"/>
+      <c r="AM4" s="118"/>
+      <c r="AN4" s="118"/>
+      <c r="AO4" s="118"/>
+      <c r="AP4" s="118"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="118"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="115" t="s">
+      <c r="AU4" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="AV4" s="115"/>
-      <c r="AW4" s="115"/>
-      <c r="AX4" s="115"/>
-      <c r="AY4" s="115"/>
-      <c r="AZ4" s="115"/>
-      <c r="BA4" s="115"/>
-      <c r="BB4" s="115"/>
-      <c r="BC4" s="115"/>
-      <c r="BD4" s="115"/>
-      <c r="BE4" s="115"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+      <c r="AY4" s="118"/>
+      <c r="AZ4" s="118"/>
+      <c r="BA4" s="118"/>
+      <c r="BB4" s="118"/>
+      <c r="BC4" s="118"/>
+      <c r="BD4" s="118"/>
+      <c r="BE4" s="118"/>
       <c r="BG4" s="8"/>
       <c r="BH4" s="3" t="s">
         <v>2</v>
@@ -27155,11 +27155,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="Q5" s="113">
+      <c r="Q5" s="116">
         <f>MAX(M13:M163)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="114"/>
+      <c r="R5" s="117"/>
       <c r="S5" s="30" t="s">
         <v>25</v>
       </c>
@@ -27176,31 +27176,31 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="12"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="115" t="s">
+      <c r="AJ5" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="115"/>
-      <c r="AM5" s="115"/>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="118"/>
+      <c r="AM5" s="118"/>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
       <c r="AT5" s="65"/>
-      <c r="AU5" s="115" t="s">
+      <c r="AU5" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="115"/>
-      <c r="BA5" s="115"/>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="118"/>
+      <c r="AZ5" s="118"/>
+      <c r="BA5" s="118"/>
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
     </row>
     <row r="6" spans="1:226" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -27211,889 +27211,889 @@
     </row>
     <row r="7" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B7" s="69"/>
-      <c r="D7" s="123" t="s">
+      <c r="D7" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="89" t="s">
+      <c r="E7" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="127" t="s">
+      <c r="I7" s="108"/>
+      <c r="J7" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="81" t="s">
+      <c r="M7" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="81" t="s">
+      <c r="O7" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="98" t="s">
+      <c r="P7" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="95">
+      <c r="Q7" s="123">
         <v>1</v>
       </c>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="96"/>
-      <c r="U7" s="96"/>
-      <c r="V7" s="96"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="96"/>
-      <c r="Y7" s="96"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="108">
+      <c r="R7" s="91"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="91"/>
+      <c r="U7" s="91"/>
+      <c r="V7" s="91"/>
+      <c r="W7" s="91"/>
+      <c r="X7" s="91"/>
+      <c r="Y7" s="91"/>
+      <c r="Z7" s="101"/>
+      <c r="AA7" s="90">
         <v>2</v>
       </c>
-      <c r="AB7" s="96"/>
-      <c r="AC7" s="96"/>
-      <c r="AD7" s="96"/>
-      <c r="AE7" s="96"/>
-      <c r="AF7" s="96"/>
-      <c r="AG7" s="96"/>
-      <c r="AH7" s="96"/>
-      <c r="AI7" s="96"/>
-      <c r="AJ7" s="97"/>
-      <c r="AK7" s="108">
+      <c r="AB7" s="91"/>
+      <c r="AC7" s="91"/>
+      <c r="AD7" s="91"/>
+      <c r="AE7" s="91"/>
+      <c r="AF7" s="91"/>
+      <c r="AG7" s="91"/>
+      <c r="AH7" s="91"/>
+      <c r="AI7" s="91"/>
+      <c r="AJ7" s="101"/>
+      <c r="AK7" s="90">
         <v>3</v>
       </c>
-      <c r="AL7" s="96"/>
-      <c r="AM7" s="96"/>
-      <c r="AN7" s="96"/>
-      <c r="AO7" s="96"/>
-      <c r="AP7" s="96"/>
-      <c r="AQ7" s="96"/>
-      <c r="AR7" s="96"/>
-      <c r="AS7" s="96"/>
-      <c r="AT7" s="97"/>
-      <c r="AU7" s="108">
+      <c r="AL7" s="91"/>
+      <c r="AM7" s="91"/>
+      <c r="AN7" s="91"/>
+      <c r="AO7" s="91"/>
+      <c r="AP7" s="91"/>
+      <c r="AQ7" s="91"/>
+      <c r="AR7" s="91"/>
+      <c r="AS7" s="91"/>
+      <c r="AT7" s="101"/>
+      <c r="AU7" s="90">
         <v>4</v>
       </c>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="96"/>
-      <c r="AX7" s="96"/>
-      <c r="AY7" s="96"/>
-      <c r="AZ7" s="96"/>
-      <c r="BA7" s="96"/>
-      <c r="BB7" s="96"/>
-      <c r="BC7" s="96"/>
-      <c r="BD7" s="97"/>
-      <c r="BE7" s="108">
+      <c r="AV7" s="91"/>
+      <c r="AW7" s="91"/>
+      <c r="AX7" s="91"/>
+      <c r="AY7" s="91"/>
+      <c r="AZ7" s="91"/>
+      <c r="BA7" s="91"/>
+      <c r="BB7" s="91"/>
+      <c r="BC7" s="91"/>
+      <c r="BD7" s="101"/>
+      <c r="BE7" s="90">
         <v>5</v>
       </c>
-      <c r="BF7" s="96"/>
-      <c r="BG7" s="96"/>
-      <c r="BH7" s="96"/>
-      <c r="BI7" s="96"/>
-      <c r="BJ7" s="96"/>
-      <c r="BK7" s="96"/>
-      <c r="BL7" s="96"/>
-      <c r="BM7" s="96"/>
-      <c r="BN7" s="97"/>
-      <c r="BO7" s="108">
+      <c r="BF7" s="91"/>
+      <c r="BG7" s="91"/>
+      <c r="BH7" s="91"/>
+      <c r="BI7" s="91"/>
+      <c r="BJ7" s="91"/>
+      <c r="BK7" s="91"/>
+      <c r="BL7" s="91"/>
+      <c r="BM7" s="91"/>
+      <c r="BN7" s="101"/>
+      <c r="BO7" s="90">
         <v>6</v>
       </c>
-      <c r="BP7" s="96"/>
-      <c r="BQ7" s="96"/>
-      <c r="BR7" s="96"/>
-      <c r="BS7" s="96"/>
-      <c r="BT7" s="96"/>
-      <c r="BU7" s="96"/>
-      <c r="BV7" s="96"/>
-      <c r="BW7" s="96"/>
-      <c r="BX7" s="97"/>
-      <c r="BY7" s="108">
+      <c r="BP7" s="91"/>
+      <c r="BQ7" s="91"/>
+      <c r="BR7" s="91"/>
+      <c r="BS7" s="91"/>
+      <c r="BT7" s="91"/>
+      <c r="BU7" s="91"/>
+      <c r="BV7" s="91"/>
+      <c r="BW7" s="91"/>
+      <c r="BX7" s="101"/>
+      <c r="BY7" s="90">
         <v>7</v>
       </c>
-      <c r="BZ7" s="96"/>
-      <c r="CA7" s="96"/>
-      <c r="CB7" s="96"/>
-      <c r="CC7" s="96"/>
-      <c r="CD7" s="96"/>
-      <c r="CE7" s="96"/>
-      <c r="CF7" s="96"/>
-      <c r="CG7" s="96"/>
-      <c r="CH7" s="97"/>
-      <c r="CI7" s="108">
+      <c r="BZ7" s="91"/>
+      <c r="CA7" s="91"/>
+      <c r="CB7" s="91"/>
+      <c r="CC7" s="91"/>
+      <c r="CD7" s="91"/>
+      <c r="CE7" s="91"/>
+      <c r="CF7" s="91"/>
+      <c r="CG7" s="91"/>
+      <c r="CH7" s="101"/>
+      <c r="CI7" s="90">
         <v>8</v>
       </c>
-      <c r="CJ7" s="96"/>
-      <c r="CK7" s="96"/>
-      <c r="CL7" s="96"/>
-      <c r="CM7" s="96"/>
-      <c r="CN7" s="96"/>
-      <c r="CO7" s="96"/>
-      <c r="CP7" s="96"/>
-      <c r="CQ7" s="96"/>
-      <c r="CR7" s="97"/>
-      <c r="CS7" s="108">
+      <c r="CJ7" s="91"/>
+      <c r="CK7" s="91"/>
+      <c r="CL7" s="91"/>
+      <c r="CM7" s="91"/>
+      <c r="CN7" s="91"/>
+      <c r="CO7" s="91"/>
+      <c r="CP7" s="91"/>
+      <c r="CQ7" s="91"/>
+      <c r="CR7" s="101"/>
+      <c r="CS7" s="90">
         <v>9</v>
       </c>
-      <c r="CT7" s="96"/>
-      <c r="CU7" s="96"/>
-      <c r="CV7" s="96"/>
-      <c r="CW7" s="96"/>
-      <c r="CX7" s="96"/>
-      <c r="CY7" s="96"/>
-      <c r="CZ7" s="96"/>
-      <c r="DA7" s="96"/>
-      <c r="DB7" s="96"/>
-      <c r="DC7" s="108">
+      <c r="CT7" s="91"/>
+      <c r="CU7" s="91"/>
+      <c r="CV7" s="91"/>
+      <c r="CW7" s="91"/>
+      <c r="CX7" s="91"/>
+      <c r="CY7" s="91"/>
+      <c r="CZ7" s="91"/>
+      <c r="DA7" s="91"/>
+      <c r="DB7" s="91"/>
+      <c r="DC7" s="90">
         <v>10</v>
       </c>
-      <c r="DD7" s="96"/>
-      <c r="DE7" s="96"/>
-      <c r="DF7" s="96"/>
-      <c r="DG7" s="96"/>
-      <c r="DH7" s="96"/>
-      <c r="DI7" s="96"/>
-      <c r="DJ7" s="96"/>
-      <c r="DK7" s="96"/>
-      <c r="DL7" s="97"/>
-      <c r="DM7" s="108">
+      <c r="DD7" s="91"/>
+      <c r="DE7" s="91"/>
+      <c r="DF7" s="91"/>
+      <c r="DG7" s="91"/>
+      <c r="DH7" s="91"/>
+      <c r="DI7" s="91"/>
+      <c r="DJ7" s="91"/>
+      <c r="DK7" s="91"/>
+      <c r="DL7" s="101"/>
+      <c r="DM7" s="90">
         <v>11</v>
       </c>
-      <c r="DN7" s="96"/>
-      <c r="DO7" s="96"/>
-      <c r="DP7" s="96"/>
-      <c r="DQ7" s="96"/>
-      <c r="DR7" s="96"/>
-      <c r="DS7" s="96"/>
-      <c r="DT7" s="96"/>
-      <c r="DU7" s="96"/>
-      <c r="DV7" s="97"/>
-      <c r="DW7" s="108">
+      <c r="DN7" s="91"/>
+      <c r="DO7" s="91"/>
+      <c r="DP7" s="91"/>
+      <c r="DQ7" s="91"/>
+      <c r="DR7" s="91"/>
+      <c r="DS7" s="91"/>
+      <c r="DT7" s="91"/>
+      <c r="DU7" s="91"/>
+      <c r="DV7" s="101"/>
+      <c r="DW7" s="90">
         <v>12</v>
       </c>
-      <c r="DX7" s="96"/>
-      <c r="DY7" s="96"/>
-      <c r="DZ7" s="96"/>
-      <c r="EA7" s="96"/>
-      <c r="EB7" s="96"/>
-      <c r="EC7" s="96"/>
-      <c r="ED7" s="96"/>
-      <c r="EE7" s="96"/>
-      <c r="EF7" s="97"/>
-      <c r="EG7" s="108">
+      <c r="DX7" s="91"/>
+      <c r="DY7" s="91"/>
+      <c r="DZ7" s="91"/>
+      <c r="EA7" s="91"/>
+      <c r="EB7" s="91"/>
+      <c r="EC7" s="91"/>
+      <c r="ED7" s="91"/>
+      <c r="EE7" s="91"/>
+      <c r="EF7" s="101"/>
+      <c r="EG7" s="90">
         <v>13</v>
       </c>
-      <c r="EH7" s="96"/>
-      <c r="EI7" s="96"/>
-      <c r="EJ7" s="96"/>
-      <c r="EK7" s="96"/>
-      <c r="EL7" s="96"/>
-      <c r="EM7" s="96"/>
-      <c r="EN7" s="96"/>
-      <c r="EO7" s="96"/>
-      <c r="EP7" s="126"/>
-      <c r="EQ7" s="96">
+      <c r="EH7" s="91"/>
+      <c r="EI7" s="91"/>
+      <c r="EJ7" s="91"/>
+      <c r="EK7" s="91"/>
+      <c r="EL7" s="91"/>
+      <c r="EM7" s="91"/>
+      <c r="EN7" s="91"/>
+      <c r="EO7" s="91"/>
+      <c r="EP7" s="92"/>
+      <c r="EQ7" s="91">
         <v>14</v>
       </c>
-      <c r="ER7" s="96"/>
-      <c r="ES7" s="96"/>
-      <c r="ET7" s="96"/>
-      <c r="EU7" s="96"/>
-      <c r="EV7" s="96"/>
-      <c r="EW7" s="96"/>
-      <c r="EX7" s="96"/>
-      <c r="EY7" s="96"/>
-      <c r="EZ7" s="97"/>
-      <c r="FA7" s="108">
+      <c r="ER7" s="91"/>
+      <c r="ES7" s="91"/>
+      <c r="ET7" s="91"/>
+      <c r="EU7" s="91"/>
+      <c r="EV7" s="91"/>
+      <c r="EW7" s="91"/>
+      <c r="EX7" s="91"/>
+      <c r="EY7" s="91"/>
+      <c r="EZ7" s="101"/>
+      <c r="FA7" s="90">
         <v>15</v>
       </c>
-      <c r="FB7" s="96"/>
-      <c r="FC7" s="96"/>
-      <c r="FD7" s="96"/>
-      <c r="FE7" s="96"/>
-      <c r="FF7" s="96"/>
-      <c r="FG7" s="96"/>
-      <c r="FH7" s="96"/>
-      <c r="FI7" s="96"/>
-      <c r="FJ7" s="97"/>
-      <c r="FK7" s="108">
+      <c r="FB7" s="91"/>
+      <c r="FC7" s="91"/>
+      <c r="FD7" s="91"/>
+      <c r="FE7" s="91"/>
+      <c r="FF7" s="91"/>
+      <c r="FG7" s="91"/>
+      <c r="FH7" s="91"/>
+      <c r="FI7" s="91"/>
+      <c r="FJ7" s="101"/>
+      <c r="FK7" s="90">
         <v>16</v>
       </c>
-      <c r="FL7" s="96"/>
-      <c r="FM7" s="96"/>
-      <c r="FN7" s="96"/>
-      <c r="FO7" s="96"/>
-      <c r="FP7" s="96"/>
-      <c r="FQ7" s="96"/>
-      <c r="FR7" s="96"/>
-      <c r="FS7" s="96"/>
-      <c r="FT7" s="97"/>
-      <c r="FU7" s="108">
+      <c r="FL7" s="91"/>
+      <c r="FM7" s="91"/>
+      <c r="FN7" s="91"/>
+      <c r="FO7" s="91"/>
+      <c r="FP7" s="91"/>
+      <c r="FQ7" s="91"/>
+      <c r="FR7" s="91"/>
+      <c r="FS7" s="91"/>
+      <c r="FT7" s="101"/>
+      <c r="FU7" s="90">
         <v>17</v>
       </c>
-      <c r="FV7" s="96"/>
-      <c r="FW7" s="96"/>
-      <c r="FX7" s="96"/>
-      <c r="FY7" s="96"/>
-      <c r="FZ7" s="96"/>
-      <c r="GA7" s="96"/>
-      <c r="GB7" s="96"/>
-      <c r="GC7" s="96"/>
-      <c r="GD7" s="97"/>
-      <c r="GE7" s="108">
+      <c r="FV7" s="91"/>
+      <c r="FW7" s="91"/>
+      <c r="FX7" s="91"/>
+      <c r="FY7" s="91"/>
+      <c r="FZ7" s="91"/>
+      <c r="GA7" s="91"/>
+      <c r="GB7" s="91"/>
+      <c r="GC7" s="91"/>
+      <c r="GD7" s="101"/>
+      <c r="GE7" s="90">
         <v>18</v>
       </c>
-      <c r="GF7" s="96"/>
-      <c r="GG7" s="96"/>
-      <c r="GH7" s="96"/>
-      <c r="GI7" s="96"/>
-      <c r="GJ7" s="96"/>
-      <c r="GK7" s="96"/>
-      <c r="GL7" s="96"/>
-      <c r="GM7" s="96"/>
-      <c r="GN7" s="97"/>
-      <c r="GO7" s="108">
+      <c r="GF7" s="91"/>
+      <c r="GG7" s="91"/>
+      <c r="GH7" s="91"/>
+      <c r="GI7" s="91"/>
+      <c r="GJ7" s="91"/>
+      <c r="GK7" s="91"/>
+      <c r="GL7" s="91"/>
+      <c r="GM7" s="91"/>
+      <c r="GN7" s="101"/>
+      <c r="GO7" s="90">
         <v>19</v>
       </c>
-      <c r="GP7" s="96"/>
-      <c r="GQ7" s="96"/>
-      <c r="GR7" s="96"/>
-      <c r="GS7" s="96"/>
-      <c r="GT7" s="96"/>
-      <c r="GU7" s="96"/>
-      <c r="GV7" s="96"/>
-      <c r="GW7" s="96"/>
-      <c r="GX7" s="97"/>
-      <c r="GY7" s="108">
+      <c r="GP7" s="91"/>
+      <c r="GQ7" s="91"/>
+      <c r="GR7" s="91"/>
+      <c r="GS7" s="91"/>
+      <c r="GT7" s="91"/>
+      <c r="GU7" s="91"/>
+      <c r="GV7" s="91"/>
+      <c r="GW7" s="91"/>
+      <c r="GX7" s="101"/>
+      <c r="GY7" s="90">
         <v>20</v>
       </c>
-      <c r="GZ7" s="96"/>
-      <c r="HA7" s="96"/>
-      <c r="HB7" s="96"/>
-      <c r="HC7" s="96"/>
-      <c r="HD7" s="96"/>
-      <c r="HE7" s="96"/>
-      <c r="HF7" s="96"/>
-      <c r="HG7" s="96"/>
-      <c r="HH7" s="97"/>
-      <c r="HI7" s="108">
+      <c r="GZ7" s="91"/>
+      <c r="HA7" s="91"/>
+      <c r="HB7" s="91"/>
+      <c r="HC7" s="91"/>
+      <c r="HD7" s="91"/>
+      <c r="HE7" s="91"/>
+      <c r="HF7" s="91"/>
+      <c r="HG7" s="91"/>
+      <c r="HH7" s="101"/>
+      <c r="HI7" s="90">
         <v>21</v>
       </c>
-      <c r="HJ7" s="96"/>
-      <c r="HK7" s="96"/>
-      <c r="HL7" s="96"/>
-      <c r="HM7" s="96"/>
-      <c r="HN7" s="96"/>
-      <c r="HO7" s="96"/>
-      <c r="HP7" s="96"/>
-      <c r="HQ7" s="96"/>
-      <c r="HR7" s="126"/>
+      <c r="HJ7" s="91"/>
+      <c r="HK7" s="91"/>
+      <c r="HL7" s="91"/>
+      <c r="HM7" s="91"/>
+      <c r="HN7" s="91"/>
+      <c r="HO7" s="91"/>
+      <c r="HP7" s="91"/>
+      <c r="HQ7" s="91"/>
+      <c r="HR7" s="92"/>
     </row>
     <row r="8" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="128"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="102">
+      <c r="D8" s="103"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="128"/>
+      <c r="N8" s="128"/>
+      <c r="O8" s="128"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="130">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],Q7),"")</f>
         <v>45040</v>
       </c>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="103"/>
-      <c r="Z8" s="104"/>
-      <c r="AA8" s="117">
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="94"/>
+      <c r="U8" s="94"/>
+      <c r="V8" s="94"/>
+      <c r="W8" s="94"/>
+      <c r="X8" s="94"/>
+      <c r="Y8" s="94"/>
+      <c r="Z8" s="95"/>
+      <c r="AA8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AA7),"")</f>
         <v>45041</v>
       </c>
-      <c r="AB8" s="103"/>
-      <c r="AC8" s="103"/>
-      <c r="AD8" s="103"/>
-      <c r="AE8" s="103"/>
-      <c r="AF8" s="103"/>
-      <c r="AG8" s="103"/>
-      <c r="AH8" s="103"/>
-      <c r="AI8" s="103"/>
-      <c r="AJ8" s="104"/>
-      <c r="AK8" s="117">
+      <c r="AB8" s="94"/>
+      <c r="AC8" s="94"/>
+      <c r="AD8" s="94"/>
+      <c r="AE8" s="94"/>
+      <c r="AF8" s="94"/>
+      <c r="AG8" s="94"/>
+      <c r="AH8" s="94"/>
+      <c r="AI8" s="94"/>
+      <c r="AJ8" s="95"/>
+      <c r="AK8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AK7),"")</f>
         <v>45042</v>
       </c>
-      <c r="AL8" s="103"/>
-      <c r="AM8" s="103"/>
-      <c r="AN8" s="103"/>
-      <c r="AO8" s="103"/>
-      <c r="AP8" s="103"/>
-      <c r="AQ8" s="103"/>
-      <c r="AR8" s="103"/>
-      <c r="AS8" s="103"/>
-      <c r="AT8" s="104"/>
-      <c r="AU8" s="117">
+      <c r="AL8" s="94"/>
+      <c r="AM8" s="94"/>
+      <c r="AN8" s="94"/>
+      <c r="AO8" s="94"/>
+      <c r="AP8" s="94"/>
+      <c r="AQ8" s="94"/>
+      <c r="AR8" s="94"/>
+      <c r="AS8" s="94"/>
+      <c r="AT8" s="95"/>
+      <c r="AU8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AU7),"")</f>
         <v>45048</v>
       </c>
-      <c r="AV8" s="103"/>
-      <c r="AW8" s="103"/>
-      <c r="AX8" s="103"/>
-      <c r="AY8" s="103"/>
-      <c r="AZ8" s="103"/>
-      <c r="BA8" s="103"/>
-      <c r="BB8" s="103"/>
-      <c r="BC8" s="103"/>
-      <c r="BD8" s="104"/>
-      <c r="BE8" s="117">
+      <c r="AV8" s="94"/>
+      <c r="AW8" s="94"/>
+      <c r="AX8" s="94"/>
+      <c r="AY8" s="94"/>
+      <c r="AZ8" s="94"/>
+      <c r="BA8" s="94"/>
+      <c r="BB8" s="94"/>
+      <c r="BC8" s="94"/>
+      <c r="BD8" s="95"/>
+      <c r="BE8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BE7),"")</f>
         <v>45049</v>
       </c>
-      <c r="BF8" s="103"/>
-      <c r="BG8" s="103"/>
-      <c r="BH8" s="103"/>
-      <c r="BI8" s="103"/>
-      <c r="BJ8" s="103"/>
-      <c r="BK8" s="103"/>
-      <c r="BL8" s="103"/>
-      <c r="BM8" s="103"/>
-      <c r="BN8" s="104"/>
-      <c r="BO8" s="117">
+      <c r="BF8" s="94"/>
+      <c r="BG8" s="94"/>
+      <c r="BH8" s="94"/>
+      <c r="BI8" s="94"/>
+      <c r="BJ8" s="94"/>
+      <c r="BK8" s="94"/>
+      <c r="BL8" s="94"/>
+      <c r="BM8" s="94"/>
+      <c r="BN8" s="95"/>
+      <c r="BO8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BO7),"")</f>
         <v>45054</v>
       </c>
-      <c r="BP8" s="103"/>
-      <c r="BQ8" s="103"/>
-      <c r="BR8" s="103"/>
-      <c r="BS8" s="103"/>
-      <c r="BT8" s="103"/>
-      <c r="BU8" s="103"/>
-      <c r="BV8" s="103"/>
-      <c r="BW8" s="103"/>
-      <c r="BX8" s="104"/>
-      <c r="BY8" s="117">
+      <c r="BP8" s="94"/>
+      <c r="BQ8" s="94"/>
+      <c r="BR8" s="94"/>
+      <c r="BS8" s="94"/>
+      <c r="BT8" s="94"/>
+      <c r="BU8" s="94"/>
+      <c r="BV8" s="94"/>
+      <c r="BW8" s="94"/>
+      <c r="BX8" s="95"/>
+      <c r="BY8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BY7),"")</f>
         <v>45055</v>
       </c>
-      <c r="BZ8" s="103"/>
-      <c r="CA8" s="103"/>
-      <c r="CB8" s="103"/>
-      <c r="CC8" s="103"/>
-      <c r="CD8" s="103"/>
-      <c r="CE8" s="103"/>
-      <c r="CF8" s="103"/>
-      <c r="CG8" s="103"/>
-      <c r="CH8" s="104"/>
-      <c r="CI8" s="117">
+      <c r="BZ8" s="94"/>
+      <c r="CA8" s="94"/>
+      <c r="CB8" s="94"/>
+      <c r="CC8" s="94"/>
+      <c r="CD8" s="94"/>
+      <c r="CE8" s="94"/>
+      <c r="CF8" s="94"/>
+      <c r="CG8" s="94"/>
+      <c r="CH8" s="95"/>
+      <c r="CI8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CI7),"")</f>
         <v>45056</v>
       </c>
-      <c r="CJ8" s="103"/>
-      <c r="CK8" s="103"/>
-      <c r="CL8" s="103"/>
-      <c r="CM8" s="103"/>
-      <c r="CN8" s="103"/>
-      <c r="CO8" s="103"/>
-      <c r="CP8" s="103"/>
-      <c r="CQ8" s="103"/>
-      <c r="CR8" s="104"/>
-      <c r="CS8" s="117">
+      <c r="CJ8" s="94"/>
+      <c r="CK8" s="94"/>
+      <c r="CL8" s="94"/>
+      <c r="CM8" s="94"/>
+      <c r="CN8" s="94"/>
+      <c r="CO8" s="94"/>
+      <c r="CP8" s="94"/>
+      <c r="CQ8" s="94"/>
+      <c r="CR8" s="95"/>
+      <c r="CS8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CS7),"")</f>
         <v>45061</v>
       </c>
-      <c r="CT8" s="103"/>
-      <c r="CU8" s="103"/>
-      <c r="CV8" s="103"/>
-      <c r="CW8" s="103"/>
-      <c r="CX8" s="103"/>
-      <c r="CY8" s="103"/>
-      <c r="CZ8" s="103"/>
-      <c r="DA8" s="103"/>
-      <c r="DB8" s="103"/>
-      <c r="DC8" s="117">
+      <c r="CT8" s="94"/>
+      <c r="CU8" s="94"/>
+      <c r="CV8" s="94"/>
+      <c r="CW8" s="94"/>
+      <c r="CX8" s="94"/>
+      <c r="CY8" s="94"/>
+      <c r="CZ8" s="94"/>
+      <c r="DA8" s="94"/>
+      <c r="DB8" s="94"/>
+      <c r="DC8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DC7),"")</f>
         <v>45062</v>
       </c>
-      <c r="DD8" s="103"/>
-      <c r="DE8" s="103"/>
-      <c r="DF8" s="103"/>
-      <c r="DG8" s="103"/>
-      <c r="DH8" s="103"/>
-      <c r="DI8" s="103"/>
-      <c r="DJ8" s="103"/>
-      <c r="DK8" s="103"/>
-      <c r="DL8" s="104"/>
-      <c r="DM8" s="117">
+      <c r="DD8" s="94"/>
+      <c r="DE8" s="94"/>
+      <c r="DF8" s="94"/>
+      <c r="DG8" s="94"/>
+      <c r="DH8" s="94"/>
+      <c r="DI8" s="94"/>
+      <c r="DJ8" s="94"/>
+      <c r="DK8" s="94"/>
+      <c r="DL8" s="95"/>
+      <c r="DM8" s="93">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DM7),"")</f>
         <v>45063</v>
       </c>
-      <c r="DN8" s="103"/>
-      <c r="DO8" s="103"/>
-      <c r="DP8" s="103"/>
-      <c r="DQ8" s="103"/>
-      <c r="DR8" s="103"/>
-      <c r="DS8" s="103"/>
-      <c r="DT8" s="103"/>
-      <c r="DU8" s="103"/>
-      <c r="DV8" s="104"/>
-      <c r="DW8" s="117" t="str">
+      <c r="DN8" s="94"/>
+      <c r="DO8" s="94"/>
+      <c r="DP8" s="94"/>
+      <c r="DQ8" s="94"/>
+      <c r="DR8" s="94"/>
+      <c r="DS8" s="94"/>
+      <c r="DT8" s="94"/>
+      <c r="DU8" s="94"/>
+      <c r="DV8" s="95"/>
+      <c r="DW8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DW7),"")</f>
         <v/>
       </c>
-      <c r="DX8" s="103"/>
-      <c r="DY8" s="103"/>
-      <c r="DZ8" s="103"/>
-      <c r="EA8" s="103"/>
-      <c r="EB8" s="103"/>
-      <c r="EC8" s="103"/>
-      <c r="ED8" s="103"/>
-      <c r="EE8" s="103"/>
-      <c r="EF8" s="104"/>
-      <c r="EG8" s="117" t="str">
+      <c r="DX8" s="94"/>
+      <c r="DY8" s="94"/>
+      <c r="DZ8" s="94"/>
+      <c r="EA8" s="94"/>
+      <c r="EB8" s="94"/>
+      <c r="EC8" s="94"/>
+      <c r="ED8" s="94"/>
+      <c r="EE8" s="94"/>
+      <c r="EF8" s="95"/>
+      <c r="EG8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EG7),"")</f>
         <v/>
       </c>
-      <c r="EH8" s="103"/>
-      <c r="EI8" s="103"/>
-      <c r="EJ8" s="103"/>
-      <c r="EK8" s="103"/>
-      <c r="EL8" s="103"/>
-      <c r="EM8" s="103"/>
-      <c r="EN8" s="103"/>
-      <c r="EO8" s="103"/>
-      <c r="EP8" s="118"/>
-      <c r="EQ8" s="103" t="str">
+      <c r="EH8" s="94"/>
+      <c r="EI8" s="94"/>
+      <c r="EJ8" s="94"/>
+      <c r="EK8" s="94"/>
+      <c r="EL8" s="94"/>
+      <c r="EM8" s="94"/>
+      <c r="EN8" s="94"/>
+      <c r="EO8" s="94"/>
+      <c r="EP8" s="96"/>
+      <c r="EQ8" s="94" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EQ7),"")</f>
         <v/>
       </c>
-      <c r="ER8" s="103"/>
-      <c r="ES8" s="103"/>
-      <c r="ET8" s="103"/>
-      <c r="EU8" s="103"/>
-      <c r="EV8" s="103"/>
-      <c r="EW8" s="103"/>
-      <c r="EX8" s="103"/>
-      <c r="EY8" s="103"/>
-      <c r="EZ8" s="104"/>
-      <c r="FA8" s="117" t="str">
+      <c r="ER8" s="94"/>
+      <c r="ES8" s="94"/>
+      <c r="ET8" s="94"/>
+      <c r="EU8" s="94"/>
+      <c r="EV8" s="94"/>
+      <c r="EW8" s="94"/>
+      <c r="EX8" s="94"/>
+      <c r="EY8" s="94"/>
+      <c r="EZ8" s="95"/>
+      <c r="FA8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FA7),"")</f>
         <v/>
       </c>
-      <c r="FB8" s="103"/>
-      <c r="FC8" s="103"/>
-      <c r="FD8" s="103"/>
-      <c r="FE8" s="103"/>
-      <c r="FF8" s="103"/>
-      <c r="FG8" s="103"/>
-      <c r="FH8" s="103"/>
-      <c r="FI8" s="103"/>
-      <c r="FJ8" s="104"/>
-      <c r="FK8" s="117" t="str">
+      <c r="FB8" s="94"/>
+      <c r="FC8" s="94"/>
+      <c r="FD8" s="94"/>
+      <c r="FE8" s="94"/>
+      <c r="FF8" s="94"/>
+      <c r="FG8" s="94"/>
+      <c r="FH8" s="94"/>
+      <c r="FI8" s="94"/>
+      <c r="FJ8" s="95"/>
+      <c r="FK8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FK7),"")</f>
         <v/>
       </c>
-      <c r="FL8" s="103"/>
-      <c r="FM8" s="103"/>
-      <c r="FN8" s="103"/>
-      <c r="FO8" s="103"/>
-      <c r="FP8" s="103"/>
-      <c r="FQ8" s="103"/>
-      <c r="FR8" s="103"/>
-      <c r="FS8" s="103"/>
-      <c r="FT8" s="104"/>
-      <c r="FU8" s="117" t="str">
+      <c r="FL8" s="94"/>
+      <c r="FM8" s="94"/>
+      <c r="FN8" s="94"/>
+      <c r="FO8" s="94"/>
+      <c r="FP8" s="94"/>
+      <c r="FQ8" s="94"/>
+      <c r="FR8" s="94"/>
+      <c r="FS8" s="94"/>
+      <c r="FT8" s="95"/>
+      <c r="FU8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FU7),"")</f>
         <v/>
       </c>
-      <c r="FV8" s="103"/>
-      <c r="FW8" s="103"/>
-      <c r="FX8" s="103"/>
-      <c r="FY8" s="103"/>
-      <c r="FZ8" s="103"/>
-      <c r="GA8" s="103"/>
-      <c r="GB8" s="103"/>
-      <c r="GC8" s="103"/>
-      <c r="GD8" s="104"/>
-      <c r="GE8" s="117" t="str">
+      <c r="FV8" s="94"/>
+      <c r="FW8" s="94"/>
+      <c r="FX8" s="94"/>
+      <c r="FY8" s="94"/>
+      <c r="FZ8" s="94"/>
+      <c r="GA8" s="94"/>
+      <c r="GB8" s="94"/>
+      <c r="GC8" s="94"/>
+      <c r="GD8" s="95"/>
+      <c r="GE8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GE7),"")</f>
         <v/>
       </c>
-      <c r="GF8" s="103"/>
-      <c r="GG8" s="103"/>
-      <c r="GH8" s="103"/>
-      <c r="GI8" s="103"/>
-      <c r="GJ8" s="103"/>
-      <c r="GK8" s="103"/>
-      <c r="GL8" s="103"/>
-      <c r="GM8" s="103"/>
-      <c r="GN8" s="104"/>
-      <c r="GO8" s="117" t="str">
+      <c r="GF8" s="94"/>
+      <c r="GG8" s="94"/>
+      <c r="GH8" s="94"/>
+      <c r="GI8" s="94"/>
+      <c r="GJ8" s="94"/>
+      <c r="GK8" s="94"/>
+      <c r="GL8" s="94"/>
+      <c r="GM8" s="94"/>
+      <c r="GN8" s="95"/>
+      <c r="GO8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GO7),"")</f>
         <v/>
       </c>
-      <c r="GP8" s="103"/>
-      <c r="GQ8" s="103"/>
-      <c r="GR8" s="103"/>
-      <c r="GS8" s="103"/>
-      <c r="GT8" s="103"/>
-      <c r="GU8" s="103"/>
-      <c r="GV8" s="103"/>
-      <c r="GW8" s="103"/>
-      <c r="GX8" s="104"/>
-      <c r="GY8" s="117" t="str">
+      <c r="GP8" s="94"/>
+      <c r="GQ8" s="94"/>
+      <c r="GR8" s="94"/>
+      <c r="GS8" s="94"/>
+      <c r="GT8" s="94"/>
+      <c r="GU8" s="94"/>
+      <c r="GV8" s="94"/>
+      <c r="GW8" s="94"/>
+      <c r="GX8" s="95"/>
+      <c r="GY8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GY7),"")</f>
         <v/>
       </c>
-      <c r="GZ8" s="103"/>
-      <c r="HA8" s="103"/>
-      <c r="HB8" s="103"/>
-      <c r="HC8" s="103"/>
-      <c r="HD8" s="103"/>
-      <c r="HE8" s="103"/>
-      <c r="HF8" s="103"/>
-      <c r="HG8" s="103"/>
-      <c r="HH8" s="104"/>
-      <c r="HI8" s="117" t="str">
+      <c r="GZ8" s="94"/>
+      <c r="HA8" s="94"/>
+      <c r="HB8" s="94"/>
+      <c r="HC8" s="94"/>
+      <c r="HD8" s="94"/>
+      <c r="HE8" s="94"/>
+      <c r="HF8" s="94"/>
+      <c r="HG8" s="94"/>
+      <c r="HH8" s="95"/>
+      <c r="HI8" s="93" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],HI7),"")</f>
         <v/>
       </c>
-      <c r="HJ8" s="103"/>
-      <c r="HK8" s="103"/>
-      <c r="HL8" s="103"/>
-      <c r="HM8" s="103"/>
-      <c r="HN8" s="103"/>
-      <c r="HO8" s="103"/>
-      <c r="HP8" s="103"/>
-      <c r="HQ8" s="103"/>
-      <c r="HR8" s="118"/>
+      <c r="HJ8" s="94"/>
+      <c r="HK8" s="94"/>
+      <c r="HL8" s="94"/>
+      <c r="HM8" s="94"/>
+      <c r="HN8" s="94"/>
+      <c r="HO8" s="94"/>
+      <c r="HP8" s="94"/>
+      <c r="HQ8" s="94"/>
+      <c r="HR8" s="96"/>
     </row>
     <row r="9" spans="1:226" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="128"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="105">
+      <c r="D9" s="103"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
+      <c r="O9" s="128"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="131">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(Q8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="107"/>
-      <c r="AA9" s="116" t="str">
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="98"/>
+      <c r="U9" s="98"/>
+      <c r="V9" s="98"/>
+      <c r="W9" s="98"/>
+      <c r="X9" s="98"/>
+      <c r="Y9" s="98"/>
+      <c r="Z9" s="99"/>
+      <c r="AA9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L1] Connexion</v>
       </c>
-      <c r="AB9" s="106"/>
-      <c r="AC9" s="106"/>
-      <c r="AD9" s="106"/>
-      <c r="AE9" s="106"/>
-      <c r="AF9" s="106"/>
-      <c r="AG9" s="106"/>
-      <c r="AH9" s="106"/>
-      <c r="AI9" s="106"/>
-      <c r="AJ9" s="107"/>
-      <c r="AK9" s="116">
+      <c r="AB9" s="98"/>
+      <c r="AC9" s="98"/>
+      <c r="AD9" s="98"/>
+      <c r="AE9" s="98"/>
+      <c r="AF9" s="98"/>
+      <c r="AG9" s="98"/>
+      <c r="AH9" s="98"/>
+      <c r="AI9" s="98"/>
+      <c r="AJ9" s="99"/>
+      <c r="AK9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="106"/>
-      <c r="AM9" s="106"/>
-      <c r="AN9" s="106"/>
-      <c r="AO9" s="106"/>
-      <c r="AP9" s="106"/>
-      <c r="AQ9" s="106"/>
-      <c r="AR9" s="106"/>
-      <c r="AS9" s="106"/>
-      <c r="AT9" s="107"/>
-      <c r="AU9" s="116" t="str">
+      <c r="AL9" s="98"/>
+      <c r="AM9" s="98"/>
+      <c r="AN9" s="98"/>
+      <c r="AO9" s="98"/>
+      <c r="AP9" s="98"/>
+      <c r="AQ9" s="98"/>
+      <c r="AR9" s="98"/>
+      <c r="AS9" s="98"/>
+      <c r="AT9" s="99"/>
+      <c r="AU9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L2] Affichage Professeur</v>
       </c>
-      <c r="AV9" s="106"/>
-      <c r="AW9" s="106"/>
-      <c r="AX9" s="106"/>
-      <c r="AY9" s="106"/>
-      <c r="AZ9" s="106"/>
-      <c r="BA9" s="106"/>
-      <c r="BB9" s="106"/>
-      <c r="BC9" s="106"/>
-      <c r="BD9" s="107"/>
-      <c r="BE9" s="116">
+      <c r="AV9" s="98"/>
+      <c r="AW9" s="98"/>
+      <c r="AX9" s="98"/>
+      <c r="AY9" s="98"/>
+      <c r="AZ9" s="98"/>
+      <c r="BA9" s="98"/>
+      <c r="BB9" s="98"/>
+      <c r="BC9" s="98"/>
+      <c r="BD9" s="99"/>
+      <c r="BE9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BF9" s="106"/>
-      <c r="BG9" s="106"/>
-      <c r="BH9" s="106"/>
-      <c r="BI9" s="106"/>
-      <c r="BJ9" s="106"/>
-      <c r="BK9" s="106"/>
-      <c r="BL9" s="106"/>
-      <c r="BM9" s="106"/>
-      <c r="BN9" s="107"/>
-      <c r="BO9" s="116" t="str">
+      <c r="BF9" s="98"/>
+      <c r="BG9" s="98"/>
+      <c r="BH9" s="98"/>
+      <c r="BI9" s="98"/>
+      <c r="BJ9" s="98"/>
+      <c r="BK9" s="98"/>
+      <c r="BL9" s="98"/>
+      <c r="BM9" s="98"/>
+      <c r="BN9" s="99"/>
+      <c r="BO9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L3] Historique</v>
       </c>
-      <c r="BP9" s="106"/>
-      <c r="BQ9" s="106"/>
-      <c r="BR9" s="106"/>
-      <c r="BS9" s="106"/>
-      <c r="BT9" s="106"/>
-      <c r="BU9" s="106"/>
-      <c r="BV9" s="106"/>
-      <c r="BW9" s="106"/>
-      <c r="BX9" s="107"/>
-      <c r="BY9" s="116">
+      <c r="BP9" s="98"/>
+      <c r="BQ9" s="98"/>
+      <c r="BR9" s="98"/>
+      <c r="BS9" s="98"/>
+      <c r="BT9" s="98"/>
+      <c r="BU9" s="98"/>
+      <c r="BV9" s="98"/>
+      <c r="BW9" s="98"/>
+      <c r="BX9" s="99"/>
+      <c r="BY9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BZ9" s="106"/>
-      <c r="CA9" s="106"/>
-      <c r="CB9" s="106"/>
-      <c r="CC9" s="106"/>
-      <c r="CD9" s="106"/>
-      <c r="CE9" s="106"/>
-      <c r="CF9" s="106"/>
-      <c r="CG9" s="106"/>
-      <c r="CH9" s="107"/>
-      <c r="CI9" s="116" t="str">
+      <c r="BZ9" s="98"/>
+      <c r="CA9" s="98"/>
+      <c r="CB9" s="98"/>
+      <c r="CC9" s="98"/>
+      <c r="CD9" s="98"/>
+      <c r="CE9" s="98"/>
+      <c r="CF9" s="98"/>
+      <c r="CG9" s="98"/>
+      <c r="CH9" s="99"/>
+      <c r="CI9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L4] Filtrage</v>
       </c>
-      <c r="CJ9" s="106"/>
-      <c r="CK9" s="106"/>
-      <c r="CL9" s="106"/>
-      <c r="CM9" s="106"/>
-      <c r="CN9" s="106"/>
-      <c r="CO9" s="106"/>
-      <c r="CP9" s="106"/>
-      <c r="CQ9" s="106"/>
-      <c r="CR9" s="107"/>
-      <c r="CS9" s="116" t="str">
+      <c r="CJ9" s="98"/>
+      <c r="CK9" s="98"/>
+      <c r="CL9" s="98"/>
+      <c r="CM9" s="98"/>
+      <c r="CN9" s="98"/>
+      <c r="CO9" s="98"/>
+      <c r="CP9" s="98"/>
+      <c r="CQ9" s="98"/>
+      <c r="CR9" s="99"/>
+      <c r="CS9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CS8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L5] Streaming multicast</v>
       </c>
-      <c r="CT9" s="106"/>
-      <c r="CU9" s="106"/>
-      <c r="CV9" s="106"/>
-      <c r="CW9" s="106"/>
-      <c r="CX9" s="106"/>
-      <c r="CY9" s="106"/>
-      <c r="CZ9" s="106"/>
-      <c r="DA9" s="106"/>
-      <c r="DB9" s="106"/>
-      <c r="DC9" s="116">
+      <c r="CT9" s="98"/>
+      <c r="CU9" s="98"/>
+      <c r="CV9" s="98"/>
+      <c r="CW9" s="98"/>
+      <c r="CX9" s="98"/>
+      <c r="CY9" s="98"/>
+      <c r="CZ9" s="98"/>
+      <c r="DA9" s="98"/>
+      <c r="DB9" s="98"/>
+      <c r="DC9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DC8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DD9" s="106"/>
-      <c r="DE9" s="106"/>
-      <c r="DF9" s="106"/>
-      <c r="DG9" s="106"/>
-      <c r="DH9" s="106"/>
-      <c r="DI9" s="106"/>
-      <c r="DJ9" s="106"/>
-      <c r="DK9" s="106"/>
-      <c r="DL9" s="107"/>
-      <c r="DM9" s="116" t="str">
+      <c r="DD9" s="98"/>
+      <c r="DE9" s="98"/>
+      <c r="DF9" s="98"/>
+      <c r="DG9" s="98"/>
+      <c r="DH9" s="98"/>
+      <c r="DI9" s="98"/>
+      <c r="DJ9" s="98"/>
+      <c r="DK9" s="98"/>
+      <c r="DL9" s="99"/>
+      <c r="DM9" s="97" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DM8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L6] Contrôle à distance</v>
       </c>
-      <c r="DN9" s="106"/>
-      <c r="DO9" s="106"/>
-      <c r="DP9" s="106"/>
-      <c r="DQ9" s="106"/>
-      <c r="DR9" s="106"/>
-      <c r="DS9" s="106"/>
-      <c r="DT9" s="106"/>
-      <c r="DU9" s="106"/>
-      <c r="DV9" s="107"/>
-      <c r="DW9" s="116">
+      <c r="DN9" s="98"/>
+      <c r="DO9" s="98"/>
+      <c r="DP9" s="98"/>
+      <c r="DQ9" s="98"/>
+      <c r="DR9" s="98"/>
+      <c r="DS9" s="98"/>
+      <c r="DT9" s="98"/>
+      <c r="DU9" s="98"/>
+      <c r="DV9" s="99"/>
+      <c r="DW9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DW8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DX9" s="106"/>
-      <c r="DY9" s="106"/>
-      <c r="DZ9" s="106"/>
-      <c r="EA9" s="106"/>
-      <c r="EB9" s="106"/>
-      <c r="EC9" s="106"/>
-      <c r="ED9" s="106"/>
-      <c r="EE9" s="106"/>
-      <c r="EF9" s="107"/>
-      <c r="EG9" s="116">
+      <c r="DX9" s="98"/>
+      <c r="DY9" s="98"/>
+      <c r="DZ9" s="98"/>
+      <c r="EA9" s="98"/>
+      <c r="EB9" s="98"/>
+      <c r="EC9" s="98"/>
+      <c r="ED9" s="98"/>
+      <c r="EE9" s="98"/>
+      <c r="EF9" s="99"/>
+      <c r="EG9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EG8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="EH9" s="106"/>
-      <c r="EI9" s="106"/>
-      <c r="EJ9" s="106"/>
-      <c r="EK9" s="106"/>
-      <c r="EL9" s="106"/>
-      <c r="EM9" s="106"/>
-      <c r="EN9" s="106"/>
-      <c r="EO9" s="106"/>
-      <c r="EP9" s="122"/>
-      <c r="EQ9" s="106">
+      <c r="EH9" s="98"/>
+      <c r="EI9" s="98"/>
+      <c r="EJ9" s="98"/>
+      <c r="EK9" s="98"/>
+      <c r="EL9" s="98"/>
+      <c r="EM9" s="98"/>
+      <c r="EN9" s="98"/>
+      <c r="EO9" s="98"/>
+      <c r="EP9" s="100"/>
+      <c r="EQ9" s="98">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EQ8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="ER9" s="106"/>
-      <c r="ES9" s="106"/>
-      <c r="ET9" s="106"/>
-      <c r="EU9" s="106"/>
-      <c r="EV9" s="106"/>
-      <c r="EW9" s="106"/>
-      <c r="EX9" s="106"/>
-      <c r="EY9" s="106"/>
-      <c r="EZ9" s="107"/>
-      <c r="FA9" s="116">
+      <c r="ER9" s="98"/>
+      <c r="ES9" s="98"/>
+      <c r="ET9" s="98"/>
+      <c r="EU9" s="98"/>
+      <c r="EV9" s="98"/>
+      <c r="EW9" s="98"/>
+      <c r="EX9" s="98"/>
+      <c r="EY9" s="98"/>
+      <c r="EZ9" s="99"/>
+      <c r="FA9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FB9" s="106"/>
-      <c r="FC9" s="106"/>
-      <c r="FD9" s="106"/>
-      <c r="FE9" s="106"/>
-      <c r="FF9" s="106"/>
-      <c r="FG9" s="106"/>
-      <c r="FH9" s="106"/>
-      <c r="FI9" s="106"/>
-      <c r="FJ9" s="107"/>
-      <c r="FK9" s="116">
+      <c r="FB9" s="98"/>
+      <c r="FC9" s="98"/>
+      <c r="FD9" s="98"/>
+      <c r="FE9" s="98"/>
+      <c r="FF9" s="98"/>
+      <c r="FG9" s="98"/>
+      <c r="FH9" s="98"/>
+      <c r="FI9" s="98"/>
+      <c r="FJ9" s="99"/>
+      <c r="FK9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FL9" s="106"/>
-      <c r="FM9" s="106"/>
-      <c r="FN9" s="106"/>
-      <c r="FO9" s="106"/>
-      <c r="FP9" s="106"/>
-      <c r="FQ9" s="106"/>
-      <c r="FR9" s="106"/>
-      <c r="FS9" s="106"/>
-      <c r="FT9" s="107"/>
-      <c r="FU9" s="116">
+      <c r="FL9" s="98"/>
+      <c r="FM9" s="98"/>
+      <c r="FN9" s="98"/>
+      <c r="FO9" s="98"/>
+      <c r="FP9" s="98"/>
+      <c r="FQ9" s="98"/>
+      <c r="FR9" s="98"/>
+      <c r="FS9" s="98"/>
+      <c r="FT9" s="99"/>
+      <c r="FU9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FV9" s="106"/>
-      <c r="FW9" s="106"/>
-      <c r="FX9" s="106"/>
-      <c r="FY9" s="106"/>
-      <c r="FZ9" s="106"/>
-      <c r="GA9" s="106"/>
-      <c r="GB9" s="106"/>
-      <c r="GC9" s="106"/>
-      <c r="GD9" s="107"/>
-      <c r="GE9" s="116">
+      <c r="FV9" s="98"/>
+      <c r="FW9" s="98"/>
+      <c r="FX9" s="98"/>
+      <c r="FY9" s="98"/>
+      <c r="FZ9" s="98"/>
+      <c r="GA9" s="98"/>
+      <c r="GB9" s="98"/>
+      <c r="GC9" s="98"/>
+      <c r="GD9" s="99"/>
+      <c r="GE9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GF9" s="106"/>
-      <c r="GG9" s="106"/>
-      <c r="GH9" s="106"/>
-      <c r="GI9" s="106"/>
-      <c r="GJ9" s="106"/>
-      <c r="GK9" s="106"/>
-      <c r="GL9" s="106"/>
-      <c r="GM9" s="106"/>
-      <c r="GN9" s="107"/>
-      <c r="GO9" s="116">
+      <c r="GF9" s="98"/>
+      <c r="GG9" s="98"/>
+      <c r="GH9" s="98"/>
+      <c r="GI9" s="98"/>
+      <c r="GJ9" s="98"/>
+      <c r="GK9" s="98"/>
+      <c r="GL9" s="98"/>
+      <c r="GM9" s="98"/>
+      <c r="GN9" s="99"/>
+      <c r="GO9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GP9" s="106"/>
-      <c r="GQ9" s="106"/>
-      <c r="GR9" s="106"/>
-      <c r="GS9" s="106"/>
-      <c r="GT9" s="106"/>
-      <c r="GU9" s="106"/>
-      <c r="GV9" s="106"/>
-      <c r="GW9" s="106"/>
-      <c r="GX9" s="107"/>
-      <c r="GY9" s="116">
+      <c r="GP9" s="98"/>
+      <c r="GQ9" s="98"/>
+      <c r="GR9" s="98"/>
+      <c r="GS9" s="98"/>
+      <c r="GT9" s="98"/>
+      <c r="GU9" s="98"/>
+      <c r="GV9" s="98"/>
+      <c r="GW9" s="98"/>
+      <c r="GX9" s="99"/>
+      <c r="GY9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GZ9" s="106"/>
-      <c r="HA9" s="106"/>
-      <c r="HB9" s="106"/>
-      <c r="HC9" s="106"/>
-      <c r="HD9" s="106"/>
-      <c r="HE9" s="106"/>
-      <c r="HF9" s="106"/>
-      <c r="HG9" s="106"/>
-      <c r="HH9" s="107"/>
-      <c r="HI9" s="116">
+      <c r="GZ9" s="98"/>
+      <c r="HA9" s="98"/>
+      <c r="HB9" s="98"/>
+      <c r="HC9" s="98"/>
+      <c r="HD9" s="98"/>
+      <c r="HE9" s="98"/>
+      <c r="HF9" s="98"/>
+      <c r="HG9" s="98"/>
+      <c r="HH9" s="99"/>
+      <c r="HI9" s="97">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(HI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="HJ9" s="106"/>
-      <c r="HK9" s="106"/>
-      <c r="HL9" s="106"/>
-      <c r="HM9" s="106"/>
-      <c r="HN9" s="106"/>
-      <c r="HO9" s="106"/>
-      <c r="HP9" s="106"/>
-      <c r="HQ9" s="106"/>
-      <c r="HR9" s="122"/>
+      <c r="HJ9" s="98"/>
+      <c r="HK9" s="98"/>
+      <c r="HL9" s="98"/>
+      <c r="HM9" s="98"/>
+      <c r="HN9" s="98"/>
+      <c r="HO9" s="98"/>
+      <c r="HP9" s="98"/>
+      <c r="HQ9" s="98"/>
+      <c r="HR9" s="100"/>
     </row>
     <row r="10" spans="1:226" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="99"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
+      <c r="N10" s="128"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="125"/>
       <c r="Q10" s="5"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="20"/>
@@ -28139,19 +28139,19 @@
       <c r="A11" s="68"/>
       <c r="B11" s="5"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="100"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="134"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
+      <c r="O11" s="129"/>
+      <c r="P11" s="126"/>
       <c r="Q11" s="51">
         <v>0</v>
       </c>
@@ -29648,17 +29648,17 @@
       </c>
     </row>
     <row r="13" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="G13" s="87" t="s">
+      <c r="E13" s="83"/>
+      <c r="G13" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="119" t="str">
+      <c r="H13" s="85" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
       </c>
@@ -29764,11 +29764,11 @@
       <c r="HR13" s="4"/>
     </row>
     <row r="14" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="134"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="101"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="119"/>
+      <c r="B14" s="81"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="83"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="85"/>
       <c r="I14" s="45" t="s">
         <v>1</v>
       </c>
@@ -30020,22 +30020,22 @@
       <c r="HR14" s="31"/>
     </row>
     <row r="15" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="134" t="s">
+      <c r="B15" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="101">
+      <c r="F15" s="83">
         <v>1</v>
       </c>
-      <c r="G15" s="87" t="s">
+      <c r="G15" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="119" t="str">
+      <c r="H15" s="85" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
       </c>
@@ -30106,12 +30106,12 @@
       <c r="HR15" s="4"/>
     </row>
     <row r="16" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="134"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="119"/>
+      <c r="B16" s="81"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="85"/>
       <c r="I16" s="45" t="s">
         <v>1</v>
       </c>
@@ -30351,20 +30351,20 @@
       <c r="HR16" s="31"/>
     </row>
     <row r="17" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="88" t="s">
+      <c r="D17" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101">
+      <c r="E17" s="83"/>
+      <c r="F17" s="83">
         <v>1</v>
       </c>
-      <c r="G17" s="87" t="s">
+      <c r="G17" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="119" t="str">
+      <c r="H17" s="85" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
       </c>
@@ -30436,12 +30436,12 @@
       <c r="HR17" s="4"/>
     </row>
     <row r="18" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="134"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="119"/>
+      <c r="B18" s="81"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="85"/>
       <c r="I18" s="45" t="s">
         <v>1</v>
       </c>
@@ -30683,22 +30683,22 @@
       <c r="HR18" s="31"/>
     </row>
     <row r="19" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="88" t="s">
+      <c r="D19" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="101" t="s">
+      <c r="E19" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="101">
+      <c r="F19" s="83">
         <v>1</v>
       </c>
-      <c r="G19" s="87" t="s">
+      <c r="G19" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="119" t="str">
+      <c r="H19" s="85" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
       </c>
@@ -30782,12 +30782,12 @@
       <c r="HR19" s="4"/>
     </row>
     <row r="20" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="134"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="119"/>
+      <c r="B20" s="81"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="85"/>
       <c r="I20" s="45" t="s">
         <v>1</v>
       </c>
@@ -31031,20 +31031,20 @@
       <c r="HR20" s="31"/>
     </row>
     <row r="21" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="134" t="s">
+      <c r="B21" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="88" t="s">
+      <c r="D21" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101">
+      <c r="E21" s="83"/>
+      <c r="F21" s="83">
         <v>1</v>
       </c>
-      <c r="G21" s="87" t="s">
+      <c r="G21" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="119" t="str">
+      <c r="H21" s="85" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
       </c>
@@ -31118,12 +31118,12 @@
       <c r="HR21" s="4"/>
     </row>
     <row r="22" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="134"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="119"/>
+      <c r="B22" s="81"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="85"/>
       <c r="I22" s="45" t="s">
         <v>1</v>
       </c>
@@ -31361,20 +31361,20 @@
       <c r="HR22" s="31"/>
     </row>
     <row r="23" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="134" t="s">
+      <c r="B23" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101">
+      <c r="E23" s="83"/>
+      <c r="F23" s="83">
         <v>1</v>
       </c>
-      <c r="G23" s="87" t="s">
+      <c r="G23" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="119" t="str">
+      <c r="H23" s="85" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
       </c>
@@ -31445,12 +31445,12 @@
       <c r="HR23" s="4"/>
     </row>
     <row r="24" spans="2:226" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="134"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="119"/>
+      <c r="B24" s="81"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="85"/>
       <c r="I24" s="45" t="s">
         <v>1</v>
       </c>
@@ -31692,20 +31692,20 @@
       <c r="HR24" s="31"/>
     </row>
     <row r="25" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="134" t="s">
+      <c r="B25" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="88" t="s">
+      <c r="D25" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101">
+      <c r="E25" s="83"/>
+      <c r="F25" s="83">
         <v>1</v>
       </c>
-      <c r="G25" s="87" t="s">
+      <c r="G25" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="119" t="str">
+      <c r="H25" s="85" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
       </c>
@@ -31775,12 +31775,12 @@
       <c r="HR25" s="4"/>
     </row>
     <row r="26" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="134"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="119"/>
+      <c r="B26" s="81"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="85"/>
       <c r="I26" s="45" t="s">
         <v>1</v>
       </c>
@@ -32020,20 +32020,20 @@
       <c r="HR26" s="31"/>
     </row>
     <row r="27" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="134" t="s">
+      <c r="B27" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="88" t="s">
+      <c r="D27" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101">
+      <c r="E27" s="83"/>
+      <c r="F27" s="83">
         <v>2</v>
       </c>
-      <c r="G27" s="87" t="s">
+      <c r="G27" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="119" t="str">
+      <c r="H27" s="85" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
       </c>
@@ -32114,12 +32114,12 @@
       <c r="HR27" s="4"/>
     </row>
     <row r="28" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="134"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="119"/>
+      <c r="B28" s="81"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="85"/>
       <c r="I28" s="45" t="s">
         <v>1</v>
       </c>
@@ -32359,22 +32359,22 @@
       <c r="HR28" s="31"/>
     </row>
     <row r="29" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="134" t="s">
+      <c r="B29" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="88" t="s">
+      <c r="D29" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="101" t="s">
+      <c r="E29" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="101">
+      <c r="F29" s="83">
         <v>2</v>
       </c>
-      <c r="G29" s="87" t="s">
+      <c r="G29" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="119" t="str">
+      <c r="H29" s="85" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v>!</v>
       </c>
@@ -32454,12 +32454,12 @@
       <c r="HR29" s="4"/>
     </row>
     <row r="30" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="134"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="119"/>
+      <c r="B30" s="81"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="45" t="s">
         <v>1</v>
       </c>
@@ -32715,22 +32715,22 @@
       <c r="HR30" s="31"/>
     </row>
     <row r="31" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="134" t="s">
+      <c r="B31" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="121" t="s">
+      <c r="D31" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="101" t="s">
+      <c r="E31" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="101">
+      <c r="F31" s="83">
         <v>2</v>
       </c>
-      <c r="G31" s="87" t="s">
+      <c r="G31" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="119" t="str">
+      <c r="H31" s="85" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
       </c>
@@ -32802,12 +32802,12 @@
       <c r="HR31" s="4"/>
     </row>
     <row r="32" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="134"/>
-      <c r="D32" s="121"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="119"/>
+      <c r="B32" s="81"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="85"/>
       <c r="I32" s="45" t="s">
         <v>1</v>
       </c>
@@ -33049,22 +33049,22 @@
       <c r="HR32" s="31"/>
     </row>
     <row r="33" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="134" t="s">
+      <c r="B33" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="121" t="s">
+      <c r="D33" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="101" t="s">
+      <c r="E33" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="101">
+      <c r="F33" s="83">
         <v>2</v>
       </c>
-      <c r="G33" s="87" t="s">
+      <c r="G33" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="119" t="str">
+      <c r="H33" s="85" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
       </c>
@@ -33140,12 +33140,12 @@
       <c r="HR33" s="4"/>
     </row>
     <row r="34" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="134"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="119"/>
+      <c r="B34" s="81"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="45" t="s">
         <v>1</v>
       </c>
@@ -33387,22 +33387,22 @@
       <c r="HR34" s="31"/>
     </row>
     <row r="35" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="134" t="s">
+      <c r="B35" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="121" t="s">
+      <c r="D35" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="101" t="s">
+      <c r="E35" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="101">
+      <c r="F35" s="83">
         <v>2</v>
       </c>
-      <c r="G35" s="87" t="s">
+      <c r="G35" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="119" t="str">
+      <c r="H35" s="85" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
       </c>
@@ -33481,12 +33481,12 @@
       <c r="HR35" s="4"/>
     </row>
     <row r="36" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="134"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="101"/>
-      <c r="F36" s="101"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="119"/>
+      <c r="B36" s="81"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="45" t="s">
         <v>1</v>
       </c>
@@ -33724,22 +33724,22 @@
       <c r="HR36" s="31"/>
     </row>
     <row r="37" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="134" t="s">
+      <c r="B37" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="121" t="s">
+      <c r="D37" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="101" t="s">
+      <c r="E37" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="101">
+      <c r="F37" s="83">
         <v>2</v>
       </c>
-      <c r="G37" s="87" t="s">
+      <c r="G37" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="119" t="str">
+      <c r="H37" s="85" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
       </c>
@@ -33813,12 +33813,12 @@
       <c r="HR37" s="4"/>
     </row>
     <row r="38" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="134"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="119"/>
+      <c r="B38" s="81"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="45" t="s">
         <v>1</v>
       </c>
@@ -34058,20 +34058,20 @@
       <c r="HR38" s="31"/>
     </row>
     <row r="39" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="121" t="s">
+      <c r="D39" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101">
+      <c r="E39" s="83"/>
+      <c r="F39" s="83">
         <v>3</v>
       </c>
-      <c r="G39" s="87" t="s">
+      <c r="G39" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="119" t="str">
+      <c r="H39" s="85" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
       </c>
@@ -34152,12 +34152,12 @@
       <c r="HR39" s="4"/>
     </row>
     <row r="40" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="134"/>
-      <c r="D40" s="121"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="119"/>
+      <c r="B40" s="81"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="85"/>
       <c r="I40" s="45" t="s">
         <v>1</v>
       </c>
@@ -34405,20 +34405,20 @@
       <c r="HR40" s="31"/>
     </row>
     <row r="41" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="134" t="s">
+      <c r="B41" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="121" t="s">
+      <c r="D41" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="101"/>
-      <c r="F41" s="101">
+      <c r="E41" s="83"/>
+      <c r="F41" s="83">
         <v>3</v>
       </c>
-      <c r="G41" s="87" t="s">
+      <c r="G41" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="119" t="str">
+      <c r="H41" s="85" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
       </c>
@@ -34492,12 +34492,12 @@
       <c r="HR41" s="4"/>
     </row>
     <row r="42" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="134"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="101"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="119"/>
+      <c r="B42" s="81"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="83"/>
+      <c r="F42" s="83"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="85"/>
       <c r="I42" s="45" t="s">
         <v>1</v>
       </c>
@@ -34737,20 +34737,20 @@
       <c r="HR42" s="31"/>
     </row>
     <row r="43" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="134" t="s">
+      <c r="B43" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="121" t="s">
+      <c r="D43" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="101"/>
-      <c r="F43" s="101">
+      <c r="E43" s="83"/>
+      <c r="F43" s="83">
         <v>3</v>
       </c>
-      <c r="G43" s="87" t="s">
+      <c r="G43" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="119" t="str">
+      <c r="H43" s="85" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
       </c>
@@ -34823,12 +34823,12 @@
       <c r="HR43" s="4"/>
     </row>
     <row r="44" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="134"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="101"/>
-      <c r="F44" s="101"/>
-      <c r="G44" s="87"/>
-      <c r="H44" s="119"/>
+      <c r="B44" s="81"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="85"/>
       <c r="I44" s="45" t="s">
         <v>1</v>
       </c>
@@ -35070,20 +35070,20 @@
       <c r="HR44" s="31"/>
     </row>
     <row r="45" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="134" t="s">
+      <c r="B45" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="121" t="s">
+      <c r="D45" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="101"/>
-      <c r="F45" s="101">
+      <c r="E45" s="83"/>
+      <c r="F45" s="83">
         <v>3</v>
       </c>
-      <c r="G45" s="87" t="s">
+      <c r="G45" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="119" t="str">
+      <c r="H45" s="85" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
       </c>
@@ -35156,12 +35156,12 @@
       <c r="HR45" s="4"/>
     </row>
     <row r="46" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="134"/>
-      <c r="D46" s="121"/>
-      <c r="E46" s="101"/>
-      <c r="F46" s="101"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="119"/>
+      <c r="B46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="85"/>
       <c r="I46" s="45" t="s">
         <v>1</v>
       </c>
@@ -35403,20 +35403,20 @@
       <c r="HR46" s="31"/>
     </row>
     <row r="47" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="134" t="s">
+      <c r="B47" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="121" t="s">
+      <c r="D47" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="101"/>
-      <c r="F47" s="101">
+      <c r="E47" s="83"/>
+      <c r="F47" s="83">
         <v>3</v>
       </c>
-      <c r="G47" s="87" t="s">
+      <c r="G47" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="119" t="str">
+      <c r="H47" s="85" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
       </c>
@@ -35486,12 +35486,12 @@
       <c r="HR47" s="4"/>
     </row>
     <row r="48" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="134"/>
-      <c r="D48" s="121"/>
-      <c r="E48" s="101"/>
-      <c r="F48" s="101"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="119"/>
+      <c r="B48" s="81"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="85"/>
       <c r="I48" s="45" t="s">
         <v>1</v>
       </c>
@@ -35733,20 +35733,20 @@
       <c r="HR48" s="31"/>
     </row>
     <row r="49" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="134" t="s">
+      <c r="B49" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="121" t="s">
+      <c r="D49" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="101"/>
-      <c r="F49" s="101">
+      <c r="E49" s="83"/>
+      <c r="F49" s="83">
         <v>4</v>
       </c>
-      <c r="G49" s="87" t="s">
+      <c r="G49" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="119" t="str">
+      <c r="H49" s="85" t="str">
         <f t="shared" ref="H49" si="65">IF(O50&gt;P49,"!","")</f>
         <v/>
       </c>
@@ -35834,12 +35834,12 @@
       <c r="HR49" s="4"/>
     </row>
     <row r="50" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="134"/>
-      <c r="D50" s="121"/>
-      <c r="E50" s="101"/>
-      <c r="F50" s="101"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="119"/>
+      <c r="B50" s="81"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="85"/>
       <c r="I50" s="45" t="s">
         <v>1</v>
       </c>
@@ -36083,20 +36083,20 @@
       <c r="HR50" s="31"/>
     </row>
     <row r="51" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="134" t="s">
+      <c r="B51" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="121" t="s">
+      <c r="D51" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="101"/>
-      <c r="F51" s="101">
+      <c r="E51" s="83"/>
+      <c r="F51" s="83">
         <v>4</v>
       </c>
-      <c r="G51" s="87" t="s">
+      <c r="G51" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="119" t="str">
+      <c r="H51" s="85" t="str">
         <f t="shared" ref="H51" si="71">IF(O52&gt;P51,"!","")</f>
         <v/>
       </c>
@@ -36173,12 +36173,12 @@
       <c r="HR51" s="4"/>
     </row>
     <row r="52" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="134"/>
-      <c r="D52" s="121"/>
-      <c r="E52" s="101"/>
-      <c r="F52" s="101"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="119"/>
+      <c r="B52" s="81"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="84"/>
+      <c r="H52" s="85"/>
       <c r="I52" s="45" t="s">
         <v>1</v>
       </c>
@@ -36422,20 +36422,20 @@
       <c r="HR52" s="31"/>
     </row>
     <row r="53" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="134" t="s">
+      <c r="B53" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="121" t="s">
+      <c r="D53" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101">
+      <c r="E53" s="83"/>
+      <c r="F53" s="83">
         <v>4</v>
       </c>
-      <c r="G53" s="87" t="s">
+      <c r="G53" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H53" s="119" t="str">
+      <c r="H53" s="85" t="str">
         <f t="shared" ref="H53" si="77">IF(O54&gt;P53,"!","")</f>
         <v/>
       </c>
@@ -36515,12 +36515,12 @@
       <c r="HR53" s="4"/>
     </row>
     <row r="54" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="134"/>
-      <c r="D54" s="121"/>
-      <c r="E54" s="101"/>
-      <c r="F54" s="101"/>
-      <c r="G54" s="87"/>
-      <c r="H54" s="119"/>
+      <c r="B54" s="81"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="83"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="85"/>
       <c r="I54" s="45" t="s">
         <v>1</v>
       </c>
@@ -36760,22 +36760,22 @@
       <c r="HR54" s="31"/>
     </row>
     <row r="55" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="134" t="s">
+      <c r="B55" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="121" t="s">
+      <c r="D55" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="101" t="s">
+      <c r="E55" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="101">
+      <c r="F55" s="83">
         <v>4</v>
       </c>
-      <c r="G55" s="87" t="s">
+      <c r="G55" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H55" s="119" t="str">
+      <c r="H55" s="85" t="str">
         <f t="shared" ref="H55" si="83">IF(O56&gt;P55,"!","")</f>
         <v/>
       </c>
@@ -36858,12 +36858,12 @@
       <c r="HR55" s="4"/>
     </row>
     <row r="56" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="134"/>
-      <c r="D56" s="121"/>
-      <c r="E56" s="101"/>
-      <c r="F56" s="101"/>
-      <c r="G56" s="87"/>
-      <c r="H56" s="119"/>
+      <c r="B56" s="81"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="83"/>
+      <c r="F56" s="83"/>
+      <c r="G56" s="84"/>
+      <c r="H56" s="85"/>
       <c r="I56" s="45" t="s">
         <v>1</v>
       </c>
@@ -37105,22 +37105,22 @@
       <c r="HR56" s="31"/>
     </row>
     <row r="57" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="134" t="s">
+      <c r="B57" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="121" t="s">
+      <c r="D57" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="101" t="s">
+      <c r="E57" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="101">
+      <c r="F57" s="83">
         <v>4</v>
       </c>
-      <c r="G57" s="87" t="s">
+      <c r="G57" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H57" s="119" t="str">
+      <c r="H57" s="85" t="str">
         <f t="shared" ref="H57" si="89">IF(O58&gt;P57,"!","")</f>
         <v/>
       </c>
@@ -37191,12 +37191,12 @@
       <c r="HR57" s="4"/>
     </row>
     <row r="58" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="134"/>
-      <c r="D58" s="121"/>
-      <c r="E58" s="101"/>
-      <c r="F58" s="101"/>
-      <c r="G58" s="87"/>
-      <c r="H58" s="119"/>
+      <c r="B58" s="81"/>
+      <c r="D58" s="82"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="85"/>
       <c r="I58" s="45" t="s">
         <v>1</v>
       </c>
@@ -37440,20 +37440,20 @@
       <c r="HR58" s="31"/>
     </row>
     <row r="59" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="134" t="s">
+      <c r="B59" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="121" t="s">
+      <c r="D59" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="101"/>
-      <c r="F59" s="101">
+      <c r="E59" s="83"/>
+      <c r="F59" s="83">
         <v>5</v>
       </c>
-      <c r="G59" s="87" t="s">
+      <c r="G59" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="119" t="str">
+      <c r="H59" s="85" t="str">
         <f t="shared" ref="H59" si="95">IF(O60&gt;P59,"!","")</f>
         <v/>
       </c>
@@ -37527,12 +37527,12 @@
       <c r="HR59" s="4"/>
     </row>
     <row r="60" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="134"/>
-      <c r="D60" s="121"/>
-      <c r="E60" s="101"/>
-      <c r="F60" s="101"/>
-      <c r="G60" s="87"/>
-      <c r="H60" s="119"/>
+      <c r="B60" s="81"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="83"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="84"/>
+      <c r="H60" s="85"/>
       <c r="I60" s="45" t="s">
         <v>1</v>
       </c>
@@ -37772,18 +37772,18 @@
       <c r="HR60" s="31"/>
     </row>
     <row r="61" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="134" t="s">
+      <c r="B61" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="121" t="s">
+      <c r="D61" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E61" s="101"/>
-      <c r="F61" s="101">
+      <c r="E61" s="83"/>
+      <c r="F61" s="83">
         <v>5</v>
       </c>
-      <c r="G61" s="87"/>
-      <c r="H61" s="119" t="str">
+      <c r="G61" s="84"/>
+      <c r="H61" s="85" t="str">
         <f t="shared" ref="H61" si="101">IF(O62&gt;P61,"!","")</f>
         <v/>
       </c>
@@ -37878,23 +37878,23 @@
       <c r="HR61" s="4"/>
     </row>
     <row r="62" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="134"/>
-      <c r="D62" s="121"/>
-      <c r="E62" s="101"/>
-      <c r="F62" s="101"/>
-      <c r="G62" s="87"/>
-      <c r="H62" s="119"/>
+      <c r="B62" s="81"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="83"/>
+      <c r="F62" s="83"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="85"/>
       <c r="I62" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J62" s="46">
         <f>IF(D61="","",COUNTIF(Echéancier!$Q62:$EP62,"r"))</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K62" s="14"/>
       <c r="L62" s="14">
         <f t="shared" ref="L62" si="104">IFERROR(L60+J62,0)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M62" s="14">
         <f t="shared" ref="M62" si="105">COUNTIF(Q62:EP62,"a")</f>
@@ -37906,7 +37906,7 @@
       </c>
       <c r="O62" s="14">
         <f>IFERROR(MATCH("ra",$Q62:$EP62,1),0)</f>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P62" s="14"/>
       <c r="Q62" s="23"/>
@@ -38004,7 +38004,9 @@
       <c r="CO62" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="CP62" s="75"/>
+      <c r="CP62" s="75" t="s">
+        <v>27</v>
+      </c>
       <c r="CQ62" s="34"/>
       <c r="CR62" s="24"/>
       <c r="CS62" s="25"/>
@@ -38139,18 +38141,18 @@
       <c r="HR62" s="31"/>
     </row>
     <row r="63" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="134" t="s">
+      <c r="B63" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="121" t="s">
+      <c r="D63" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="101"/>
-      <c r="F63" s="101">
+      <c r="E63" s="83"/>
+      <c r="F63" s="83">
         <v>5</v>
       </c>
-      <c r="G63" s="87"/>
-      <c r="H63" s="119" t="str">
+      <c r="G63" s="84"/>
+      <c r="H63" s="85" t="str">
         <f t="shared" ref="H63" si="107">IF(O64&gt;P63,"!","")</f>
         <v/>
       </c>
@@ -38235,23 +38237,23 @@
       <c r="HR63" s="4"/>
     </row>
     <row r="64" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="134"/>
-      <c r="D64" s="121"/>
-      <c r="E64" s="101"/>
-      <c r="F64" s="101"/>
-      <c r="G64" s="87"/>
-      <c r="H64" s="119"/>
+      <c r="B64" s="81"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="83"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="85"/>
       <c r="I64" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J64" s="46">
         <f>IF(D63="","",COUNTIF(Echéancier!$Q64:$EP64,"r"))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K64" s="14"/>
       <c r="L64" s="14">
         <f t="shared" ref="L64" si="110">IFERROR(L62+J64,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M64" s="14">
         <f t="shared" ref="M64" si="111">COUNTIF(Q64:EP64,"a")</f>
@@ -38263,7 +38265,7 @@
       </c>
       <c r="O64" s="14">
         <f>IFERROR(MATCH("ra",$Q64:$EP64,1),0)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="P64" s="14"/>
       <c r="Q64" s="23"/>
@@ -38344,8 +38346,12 @@
       <c r="CN64" s="34"/>
       <c r="CO64" s="34"/>
       <c r="CP64" s="75"/>
-      <c r="CQ64" s="75"/>
-      <c r="CR64" s="74"/>
+      <c r="CQ64" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="CR64" s="74" t="s">
+        <v>27</v>
+      </c>
       <c r="CS64" s="76"/>
       <c r="CT64" s="34"/>
       <c r="CU64" s="34"/>
@@ -38478,18 +38484,18 @@
       <c r="HR64" s="31"/>
     </row>
     <row r="65" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="134" t="s">
+      <c r="B65" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="121" t="s">
+      <c r="D65" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="101"/>
-      <c r="F65" s="101">
+      <c r="E65" s="83"/>
+      <c r="F65" s="83">
         <v>6</v>
       </c>
-      <c r="G65" s="87"/>
-      <c r="H65" s="119" t="str">
+      <c r="G65" s="84"/>
+      <c r="H65" s="85" t="str">
         <f t="shared" ref="H65" si="113">IF(O66&gt;P65,"!","")</f>
         <v/>
       </c>
@@ -38567,12 +38573,12 @@
       <c r="HR65" s="4"/>
     </row>
     <row r="66" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="134"/>
-      <c r="D66" s="121"/>
-      <c r="E66" s="101"/>
-      <c r="F66" s="101"/>
-      <c r="G66" s="87"/>
-      <c r="H66" s="119"/>
+      <c r="B66" s="81"/>
+      <c r="D66" s="82"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="85"/>
       <c r="I66" s="45" t="s">
         <v>1</v>
       </c>
@@ -38583,7 +38589,7 @@
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -38810,20 +38816,20 @@
       <c r="HR66" s="31"/>
     </row>
     <row r="67" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="134" t="s">
+      <c r="B67" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="121" t="s">
+      <c r="D67" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="101" t="s">
+      <c r="E67" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="F67" s="101">
+      <c r="F67" s="83">
         <v>6</v>
       </c>
-      <c r="G67" s="87"/>
-      <c r="H67" s="119" t="str">
+      <c r="G67" s="84"/>
+      <c r="H67" s="85" t="str">
         <f t="shared" ref="H67" si="119">IF(O68&gt;P67,"!","")</f>
         <v/>
       </c>
@@ -38918,12 +38924,12 @@
       <c r="HR67" s="4"/>
     </row>
     <row r="68" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="134"/>
-      <c r="D68" s="121"/>
-      <c r="E68" s="101"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="87"/>
-      <c r="H68" s="119"/>
+      <c r="B68" s="81"/>
+      <c r="D68" s="82"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="85"/>
       <c r="I68" s="45" t="s">
         <v>1</v>
       </c>
@@ -38934,7 +38940,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -39161,20 +39167,20 @@
       <c r="HR68" s="31"/>
     </row>
     <row r="69" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="134" t="s">
+      <c r="B69" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="121" t="s">
+      <c r="D69" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="101" t="s">
+      <c r="E69" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="F69" s="101">
+      <c r="F69" s="83">
         <v>6</v>
       </c>
-      <c r="G69" s="87"/>
-      <c r="H69" s="119" t="str">
+      <c r="G69" s="84"/>
+      <c r="H69" s="85" t="str">
         <f t="shared" ref="H69" si="127">IF(O70&gt;P69,"!","")</f>
         <v/>
       </c>
@@ -39251,12 +39257,12 @@
       <c r="HR69" s="4"/>
     </row>
     <row r="70" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="134"/>
-      <c r="D70" s="121"/>
-      <c r="E70" s="101"/>
-      <c r="F70" s="101"/>
-      <c r="G70" s="87"/>
-      <c r="H70" s="119"/>
+      <c r="B70" s="81"/>
+      <c r="D70" s="82"/>
+      <c r="E70" s="83"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="85"/>
       <c r="I70" s="45" t="s">
         <v>1</v>
       </c>
@@ -39267,7 +39273,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -39494,20 +39500,20 @@
       <c r="HR70" s="31"/>
     </row>
     <row r="71" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="134" t="s">
+      <c r="B71" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="121" t="s">
+      <c r="D71" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="E71" s="101" t="s">
+      <c r="E71" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="F71" s="101">
+      <c r="F71" s="83">
         <v>6</v>
       </c>
-      <c r="G71" s="87"/>
-      <c r="H71" s="119" t="str">
+      <c r="G71" s="84"/>
+      <c r="H71" s="85" t="str">
         <f t="shared" ref="H71" si="133">IF(O72&gt;P71,"!","")</f>
         <v/>
       </c>
@@ -39583,12 +39589,12 @@
       <c r="HR71" s="4"/>
     </row>
     <row r="72" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="134"/>
-      <c r="D72" s="121"/>
-      <c r="E72" s="101"/>
-      <c r="F72" s="101"/>
-      <c r="G72" s="87"/>
-      <c r="H72" s="119"/>
+      <c r="B72" s="81"/>
+      <c r="D72" s="82"/>
+      <c r="E72" s="83"/>
+      <c r="F72" s="83"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="85"/>
       <c r="I72" s="45" t="s">
         <v>1</v>
       </c>
@@ -39599,7 +39605,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -39915,13 +39921,13 @@
     </row>
     <row r="73" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="121" t="s">
+      <c r="D73" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="101"/>
-      <c r="F73" s="101"/>
-      <c r="G73" s="87"/>
-      <c r="H73" s="119" t="str">
+      <c r="E73" s="83"/>
+      <c r="F73" s="83"/>
+      <c r="G73" s="84"/>
+      <c r="H73" s="85" t="str">
         <f t="shared" ref="H73" si="139">IF(O74&gt;P73,"!","")</f>
         <v/>
       </c>
@@ -39989,11 +39995,11 @@
     </row>
     <row r="74" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="D74" s="121"/>
-      <c r="E74" s="101"/>
-      <c r="F74" s="101"/>
-      <c r="G74" s="87"/>
-      <c r="H74" s="119"/>
+      <c r="D74" s="82"/>
+      <c r="E74" s="83"/>
+      <c r="F74" s="83"/>
+      <c r="G74" s="84"/>
+      <c r="H74" s="85"/>
       <c r="I74" s="45" t="s">
         <v>1</v>
       </c>
@@ -40004,7 +40010,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>
@@ -40232,13 +40238,13 @@
     </row>
     <row r="75" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="121" t="s">
+      <c r="D75" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="101"/>
-      <c r="F75" s="101"/>
-      <c r="G75" s="87"/>
-      <c r="H75" s="119" t="str">
+      <c r="E75" s="83"/>
+      <c r="F75" s="83"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="85" t="str">
         <f t="shared" ref="H75" si="145">IF(O76&gt;P75,"!","")</f>
         <v/>
       </c>
@@ -40310,11 +40316,11 @@
     </row>
     <row r="76" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
-      <c r="D76" s="121"/>
-      <c r="E76" s="101"/>
-      <c r="F76" s="101"/>
-      <c r="G76" s="87"/>
-      <c r="H76" s="119"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="83"/>
+      <c r="F76" s="83"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="85"/>
       <c r="I76" s="45" t="s">
         <v>1</v>
       </c>
@@ -40325,7 +40331,7 @@
       <c r="K76" s="14"/>
       <c r="L76" s="14">
         <f t="shared" ref="L76" si="148">IFERROR(L74+J76,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M76" s="14">
         <f t="shared" ref="M76" si="149">COUNTIF(Q76:EP76,"a")</f>
@@ -40553,13 +40559,13 @@
     </row>
     <row r="77" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
-      <c r="D77" s="121" t="s">
+      <c r="D77" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="E77" s="101"/>
-      <c r="F77" s="101"/>
-      <c r="G77" s="87"/>
-      <c r="H77" s="119" t="str">
+      <c r="E77" s="83"/>
+      <c r="F77" s="83"/>
+      <c r="G77" s="84"/>
+      <c r="H77" s="85" t="str">
         <f t="shared" ref="H77" si="151">IF(O78&gt;P77,"!","")</f>
         <v/>
       </c>
@@ -40648,11 +40654,11 @@
     </row>
     <row r="78" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="121"/>
-      <c r="E78" s="101"/>
-      <c r="F78" s="101"/>
-      <c r="G78" s="87"/>
-      <c r="H78" s="119"/>
+      <c r="D78" s="82"/>
+      <c r="E78" s="83"/>
+      <c r="F78" s="83"/>
+      <c r="G78" s="84"/>
+      <c r="H78" s="85"/>
       <c r="I78" s="45" t="s">
         <v>1</v>
       </c>
@@ -40663,7 +40669,7 @@
       <c r="K78" s="14"/>
       <c r="L78" s="14">
         <f t="shared" ref="L78" si="154">IFERROR(L76+J78,0)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M78" s="14">
         <f t="shared" ref="M78" si="155">COUNTIF(Q78:EP78,"a")</f>
@@ -40891,11 +40897,11 @@
     </row>
     <row r="79" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="D79" s="121"/>
-      <c r="E79" s="101"/>
-      <c r="F79" s="101"/>
-      <c r="G79" s="87"/>
-      <c r="H79" s="119" t="str">
+      <c r="D79" s="82"/>
+      <c r="E79" s="83"/>
+      <c r="F79" s="83"/>
+      <c r="G79" s="84"/>
+      <c r="H79" s="85" t="str">
         <f t="shared" ref="H79" si="157">IF(O80&gt;P79,"!","")</f>
         <v/>
       </c>
@@ -40964,11 +40970,11 @@
     </row>
     <row r="80" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
-      <c r="D80" s="121"/>
-      <c r="E80" s="101"/>
-      <c r="F80" s="101"/>
-      <c r="G80" s="87"/>
-      <c r="H80" s="119"/>
+      <c r="D80" s="82"/>
+      <c r="E80" s="83"/>
+      <c r="F80" s="83"/>
+      <c r="G80" s="84"/>
+      <c r="H80" s="85"/>
       <c r="I80" s="45" t="s">
         <v>1</v>
       </c>
@@ -41207,11 +41213,11 @@
     </row>
     <row r="81" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="D81" s="121"/>
-      <c r="E81" s="101"/>
-      <c r="F81" s="101"/>
-      <c r="G81" s="87"/>
-      <c r="H81" s="119" t="str">
+      <c r="D81" s="82"/>
+      <c r="E81" s="83"/>
+      <c r="F81" s="83"/>
+      <c r="G81" s="84"/>
+      <c r="H81" s="85" t="str">
         <f t="shared" ref="H81" si="163">IF(O82&gt;P81,"!","")</f>
         <v/>
       </c>
@@ -41280,11 +41286,11 @@
     </row>
     <row r="82" spans="2:226" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="70"/>
-      <c r="D82" s="130"/>
-      <c r="E82" s="131"/>
-      <c r="F82" s="131"/>
-      <c r="G82" s="132"/>
-      <c r="H82" s="133"/>
+      <c r="D82" s="86"/>
+      <c r="E82" s="87"/>
+      <c r="F82" s="87"/>
+      <c r="G82" s="88"/>
+      <c r="H82" s="89"/>
       <c r="I82" s="47" t="s">
         <v>1</v>
       </c>
@@ -41523,136 +41529,139 @@
     </row>
   </sheetData>
   <mergeCells count="287">
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="Q7:Z7"/>
+    <mergeCell ref="P7:P11"/>
+    <mergeCell ref="O7:O11"/>
+    <mergeCell ref="N7:N11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="Q8:Z8"/>
+    <mergeCell ref="Q9:Z9"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="AA7:AJ7"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AU7:BD7"/>
+    <mergeCell ref="BE7:BN7"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="DC7:DL7"/>
+    <mergeCell ref="DM7:DV7"/>
+    <mergeCell ref="AJ4:AR4"/>
+    <mergeCell ref="AJ5:AR5"/>
+    <mergeCell ref="AU5:BE5"/>
+    <mergeCell ref="AU4:BE4"/>
+    <mergeCell ref="BY9:CH9"/>
+    <mergeCell ref="CI9:CR9"/>
+    <mergeCell ref="CS9:DB9"/>
+    <mergeCell ref="DC9:DL9"/>
+    <mergeCell ref="DM9:DV9"/>
+    <mergeCell ref="DW9:EF9"/>
+    <mergeCell ref="DM8:DV8"/>
+    <mergeCell ref="DW8:EF8"/>
+    <mergeCell ref="EG8:EP8"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="AK9:AT9"/>
+    <mergeCell ref="AU9:BD9"/>
+    <mergeCell ref="BE9:BN9"/>
+    <mergeCell ref="BO9:BX9"/>
+    <mergeCell ref="EG9:EP9"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="FK7:FT7"/>
+    <mergeCell ref="FU7:GD7"/>
+    <mergeCell ref="GE7:GN7"/>
+    <mergeCell ref="GO7:GX7"/>
+    <mergeCell ref="GY7:HH7"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="BO7:BX7"/>
+    <mergeCell ref="EG7:EP7"/>
+    <mergeCell ref="AA8:AJ8"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AU8:BD8"/>
+    <mergeCell ref="BE8:BN8"/>
+    <mergeCell ref="BO8:BX8"/>
+    <mergeCell ref="BY8:CH8"/>
+    <mergeCell ref="CI8:CR8"/>
+    <mergeCell ref="CS8:DB8"/>
+    <mergeCell ref="DC8:DL8"/>
+    <mergeCell ref="BY7:CH7"/>
+    <mergeCell ref="CI7:CR7"/>
+    <mergeCell ref="CS7:DB7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="DW7:EF7"/>
+    <mergeCell ref="AA9:AJ9"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="F41:F42"/>
@@ -41677,139 +41686,136 @@
     <mergeCell ref="EQ8:EZ8"/>
     <mergeCell ref="EQ9:EZ9"/>
     <mergeCell ref="FA7:FJ7"/>
-    <mergeCell ref="FK7:FT7"/>
-    <mergeCell ref="FU7:GD7"/>
-    <mergeCell ref="GE7:GN7"/>
-    <mergeCell ref="GO7:GX7"/>
-    <mergeCell ref="GY7:HH7"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="BO7:BX7"/>
-    <mergeCell ref="EG7:EP7"/>
-    <mergeCell ref="AA8:AJ8"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AU8:BD8"/>
-    <mergeCell ref="BE8:BN8"/>
-    <mergeCell ref="BO8:BX8"/>
-    <mergeCell ref="BY8:CH8"/>
-    <mergeCell ref="CI8:CR8"/>
-    <mergeCell ref="CS8:DB8"/>
-    <mergeCell ref="DC8:DL8"/>
-    <mergeCell ref="BY7:CH7"/>
-    <mergeCell ref="CI7:CR7"/>
-    <mergeCell ref="CS7:DB7"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="DW7:EF7"/>
-    <mergeCell ref="AA9:AJ9"/>
-    <mergeCell ref="AK9:AT9"/>
-    <mergeCell ref="AU9:BD9"/>
-    <mergeCell ref="BE9:BN9"/>
-    <mergeCell ref="BO9:BX9"/>
-    <mergeCell ref="EG9:EP9"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="BY9:CH9"/>
-    <mergeCell ref="CI9:CR9"/>
-    <mergeCell ref="CS9:DB9"/>
-    <mergeCell ref="DC9:DL9"/>
-    <mergeCell ref="DM9:DV9"/>
-    <mergeCell ref="DW9:EF9"/>
-    <mergeCell ref="DM8:DV8"/>
-    <mergeCell ref="DW8:EF8"/>
-    <mergeCell ref="EG8:EP8"/>
-    <mergeCell ref="AA7:AJ7"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AU7:BD7"/>
-    <mergeCell ref="BE7:BN7"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="DC7:DL7"/>
-    <mergeCell ref="DM7:DV7"/>
-    <mergeCell ref="AJ4:AR4"/>
-    <mergeCell ref="AJ5:AR5"/>
-    <mergeCell ref="AU5:BE5"/>
-    <mergeCell ref="AU4:BE4"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="Q7:Z7"/>
-    <mergeCell ref="P7:P11"/>
-    <mergeCell ref="O7:O11"/>
-    <mergeCell ref="N7:N11"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="Q8:Z8"/>
-    <mergeCell ref="Q9:Z9"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7:HR8">
     <cfRule type="expression" dxfId="2730" priority="3963">
@@ -52029,9 +52035,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52258,27 +52267,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
-    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -52304,9 +52301,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
+    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Documentation et changement de configuration
</commit_message>
<xml_diff>
--- a/Planification/Gantt_Modele.xlsx
+++ b/Planification/Gantt_Modele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git\tpi-impero-v2\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1251FAB5-1F18-4DFB-8529-6E29545B22FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C4515D-AA09-4BC1-A9F1-9976335E464E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8430" tabRatio="445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="101">
   <si>
     <t>Prévu, non terminé</t>
   </si>
@@ -939,43 +939,70 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -984,10 +1011,7 @@
     <xf numFmtId="14" fontId="1" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -996,41 +1020,8 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1053,53 +1044,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -27022,8 +27022,8 @@
   </sheetPr>
   <dimension ref="A1:HR82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="AA49" sqref="AA49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="DD71" sqref="DD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27069,11 +27069,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="Q3" s="112">
+      <c r="Q3" s="109">
         <f>MAX(K13:K163)</f>
         <v>64</v>
       </c>
-      <c r="R3" s="113"/>
+      <c r="R3" s="110"/>
       <c r="S3" s="28" t="s">
         <v>23</v>
       </c>
@@ -27098,11 +27098,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="Q4" s="114">
+      <c r="Q4" s="111">
         <f>MAX(L13:L163)-L12</f>
-        <v>38</v>
-      </c>
-      <c r="R4" s="115"/>
+        <v>42</v>
+      </c>
+      <c r="R4" s="112"/>
       <c r="S4" s="29" t="s">
         <v>24</v>
       </c>
@@ -27119,31 +27119,31 @@
       <c r="AD4" s="26"/>
       <c r="AE4" s="27"/>
       <c r="AI4" s="66"/>
-      <c r="AJ4" s="118" t="s">
+      <c r="AJ4" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="AK4" s="118"/>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="118"/>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118"/>
+      <c r="AK4" s="115"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="118" t="s">
+      <c r="AU4" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118"/>
-      <c r="AZ4" s="118"/>
-      <c r="BA4" s="118"/>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="115"/>
+      <c r="BC4" s="115"/>
+      <c r="BD4" s="115"/>
+      <c r="BE4" s="115"/>
       <c r="BG4" s="8"/>
       <c r="BH4" s="3" t="s">
         <v>2</v>
@@ -27155,11 +27155,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="Q5" s="116">
+      <c r="Q5" s="113">
         <f>MAX(M13:M163)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="117"/>
+      <c r="R5" s="114"/>
       <c r="S5" s="30" t="s">
         <v>25</v>
       </c>
@@ -27176,31 +27176,31 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="12"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="118" t="s">
+      <c r="AJ5" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="118"/>
-      <c r="AM5" s="118"/>
-      <c r="AN5" s="118"/>
-      <c r="AO5" s="118"/>
-      <c r="AP5" s="118"/>
-      <c r="AQ5" s="118"/>
-      <c r="AR5" s="118"/>
+      <c r="AK5" s="115"/>
+      <c r="AL5" s="115"/>
+      <c r="AM5" s="115"/>
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="115"/>
       <c r="AT5" s="65"/>
-      <c r="AU5" s="118" t="s">
+      <c r="AU5" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="118"/>
-      <c r="AZ5" s="118"/>
-      <c r="BA5" s="118"/>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="115"/>
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="115"/>
+      <c r="BA5" s="115"/>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="115"/>
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="115"/>
     </row>
     <row r="6" spans="1:226" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3"/>
@@ -27211,889 +27211,889 @@
     </row>
     <row r="7" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B7" s="69"/>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="108" t="s">
+      <c r="F7" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="108" t="s">
+      <c r="G7" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="108" t="s">
+      <c r="H7" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="108"/>
-      <c r="J7" s="105" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="132" t="s">
+      <c r="K7" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="127" t="s">
+      <c r="L7" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="127" t="s">
+      <c r="M7" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="127" t="s">
+      <c r="N7" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="127" t="s">
+      <c r="O7" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="124" t="s">
+      <c r="P7" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="123">
+      <c r="Q7" s="95">
         <v>1</v>
       </c>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="91"/>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="101"/>
-      <c r="AA7" s="90">
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="96"/>
+      <c r="V7" s="96"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="97"/>
+      <c r="AA7" s="108">
         <v>2</v>
       </c>
-      <c r="AB7" s="91"/>
-      <c r="AC7" s="91"/>
-      <c r="AD7" s="91"/>
-      <c r="AE7" s="91"/>
-      <c r="AF7" s="91"/>
-      <c r="AG7" s="91"/>
-      <c r="AH7" s="91"/>
-      <c r="AI7" s="91"/>
-      <c r="AJ7" s="101"/>
-      <c r="AK7" s="90">
+      <c r="AB7" s="96"/>
+      <c r="AC7" s="96"/>
+      <c r="AD7" s="96"/>
+      <c r="AE7" s="96"/>
+      <c r="AF7" s="96"/>
+      <c r="AG7" s="96"/>
+      <c r="AH7" s="96"/>
+      <c r="AI7" s="96"/>
+      <c r="AJ7" s="97"/>
+      <c r="AK7" s="108">
         <v>3</v>
       </c>
-      <c r="AL7" s="91"/>
-      <c r="AM7" s="91"/>
-      <c r="AN7" s="91"/>
-      <c r="AO7" s="91"/>
-      <c r="AP7" s="91"/>
-      <c r="AQ7" s="91"/>
-      <c r="AR7" s="91"/>
-      <c r="AS7" s="91"/>
-      <c r="AT7" s="101"/>
-      <c r="AU7" s="90">
+      <c r="AL7" s="96"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="96"/>
+      <c r="AO7" s="96"/>
+      <c r="AP7" s="96"/>
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="96"/>
+      <c r="AS7" s="96"/>
+      <c r="AT7" s="97"/>
+      <c r="AU7" s="108">
         <v>4</v>
       </c>
-      <c r="AV7" s="91"/>
-      <c r="AW7" s="91"/>
-      <c r="AX7" s="91"/>
-      <c r="AY7" s="91"/>
-      <c r="AZ7" s="91"/>
-      <c r="BA7" s="91"/>
-      <c r="BB7" s="91"/>
-      <c r="BC7" s="91"/>
-      <c r="BD7" s="101"/>
-      <c r="BE7" s="90">
+      <c r="AV7" s="96"/>
+      <c r="AW7" s="96"/>
+      <c r="AX7" s="96"/>
+      <c r="AY7" s="96"/>
+      <c r="AZ7" s="96"/>
+      <c r="BA7" s="96"/>
+      <c r="BB7" s="96"/>
+      <c r="BC7" s="96"/>
+      <c r="BD7" s="97"/>
+      <c r="BE7" s="108">
         <v>5</v>
       </c>
-      <c r="BF7" s="91"/>
-      <c r="BG7" s="91"/>
-      <c r="BH7" s="91"/>
-      <c r="BI7" s="91"/>
-      <c r="BJ7" s="91"/>
-      <c r="BK7" s="91"/>
-      <c r="BL7" s="91"/>
-      <c r="BM7" s="91"/>
-      <c r="BN7" s="101"/>
-      <c r="BO7" s="90">
+      <c r="BF7" s="96"/>
+      <c r="BG7" s="96"/>
+      <c r="BH7" s="96"/>
+      <c r="BI7" s="96"/>
+      <c r="BJ7" s="96"/>
+      <c r="BK7" s="96"/>
+      <c r="BL7" s="96"/>
+      <c r="BM7" s="96"/>
+      <c r="BN7" s="97"/>
+      <c r="BO7" s="108">
         <v>6</v>
       </c>
-      <c r="BP7" s="91"/>
-      <c r="BQ7" s="91"/>
-      <c r="BR7" s="91"/>
-      <c r="BS7" s="91"/>
-      <c r="BT7" s="91"/>
-      <c r="BU7" s="91"/>
-      <c r="BV7" s="91"/>
-      <c r="BW7" s="91"/>
-      <c r="BX7" s="101"/>
-      <c r="BY7" s="90">
+      <c r="BP7" s="96"/>
+      <c r="BQ7" s="96"/>
+      <c r="BR7" s="96"/>
+      <c r="BS7" s="96"/>
+      <c r="BT7" s="96"/>
+      <c r="BU7" s="96"/>
+      <c r="BV7" s="96"/>
+      <c r="BW7" s="96"/>
+      <c r="BX7" s="97"/>
+      <c r="BY7" s="108">
         <v>7</v>
       </c>
-      <c r="BZ7" s="91"/>
-      <c r="CA7" s="91"/>
-      <c r="CB7" s="91"/>
-      <c r="CC7" s="91"/>
-      <c r="CD7" s="91"/>
-      <c r="CE7" s="91"/>
-      <c r="CF7" s="91"/>
-      <c r="CG7" s="91"/>
-      <c r="CH7" s="101"/>
-      <c r="CI7" s="90">
+      <c r="BZ7" s="96"/>
+      <c r="CA7" s="96"/>
+      <c r="CB7" s="96"/>
+      <c r="CC7" s="96"/>
+      <c r="CD7" s="96"/>
+      <c r="CE7" s="96"/>
+      <c r="CF7" s="96"/>
+      <c r="CG7" s="96"/>
+      <c r="CH7" s="97"/>
+      <c r="CI7" s="108">
         <v>8</v>
       </c>
-      <c r="CJ7" s="91"/>
-      <c r="CK7" s="91"/>
-      <c r="CL7" s="91"/>
-      <c r="CM7" s="91"/>
-      <c r="CN7" s="91"/>
-      <c r="CO7" s="91"/>
-      <c r="CP7" s="91"/>
-      <c r="CQ7" s="91"/>
-      <c r="CR7" s="101"/>
-      <c r="CS7" s="90">
+      <c r="CJ7" s="96"/>
+      <c r="CK7" s="96"/>
+      <c r="CL7" s="96"/>
+      <c r="CM7" s="96"/>
+      <c r="CN7" s="96"/>
+      <c r="CO7" s="96"/>
+      <c r="CP7" s="96"/>
+      <c r="CQ7" s="96"/>
+      <c r="CR7" s="97"/>
+      <c r="CS7" s="108">
         <v>9</v>
       </c>
-      <c r="CT7" s="91"/>
-      <c r="CU7" s="91"/>
-      <c r="CV7" s="91"/>
-      <c r="CW7" s="91"/>
-      <c r="CX7" s="91"/>
-      <c r="CY7" s="91"/>
-      <c r="CZ7" s="91"/>
-      <c r="DA7" s="91"/>
-      <c r="DB7" s="91"/>
-      <c r="DC7" s="90">
+      <c r="CT7" s="96"/>
+      <c r="CU7" s="96"/>
+      <c r="CV7" s="96"/>
+      <c r="CW7" s="96"/>
+      <c r="CX7" s="96"/>
+      <c r="CY7" s="96"/>
+      <c r="CZ7" s="96"/>
+      <c r="DA7" s="96"/>
+      <c r="DB7" s="96"/>
+      <c r="DC7" s="108">
         <v>10</v>
       </c>
-      <c r="DD7" s="91"/>
-      <c r="DE7" s="91"/>
-      <c r="DF7" s="91"/>
-      <c r="DG7" s="91"/>
-      <c r="DH7" s="91"/>
-      <c r="DI7" s="91"/>
-      <c r="DJ7" s="91"/>
-      <c r="DK7" s="91"/>
-      <c r="DL7" s="101"/>
-      <c r="DM7" s="90">
+      <c r="DD7" s="96"/>
+      <c r="DE7" s="96"/>
+      <c r="DF7" s="96"/>
+      <c r="DG7" s="96"/>
+      <c r="DH7" s="96"/>
+      <c r="DI7" s="96"/>
+      <c r="DJ7" s="96"/>
+      <c r="DK7" s="96"/>
+      <c r="DL7" s="97"/>
+      <c r="DM7" s="108">
         <v>11</v>
       </c>
-      <c r="DN7" s="91"/>
-      <c r="DO7" s="91"/>
-      <c r="DP7" s="91"/>
-      <c r="DQ7" s="91"/>
-      <c r="DR7" s="91"/>
-      <c r="DS7" s="91"/>
-      <c r="DT7" s="91"/>
-      <c r="DU7" s="91"/>
-      <c r="DV7" s="101"/>
-      <c r="DW7" s="90">
+      <c r="DN7" s="96"/>
+      <c r="DO7" s="96"/>
+      <c r="DP7" s="96"/>
+      <c r="DQ7" s="96"/>
+      <c r="DR7" s="96"/>
+      <c r="DS7" s="96"/>
+      <c r="DT7" s="96"/>
+      <c r="DU7" s="96"/>
+      <c r="DV7" s="97"/>
+      <c r="DW7" s="108">
         <v>12</v>
       </c>
-      <c r="DX7" s="91"/>
-      <c r="DY7" s="91"/>
-      <c r="DZ7" s="91"/>
-      <c r="EA7" s="91"/>
-      <c r="EB7" s="91"/>
-      <c r="EC7" s="91"/>
-      <c r="ED7" s="91"/>
-      <c r="EE7" s="91"/>
-      <c r="EF7" s="101"/>
-      <c r="EG7" s="90">
+      <c r="DX7" s="96"/>
+      <c r="DY7" s="96"/>
+      <c r="DZ7" s="96"/>
+      <c r="EA7" s="96"/>
+      <c r="EB7" s="96"/>
+      <c r="EC7" s="96"/>
+      <c r="ED7" s="96"/>
+      <c r="EE7" s="96"/>
+      <c r="EF7" s="97"/>
+      <c r="EG7" s="108">
         <v>13</v>
       </c>
-      <c r="EH7" s="91"/>
-      <c r="EI7" s="91"/>
-      <c r="EJ7" s="91"/>
-      <c r="EK7" s="91"/>
-      <c r="EL7" s="91"/>
-      <c r="EM7" s="91"/>
-      <c r="EN7" s="91"/>
-      <c r="EO7" s="91"/>
-      <c r="EP7" s="92"/>
-      <c r="EQ7" s="91">
+      <c r="EH7" s="96"/>
+      <c r="EI7" s="96"/>
+      <c r="EJ7" s="96"/>
+      <c r="EK7" s="96"/>
+      <c r="EL7" s="96"/>
+      <c r="EM7" s="96"/>
+      <c r="EN7" s="96"/>
+      <c r="EO7" s="96"/>
+      <c r="EP7" s="126"/>
+      <c r="EQ7" s="96">
         <v>14</v>
       </c>
-      <c r="ER7" s="91"/>
-      <c r="ES7" s="91"/>
-      <c r="ET7" s="91"/>
-      <c r="EU7" s="91"/>
-      <c r="EV7" s="91"/>
-      <c r="EW7" s="91"/>
-      <c r="EX7" s="91"/>
-      <c r="EY7" s="91"/>
-      <c r="EZ7" s="101"/>
-      <c r="FA7" s="90">
+      <c r="ER7" s="96"/>
+      <c r="ES7" s="96"/>
+      <c r="ET7" s="96"/>
+      <c r="EU7" s="96"/>
+      <c r="EV7" s="96"/>
+      <c r="EW7" s="96"/>
+      <c r="EX7" s="96"/>
+      <c r="EY7" s="96"/>
+      <c r="EZ7" s="97"/>
+      <c r="FA7" s="108">
         <v>15</v>
       </c>
-      <c r="FB7" s="91"/>
-      <c r="FC7" s="91"/>
-      <c r="FD7" s="91"/>
-      <c r="FE7" s="91"/>
-      <c r="FF7" s="91"/>
-      <c r="FG7" s="91"/>
-      <c r="FH7" s="91"/>
-      <c r="FI7" s="91"/>
-      <c r="FJ7" s="101"/>
-      <c r="FK7" s="90">
+      <c r="FB7" s="96"/>
+      <c r="FC7" s="96"/>
+      <c r="FD7" s="96"/>
+      <c r="FE7" s="96"/>
+      <c r="FF7" s="96"/>
+      <c r="FG7" s="96"/>
+      <c r="FH7" s="96"/>
+      <c r="FI7" s="96"/>
+      <c r="FJ7" s="97"/>
+      <c r="FK7" s="108">
         <v>16</v>
       </c>
-      <c r="FL7" s="91"/>
-      <c r="FM7" s="91"/>
-      <c r="FN7" s="91"/>
-      <c r="FO7" s="91"/>
-      <c r="FP7" s="91"/>
-      <c r="FQ7" s="91"/>
-      <c r="FR7" s="91"/>
-      <c r="FS7" s="91"/>
-      <c r="FT7" s="101"/>
-      <c r="FU7" s="90">
+      <c r="FL7" s="96"/>
+      <c r="FM7" s="96"/>
+      <c r="FN7" s="96"/>
+      <c r="FO7" s="96"/>
+      <c r="FP7" s="96"/>
+      <c r="FQ7" s="96"/>
+      <c r="FR7" s="96"/>
+      <c r="FS7" s="96"/>
+      <c r="FT7" s="97"/>
+      <c r="FU7" s="108">
         <v>17</v>
       </c>
-      <c r="FV7" s="91"/>
-      <c r="FW7" s="91"/>
-      <c r="FX7" s="91"/>
-      <c r="FY7" s="91"/>
-      <c r="FZ7" s="91"/>
-      <c r="GA7" s="91"/>
-      <c r="GB7" s="91"/>
-      <c r="GC7" s="91"/>
-      <c r="GD7" s="101"/>
-      <c r="GE7" s="90">
+      <c r="FV7" s="96"/>
+      <c r="FW7" s="96"/>
+      <c r="FX7" s="96"/>
+      <c r="FY7" s="96"/>
+      <c r="FZ7" s="96"/>
+      <c r="GA7" s="96"/>
+      <c r="GB7" s="96"/>
+      <c r="GC7" s="96"/>
+      <c r="GD7" s="97"/>
+      <c r="GE7" s="108">
         <v>18</v>
       </c>
-      <c r="GF7" s="91"/>
-      <c r="GG7" s="91"/>
-      <c r="GH7" s="91"/>
-      <c r="GI7" s="91"/>
-      <c r="GJ7" s="91"/>
-      <c r="GK7" s="91"/>
-      <c r="GL7" s="91"/>
-      <c r="GM7" s="91"/>
-      <c r="GN7" s="101"/>
-      <c r="GO7" s="90">
+      <c r="GF7" s="96"/>
+      <c r="GG7" s="96"/>
+      <c r="GH7" s="96"/>
+      <c r="GI7" s="96"/>
+      <c r="GJ7" s="96"/>
+      <c r="GK7" s="96"/>
+      <c r="GL7" s="96"/>
+      <c r="GM7" s="96"/>
+      <c r="GN7" s="97"/>
+      <c r="GO7" s="108">
         <v>19</v>
       </c>
-      <c r="GP7" s="91"/>
-      <c r="GQ7" s="91"/>
-      <c r="GR7" s="91"/>
-      <c r="GS7" s="91"/>
-      <c r="GT7" s="91"/>
-      <c r="GU7" s="91"/>
-      <c r="GV7" s="91"/>
-      <c r="GW7" s="91"/>
-      <c r="GX7" s="101"/>
-      <c r="GY7" s="90">
+      <c r="GP7" s="96"/>
+      <c r="GQ7" s="96"/>
+      <c r="GR7" s="96"/>
+      <c r="GS7" s="96"/>
+      <c r="GT7" s="96"/>
+      <c r="GU7" s="96"/>
+      <c r="GV7" s="96"/>
+      <c r="GW7" s="96"/>
+      <c r="GX7" s="97"/>
+      <c r="GY7" s="108">
         <v>20</v>
       </c>
-      <c r="GZ7" s="91"/>
-      <c r="HA7" s="91"/>
-      <c r="HB7" s="91"/>
-      <c r="HC7" s="91"/>
-      <c r="HD7" s="91"/>
-      <c r="HE7" s="91"/>
-      <c r="HF7" s="91"/>
-      <c r="HG7" s="91"/>
-      <c r="HH7" s="101"/>
-      <c r="HI7" s="90">
+      <c r="GZ7" s="96"/>
+      <c r="HA7" s="96"/>
+      <c r="HB7" s="96"/>
+      <c r="HC7" s="96"/>
+      <c r="HD7" s="96"/>
+      <c r="HE7" s="96"/>
+      <c r="HF7" s="96"/>
+      <c r="HG7" s="96"/>
+      <c r="HH7" s="97"/>
+      <c r="HI7" s="108">
         <v>21</v>
       </c>
-      <c r="HJ7" s="91"/>
-      <c r="HK7" s="91"/>
-      <c r="HL7" s="91"/>
-      <c r="HM7" s="91"/>
-      <c r="HN7" s="91"/>
-      <c r="HO7" s="91"/>
-      <c r="HP7" s="91"/>
-      <c r="HQ7" s="91"/>
-      <c r="HR7" s="92"/>
+      <c r="HJ7" s="96"/>
+      <c r="HK7" s="96"/>
+      <c r="HL7" s="96"/>
+      <c r="HM7" s="96"/>
+      <c r="HN7" s="96"/>
+      <c r="HO7" s="96"/>
+      <c r="HP7" s="96"/>
+      <c r="HQ7" s="96"/>
+      <c r="HR7" s="126"/>
     </row>
     <row r="8" spans="1:226" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="128"/>
-      <c r="M8" s="128"/>
-      <c r="N8" s="128"/>
-      <c r="O8" s="128"/>
-      <c r="P8" s="125"/>
-      <c r="Q8" s="130">
+      <c r="D8" s="124"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="102">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],Q7),"")</f>
         <v>45040</v>
       </c>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
-      <c r="U8" s="94"/>
-      <c r="V8" s="94"/>
-      <c r="W8" s="94"/>
-      <c r="X8" s="94"/>
-      <c r="Y8" s="94"/>
-      <c r="Z8" s="95"/>
-      <c r="AA8" s="93">
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="103"/>
+      <c r="Z8" s="104"/>
+      <c r="AA8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AA7),"")</f>
         <v>45041</v>
       </c>
-      <c r="AB8" s="94"/>
-      <c r="AC8" s="94"/>
-      <c r="AD8" s="94"/>
-      <c r="AE8" s="94"/>
-      <c r="AF8" s="94"/>
-      <c r="AG8" s="94"/>
-      <c r="AH8" s="94"/>
-      <c r="AI8" s="94"/>
-      <c r="AJ8" s="95"/>
-      <c r="AK8" s="93">
+      <c r="AB8" s="103"/>
+      <c r="AC8" s="103"/>
+      <c r="AD8" s="103"/>
+      <c r="AE8" s="103"/>
+      <c r="AF8" s="103"/>
+      <c r="AG8" s="103"/>
+      <c r="AH8" s="103"/>
+      <c r="AI8" s="103"/>
+      <c r="AJ8" s="104"/>
+      <c r="AK8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AK7),"")</f>
         <v>45042</v>
       </c>
-      <c r="AL8" s="94"/>
-      <c r="AM8" s="94"/>
-      <c r="AN8" s="94"/>
-      <c r="AO8" s="94"/>
-      <c r="AP8" s="94"/>
-      <c r="AQ8" s="94"/>
-      <c r="AR8" s="94"/>
-      <c r="AS8" s="94"/>
-      <c r="AT8" s="95"/>
-      <c r="AU8" s="93">
+      <c r="AL8" s="103"/>
+      <c r="AM8" s="103"/>
+      <c r="AN8" s="103"/>
+      <c r="AO8" s="103"/>
+      <c r="AP8" s="103"/>
+      <c r="AQ8" s="103"/>
+      <c r="AR8" s="103"/>
+      <c r="AS8" s="103"/>
+      <c r="AT8" s="104"/>
+      <c r="AU8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],AU7),"")</f>
         <v>45048</v>
       </c>
-      <c r="AV8" s="94"/>
-      <c r="AW8" s="94"/>
-      <c r="AX8" s="94"/>
-      <c r="AY8" s="94"/>
-      <c r="AZ8" s="94"/>
-      <c r="BA8" s="94"/>
-      <c r="BB8" s="94"/>
-      <c r="BC8" s="94"/>
-      <c r="BD8" s="95"/>
-      <c r="BE8" s="93">
+      <c r="AV8" s="103"/>
+      <c r="AW8" s="103"/>
+      <c r="AX8" s="103"/>
+      <c r="AY8" s="103"/>
+      <c r="AZ8" s="103"/>
+      <c r="BA8" s="103"/>
+      <c r="BB8" s="103"/>
+      <c r="BC8" s="103"/>
+      <c r="BD8" s="104"/>
+      <c r="BE8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BE7),"")</f>
         <v>45049</v>
       </c>
-      <c r="BF8" s="94"/>
-      <c r="BG8" s="94"/>
-      <c r="BH8" s="94"/>
-      <c r="BI8" s="94"/>
-      <c r="BJ8" s="94"/>
-      <c r="BK8" s="94"/>
-      <c r="BL8" s="94"/>
-      <c r="BM8" s="94"/>
-      <c r="BN8" s="95"/>
-      <c r="BO8" s="93">
+      <c r="BF8" s="103"/>
+      <c r="BG8" s="103"/>
+      <c r="BH8" s="103"/>
+      <c r="BI8" s="103"/>
+      <c r="BJ8" s="103"/>
+      <c r="BK8" s="103"/>
+      <c r="BL8" s="103"/>
+      <c r="BM8" s="103"/>
+      <c r="BN8" s="104"/>
+      <c r="BO8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BO7),"")</f>
         <v>45054</v>
       </c>
-      <c r="BP8" s="94"/>
-      <c r="BQ8" s="94"/>
-      <c r="BR8" s="94"/>
-      <c r="BS8" s="94"/>
-      <c r="BT8" s="94"/>
-      <c r="BU8" s="94"/>
-      <c r="BV8" s="94"/>
-      <c r="BW8" s="94"/>
-      <c r="BX8" s="95"/>
-      <c r="BY8" s="93">
+      <c r="BP8" s="103"/>
+      <c r="BQ8" s="103"/>
+      <c r="BR8" s="103"/>
+      <c r="BS8" s="103"/>
+      <c r="BT8" s="103"/>
+      <c r="BU8" s="103"/>
+      <c r="BV8" s="103"/>
+      <c r="BW8" s="103"/>
+      <c r="BX8" s="104"/>
+      <c r="BY8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],BY7),"")</f>
         <v>45055</v>
       </c>
-      <c r="BZ8" s="94"/>
-      <c r="CA8" s="94"/>
-      <c r="CB8" s="94"/>
-      <c r="CC8" s="94"/>
-      <c r="CD8" s="94"/>
-      <c r="CE8" s="94"/>
-      <c r="CF8" s="94"/>
-      <c r="CG8" s="94"/>
-      <c r="CH8" s="95"/>
-      <c r="CI8" s="93">
+      <c r="BZ8" s="103"/>
+      <c r="CA8" s="103"/>
+      <c r="CB8" s="103"/>
+      <c r="CC8" s="103"/>
+      <c r="CD8" s="103"/>
+      <c r="CE8" s="103"/>
+      <c r="CF8" s="103"/>
+      <c r="CG8" s="103"/>
+      <c r="CH8" s="104"/>
+      <c r="CI8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CI7),"")</f>
         <v>45056</v>
       </c>
-      <c r="CJ8" s="94"/>
-      <c r="CK8" s="94"/>
-      <c r="CL8" s="94"/>
-      <c r="CM8" s="94"/>
-      <c r="CN8" s="94"/>
-      <c r="CO8" s="94"/>
-      <c r="CP8" s="94"/>
-      <c r="CQ8" s="94"/>
-      <c r="CR8" s="95"/>
-      <c r="CS8" s="93">
+      <c r="CJ8" s="103"/>
+      <c r="CK8" s="103"/>
+      <c r="CL8" s="103"/>
+      <c r="CM8" s="103"/>
+      <c r="CN8" s="103"/>
+      <c r="CO8" s="103"/>
+      <c r="CP8" s="103"/>
+      <c r="CQ8" s="103"/>
+      <c r="CR8" s="104"/>
+      <c r="CS8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],CS7),"")</f>
         <v>45061</v>
       </c>
-      <c r="CT8" s="94"/>
-      <c r="CU8" s="94"/>
-      <c r="CV8" s="94"/>
-      <c r="CW8" s="94"/>
-      <c r="CX8" s="94"/>
-      <c r="CY8" s="94"/>
-      <c r="CZ8" s="94"/>
-      <c r="DA8" s="94"/>
-      <c r="DB8" s="94"/>
-      <c r="DC8" s="93">
+      <c r="CT8" s="103"/>
+      <c r="CU8" s="103"/>
+      <c r="CV8" s="103"/>
+      <c r="CW8" s="103"/>
+      <c r="CX8" s="103"/>
+      <c r="CY8" s="103"/>
+      <c r="CZ8" s="103"/>
+      <c r="DA8" s="103"/>
+      <c r="DB8" s="103"/>
+      <c r="DC8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DC7),"")</f>
         <v>45062</v>
       </c>
-      <c r="DD8" s="94"/>
-      <c r="DE8" s="94"/>
-      <c r="DF8" s="94"/>
-      <c r="DG8" s="94"/>
-      <c r="DH8" s="94"/>
-      <c r="DI8" s="94"/>
-      <c r="DJ8" s="94"/>
-      <c r="DK8" s="94"/>
-      <c r="DL8" s="95"/>
-      <c r="DM8" s="93">
+      <c r="DD8" s="103"/>
+      <c r="DE8" s="103"/>
+      <c r="DF8" s="103"/>
+      <c r="DG8" s="103"/>
+      <c r="DH8" s="103"/>
+      <c r="DI8" s="103"/>
+      <c r="DJ8" s="103"/>
+      <c r="DK8" s="103"/>
+      <c r="DL8" s="104"/>
+      <c r="DM8" s="117">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DM7),"")</f>
         <v>45063</v>
       </c>
-      <c r="DN8" s="94"/>
-      <c r="DO8" s="94"/>
-      <c r="DP8" s="94"/>
-      <c r="DQ8" s="94"/>
-      <c r="DR8" s="94"/>
-      <c r="DS8" s="94"/>
-      <c r="DT8" s="94"/>
-      <c r="DU8" s="94"/>
-      <c r="DV8" s="95"/>
-      <c r="DW8" s="93" t="str">
+      <c r="DN8" s="103"/>
+      <c r="DO8" s="103"/>
+      <c r="DP8" s="103"/>
+      <c r="DQ8" s="103"/>
+      <c r="DR8" s="103"/>
+      <c r="DS8" s="103"/>
+      <c r="DT8" s="103"/>
+      <c r="DU8" s="103"/>
+      <c r="DV8" s="104"/>
+      <c r="DW8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],DW7),"")</f>
         <v/>
       </c>
-      <c r="DX8" s="94"/>
-      <c r="DY8" s="94"/>
-      <c r="DZ8" s="94"/>
-      <c r="EA8" s="94"/>
-      <c r="EB8" s="94"/>
-      <c r="EC8" s="94"/>
-      <c r="ED8" s="94"/>
-      <c r="EE8" s="94"/>
-      <c r="EF8" s="95"/>
-      <c r="EG8" s="93" t="str">
+      <c r="DX8" s="103"/>
+      <c r="DY8" s="103"/>
+      <c r="DZ8" s="103"/>
+      <c r="EA8" s="103"/>
+      <c r="EB8" s="103"/>
+      <c r="EC8" s="103"/>
+      <c r="ED8" s="103"/>
+      <c r="EE8" s="103"/>
+      <c r="EF8" s="104"/>
+      <c r="EG8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EG7),"")</f>
         <v/>
       </c>
-      <c r="EH8" s="94"/>
-      <c r="EI8" s="94"/>
-      <c r="EJ8" s="94"/>
-      <c r="EK8" s="94"/>
-      <c r="EL8" s="94"/>
-      <c r="EM8" s="94"/>
-      <c r="EN8" s="94"/>
-      <c r="EO8" s="94"/>
-      <c r="EP8" s="96"/>
-      <c r="EQ8" s="94" t="str">
+      <c r="EH8" s="103"/>
+      <c r="EI8" s="103"/>
+      <c r="EJ8" s="103"/>
+      <c r="EK8" s="103"/>
+      <c r="EL8" s="103"/>
+      <c r="EM8" s="103"/>
+      <c r="EN8" s="103"/>
+      <c r="EO8" s="103"/>
+      <c r="EP8" s="118"/>
+      <c r="EQ8" s="103" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],EQ7),"")</f>
         <v/>
       </c>
-      <c r="ER8" s="94"/>
-      <c r="ES8" s="94"/>
-      <c r="ET8" s="94"/>
-      <c r="EU8" s="94"/>
-      <c r="EV8" s="94"/>
-      <c r="EW8" s="94"/>
-      <c r="EX8" s="94"/>
-      <c r="EY8" s="94"/>
-      <c r="EZ8" s="95"/>
-      <c r="FA8" s="93" t="str">
+      <c r="ER8" s="103"/>
+      <c r="ES8" s="103"/>
+      <c r="ET8" s="103"/>
+      <c r="EU8" s="103"/>
+      <c r="EV8" s="103"/>
+      <c r="EW8" s="103"/>
+      <c r="EX8" s="103"/>
+      <c r="EY8" s="103"/>
+      <c r="EZ8" s="104"/>
+      <c r="FA8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FA7),"")</f>
         <v/>
       </c>
-      <c r="FB8" s="94"/>
-      <c r="FC8" s="94"/>
-      <c r="FD8" s="94"/>
-      <c r="FE8" s="94"/>
-      <c r="FF8" s="94"/>
-      <c r="FG8" s="94"/>
-      <c r="FH8" s="94"/>
-      <c r="FI8" s="94"/>
-      <c r="FJ8" s="95"/>
-      <c r="FK8" s="93" t="str">
+      <c r="FB8" s="103"/>
+      <c r="FC8" s="103"/>
+      <c r="FD8" s="103"/>
+      <c r="FE8" s="103"/>
+      <c r="FF8" s="103"/>
+      <c r="FG8" s="103"/>
+      <c r="FH8" s="103"/>
+      <c r="FI8" s="103"/>
+      <c r="FJ8" s="104"/>
+      <c r="FK8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FK7),"")</f>
         <v/>
       </c>
-      <c r="FL8" s="94"/>
-      <c r="FM8" s="94"/>
-      <c r="FN8" s="94"/>
-      <c r="FO8" s="94"/>
-      <c r="FP8" s="94"/>
-      <c r="FQ8" s="94"/>
-      <c r="FR8" s="94"/>
-      <c r="FS8" s="94"/>
-      <c r="FT8" s="95"/>
-      <c r="FU8" s="93" t="str">
+      <c r="FL8" s="103"/>
+      <c r="FM8" s="103"/>
+      <c r="FN8" s="103"/>
+      <c r="FO8" s="103"/>
+      <c r="FP8" s="103"/>
+      <c r="FQ8" s="103"/>
+      <c r="FR8" s="103"/>
+      <c r="FS8" s="103"/>
+      <c r="FT8" s="104"/>
+      <c r="FU8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],FU7),"")</f>
         <v/>
       </c>
-      <c r="FV8" s="94"/>
-      <c r="FW8" s="94"/>
-      <c r="FX8" s="94"/>
-      <c r="FY8" s="94"/>
-      <c r="FZ8" s="94"/>
-      <c r="GA8" s="94"/>
-      <c r="GB8" s="94"/>
-      <c r="GC8" s="94"/>
-      <c r="GD8" s="95"/>
-      <c r="GE8" s="93" t="str">
+      <c r="FV8" s="103"/>
+      <c r="FW8" s="103"/>
+      <c r="FX8" s="103"/>
+      <c r="FY8" s="103"/>
+      <c r="FZ8" s="103"/>
+      <c r="GA8" s="103"/>
+      <c r="GB8" s="103"/>
+      <c r="GC8" s="103"/>
+      <c r="GD8" s="104"/>
+      <c r="GE8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GE7),"")</f>
         <v/>
       </c>
-      <c r="GF8" s="94"/>
-      <c r="GG8" s="94"/>
-      <c r="GH8" s="94"/>
-      <c r="GI8" s="94"/>
-      <c r="GJ8" s="94"/>
-      <c r="GK8" s="94"/>
-      <c r="GL8" s="94"/>
-      <c r="GM8" s="94"/>
-      <c r="GN8" s="95"/>
-      <c r="GO8" s="93" t="str">
+      <c r="GF8" s="103"/>
+      <c r="GG8" s="103"/>
+      <c r="GH8" s="103"/>
+      <c r="GI8" s="103"/>
+      <c r="GJ8" s="103"/>
+      <c r="GK8" s="103"/>
+      <c r="GL8" s="103"/>
+      <c r="GM8" s="103"/>
+      <c r="GN8" s="104"/>
+      <c r="GO8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GO7),"")</f>
         <v/>
       </c>
-      <c r="GP8" s="94"/>
-      <c r="GQ8" s="94"/>
-      <c r="GR8" s="94"/>
-      <c r="GS8" s="94"/>
-      <c r="GT8" s="94"/>
-      <c r="GU8" s="94"/>
-      <c r="GV8" s="94"/>
-      <c r="GW8" s="94"/>
-      <c r="GX8" s="95"/>
-      <c r="GY8" s="93" t="str">
+      <c r="GP8" s="103"/>
+      <c r="GQ8" s="103"/>
+      <c r="GR8" s="103"/>
+      <c r="GS8" s="103"/>
+      <c r="GT8" s="103"/>
+      <c r="GU8" s="103"/>
+      <c r="GV8" s="103"/>
+      <c r="GW8" s="103"/>
+      <c r="GX8" s="104"/>
+      <c r="GY8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],GY7),"")</f>
         <v/>
       </c>
-      <c r="GZ8" s="94"/>
-      <c r="HA8" s="94"/>
-      <c r="HB8" s="94"/>
-      <c r="HC8" s="94"/>
-      <c r="HD8" s="94"/>
-      <c r="HE8" s="94"/>
-      <c r="HF8" s="94"/>
-      <c r="HG8" s="94"/>
-      <c r="HH8" s="95"/>
-      <c r="HI8" s="93" t="str">
+      <c r="GZ8" s="103"/>
+      <c r="HA8" s="103"/>
+      <c r="HB8" s="103"/>
+      <c r="HC8" s="103"/>
+      <c r="HD8" s="103"/>
+      <c r="HE8" s="103"/>
+      <c r="HF8" s="103"/>
+      <c r="HG8" s="103"/>
+      <c r="HH8" s="104"/>
+      <c r="HI8" s="117" t="str">
         <f>IFERROR(SMALL(TabDates[[Date TPI]:[Date TPI]],HI7),"")</f>
         <v/>
       </c>
-      <c r="HJ8" s="94"/>
-      <c r="HK8" s="94"/>
-      <c r="HL8" s="94"/>
-      <c r="HM8" s="94"/>
-      <c r="HN8" s="94"/>
-      <c r="HO8" s="94"/>
-      <c r="HP8" s="94"/>
-      <c r="HQ8" s="94"/>
-      <c r="HR8" s="96"/>
+      <c r="HJ8" s="103"/>
+      <c r="HK8" s="103"/>
+      <c r="HL8" s="103"/>
+      <c r="HM8" s="103"/>
+      <c r="HN8" s="103"/>
+      <c r="HO8" s="103"/>
+      <c r="HP8" s="103"/>
+      <c r="HQ8" s="103"/>
+      <c r="HR8" s="118"/>
     </row>
     <row r="9" spans="1:226" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="133"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="131">
+      <c r="D9" s="124"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="99"/>
+      <c r="Q9" s="105">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(Q8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="98"/>
-      <c r="Z9" s="99"/>
-      <c r="AA9" s="97" t="str">
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="106"/>
+      <c r="V9" s="106"/>
+      <c r="W9" s="106"/>
+      <c r="X9" s="106"/>
+      <c r="Y9" s="106"/>
+      <c r="Z9" s="107"/>
+      <c r="AA9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L1] Connexion</v>
       </c>
-      <c r="AB9" s="98"/>
-      <c r="AC9" s="98"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="98"/>
-      <c r="AF9" s="98"/>
-      <c r="AG9" s="98"/>
-      <c r="AH9" s="98"/>
-      <c r="AI9" s="98"/>
-      <c r="AJ9" s="99"/>
-      <c r="AK9" s="97">
+      <c r="AB9" s="106"/>
+      <c r="AC9" s="106"/>
+      <c r="AD9" s="106"/>
+      <c r="AE9" s="106"/>
+      <c r="AF9" s="106"/>
+      <c r="AG9" s="106"/>
+      <c r="AH9" s="106"/>
+      <c r="AI9" s="106"/>
+      <c r="AJ9" s="107"/>
+      <c r="AK9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="98"/>
-      <c r="AM9" s="98"/>
-      <c r="AN9" s="98"/>
-      <c r="AO9" s="98"/>
-      <c r="AP9" s="98"/>
-      <c r="AQ9" s="98"/>
-      <c r="AR9" s="98"/>
-      <c r="AS9" s="98"/>
-      <c r="AT9" s="99"/>
-      <c r="AU9" s="97" t="str">
+      <c r="AL9" s="106"/>
+      <c r="AM9" s="106"/>
+      <c r="AN9" s="106"/>
+      <c r="AO9" s="106"/>
+      <c r="AP9" s="106"/>
+      <c r="AQ9" s="106"/>
+      <c r="AR9" s="106"/>
+      <c r="AS9" s="106"/>
+      <c r="AT9" s="107"/>
+      <c r="AU9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(AU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L2] Affichage Professeur</v>
       </c>
-      <c r="AV9" s="98"/>
-      <c r="AW9" s="98"/>
-      <c r="AX9" s="98"/>
-      <c r="AY9" s="98"/>
-      <c r="AZ9" s="98"/>
-      <c r="BA9" s="98"/>
-      <c r="BB9" s="98"/>
-      <c r="BC9" s="98"/>
-      <c r="BD9" s="99"/>
-      <c r="BE9" s="97">
+      <c r="AV9" s="106"/>
+      <c r="AW9" s="106"/>
+      <c r="AX9" s="106"/>
+      <c r="AY9" s="106"/>
+      <c r="AZ9" s="106"/>
+      <c r="BA9" s="106"/>
+      <c r="BB9" s="106"/>
+      <c r="BC9" s="106"/>
+      <c r="BD9" s="107"/>
+      <c r="BE9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BF9" s="98"/>
-      <c r="BG9" s="98"/>
-      <c r="BH9" s="98"/>
-      <c r="BI9" s="98"/>
-      <c r="BJ9" s="98"/>
-      <c r="BK9" s="98"/>
-      <c r="BL9" s="98"/>
-      <c r="BM9" s="98"/>
-      <c r="BN9" s="99"/>
-      <c r="BO9" s="97" t="str">
+      <c r="BF9" s="106"/>
+      <c r="BG9" s="106"/>
+      <c r="BH9" s="106"/>
+      <c r="BI9" s="106"/>
+      <c r="BJ9" s="106"/>
+      <c r="BK9" s="106"/>
+      <c r="BL9" s="106"/>
+      <c r="BM9" s="106"/>
+      <c r="BN9" s="107"/>
+      <c r="BO9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L3] Historique</v>
       </c>
-      <c r="BP9" s="98"/>
-      <c r="BQ9" s="98"/>
-      <c r="BR9" s="98"/>
-      <c r="BS9" s="98"/>
-      <c r="BT9" s="98"/>
-      <c r="BU9" s="98"/>
-      <c r="BV9" s="98"/>
-      <c r="BW9" s="98"/>
-      <c r="BX9" s="99"/>
-      <c r="BY9" s="97">
+      <c r="BP9" s="106"/>
+      <c r="BQ9" s="106"/>
+      <c r="BR9" s="106"/>
+      <c r="BS9" s="106"/>
+      <c r="BT9" s="106"/>
+      <c r="BU9" s="106"/>
+      <c r="BV9" s="106"/>
+      <c r="BW9" s="106"/>
+      <c r="BX9" s="107"/>
+      <c r="BY9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(BY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="BZ9" s="98"/>
-      <c r="CA9" s="98"/>
-      <c r="CB9" s="98"/>
-      <c r="CC9" s="98"/>
-      <c r="CD9" s="98"/>
-      <c r="CE9" s="98"/>
-      <c r="CF9" s="98"/>
-      <c r="CG9" s="98"/>
-      <c r="CH9" s="99"/>
-      <c r="CI9" s="97" t="str">
+      <c r="BZ9" s="106"/>
+      <c r="CA9" s="106"/>
+      <c r="CB9" s="106"/>
+      <c r="CC9" s="106"/>
+      <c r="CD9" s="106"/>
+      <c r="CE9" s="106"/>
+      <c r="CF9" s="106"/>
+      <c r="CG9" s="106"/>
+      <c r="CH9" s="107"/>
+      <c r="CI9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L4] Filtrage</v>
       </c>
-      <c r="CJ9" s="98"/>
-      <c r="CK9" s="98"/>
-      <c r="CL9" s="98"/>
-      <c r="CM9" s="98"/>
-      <c r="CN9" s="98"/>
-      <c r="CO9" s="98"/>
-      <c r="CP9" s="98"/>
-      <c r="CQ9" s="98"/>
-      <c r="CR9" s="99"/>
-      <c r="CS9" s="97" t="str">
+      <c r="CJ9" s="106"/>
+      <c r="CK9" s="106"/>
+      <c r="CL9" s="106"/>
+      <c r="CM9" s="106"/>
+      <c r="CN9" s="106"/>
+      <c r="CO9" s="106"/>
+      <c r="CP9" s="106"/>
+      <c r="CQ9" s="106"/>
+      <c r="CR9" s="107"/>
+      <c r="CS9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(CS8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L5] Streaming multicast</v>
       </c>
-      <c r="CT9" s="98"/>
-      <c r="CU9" s="98"/>
-      <c r="CV9" s="98"/>
-      <c r="CW9" s="98"/>
-      <c r="CX9" s="98"/>
-      <c r="CY9" s="98"/>
-      <c r="CZ9" s="98"/>
-      <c r="DA9" s="98"/>
-      <c r="DB9" s="98"/>
-      <c r="DC9" s="97">
+      <c r="CT9" s="106"/>
+      <c r="CU9" s="106"/>
+      <c r="CV9" s="106"/>
+      <c r="CW9" s="106"/>
+      <c r="CX9" s="106"/>
+      <c r="CY9" s="106"/>
+      <c r="CZ9" s="106"/>
+      <c r="DA9" s="106"/>
+      <c r="DB9" s="106"/>
+      <c r="DC9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DC8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DD9" s="98"/>
-      <c r="DE9" s="98"/>
-      <c r="DF9" s="98"/>
-      <c r="DG9" s="98"/>
-      <c r="DH9" s="98"/>
-      <c r="DI9" s="98"/>
-      <c r="DJ9" s="98"/>
-      <c r="DK9" s="98"/>
-      <c r="DL9" s="99"/>
-      <c r="DM9" s="97" t="str">
+      <c r="DD9" s="106"/>
+      <c r="DE9" s="106"/>
+      <c r="DF9" s="106"/>
+      <c r="DG9" s="106"/>
+      <c r="DH9" s="106"/>
+      <c r="DI9" s="106"/>
+      <c r="DJ9" s="106"/>
+      <c r="DK9" s="106"/>
+      <c r="DL9" s="107"/>
+      <c r="DM9" s="116" t="str">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DM8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>[L6] Contrôle à distance</v>
       </c>
-      <c r="DN9" s="98"/>
-      <c r="DO9" s="98"/>
-      <c r="DP9" s="98"/>
-      <c r="DQ9" s="98"/>
-      <c r="DR9" s="98"/>
-      <c r="DS9" s="98"/>
-      <c r="DT9" s="98"/>
-      <c r="DU9" s="98"/>
-      <c r="DV9" s="99"/>
-      <c r="DW9" s="97">
+      <c r="DN9" s="106"/>
+      <c r="DO9" s="106"/>
+      <c r="DP9" s="106"/>
+      <c r="DQ9" s="106"/>
+      <c r="DR9" s="106"/>
+      <c r="DS9" s="106"/>
+      <c r="DT9" s="106"/>
+      <c r="DU9" s="106"/>
+      <c r="DV9" s="107"/>
+      <c r="DW9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(DW8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="DX9" s="98"/>
-      <c r="DY9" s="98"/>
-      <c r="DZ9" s="98"/>
-      <c r="EA9" s="98"/>
-      <c r="EB9" s="98"/>
-      <c r="EC9" s="98"/>
-      <c r="ED9" s="98"/>
-      <c r="EE9" s="98"/>
-      <c r="EF9" s="99"/>
-      <c r="EG9" s="97">
+      <c r="DX9" s="106"/>
+      <c r="DY9" s="106"/>
+      <c r="DZ9" s="106"/>
+      <c r="EA9" s="106"/>
+      <c r="EB9" s="106"/>
+      <c r="EC9" s="106"/>
+      <c r="ED9" s="106"/>
+      <c r="EE9" s="106"/>
+      <c r="EF9" s="107"/>
+      <c r="EG9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EG8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="EH9" s="98"/>
-      <c r="EI9" s="98"/>
-      <c r="EJ9" s="98"/>
-      <c r="EK9" s="98"/>
-      <c r="EL9" s="98"/>
-      <c r="EM9" s="98"/>
-      <c r="EN9" s="98"/>
-      <c r="EO9" s="98"/>
-      <c r="EP9" s="100"/>
-      <c r="EQ9" s="98">
+      <c r="EH9" s="106"/>
+      <c r="EI9" s="106"/>
+      <c r="EJ9" s="106"/>
+      <c r="EK9" s="106"/>
+      <c r="EL9" s="106"/>
+      <c r="EM9" s="106"/>
+      <c r="EN9" s="106"/>
+      <c r="EO9" s="106"/>
+      <c r="EP9" s="122"/>
+      <c r="EQ9" s="106">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(EQ8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="ER9" s="98"/>
-      <c r="ES9" s="98"/>
-      <c r="ET9" s="98"/>
-      <c r="EU9" s="98"/>
-      <c r="EV9" s="98"/>
-      <c r="EW9" s="98"/>
-      <c r="EX9" s="98"/>
-      <c r="EY9" s="98"/>
-      <c r="EZ9" s="99"/>
-      <c r="FA9" s="97">
+      <c r="ER9" s="106"/>
+      <c r="ES9" s="106"/>
+      <c r="ET9" s="106"/>
+      <c r="EU9" s="106"/>
+      <c r="EV9" s="106"/>
+      <c r="EW9" s="106"/>
+      <c r="EX9" s="106"/>
+      <c r="EY9" s="106"/>
+      <c r="EZ9" s="107"/>
+      <c r="FA9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FA8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FB9" s="98"/>
-      <c r="FC9" s="98"/>
-      <c r="FD9" s="98"/>
-      <c r="FE9" s="98"/>
-      <c r="FF9" s="98"/>
-      <c r="FG9" s="98"/>
-      <c r="FH9" s="98"/>
-      <c r="FI9" s="98"/>
-      <c r="FJ9" s="99"/>
-      <c r="FK9" s="97">
+      <c r="FB9" s="106"/>
+      <c r="FC9" s="106"/>
+      <c r="FD9" s="106"/>
+      <c r="FE9" s="106"/>
+      <c r="FF9" s="106"/>
+      <c r="FG9" s="106"/>
+      <c r="FH9" s="106"/>
+      <c r="FI9" s="106"/>
+      <c r="FJ9" s="107"/>
+      <c r="FK9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FK8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FL9" s="98"/>
-      <c r="FM9" s="98"/>
-      <c r="FN9" s="98"/>
-      <c r="FO9" s="98"/>
-      <c r="FP9" s="98"/>
-      <c r="FQ9" s="98"/>
-      <c r="FR9" s="98"/>
-      <c r="FS9" s="98"/>
-      <c r="FT9" s="99"/>
-      <c r="FU9" s="97">
+      <c r="FL9" s="106"/>
+      <c r="FM9" s="106"/>
+      <c r="FN9" s="106"/>
+      <c r="FO9" s="106"/>
+      <c r="FP9" s="106"/>
+      <c r="FQ9" s="106"/>
+      <c r="FR9" s="106"/>
+      <c r="FS9" s="106"/>
+      <c r="FT9" s="107"/>
+      <c r="FU9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(FU8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="FV9" s="98"/>
-      <c r="FW9" s="98"/>
-      <c r="FX9" s="98"/>
-      <c r="FY9" s="98"/>
-      <c r="FZ9" s="98"/>
-      <c r="GA9" s="98"/>
-      <c r="GB9" s="98"/>
-      <c r="GC9" s="98"/>
-      <c r="GD9" s="99"/>
-      <c r="GE9" s="97">
+      <c r="FV9" s="106"/>
+      <c r="FW9" s="106"/>
+      <c r="FX9" s="106"/>
+      <c r="FY9" s="106"/>
+      <c r="FZ9" s="106"/>
+      <c r="GA9" s="106"/>
+      <c r="GB9" s="106"/>
+      <c r="GC9" s="106"/>
+      <c r="GD9" s="107"/>
+      <c r="GE9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GE8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GF9" s="98"/>
-      <c r="GG9" s="98"/>
-      <c r="GH9" s="98"/>
-      <c r="GI9" s="98"/>
-      <c r="GJ9" s="98"/>
-      <c r="GK9" s="98"/>
-      <c r="GL9" s="98"/>
-      <c r="GM9" s="98"/>
-      <c r="GN9" s="99"/>
-      <c r="GO9" s="97">
+      <c r="GF9" s="106"/>
+      <c r="GG9" s="106"/>
+      <c r="GH9" s="106"/>
+      <c r="GI9" s="106"/>
+      <c r="GJ9" s="106"/>
+      <c r="GK9" s="106"/>
+      <c r="GL9" s="106"/>
+      <c r="GM9" s="106"/>
+      <c r="GN9" s="107"/>
+      <c r="GO9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GO8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GP9" s="98"/>
-      <c r="GQ9" s="98"/>
-      <c r="GR9" s="98"/>
-      <c r="GS9" s="98"/>
-      <c r="GT9" s="98"/>
-      <c r="GU9" s="98"/>
-      <c r="GV9" s="98"/>
-      <c r="GW9" s="98"/>
-      <c r="GX9" s="99"/>
-      <c r="GY9" s="97">
+      <c r="GP9" s="106"/>
+      <c r="GQ9" s="106"/>
+      <c r="GR9" s="106"/>
+      <c r="GS9" s="106"/>
+      <c r="GT9" s="106"/>
+      <c r="GU9" s="106"/>
+      <c r="GV9" s="106"/>
+      <c r="GW9" s="106"/>
+      <c r="GX9" s="107"/>
+      <c r="GY9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(GY8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="GZ9" s="98"/>
-      <c r="HA9" s="98"/>
-      <c r="HB9" s="98"/>
-      <c r="HC9" s="98"/>
-      <c r="HD9" s="98"/>
-      <c r="HE9" s="98"/>
-      <c r="HF9" s="98"/>
-      <c r="HG9" s="98"/>
-      <c r="HH9" s="99"/>
-      <c r="HI9" s="97">
+      <c r="GZ9" s="106"/>
+      <c r="HA9" s="106"/>
+      <c r="HB9" s="106"/>
+      <c r="HC9" s="106"/>
+      <c r="HD9" s="106"/>
+      <c r="HE9" s="106"/>
+      <c r="HF9" s="106"/>
+      <c r="HG9" s="106"/>
+      <c r="HH9" s="107"/>
+      <c r="HI9" s="116">
         <f>INDEX(TabDates[[Livrables / infos]:[Livrables / infos]],MATCH(HI8,TabDates[[Date TPI]:[Date TPI]]))</f>
         <v>0</v>
       </c>
-      <c r="HJ9" s="98"/>
-      <c r="HK9" s="98"/>
-      <c r="HL9" s="98"/>
-      <c r="HM9" s="98"/>
-      <c r="HN9" s="98"/>
-      <c r="HO9" s="98"/>
-      <c r="HP9" s="98"/>
-      <c r="HQ9" s="98"/>
-      <c r="HR9" s="100"/>
+      <c r="HJ9" s="106"/>
+      <c r="HK9" s="106"/>
+      <c r="HL9" s="106"/>
+      <c r="HM9" s="106"/>
+      <c r="HN9" s="106"/>
+      <c r="HO9" s="106"/>
+      <c r="HP9" s="106"/>
+      <c r="HQ9" s="106"/>
+      <c r="HR9" s="122"/>
     </row>
     <row r="10" spans="1:226" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="133"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="125"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="99"/>
       <c r="Q10" s="5"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="20"/>
@@ -28139,19 +28139,19 @@
       <c r="A11" s="68"/>
       <c r="B11" s="5"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
-      <c r="O11" s="129"/>
-      <c r="P11" s="126"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="100"/>
       <c r="Q11" s="51">
         <v>0</v>
       </c>
@@ -29648,17 +29648,17 @@
       </c>
     </row>
     <row r="13" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="111" t="s">
+      <c r="D13" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="83"/>
-      <c r="G13" s="84" t="s">
+      <c r="E13" s="101"/>
+      <c r="G13" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="85" t="str">
+      <c r="H13" s="119" t="str">
         <f>IF(O14&gt;P13,"!","")</f>
         <v>!</v>
       </c>
@@ -29764,11 +29764,11 @@
       <c r="HR13" s="4"/>
     </row>
     <row r="14" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="83"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="85"/>
+      <c r="B14" s="134"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="101"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="119"/>
       <c r="I14" s="45" t="s">
         <v>1</v>
       </c>
@@ -30020,22 +30020,22 @@
       <c r="HR14" s="31"/>
     </row>
     <row r="15" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="83" t="s">
+      <c r="E15" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="83">
+      <c r="F15" s="101">
         <v>1</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="85" t="str">
+      <c r="H15" s="119" t="str">
         <f t="shared" ref="H15" si="4">IF(O16&gt;P15,"!","")</f>
         <v/>
       </c>
@@ -30106,12 +30106,12 @@
       <c r="HR15" s="4"/>
     </row>
     <row r="16" spans="1:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="81"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="85"/>
+      <c r="B16" s="134"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="119"/>
       <c r="I16" s="45" t="s">
         <v>1</v>
       </c>
@@ -30351,20 +30351,20 @@
       <c r="HR16" s="31"/>
     </row>
     <row r="17" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83">
+      <c r="E17" s="101"/>
+      <c r="F17" s="101">
         <v>1</v>
       </c>
-      <c r="G17" s="84" t="s">
+      <c r="G17" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="85" t="str">
+      <c r="H17" s="119" t="str">
         <f t="shared" ref="H17" si="7">IF(O18&gt;P17,"!","")</f>
         <v/>
       </c>
@@ -30436,12 +30436,12 @@
       <c r="HR17" s="4"/>
     </row>
     <row r="18" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="85"/>
+      <c r="B18" s="134"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="119"/>
       <c r="I18" s="45" t="s">
         <v>1</v>
       </c>
@@ -30683,22 +30683,22 @@
       <c r="HR18" s="31"/>
     </row>
     <row r="19" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="111" t="s">
+      <c r="D19" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E19" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="83">
+      <c r="F19" s="101">
         <v>1</v>
       </c>
-      <c r="G19" s="84" t="s">
+      <c r="G19" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="85" t="str">
+      <c r="H19" s="119" t="str">
         <f t="shared" ref="H19" si="10">IF(O20&gt;P19,"!","")</f>
         <v/>
       </c>
@@ -30782,12 +30782,12 @@
       <c r="HR19" s="4"/>
     </row>
     <row r="20" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="81"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="85"/>
+      <c r="B20" s="134"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="119"/>
       <c r="I20" s="45" t="s">
         <v>1</v>
       </c>
@@ -31031,20 +31031,20 @@
       <c r="HR20" s="31"/>
     </row>
     <row r="21" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83">
+      <c r="E21" s="101"/>
+      <c r="F21" s="101">
         <v>1</v>
       </c>
-      <c r="G21" s="84" t="s">
+      <c r="G21" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="85" t="str">
+      <c r="H21" s="119" t="str">
         <f t="shared" ref="H21" si="12">IF(O22&gt;P21,"!","")</f>
         <v/>
       </c>
@@ -31118,12 +31118,12 @@
       <c r="HR21" s="4"/>
     </row>
     <row r="22" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="81"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="85"/>
+      <c r="B22" s="134"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="119"/>
       <c r="I22" s="45" t="s">
         <v>1</v>
       </c>
@@ -31361,20 +31361,20 @@
       <c r="HR22" s="31"/>
     </row>
     <row r="23" spans="2:226" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="111" t="s">
+      <c r="D23" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83">
+      <c r="E23" s="101"/>
+      <c r="F23" s="101">
         <v>1</v>
       </c>
-      <c r="G23" s="84" t="s">
+      <c r="G23" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="85" t="str">
+      <c r="H23" s="119" t="str">
         <f t="shared" ref="H23" si="15">IF(O24&gt;P23,"!","")</f>
         <v/>
       </c>
@@ -31445,12 +31445,12 @@
       <c r="HR23" s="4"/>
     </row>
     <row r="24" spans="2:226" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="81"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="85"/>
+      <c r="B24" s="134"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="119"/>
       <c r="I24" s="45" t="s">
         <v>1</v>
       </c>
@@ -31692,20 +31692,20 @@
       <c r="HR24" s="31"/>
     </row>
     <row r="25" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83">
+      <c r="E25" s="101"/>
+      <c r="F25" s="101">
         <v>1</v>
       </c>
-      <c r="G25" s="84" t="s">
+      <c r="G25" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="85" t="str">
+      <c r="H25" s="119" t="str">
         <f t="shared" ref="H25" si="18">IF(O26&gt;P25,"!","")</f>
         <v/>
       </c>
@@ -31775,12 +31775,12 @@
       <c r="HR25" s="4"/>
     </row>
     <row r="26" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="81"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="85"/>
+      <c r="B26" s="134"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="119"/>
       <c r="I26" s="45" t="s">
         <v>1</v>
       </c>
@@ -32020,20 +32020,20 @@
       <c r="HR26" s="31"/>
     </row>
     <row r="27" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="111" t="s">
+      <c r="D27" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83">
+      <c r="E27" s="101"/>
+      <c r="F27" s="101">
         <v>2</v>
       </c>
-      <c r="G27" s="84" t="s">
+      <c r="G27" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="85" t="str">
+      <c r="H27" s="119" t="str">
         <f t="shared" ref="H27" si="22">IF(O28&gt;P27,"!","")</f>
         <v/>
       </c>
@@ -32114,12 +32114,12 @@
       <c r="HR27" s="4"/>
     </row>
     <row r="28" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="81"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="85"/>
+      <c r="B28" s="134"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="119"/>
       <c r="I28" s="45" t="s">
         <v>1</v>
       </c>
@@ -32359,22 +32359,22 @@
       <c r="HR28" s="31"/>
     </row>
     <row r="29" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="83" t="s">
+      <c r="E29" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="83">
+      <c r="F29" s="101">
         <v>2</v>
       </c>
-      <c r="G29" s="84" t="s">
+      <c r="G29" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="85" t="str">
+      <c r="H29" s="119" t="str">
         <f t="shared" ref="H29" si="26">IF(O30&gt;P29,"!","")</f>
         <v>!</v>
       </c>
@@ -32454,12 +32454,12 @@
       <c r="HR29" s="4"/>
     </row>
     <row r="30" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="81"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="B30" s="134"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="119"/>
       <c r="I30" s="45" t="s">
         <v>1</v>
       </c>
@@ -32715,22 +32715,22 @@
       <c r="HR30" s="31"/>
     </row>
     <row r="31" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="82" t="s">
+      <c r="D31" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="83" t="s">
+      <c r="E31" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="83">
+      <c r="F31" s="101">
         <v>2</v>
       </c>
-      <c r="G31" s="84" t="s">
+      <c r="G31" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="85" t="str">
+      <c r="H31" s="119" t="str">
         <f t="shared" ref="H31" si="30">IF(O32&gt;P31,"!","")</f>
         <v/>
       </c>
@@ -32802,12 +32802,12 @@
       <c r="HR31" s="4"/>
     </row>
     <row r="32" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="81"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="85"/>
+      <c r="B32" s="134"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="119"/>
       <c r="I32" s="45" t="s">
         <v>1</v>
       </c>
@@ -33049,22 +33049,22 @@
       <c r="HR32" s="31"/>
     </row>
     <row r="33" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="134" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="82" t="s">
+      <c r="D33" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="83" t="s">
+      <c r="E33" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="83">
+      <c r="F33" s="101">
         <v>2</v>
       </c>
-      <c r="G33" s="84" t="s">
+      <c r="G33" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="85" t="str">
+      <c r="H33" s="119" t="str">
         <f t="shared" ref="H33" si="34">IF(O34&gt;P33,"!","")</f>
         <v/>
       </c>
@@ -33140,12 +33140,12 @@
       <c r="HR33" s="4"/>
     </row>
     <row r="34" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="81"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="84"/>
-      <c r="H34" s="85"/>
+      <c r="B34" s="134"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="45" t="s">
         <v>1</v>
       </c>
@@ -33387,22 +33387,22 @@
       <c r="HR34" s="31"/>
     </row>
     <row r="35" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="81" t="s">
+      <c r="B35" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="83" t="s">
+      <c r="E35" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="83">
+      <c r="F35" s="101">
         <v>2</v>
       </c>
-      <c r="G35" s="84" t="s">
+      <c r="G35" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="85" t="str">
+      <c r="H35" s="119" t="str">
         <f t="shared" ref="H35" si="38">IF(O36&gt;P35,"!","")</f>
         <v/>
       </c>
@@ -33481,12 +33481,12 @@
       <c r="HR35" s="4"/>
     </row>
     <row r="36" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="81"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="85"/>
+      <c r="B36" s="134"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="119"/>
       <c r="I36" s="45" t="s">
         <v>1</v>
       </c>
@@ -33724,22 +33724,22 @@
       <c r="HR36" s="31"/>
     </row>
     <row r="37" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="81" t="s">
+      <c r="B37" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="121" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="83">
+      <c r="F37" s="101">
         <v>2</v>
       </c>
-      <c r="G37" s="84" t="s">
+      <c r="G37" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="85" t="str">
+      <c r="H37" s="119" t="str">
         <f t="shared" ref="H37" si="42">IF(O38&gt;P37,"!","")</f>
         <v/>
       </c>
@@ -33813,12 +33813,12 @@
       <c r="HR37" s="4"/>
     </row>
     <row r="38" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="81"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="84"/>
-      <c r="H38" s="85"/>
+      <c r="B38" s="134"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="101"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="119"/>
       <c r="I38" s="45" t="s">
         <v>1</v>
       </c>
@@ -34058,20 +34058,20 @@
       <c r="HR38" s="31"/>
     </row>
     <row r="39" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="81" t="s">
+      <c r="B39" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="82" t="s">
+      <c r="D39" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83">
+      <c r="E39" s="101"/>
+      <c r="F39" s="101">
         <v>3</v>
       </c>
-      <c r="G39" s="84" t="s">
+      <c r="G39" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="85" t="str">
+      <c r="H39" s="119" t="str">
         <f t="shared" ref="H39" si="46">IF(O40&gt;P39,"!","")</f>
         <v/>
       </c>
@@ -34152,12 +34152,12 @@
       <c r="HR39" s="4"/>
     </row>
     <row r="40" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="81"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="85"/>
+      <c r="B40" s="134"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="119"/>
       <c r="I40" s="45" t="s">
         <v>1</v>
       </c>
@@ -34405,20 +34405,20 @@
       <c r="HR40" s="31"/>
     </row>
     <row r="41" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="81" t="s">
+      <c r="B41" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="82" t="s">
+      <c r="D41" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83">
+      <c r="E41" s="101"/>
+      <c r="F41" s="101">
         <v>3</v>
       </c>
-      <c r="G41" s="84" t="s">
+      <c r="G41" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="85" t="str">
+      <c r="H41" s="119" t="str">
         <f t="shared" ref="H41" si="48">IF(O42&gt;P41,"!","")</f>
         <v/>
       </c>
@@ -34492,12 +34492,12 @@
       <c r="HR41" s="4"/>
     </row>
     <row r="42" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="81"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="83"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="84"/>
-      <c r="H42" s="85"/>
+      <c r="B42" s="134"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="101"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="119"/>
       <c r="I42" s="45" t="s">
         <v>1</v>
       </c>
@@ -34737,20 +34737,20 @@
       <c r="HR42" s="31"/>
     </row>
     <row r="43" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="81" t="s">
+      <c r="B43" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="83"/>
-      <c r="F43" s="83">
+      <c r="E43" s="101"/>
+      <c r="F43" s="101">
         <v>3</v>
       </c>
-      <c r="G43" s="84" t="s">
+      <c r="G43" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="85" t="str">
+      <c r="H43" s="119" t="str">
         <f t="shared" ref="H43" si="51">IF(O44&gt;P43,"!","")</f>
         <v/>
       </c>
@@ -34823,12 +34823,12 @@
       <c r="HR43" s="4"/>
     </row>
     <row r="44" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="81"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="83"/>
-      <c r="F44" s="83"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="85"/>
+      <c r="B44" s="134"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="101"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="45" t="s">
         <v>1</v>
       </c>
@@ -35070,20 +35070,20 @@
       <c r="HR44" s="31"/>
     </row>
     <row r="45" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="81" t="s">
+      <c r="B45" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="82" t="s">
+      <c r="D45" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="83"/>
-      <c r="F45" s="83">
+      <c r="E45" s="101"/>
+      <c r="F45" s="101">
         <v>3</v>
       </c>
-      <c r="G45" s="84" t="s">
+      <c r="G45" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="85" t="str">
+      <c r="H45" s="119" t="str">
         <f t="shared" ref="H45" si="57">IF(O46&gt;P45,"!","")</f>
         <v/>
       </c>
@@ -35156,12 +35156,12 @@
       <c r="HR45" s="4"/>
     </row>
     <row r="46" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="81"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="85"/>
+      <c r="B46" s="134"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="101"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="45" t="s">
         <v>1</v>
       </c>
@@ -35403,20 +35403,20 @@
       <c r="HR46" s="31"/>
     </row>
     <row r="47" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="81" t="s">
+      <c r="B47" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="82" t="s">
+      <c r="D47" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83">
+      <c r="E47" s="101"/>
+      <c r="F47" s="101">
         <v>3</v>
       </c>
-      <c r="G47" s="84" t="s">
+      <c r="G47" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="85" t="str">
+      <c r="H47" s="119" t="str">
         <f t="shared" ref="H47" si="62">IF(O48&gt;P47,"!","")</f>
         <v/>
       </c>
@@ -35486,12 +35486,12 @@
       <c r="HR47" s="4"/>
     </row>
     <row r="48" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="81"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="84"/>
-      <c r="H48" s="85"/>
+      <c r="B48" s="134"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="101"/>
+      <c r="F48" s="101"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="119"/>
       <c r="I48" s="45" t="s">
         <v>1</v>
       </c>
@@ -35733,20 +35733,20 @@
       <c r="HR48" s="31"/>
     </row>
     <row r="49" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="82" t="s">
+      <c r="D49" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83">
+      <c r="E49" s="101"/>
+      <c r="F49" s="101">
         <v>4</v>
       </c>
-      <c r="G49" s="84" t="s">
+      <c r="G49" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="85" t="str">
+      <c r="H49" s="119" t="str">
         <f t="shared" ref="H49" si="65">IF(O50&gt;P49,"!","")</f>
         <v/>
       </c>
@@ -35834,12 +35834,12 @@
       <c r="HR49" s="4"/>
     </row>
     <row r="50" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="81"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="85"/>
+      <c r="B50" s="134"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="101"/>
+      <c r="F50" s="101"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="119"/>
       <c r="I50" s="45" t="s">
         <v>1</v>
       </c>
@@ -36083,20 +36083,20 @@
       <c r="HR50" s="31"/>
     </row>
     <row r="51" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="81" t="s">
+      <c r="B51" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="82" t="s">
+      <c r="D51" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83">
+      <c r="E51" s="101"/>
+      <c r="F51" s="101">
         <v>4</v>
       </c>
-      <c r="G51" s="84" t="s">
+      <c r="G51" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="85" t="str">
+      <c r="H51" s="119" t="str">
         <f t="shared" ref="H51" si="71">IF(O52&gt;P51,"!","")</f>
         <v/>
       </c>
@@ -36173,12 +36173,12 @@
       <c r="HR51" s="4"/>
     </row>
     <row r="52" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="81"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="84"/>
-      <c r="H52" s="85"/>
+      <c r="B52" s="134"/>
+      <c r="D52" s="121"/>
+      <c r="E52" s="101"/>
+      <c r="F52" s="101"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="119"/>
       <c r="I52" s="45" t="s">
         <v>1</v>
       </c>
@@ -36422,20 +36422,20 @@
       <c r="HR52" s="31"/>
     </row>
     <row r="53" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="81" t="s">
+      <c r="B53" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="82" t="s">
+      <c r="D53" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="83"/>
-      <c r="F53" s="83">
+      <c r="E53" s="101"/>
+      <c r="F53" s="101">
         <v>4</v>
       </c>
-      <c r="G53" s="84" t="s">
+      <c r="G53" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H53" s="85" t="str">
+      <c r="H53" s="119" t="str">
         <f t="shared" ref="H53" si="77">IF(O54&gt;P53,"!","")</f>
         <v/>
       </c>
@@ -36515,12 +36515,12 @@
       <c r="HR53" s="4"/>
     </row>
     <row r="54" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="81"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="85"/>
+      <c r="B54" s="134"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="87"/>
+      <c r="H54" s="119"/>
       <c r="I54" s="45" t="s">
         <v>1</v>
       </c>
@@ -36760,22 +36760,22 @@
       <c r="HR54" s="31"/>
     </row>
     <row r="55" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="81" t="s">
+      <c r="B55" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="82" t="s">
+      <c r="D55" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="83" t="s">
+      <c r="E55" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="83">
+      <c r="F55" s="101">
         <v>4</v>
       </c>
-      <c r="G55" s="84" t="s">
+      <c r="G55" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H55" s="85" t="str">
+      <c r="H55" s="119" t="str">
         <f t="shared" ref="H55" si="83">IF(O56&gt;P55,"!","")</f>
         <v/>
       </c>
@@ -36858,12 +36858,12 @@
       <c r="HR55" s="4"/>
     </row>
     <row r="56" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="81"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="83"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="85"/>
+      <c r="B56" s="134"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="87"/>
+      <c r="H56" s="119"/>
       <c r="I56" s="45" t="s">
         <v>1</v>
       </c>
@@ -37105,22 +37105,22 @@
       <c r="HR56" s="31"/>
     </row>
     <row r="57" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="81" t="s">
+      <c r="B57" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="82" t="s">
+      <c r="D57" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="83" t="s">
+      <c r="E57" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="83">
+      <c r="F57" s="101">
         <v>4</v>
       </c>
-      <c r="G57" s="84" t="s">
+      <c r="G57" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H57" s="85" t="str">
+      <c r="H57" s="119" t="str">
         <f t="shared" ref="H57" si="89">IF(O58&gt;P57,"!","")</f>
         <v/>
       </c>
@@ -37191,12 +37191,12 @@
       <c r="HR57" s="4"/>
     </row>
     <row r="58" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="81"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="83"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="85"/>
+      <c r="B58" s="134"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="101"/>
+      <c r="F58" s="101"/>
+      <c r="G58" s="87"/>
+      <c r="H58" s="119"/>
       <c r="I58" s="45" t="s">
         <v>1</v>
       </c>
@@ -37440,20 +37440,20 @@
       <c r="HR58" s="31"/>
     </row>
     <row r="59" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="81" t="s">
+      <c r="B59" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="82" t="s">
+      <c r="D59" s="121" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="83"/>
-      <c r="F59" s="83">
+      <c r="E59" s="101"/>
+      <c r="F59" s="101">
         <v>5</v>
       </c>
-      <c r="G59" s="84" t="s">
+      <c r="G59" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="85" t="str">
+      <c r="H59" s="119" t="str">
         <f t="shared" ref="H59" si="95">IF(O60&gt;P59,"!","")</f>
         <v/>
       </c>
@@ -37527,12 +37527,12 @@
       <c r="HR59" s="4"/>
     </row>
     <row r="60" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="81"/>
-      <c r="D60" s="82"/>
-      <c r="E60" s="83"/>
-      <c r="F60" s="83"/>
-      <c r="G60" s="84"/>
-      <c r="H60" s="85"/>
+      <c r="B60" s="134"/>
+      <c r="D60" s="121"/>
+      <c r="E60" s="101"/>
+      <c r="F60" s="101"/>
+      <c r="G60" s="87"/>
+      <c r="H60" s="119"/>
       <c r="I60" s="45" t="s">
         <v>1</v>
       </c>
@@ -37772,20 +37772,20 @@
       <c r="HR60" s="31"/>
     </row>
     <row r="61" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="81" t="s">
+      <c r="B61" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="82" t="s">
+      <c r="D61" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="E61" s="83"/>
-      <c r="F61" s="83">
+      <c r="E61" s="101"/>
+      <c r="F61" s="101">
         <v>5</v>
       </c>
-      <c r="G61" s="84" t="s">
+      <c r="G61" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H61" s="85" t="str">
+      <c r="H61" s="119" t="str">
         <f t="shared" ref="H61" si="101">IF(O62&gt;P61,"!","")</f>
         <v/>
       </c>
@@ -37880,12 +37880,12 @@
       <c r="HR61" s="4"/>
     </row>
     <row r="62" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="81"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="84"/>
-      <c r="H62" s="85"/>
+      <c r="B62" s="134"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="101"/>
+      <c r="F62" s="101"/>
+      <c r="G62" s="87"/>
+      <c r="H62" s="119"/>
       <c r="I62" s="45" t="s">
         <v>1</v>
       </c>
@@ -38145,20 +38145,20 @@
       <c r="HR62" s="31"/>
     </row>
     <row r="63" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="81" t="s">
+      <c r="B63" s="134" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="82" t="s">
+      <c r="D63" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="83"/>
-      <c r="F63" s="83">
+      <c r="E63" s="101"/>
+      <c r="F63" s="101">
         <v>5</v>
       </c>
-      <c r="G63" s="84" t="s">
+      <c r="G63" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="H63" s="85" t="str">
+      <c r="H63" s="119" t="str">
         <f t="shared" ref="H63" si="107">IF(O64&gt;P63,"!","")</f>
         <v/>
       </c>
@@ -38243,12 +38243,12 @@
       <c r="HR63" s="4"/>
     </row>
     <row r="64" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="81"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="83"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="85"/>
+      <c r="B64" s="134"/>
+      <c r="D64" s="121"/>
+      <c r="E64" s="101"/>
+      <c r="F64" s="101"/>
+      <c r="G64" s="87"/>
+      <c r="H64" s="119"/>
       <c r="I64" s="45" t="s">
         <v>1</v>
       </c>
@@ -38502,18 +38502,18 @@
       <c r="HR64" s="31"/>
     </row>
     <row r="65" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="81" t="s">
+      <c r="B65" s="134" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="82" t="s">
+      <c r="D65" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="83"/>
-      <c r="F65" s="83">
+      <c r="E65" s="101"/>
+      <c r="F65" s="101">
         <v>6</v>
       </c>
-      <c r="G65" s="84"/>
-      <c r="H65" s="85" t="str">
+      <c r="G65" s="87"/>
+      <c r="H65" s="119" t="str">
         <f t="shared" ref="H65" si="113">IF(O66&gt;P65,"!","")</f>
         <v/>
       </c>
@@ -38591,23 +38591,23 @@
       <c r="HR65" s="4"/>
     </row>
     <row r="66" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="81"/>
-      <c r="D66" s="82"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="84"/>
-      <c r="H66" s="85"/>
+      <c r="B66" s="134"/>
+      <c r="D66" s="121"/>
+      <c r="E66" s="101"/>
+      <c r="F66" s="101"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="119"/>
       <c r="I66" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J66" s="46">
         <f>IF(D65="","",COUNTIF(Echéancier!$Q66:$EP66,"r"))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K66" s="14"/>
       <c r="L66" s="14">
         <f t="shared" ref="L66" si="116">IFERROR(L64+J66,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ref="M66" si="117">COUNTIF(Q66:EP66,"a")</f>
@@ -38619,7 +38619,7 @@
       </c>
       <c r="O66" s="14">
         <f>IFERROR(MATCH("ra",$Q66:$EP66,1),0)</f>
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="P66" s="14"/>
       <c r="Q66" s="23"/>
@@ -38712,10 +38712,18 @@
       <c r="CZ66" s="75"/>
       <c r="DA66" s="75"/>
       <c r="DB66" s="75"/>
-      <c r="DC66" s="25"/>
-      <c r="DD66" s="34"/>
-      <c r="DE66" s="34"/>
-      <c r="DF66" s="34"/>
+      <c r="DC66" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="DD66" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="DE66" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="DF66" s="34" t="s">
+        <v>27</v>
+      </c>
       <c r="DG66" s="34"/>
       <c r="DH66" s="34"/>
       <c r="DI66" s="34"/>
@@ -38834,20 +38842,20 @@
       <c r="HR66" s="31"/>
     </row>
     <row r="67" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="81" t="s">
+      <c r="B67" s="134" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="82" t="s">
+      <c r="D67" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="E67" s="83" t="s">
+      <c r="E67" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="F67" s="83">
+      <c r="F67" s="101">
         <v>6</v>
       </c>
-      <c r="G67" s="84"/>
-      <c r="H67" s="85" t="str">
+      <c r="G67" s="87"/>
+      <c r="H67" s="119" t="str">
         <f t="shared" ref="H67" si="119">IF(O68&gt;P67,"!","")</f>
         <v/>
       </c>
@@ -38942,12 +38950,12 @@
       <c r="HR67" s="4"/>
     </row>
     <row r="68" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="81"/>
-      <c r="D68" s="82"/>
-      <c r="E68" s="83"/>
-      <c r="F68" s="83"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="85"/>
+      <c r="B68" s="134"/>
+      <c r="D68" s="121"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="87"/>
+      <c r="H68" s="119"/>
       <c r="I68" s="45" t="s">
         <v>1</v>
       </c>
@@ -38958,7 +38966,7 @@
       <c r="K68" s="14"/>
       <c r="L68" s="14">
         <f t="shared" ref="L68" si="123">IFERROR(L66+J68,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M68" s="14">
         <f t="shared" ref="M68" si="124">COUNTIF(Q68:EP68,"a")</f>
@@ -39185,20 +39193,20 @@
       <c r="HR68" s="31"/>
     </row>
     <row r="69" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="81" t="s">
+      <c r="B69" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="82" t="s">
+      <c r="D69" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="83" t="s">
+      <c r="E69" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F69" s="83">
+      <c r="F69" s="101">
         <v>6</v>
       </c>
-      <c r="G69" s="84"/>
-      <c r="H69" s="85" t="str">
+      <c r="G69" s="87"/>
+      <c r="H69" s="119" t="str">
         <f t="shared" ref="H69" si="127">IF(O70&gt;P69,"!","")</f>
         <v/>
       </c>
@@ -39275,12 +39283,12 @@
       <c r="HR69" s="4"/>
     </row>
     <row r="70" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="81"/>
-      <c r="D70" s="82"/>
-      <c r="E70" s="83"/>
-      <c r="F70" s="83"/>
-      <c r="G70" s="84"/>
-      <c r="H70" s="85"/>
+      <c r="B70" s="134"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="101"/>
+      <c r="F70" s="101"/>
+      <c r="G70" s="87"/>
+      <c r="H70" s="119"/>
       <c r="I70" s="45" t="s">
         <v>1</v>
       </c>
@@ -39291,7 +39299,7 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f t="shared" ref="L70" si="130">IFERROR(L68+J70,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M70" s="14">
         <f t="shared" ref="M70" si="131">COUNTIF(Q70:EP70,"a")</f>
@@ -39518,20 +39526,20 @@
       <c r="HR70" s="31"/>
     </row>
     <row r="71" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="81" t="s">
+      <c r="B71" s="134" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="82" t="s">
+      <c r="D71" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="E71" s="83" t="s">
+      <c r="E71" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F71" s="83">
+      <c r="F71" s="101">
         <v>6</v>
       </c>
-      <c r="G71" s="84"/>
-      <c r="H71" s="85" t="str">
+      <c r="G71" s="87"/>
+      <c r="H71" s="119" t="str">
         <f t="shared" ref="H71" si="133">IF(O72&gt;P71,"!","")</f>
         <v/>
       </c>
@@ -39607,12 +39615,12 @@
       <c r="HR71" s="4"/>
     </row>
     <row r="72" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="81"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="83"/>
-      <c r="F72" s="83"/>
-      <c r="G72" s="84"/>
-      <c r="H72" s="85"/>
+      <c r="B72" s="134"/>
+      <c r="D72" s="121"/>
+      <c r="E72" s="101"/>
+      <c r="F72" s="101"/>
+      <c r="G72" s="87"/>
+      <c r="H72" s="119"/>
       <c r="I72" s="45" t="s">
         <v>1</v>
       </c>
@@ -39623,7 +39631,7 @@
       <c r="K72" s="14"/>
       <c r="L72" s="14">
         <f t="shared" ref="L72" si="136">IFERROR(L70+J72,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M72" s="14">
         <f t="shared" ref="M72" si="137">COUNTIF(Q72:EP72,"a")</f>
@@ -39939,13 +39947,13 @@
     </row>
     <row r="73" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="82" t="s">
+      <c r="D73" s="121" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="83"/>
-      <c r="F73" s="83"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="85" t="str">
+      <c r="E73" s="101"/>
+      <c r="F73" s="101"/>
+      <c r="G73" s="87"/>
+      <c r="H73" s="119" t="str">
         <f t="shared" ref="H73" si="139">IF(O74&gt;P73,"!","")</f>
         <v/>
       </c>
@@ -40013,11 +40021,11 @@
     </row>
     <row r="74" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="D74" s="82"/>
-      <c r="E74" s="83"/>
-      <c r="F74" s="83"/>
-      <c r="G74" s="84"/>
-      <c r="H74" s="85"/>
+      <c r="D74" s="121"/>
+      <c r="E74" s="101"/>
+      <c r="F74" s="101"/>
+      <c r="G74" s="87"/>
+      <c r="H74" s="119"/>
       <c r="I74" s="45" t="s">
         <v>1</v>
       </c>
@@ -40028,7 +40036,7 @@
       <c r="K74" s="14"/>
       <c r="L74" s="14">
         <f t="shared" ref="L74" si="142">IFERROR(L72+J74,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M74" s="14">
         <f t="shared" ref="M74" si="143">COUNTIF(Q74:EP74,"a")</f>
@@ -40137,8 +40145,8 @@
       <c r="DD74" s="75"/>
       <c r="DE74" s="75"/>
       <c r="DF74" s="75"/>
-      <c r="DG74" s="75"/>
-      <c r="DH74" s="75"/>
+      <c r="DG74" s="79"/>
+      <c r="DH74" s="79"/>
       <c r="DI74" s="75"/>
       <c r="DJ74" s="75"/>
       <c r="DK74" s="75"/>
@@ -40256,13 +40264,13 @@
     </row>
     <row r="75" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="82" t="s">
+      <c r="D75" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="83"/>
-      <c r="F75" s="83"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="85" t="str">
+      <c r="E75" s="101"/>
+      <c r="F75" s="101"/>
+      <c r="G75" s="87"/>
+      <c r="H75" s="119" t="str">
         <f t="shared" ref="H75" si="145">IF(O76&gt;P75,"!","")</f>
         <v/>
       </c>
@@ -40334,11 +40342,11 @@
     </row>
     <row r="76" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
-      <c r="D76" s="82"/>
-      <c r="E76" s="83"/>
-      <c r="F76" s="83"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="85"/>
+      <c r="D76" s="121"/>
+      <c r="E76" s="101"/>
+      <c r="F76" s="101"/>
+      <c r="G76" s="87"/>
+      <c r="H76" s="119"/>
       <c r="I76" s="45" t="s">
         <v>1</v>
       </c>
@@ -40349,7 +40357,7 @@
       <c r="K76" s="14"/>
       <c r="L76" s="14">
         <f t="shared" ref="L76" si="148">IFERROR(L74+J76,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M76" s="14">
         <f t="shared" ref="M76" si="149">COUNTIF(Q76:EP76,"a")</f>
@@ -40577,13 +40585,13 @@
     </row>
     <row r="77" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
-      <c r="D77" s="82" t="s">
+      <c r="D77" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="E77" s="83"/>
-      <c r="F77" s="83"/>
-      <c r="G77" s="84"/>
-      <c r="H77" s="85" t="str">
+      <c r="E77" s="101"/>
+      <c r="F77" s="101"/>
+      <c r="G77" s="87"/>
+      <c r="H77" s="119" t="str">
         <f t="shared" ref="H77" si="151">IF(O78&gt;P77,"!","")</f>
         <v/>
       </c>
@@ -40672,11 +40680,11 @@
     </row>
     <row r="78" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="82"/>
-      <c r="E78" s="83"/>
-      <c r="F78" s="83"/>
-      <c r="G78" s="84"/>
-      <c r="H78" s="85"/>
+      <c r="D78" s="121"/>
+      <c r="E78" s="101"/>
+      <c r="F78" s="101"/>
+      <c r="G78" s="87"/>
+      <c r="H78" s="119"/>
       <c r="I78" s="45" t="s">
         <v>1</v>
       </c>
@@ -40687,7 +40695,7 @@
       <c r="K78" s="14"/>
       <c r="L78" s="14">
         <f t="shared" ref="L78" si="154">IFERROR(L76+J78,0)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M78" s="14">
         <f t="shared" ref="M78" si="155">COUNTIF(Q78:EP78,"a")</f>
@@ -40915,11 +40923,11 @@
     </row>
     <row r="79" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="D79" s="82"/>
-      <c r="E79" s="83"/>
-      <c r="F79" s="83"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="85" t="str">
+      <c r="D79" s="121"/>
+      <c r="E79" s="101"/>
+      <c r="F79" s="101"/>
+      <c r="G79" s="87"/>
+      <c r="H79" s="119" t="str">
         <f t="shared" ref="H79" si="157">IF(O80&gt;P79,"!","")</f>
         <v/>
       </c>
@@ -40988,11 +40996,11 @@
     </row>
     <row r="80" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
-      <c r="D80" s="82"/>
-      <c r="E80" s="83"/>
-      <c r="F80" s="83"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="85"/>
+      <c r="D80" s="121"/>
+      <c r="E80" s="101"/>
+      <c r="F80" s="101"/>
+      <c r="G80" s="87"/>
+      <c r="H80" s="119"/>
       <c r="I80" s="45" t="s">
         <v>1</v>
       </c>
@@ -41231,11 +41239,11 @@
     </row>
     <row r="81" spans="2:226" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="D81" s="82"/>
-      <c r="E81" s="83"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="85" t="str">
+      <c r="D81" s="121"/>
+      <c r="E81" s="101"/>
+      <c r="F81" s="101"/>
+      <c r="G81" s="87"/>
+      <c r="H81" s="119" t="str">
         <f t="shared" ref="H81" si="163">IF(O82&gt;P81,"!","")</f>
         <v/>
       </c>
@@ -41304,11 +41312,11 @@
     </row>
     <row r="82" spans="2:226" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="70"/>
-      <c r="D82" s="86"/>
-      <c r="E82" s="87"/>
-      <c r="F82" s="87"/>
-      <c r="G82" s="88"/>
-      <c r="H82" s="89"/>
+      <c r="D82" s="130"/>
+      <c r="E82" s="131"/>
+      <c r="F82" s="131"/>
+      <c r="G82" s="132"/>
+      <c r="H82" s="133"/>
       <c r="I82" s="47" t="s">
         <v>1</v>
       </c>
@@ -41547,15 +41555,260 @@
     </row>
   </sheetData>
   <mergeCells count="287">
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="HI7:HR7"/>
+    <mergeCell ref="FA8:FJ8"/>
+    <mergeCell ref="FK8:FT8"/>
+    <mergeCell ref="FU8:GD8"/>
+    <mergeCell ref="GE8:GN8"/>
+    <mergeCell ref="GO8:GX8"/>
+    <mergeCell ref="GY8:HH8"/>
+    <mergeCell ref="HI8:HR8"/>
+    <mergeCell ref="FA9:FJ9"/>
+    <mergeCell ref="FK9:FT9"/>
+    <mergeCell ref="FU9:GD9"/>
+    <mergeCell ref="GE9:GN9"/>
+    <mergeCell ref="GO9:GX9"/>
+    <mergeCell ref="GY9:HH9"/>
+    <mergeCell ref="HI9:HR9"/>
+    <mergeCell ref="EQ7:EZ7"/>
+    <mergeCell ref="EQ8:EZ8"/>
+    <mergeCell ref="EQ9:EZ9"/>
+    <mergeCell ref="FA7:FJ7"/>
+    <mergeCell ref="FK7:FT7"/>
+    <mergeCell ref="FU7:GD7"/>
+    <mergeCell ref="GE7:GN7"/>
+    <mergeCell ref="GO7:GX7"/>
+    <mergeCell ref="GY7:HH7"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="BO7:BX7"/>
+    <mergeCell ref="EG7:EP7"/>
+    <mergeCell ref="AA8:AJ8"/>
+    <mergeCell ref="AK8:AT8"/>
+    <mergeCell ref="AU8:BD8"/>
+    <mergeCell ref="BE8:BN8"/>
+    <mergeCell ref="BO8:BX8"/>
+    <mergeCell ref="BY8:CH8"/>
+    <mergeCell ref="CI8:CR8"/>
+    <mergeCell ref="CS8:DB8"/>
+    <mergeCell ref="DC8:DL8"/>
+    <mergeCell ref="BY7:CH7"/>
+    <mergeCell ref="CI7:CR7"/>
+    <mergeCell ref="CS7:DB7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="DW7:EF7"/>
+    <mergeCell ref="AA9:AJ9"/>
+    <mergeCell ref="AK9:AT9"/>
+    <mergeCell ref="AU9:BD9"/>
+    <mergeCell ref="BE9:BN9"/>
+    <mergeCell ref="BO9:BX9"/>
+    <mergeCell ref="EG9:EP9"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="BY9:CH9"/>
+    <mergeCell ref="CI9:CR9"/>
+    <mergeCell ref="CS9:DB9"/>
+    <mergeCell ref="DC9:DL9"/>
+    <mergeCell ref="DM9:DV9"/>
+    <mergeCell ref="DW9:EF9"/>
+    <mergeCell ref="DM8:DV8"/>
+    <mergeCell ref="DW8:EF8"/>
+    <mergeCell ref="EG8:EP8"/>
+    <mergeCell ref="AA7:AJ7"/>
+    <mergeCell ref="AK7:AT7"/>
+    <mergeCell ref="AU7:BD7"/>
+    <mergeCell ref="BE7:BN7"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="DC7:DL7"/>
+    <mergeCell ref="DM7:DV7"/>
+    <mergeCell ref="AJ4:AR4"/>
+    <mergeCell ref="AJ5:AR5"/>
+    <mergeCell ref="AU5:BE5"/>
+    <mergeCell ref="AU4:BE4"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D19:D20"/>
@@ -41580,260 +41833,15 @@
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="AA7:AJ7"/>
-    <mergeCell ref="AK7:AT7"/>
-    <mergeCell ref="AU7:BD7"/>
-    <mergeCell ref="BE7:BN7"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="DC7:DL7"/>
-    <mergeCell ref="DM7:DV7"/>
-    <mergeCell ref="AJ4:AR4"/>
-    <mergeCell ref="AJ5:AR5"/>
-    <mergeCell ref="AU5:BE5"/>
-    <mergeCell ref="AU4:BE4"/>
-    <mergeCell ref="BY9:CH9"/>
-    <mergeCell ref="CI9:CR9"/>
-    <mergeCell ref="CS9:DB9"/>
-    <mergeCell ref="DC9:DL9"/>
-    <mergeCell ref="DM9:DV9"/>
-    <mergeCell ref="DW9:EF9"/>
-    <mergeCell ref="DM8:DV8"/>
-    <mergeCell ref="DW8:EF8"/>
-    <mergeCell ref="EG8:EP8"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="AK9:AT9"/>
-    <mergeCell ref="AU9:BD9"/>
-    <mergeCell ref="BE9:BN9"/>
-    <mergeCell ref="BO9:BX9"/>
-    <mergeCell ref="EG9:EP9"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="FK7:FT7"/>
-    <mergeCell ref="FU7:GD7"/>
-    <mergeCell ref="GE7:GN7"/>
-    <mergeCell ref="GO7:GX7"/>
-    <mergeCell ref="GY7:HH7"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="BO7:BX7"/>
-    <mergeCell ref="EG7:EP7"/>
-    <mergeCell ref="AA8:AJ8"/>
-    <mergeCell ref="AK8:AT8"/>
-    <mergeCell ref="AU8:BD8"/>
-    <mergeCell ref="BE8:BN8"/>
-    <mergeCell ref="BO8:BX8"/>
-    <mergeCell ref="BY8:CH8"/>
-    <mergeCell ref="CI8:CR8"/>
-    <mergeCell ref="CS8:DB8"/>
-    <mergeCell ref="DC8:DL8"/>
-    <mergeCell ref="BY7:CH7"/>
-    <mergeCell ref="CI7:CR7"/>
-    <mergeCell ref="CS7:DB7"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="DW7:EF7"/>
-    <mergeCell ref="AA9:AJ9"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="HI7:HR7"/>
-    <mergeCell ref="FA8:FJ8"/>
-    <mergeCell ref="FK8:FT8"/>
-    <mergeCell ref="FU8:GD8"/>
-    <mergeCell ref="GE8:GN8"/>
-    <mergeCell ref="GO8:GX8"/>
-    <mergeCell ref="GY8:HH8"/>
-    <mergeCell ref="HI8:HR8"/>
-    <mergeCell ref="FA9:FJ9"/>
-    <mergeCell ref="FK9:FT9"/>
-    <mergeCell ref="FU9:GD9"/>
-    <mergeCell ref="GE9:GN9"/>
-    <mergeCell ref="GO9:GX9"/>
-    <mergeCell ref="GY9:HH9"/>
-    <mergeCell ref="HI9:HR9"/>
-    <mergeCell ref="EQ7:EZ7"/>
-    <mergeCell ref="EQ8:EZ8"/>
-    <mergeCell ref="EQ9:EZ9"/>
-    <mergeCell ref="FA7:FJ7"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7:HR8">
     <cfRule type="expression" dxfId="2730" priority="3963">
@@ -52053,12 +52061,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52285,15 +52290,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
+    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -52319,18 +52336,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B985B041-1012-4541-AB08-AA1D47D3BF0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7FE3E6-312C-49C0-9315-4EA06ADA0F8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4ac6eee3-51d7-4451-8ac6-6ed436adb6f6"/>
-    <ds:schemaRef ds:uri="96810def-8b86-4bdd-a51c-5b227b1404e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>